<commit_message>
visualized llama, 4o, 4o-mini base results. good
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-management-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AD92E0-DA6C-2942-A052-8EB7874B4FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4506395-C32A-734C-9FC4-38D094235BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4840" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="5340" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="1" bestFit="1" customWidth="1"/>
@@ -546,7 +546,7 @@
       <c r="H1" s="8"/>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="4" t="s">
@@ -809,7 +809,7 @@
     <col min="1" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
       <c r="C1" s="10" t="s">
         <v>13</v>
@@ -826,7 +826,7 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
         <v>1</v>
       </c>
@@ -858,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0.84620399999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>9</v>
@@ -932,7 +932,7 @@
         <v>0.82469899999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -968,7 +968,7 @@
         <v>0.93776499999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -1004,7 +1004,7 @@
         <v>0.93646099999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
@@ -1040,7 +1040,7 @@
         <v>0.95829299999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>0.124471</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -1114,7 +1114,7 @@
         <v>0.122515</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -1150,7 +1150,7 @@
         <v>4.9528000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>1</v>
@@ -1186,7 +1186,7 @@
         <v>5.0831000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>2</v>
@@ -1222,7 +1222,7 @@
         <v>3.5841999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>2.9326000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="3" t="s">
         <v>9</v>
@@ -1296,7 +1296,7 @@
         <v>5.2786E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>0</v>
@@ -1332,7 +1332,7 @@
         <v>1.2708000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>1</v>
@@ -1368,7 +1368,7 @@
         <v>1.2708000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
@@ -1421,7 +1421,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1479,12 +1479,24 @@
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="C3" s="6">
+        <v>0.51629072681704202</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.10025062656641601</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.383458646616541</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.581453634085213</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.17794486215538799</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.24060150375939801</v>
+      </c>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1505,12 +1517,24 @@
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="C5" s="6">
+        <v>0.42857142857142799</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.5062656641604E-3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.56892230576441105</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.77443609022556303</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.22556390977443599</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1518,12 +1542,24 @@
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="C6" s="6">
+        <v>0.581453634085213</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5.0125313283208E-3</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.41353383458646598</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.95989974937343303</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2.00501253132832E-2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.00501253132832E-2</v>
+      </c>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1533,12 +1569,24 @@
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="C7" s="6">
+        <v>0.38847117794486202</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.7543859649122799E-2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.581453634085213</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.62406015037593898</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4.5112781954887202E-2</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.31578947368421001</v>
+      </c>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1559,12 +1607,24 @@
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="6">
+        <v>0.57644110275689198</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.2531328320802001E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.41102756892230502</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.81954887218045103</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.17794486215538799</v>
+      </c>
+      <c r="H9" s="6">
+        <v>2.5062656641604E-3</v>
+      </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1572,12 +1632,24 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="C10" s="6">
+        <v>0.77694235588972405</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.21052631578947301</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1.2531328320802001E-2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.907268170426065</v>
+      </c>
+      <c r="G10" s="6">
+        <v>8.7719298245614002E-2</v>
+      </c>
+      <c r="H10" s="6">
+        <v>5.0125313283208E-3</v>
+      </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated base results visualization
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-management-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4506395-C32A-734C-9FC4-38D094235BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5C20AB-2084-F040-BE19-8CBBBBF66B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="5340" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -148,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -181,6 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1421,7 +1422,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1504,12 +1505,24 @@
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="C4" s="6">
+        <v>0.59398496240601495</v>
+      </c>
+      <c r="D4" s="12">
+        <v>9.2731829573934804E-2</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.31328320802005</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.62656641604009999</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.21804511278195399</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.15538847117794399</v>
+      </c>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -1594,12 +1607,24 @@
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="C8" s="12">
+        <v>0.360902255639097</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0.63909774436090205</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.39348370927318199</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0.60651629072681701</v>
+      </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated a table that we need to fill in
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688DEF14-1D3C-174E-A3B9-68E36315ABC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216C1CA2-9721-054A-83C9-989054C43609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="8500" windowWidth="28800" windowHeight="16100" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="7100" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
     <sheet name="join-with-learning" sheetId="2" r:id="rId2"/>
     <sheet name="union-no-learning" sheetId="4" r:id="rId3"/>
     <sheet name="union-with-learning" sheetId="5" r:id="rId4"/>
+    <sheet name="new-results" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="40">
   <si>
     <t>llama</t>
   </si>
@@ -84,6 +85,91 @@
   </si>
   <si>
     <t>max_area</t>
+  </si>
+  <si>
+    <t>comb-worst</t>
+  </si>
+  <si>
+    <t>comb-best</t>
+  </si>
+  <si>
+    <t>Heuristic-Driven 
+Approaches</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>angle-worst
+(min_angle=1)</t>
+  </si>
+  <si>
+    <t>distance-worst
+(min_distance=1)</t>
+  </si>
+  <si>
+    <t>angle-best
+(min_angle=10)</t>
+  </si>
+  <si>
+    <t>distance-best
+(min_distance=3)</t>
+  </si>
+  <si>
+    <t>no-heuristics</t>
+  </si>
+  <si>
+    <t>with-heuristics-value (degree)</t>
+  </si>
+  <si>
+    <t>with-heuristics-hint (degree)</t>
+  </si>
+  <si>
+    <t>with-heuristics-hint (distance)</t>
+  </si>
+  <si>
+    <t>with-heuristics-hint (comb)</t>
+  </si>
+  <si>
+    <t>with-heuristics-value (distance)</t>
+  </si>
+  <si>
+    <t>with-heuristics-value (comb)</t>
+  </si>
+  <si>
+    <t>Without
+ Fine-Tuning</t>
+  </si>
+  <si>
+    <t>Zero
+Shot</t>
+  </si>
+  <si>
+    <t>Few
+Shot</t>
+  </si>
+  <si>
+    <t>With 
+Fine-Tuning</t>
+  </si>
+  <si>
+    <t>noisy labels</t>
+  </si>
+  <si>
+    <t>ground truth labels</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>Spatial Join Task</t>
+  </si>
+  <si>
+    <t>representation</t>
+  </si>
+  <si>
+    <t>Machine/Deep Learning
+Approaches</t>
   </si>
 </sst>
 </file>
@@ -93,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +220,19 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -198,6 +297,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -822,12 +948,15 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E4" sqref="E4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
@@ -1622,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861F195A-92DD-DC4F-8798-7EB3A813CF21}">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2142,4 +2271,311 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="16"/>
+    <col min="5" max="5" width="14.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.85728300000000002</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0.84620399999999996</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.86510299999999996</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.95894400000000002</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.95633800000000002</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.97034900000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated base evaluaton code
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216C1CA2-9721-054A-83C9-989054C43609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C13E9F1-F80E-4C46-9D95-8B8624EF8CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="7100" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -119,12 +119,6 @@
     <t>no-heuristics</t>
   </si>
   <si>
-    <t>with-heuristics-value (degree)</t>
-  </si>
-  <si>
-    <t>with-heuristics-hint (degree)</t>
-  </si>
-  <si>
     <t>with-heuristics-hint (distance)</t>
   </si>
   <si>
@@ -170,6 +164,12 @@
   <si>
     <t>Machine/Deep Learning
 Approaches</t>
+  </si>
+  <si>
+    <t>with-heuristics-hint (angle)</t>
+  </si>
+  <si>
+    <t>with-heuristics-value (angle)</t>
   </si>
 </sst>
 </file>
@@ -254,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -287,6 +287,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,22 +309,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -323,8 +320,14 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,7 +666,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection sqref="A1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,23 +680,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="12" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -715,7 +718,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -742,7 +745,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -767,7 +770,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -792,7 +795,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -817,7 +820,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -844,7 +847,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -869,7 +872,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -894,7 +897,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -961,20 +964,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1009,7 +1012,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1047,7 +1050,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1083,7 +1086,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1122,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1158,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1193,7 +1196,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +1232,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1265,7 +1268,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1301,7 +1304,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1339,7 +1342,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1378,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1411,7 +1414,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1481,23 +1484,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="12" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1519,7 +1522,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1546,7 +1549,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1571,7 +1574,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1596,7 +1599,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1621,7 +1624,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1648,7 +1651,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1673,7 +1676,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1698,7 +1701,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1765,20 +1768,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1813,7 +1816,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1851,7 +1854,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1887,7 +1890,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1923,7 +1926,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1959,7 +1962,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2007,7 +2010,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +2047,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2080,7 +2083,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2116,7 +2119,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2154,7 +2157,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2190,7 +2193,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2226,7 +2229,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2278,264 +2281,336 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="16"/>
-    <col min="5" max="5" width="14.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="16"/>
+    <col min="1" max="1" width="16.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="12"/>
+    <col min="5" max="5" width="14.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="22">
+        <v>0.85728300000000002</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.84620399999999996</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0.86510299999999996</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="40" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="23">
-        <v>0.85728300000000002</v>
-      </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:6" ht="40" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="23">
-        <v>0.84620399999999996</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:6" ht="40" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="23">
-        <v>0.94330400000000003</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:6" ht="40" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="23">
-        <v>0.86510299999999996</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="25">
+        <v>0.48843271423916501</v>
+      </c>
+      <c r="E11" s="25">
+        <v>0.58390355164548702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="25">
+        <v>0.52362333007494299</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0.58162267839687198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="25">
+        <v>0.51156728576083399</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0.58129683936135501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="25">
+        <v>0.483870967741935</v>
+      </c>
+      <c r="E14" s="25">
+        <v>0.57999348321928901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="18" t="s">
+      <c r="D15" s="25">
+        <v>0.55979146301726901</v>
+      </c>
+      <c r="E15" s="25">
+        <v>0.63701531443466897</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="25">
+        <v>0.54154447702834796</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0.57771260997067397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="25">
+        <v>0.54089279895731501</v>
+      </c>
+      <c r="E17" s="25">
+        <v>0.576083414793092</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="25">
+        <v>0.47018572825024402</v>
+      </c>
+      <c r="E18" s="25">
+        <v>0.44020853698272999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="20" t="s">
+      <c r="D19" s="25">
+        <v>0.47539915281850698</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0.49266862170087899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="25">
+        <v>0.44639947865754298</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0.51938742261322901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="25">
+        <v>0.44965786901270699</v>
+      </c>
+      <c r="E21" s="25">
+        <v>0.45389377647442097</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="25">
+        <v>0.60019550342130901</v>
+      </c>
+      <c r="E22" s="25">
+        <v>0.784620397523623</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="25">
+        <v>0.44542196155099301</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0.53176930596285399</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="25">
+        <v>0.453567937438905</v>
+      </c>
+      <c r="E24" s="25">
+        <v>0.48061257738676999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20" t="s">
+      <c r="B25" s="21"/>
+      <c r="C25" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="18"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="18"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="16" t="s">
-        <v>35</v>
       </c>
       <c r="D26" s="5">
         <v>0.95894400000000002</v>

</xml_diff>

<commit_message>
updated gpt base evaluation code; added gpt finetune with weak label
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C13E9F1-F80E-4C46-9D95-8B8624EF8CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D632C11D-5E51-8040-9D1F-32C6F84A42E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="7100" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
-    <sheet name="join-with-learning" sheetId="2" r:id="rId2"/>
+    <sheet name="join-cross-data-results" sheetId="2" r:id="rId2"/>
     <sheet name="union-no-learning" sheetId="4" r:id="rId3"/>
     <sheet name="union-with-learning" sheetId="5" r:id="rId4"/>
-    <sheet name="new-results" sheetId="6" r:id="rId5"/>
+    <sheet name="new-join-results" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
   <si>
     <t>llama</t>
   </si>
@@ -87,66 +87,12 @@
     <t>max_area</t>
   </si>
   <si>
-    <t>comb-worst</t>
-  </si>
-  <si>
-    <t>comb-best</t>
-  </si>
-  <si>
-    <t>Heuristic-Driven 
-Approaches</t>
-  </si>
-  <si>
     <t>XGBoost</t>
   </si>
   <si>
-    <t>angle-worst
-(min_angle=1)</t>
-  </si>
-  <si>
-    <t>distance-worst
-(min_distance=1)</t>
-  </si>
-  <si>
-    <t>angle-best
-(min_angle=10)</t>
-  </si>
-  <si>
-    <t>distance-best
-(min_distance=3)</t>
-  </si>
-  <si>
     <t>no-heuristics</t>
   </si>
   <si>
-    <t>with-heuristics-hint (distance)</t>
-  </si>
-  <si>
-    <t>with-heuristics-hint (comb)</t>
-  </si>
-  <si>
-    <t>with-heuristics-value (distance)</t>
-  </si>
-  <si>
-    <t>with-heuristics-value (comb)</t>
-  </si>
-  <si>
-    <t>Without
- Fine-Tuning</t>
-  </si>
-  <si>
-    <t>Zero
-Shot</t>
-  </si>
-  <si>
-    <t>Few
-Shot</t>
-  </si>
-  <si>
-    <t>With 
-Fine-Tuning</t>
-  </si>
-  <si>
     <t>noisy labels</t>
   </si>
   <si>
@@ -156,20 +102,61 @@
     <t>Methods</t>
   </si>
   <si>
-    <t>Spatial Join Task</t>
-  </si>
-  <si>
     <t>representation</t>
   </si>
   <si>
-    <t>Machine/Deep Learning
-Approaches</t>
-  </si>
-  <si>
-    <t>with-heuristics-hint (angle)</t>
-  </si>
-  <si>
-    <t>with-heuristics-value (angle)</t>
+    <t>Heuristic-Driven</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Hint</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>comb</t>
+  </si>
+  <si>
+    <t>worst (min_angle=1)</t>
+  </si>
+  <si>
+    <t>best (min_angle=10)</t>
+  </si>
+  <si>
+    <t>best (min_dist=3)</t>
+  </si>
+  <si>
+    <t>worst (min_dist=1)</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>worst</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Without Fine-Tuning</t>
+  </si>
+  <si>
+    <t>With Fine-Tuning</t>
+  </si>
+  <si>
+    <t>min_dist</t>
+  </si>
+  <si>
+    <t>llama3</t>
   </si>
 </sst>
 </file>
@@ -179,7 +166,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,13 +220,26 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,23 +311,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2278,375 +2296,473 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="12"/>
-    <col min="5" max="5" width="14.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="12"/>
+    <col min="1" max="2" width="4.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" s="23"/>
-      <c r="C3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="22">
+      <c r="C3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="20">
         <v>0.85728300000000002</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="22">
-        <v>0.84620399999999996</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="23"/>
+      <c r="D4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="C5" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0.84620399999999996</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="22">
-        <v>0.94330400000000003</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" ht="40" x14ac:dyDescent="0.25">
+      <c r="C6" s="23"/>
+      <c r="D6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0.86510299999999996</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="22">
-        <v>0.86510299999999996</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="9" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>37</v>
+      <c r="C8" s="23"/>
+      <c r="D8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="19"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="19"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
-    </row>
-    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="25">
-        <v>0.48843271423916501</v>
-      </c>
-      <c r="E11" s="25">
-        <v>0.58390355164548702</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="25">
-        <v>0.52362333007494299</v>
-      </c>
-      <c r="E12" s="25">
-        <v>0.58162267839687198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
-      <c r="C13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="25">
-        <v>0.51156728576083399</v>
-      </c>
-      <c r="E13" s="25">
-        <v>0.58129683936135501</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="23"/>
+      <c r="D13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
-      <c r="C14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="25">
-        <v>0.483870967741935</v>
-      </c>
-      <c r="E14" s="25">
-        <v>0.57999348321928901</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="23"/>
+      <c r="D14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="25">
-        <v>0.55979146301726901</v>
-      </c>
-      <c r="E15" s="25">
-        <v>0.63701531443466897</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="25">
-        <v>0.54154447702834796</v>
-      </c>
-      <c r="E16" s="25">
-        <v>0.57771260997067397</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="25">
-        <v>0.54089279895731501</v>
-      </c>
-      <c r="E17" s="25">
-        <v>0.576083414793092</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="25">
-        <v>0.47018572825024402</v>
-      </c>
-      <c r="E18" s="25">
-        <v>0.44020853698272999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="25">
-        <v>0.47539915281850698</v>
-      </c>
-      <c r="E19" s="25">
-        <v>0.49266862170087899</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="25">
-        <v>0.44639947865754298</v>
-      </c>
-      <c r="E20" s="25">
-        <v>0.51938742261322901</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="13" t="s">
+      <c r="D22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="25">
-        <v>0.44965786901270699</v>
-      </c>
-      <c r="E21" s="25">
-        <v>0.45389377647442097</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="25">
-        <v>0.60019550342130901</v>
-      </c>
-      <c r="E22" s="25">
-        <v>0.784620397523623</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="25">
-        <v>0.44542196155099301</v>
-      </c>
-      <c r="E23" s="25">
-        <v>0.53176930596285399</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="25">
-        <v>0.453567937438905</v>
-      </c>
-      <c r="E24" s="25">
-        <v>0.48061257738676999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0.95894400000000002</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0.95633800000000002</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0.97034900000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+    </row>
+    <row r="25" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="13">
+        <v>1</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="13">
+        <v>2</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="13">
+        <v>5</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="13">
+        <v>10</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="13">
+        <v>20</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="13">
+        <v>1</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="13">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="13">
+        <v>3</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
+  <mergeCells count="27">
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
     <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A9:B10"/>
     <mergeCell ref="A11:A24"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="B18:B24"/>

</xml_diff>

<commit_message>
updated weak label finetuning code; added 4omini weak label results, degree=1
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354EF0E2-A16F-B149-A097-B9EA8270CC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A77E0A5-8510-9D44-8313-4B64E7B473EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="10340" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="39">
   <si>
     <t>llama</t>
   </si>
@@ -248,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,6 +302,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -314,6 +317,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -321,22 +327,10 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,23 +683,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="19" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -727,7 +721,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -754,7 +748,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -779,7 +773,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -804,7 +798,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -829,7 +823,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -856,7 +850,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -881,7 +875,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -906,7 +900,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -973,20 +967,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1021,7 +1015,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1059,7 +1053,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1089,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1131,7 +1125,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1161,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1205,7 +1199,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1235,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1277,7 +1271,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1313,7 +1307,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1351,7 +1345,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +1381,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1423,7 +1417,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1493,23 +1487,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="19" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1531,7 +1525,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1558,7 +1552,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1583,7 +1577,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1608,7 +1602,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1633,7 +1627,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1660,7 +1654,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1685,7 +1679,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1710,7 +1704,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1777,20 +1771,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1825,7 +1819,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1863,7 +1857,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1899,7 +1893,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1935,7 +1929,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1971,7 +1965,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2019,7 +2013,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2050,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2092,7 +2086,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2128,7 +2122,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2166,7 +2160,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2202,7 +2196,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2238,7 +2232,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2287,10 +2281,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2298,537 +2292,469 @@
     <col min="1" max="2" width="4.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" style="12" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="12"/>
+    <col min="5" max="5" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="24">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-    </row>
-    <row r="4" spans="1:7" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="24">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24" t="s">
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="24">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="24">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24" t="s">
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="24">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="25">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-    </row>
-    <row r="11" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="19">
         <v>0.49234278266536302</v>
       </c>
-      <c r="F11" s="28">
-        <v>0.60247637666992504</v>
-      </c>
-      <c r="G11" s="28">
+      <c r="F11" s="19">
         <v>0.40795047246660099</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="19">
         <v>0.51710654936461298</v>
       </c>
-      <c r="F12" s="28">
-        <v>0.60084718149234195</v>
-      </c>
-      <c r="G12" s="28">
+      <c r="F12" s="19">
         <v>0.59237536656891498</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="19">
         <v>0.54089279895731501</v>
       </c>
-      <c r="F13" s="28">
-        <v>0.59954382535027695</v>
-      </c>
-      <c r="G13" s="28">
+      <c r="F13" s="19">
         <v>0.50667970022808695</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="19">
         <v>0.49201694362984599</v>
       </c>
-      <c r="F14" s="28">
-        <v>0.59921798631475998</v>
-      </c>
-      <c r="G14" s="28">
+      <c r="F14" s="19">
         <v>0.46757901596611201</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="19">
         <v>0.596285434995112</v>
       </c>
-      <c r="F15" s="28">
-        <v>0.65786901270772202</v>
-      </c>
-      <c r="G15" s="28">
+      <c r="F15" s="19">
         <v>0.93385467579015902</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="19">
         <v>0.55751058976865397</v>
       </c>
-      <c r="F16" s="28">
-        <v>0.598892147279244</v>
-      </c>
-      <c r="G16" s="28">
+      <c r="F16" s="19">
         <v>0.76050830889540499</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="19">
         <v>0.55131964809384104</v>
       </c>
-      <c r="F17" s="28">
-        <v>0.598892147279244</v>
-      </c>
-      <c r="G17" s="28">
+      <c r="F17" s="19">
         <v>0.88367546432062505</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="19">
         <v>0.47214076246334302</v>
       </c>
-      <c r="F18" s="28">
-        <v>0.45454545454545398</v>
-      </c>
-      <c r="G18" s="28">
+      <c r="F18" s="19">
         <v>0.493320299771912</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="19">
         <v>0.46953405017921102</v>
       </c>
-      <c r="F19" s="28">
-        <v>0.52916259367872198</v>
-      </c>
-      <c r="G19" s="28">
+      <c r="F19" s="19">
         <v>0.60182469859889198</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="19">
         <v>0.50993809058325101</v>
       </c>
-      <c r="F20" s="28">
-        <v>0.67676767676767602</v>
-      </c>
-      <c r="G20" s="28">
+      <c r="F20" s="19">
         <v>0.516780710329097</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="19">
         <v>0.50863473444118601</v>
       </c>
-      <c r="F21" s="28">
-        <v>0.57543173672205905</v>
-      </c>
-      <c r="G21" s="28">
+      <c r="F21" s="19">
         <v>0.53828608667318301</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E22" s="19">
         <v>0.598892147279244</v>
       </c>
-      <c r="F22" s="28">
-        <v>0.85174323884001302</v>
-      </c>
-      <c r="G22" s="28">
+      <c r="F22" s="19">
         <v>0.92049527533398501</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="19">
         <v>0.503421309872922</v>
       </c>
-      <c r="F23" s="28">
-        <v>0.59824046920821095</v>
-      </c>
-      <c r="G23" s="28">
+      <c r="F23" s="19">
         <v>0.83447376995764</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="19">
         <v>0.51482567611599805</v>
       </c>
-      <c r="F24" s="28">
-        <v>0.58520690778755202</v>
-      </c>
-      <c r="G24" s="28">
+      <c r="F24" s="19">
         <v>0.916585206907787</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="26" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
         <v>1</v>
       </c>
       <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
       <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
       <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
       <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
       <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24" t="s">
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
         <v>1</v>
       </c>
       <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+      <c r="F30" s="13"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="23" t="s">
+      <c r="A35" s="28"/>
+      <c r="B35" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2838,14 +2764,32 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
+  <conditionalFormatting sqref="E3:F35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="percentile" val="0"/>
+        <cfvo type="percentile" val="65"/>
+        <cfvo type="max"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
weak label results are not good
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A77E0A5-8510-9D44-8313-4B64E7B473EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B52558-71FF-2242-87D5-6DE4110FCCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="10340" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -248,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,6 +305,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,20 +320,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,23 +686,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -721,7 +724,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -748,7 +751,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -773,7 +776,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -798,7 +801,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -823,7 +826,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -850,7 +853,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -875,7 +878,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -900,7 +903,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -967,20 +970,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1015,7 +1018,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1053,7 +1056,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1092,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1125,7 +1128,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1161,7 +1164,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1199,7 +1202,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1238,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1271,7 +1274,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1307,7 +1310,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1345,7 +1348,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1384,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1417,7 +1420,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1487,23 +1490,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="20" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1525,7 +1528,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1552,7 +1555,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1580,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1602,7 +1605,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1630,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1654,7 +1657,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1679,7 +1682,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1704,7 +1707,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1771,20 +1774,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1819,7 +1822,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1857,7 +1860,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1893,7 +1896,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1929,7 +1932,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1965,7 +1968,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2013,7 +2016,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2050,7 +2053,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2086,7 +2089,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2122,7 +2125,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2160,7 +2163,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2196,7 +2199,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2232,7 +2235,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2284,7 +2287,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2298,22 +2301,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2322,112 +2325,112 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="29">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="29">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="29">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="29">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="29">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2442,9 +2445,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2458,9 +2461,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2472,9 +2475,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2486,9 +2489,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2502,9 +2505,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2516,9 +2519,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2530,8 +2533,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2546,9 +2549,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2562,9 +2565,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2576,9 +2579,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2590,9 +2593,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2606,9 +2609,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2620,9 +2623,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2634,55 +2637,61 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="25" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
         <v>1</v>
       </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="13"/>
+      <c r="E25" s="8">
+        <v>0.83805799999999997</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.86933899999999997</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
       <c r="E26" s="16"/>
-      <c r="F26" s="13"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
       <c r="E27" s="16"/>
-      <c r="F27" s="13"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="13"/>
+      <c r="E28" s="8">
+        <v>0.92701199999999995</v>
+      </c>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
@@ -2690,9 +2699,9 @@
       <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26" t="s">
+      <c r="A30" s="26"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2702,9 +2711,9 @@
       <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
@@ -2712,9 +2721,9 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
@@ -2722,39 +2731,47 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="25" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2764,21 +2781,13 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:F35">
+  <conditionalFormatting sqref="E3:F24 E26:F27 E29:F35 F28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percentile" val="0"/>

</xml_diff>

<commit_message>
added code to finetune on gt labels
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B52558-71FF-2242-87D5-6DE4110FCCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484ED3F7-39E0-6D4E-9F15-6A92F5BADDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="10340" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="10840" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>llama</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>best (10,2)</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -320,20 +323,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,7 +675,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H10"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +960,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E6"/>
+      <selection activeCell="C4" sqref="C4:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2287,7 +2290,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2325,112 +2328,112 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="25">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="25">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="25">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="25">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="29"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="25">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="25"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2445,9 +2448,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2461,9 +2464,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2475,9 +2478,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2489,9 +2492,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2505,9 +2508,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2519,9 +2522,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2533,8 +2536,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2549,9 +2552,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2565,9 +2568,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2579,9 +2582,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2593,9 +2596,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2609,9 +2612,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2623,9 +2626,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2637,13 +2640,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
@@ -2657,9 +2660,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
@@ -2667,9 +2670,9 @@
       <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
@@ -2677,9 +2680,9 @@
       <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
@@ -2689,9 +2692,9 @@
       <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
@@ -2699,9 +2702,9 @@
       <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2711,9 +2714,9 @@
       <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
@@ -2721,57 +2724,52 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="29"/>
+      <c r="B35" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2781,11 +2779,19 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:F24 E26:F27 E29:F35 F28">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
idea lf self-correction; LLM
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484ED3F7-39E0-6D4E-9F15-6A92F5BADDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BE8707-524A-1247-A689-5DA25D87B60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="10840" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
   <si>
     <t>llama</t>
   </si>
@@ -160,13 +160,20 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>zero-shot correction</t>
+  </si>
+  <si>
+    <t>few-shot correction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
@@ -251,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,20 +330,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2287,10 +2297,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2300,10 +2310,13 @@
     <col min="4" max="4" width="20.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="12"/>
+    <col min="7" max="7" width="10.83203125" style="12"/>
+    <col min="8" max="8" width="20" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
@@ -2315,7 +2328,7 @@
       </c>
       <c r="F1" s="28"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -2327,113 +2340,113 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="29">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="25"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="29">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="25"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
+      <c r="F4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="29">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="25"/>
-    </row>
-    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="F5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="29">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="25"/>
-    </row>
-    <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27" t="s">
+      <c r="F6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="29">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="F7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="27">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-    </row>
-    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2446,11 +2459,12 @@
       <c r="F11" s="19">
         <v>0.40795047246660099</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27" t="s">
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2463,10 +2477,10 @@
         <v>0.59237536656891498</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2477,10 +2491,10 @@
         <v>0.50667970022808695</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2491,10 +2505,10 @@
         <v>0.46757901596611201</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2507,10 +2521,10 @@
         <v>0.93385467579015902</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2521,10 +2535,10 @@
         <v>0.76050830889540499</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2535,9 +2549,9 @@
         <v>0.88367546432062505</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2551,10 +2565,10 @@
         <v>0.493320299771912</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2567,10 +2581,10 @@
         <v>0.60182469859889198</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2581,10 +2595,10 @@
         <v>0.516780710329097</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2595,10 +2609,10 @@
         <v>0.53828608667318301</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2611,10 +2625,10 @@
         <v>0.92049527533398501</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2625,10 +2639,10 @@
         <v>0.83447376995764</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2639,14 +2653,14 @@
         <v>0.916585206907787</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+    <row r="25" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="25" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
@@ -2658,31 +2672,37 @@
       <c r="F25" s="8">
         <v>0.86933899999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="H25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+    <row r="27" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
@@ -2691,20 +2711,20 @@
       </c>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2713,20 +2733,20 @@
       <c r="E30" s="16"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
@@ -2734,28 +2754,28 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="26" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="12" t="s">
         <v>39</v>
       </c>
@@ -2765,11 +2785,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2779,19 +2807,11 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:F24 E26:F27 E29:F35 F28">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
experimenetd with self correction
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BE8707-524A-1247-A689-5DA25D87B60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE35CF31-B6B0-064B-AC9D-3D109E512F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="10840" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>llama</t>
   </si>
@@ -160,12 +160,6 @@
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>zero-shot correction</t>
-  </si>
-  <si>
-    <t>few-shot correction</t>
   </si>
 </sst>
 </file>
@@ -318,6 +312,9 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,23 +327,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,23 +693,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -737,7 +731,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -764,7 +758,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -789,7 +783,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -814,7 +808,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -839,7 +833,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -866,7 +860,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -891,7 +885,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -916,7 +910,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -983,20 +977,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1031,7 +1025,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1069,7 +1063,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1099,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1141,7 +1135,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1177,7 +1171,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1215,7 +1209,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1245,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1287,7 +1281,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1323,7 +1317,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1361,7 +1355,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1391,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1433,7 +1427,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1503,23 +1497,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +1535,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1568,7 +1562,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1593,7 +1587,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1618,7 +1612,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1643,7 +1637,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1670,7 +1664,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1695,7 +1689,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1714,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1787,20 +1781,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1835,7 +1829,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1873,7 +1867,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1909,7 +1903,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1945,7 +1939,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1981,7 +1975,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2029,7 +2023,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2066,7 +2060,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2102,7 +2096,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2138,7 +2132,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2176,7 +2170,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2206,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2248,7 +2242,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2297,10 +2291,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2317,22 +2311,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="28"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2341,77 +2335,77 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="26">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="26">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="26">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="26">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="29"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="26">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
@@ -2421,11 +2415,11 @@
       <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
@@ -2433,9 +2427,9 @@
       <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
@@ -2443,10 +2437,10 @@
       <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2459,12 +2453,12 @@
       <c r="F11" s="19">
         <v>0.40795047246660099</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2478,9 +2472,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2492,9 +2486,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2506,9 +2500,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2522,9 +2516,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2535,10 +2529,10 @@
         <v>0.76050830889540499</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2549,9 +2543,9 @@
         <v>0.88367546432062505</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2565,10 +2559,10 @@
         <v>0.493320299771912</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2581,10 +2575,10 @@
         <v>0.60182469859889198</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2595,10 +2589,10 @@
         <v>0.516780710329097</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2609,10 +2603,10 @@
         <v>0.53828608667318301</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2625,10 +2619,10 @@
         <v>0.92049527533398501</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2639,10 +2633,10 @@
         <v>0.83447376995764</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2653,14 +2647,14 @@
         <v>0.916585206907787</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
@@ -2672,37 +2666,31 @@
       <c r="F25" s="8">
         <v>0.86933899999999997</v>
       </c>
-      <c r="H25" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+    <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
@@ -2711,20 +2699,20 @@
       </c>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2733,20 +2721,20 @@
       <c r="E30" s="16"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
@@ -2754,23 +2742,23 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="27" t="s">
         <v>18</v>
       </c>
@@ -2785,19 +2773,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2807,11 +2787,19 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:F24 E26:F27 E29:F35 F28">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
added gpt self-correction code
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE35CF31-B6B0-064B-AC9D-3D109E512F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E267BD6-BAD4-0047-8B77-05AB2CCF7DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="10840" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="union-no-learning" sheetId="4" r:id="rId3"/>
     <sheet name="union-with-learning" sheetId="5" r:id="rId4"/>
     <sheet name="new-join-results" sheetId="6" r:id="rId5"/>
+    <sheet name="new-join-results (2)" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="49">
   <si>
     <t>llama</t>
   </si>
@@ -160,17 +161,49 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Heuristic
+Driven</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Few-
+Shot</t>
+  </si>
+  <si>
+    <t>Zero-
+Shot</t>
+  </si>
+  <si>
+    <t>No Fine-Tuning</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>value+
+self-correction</t>
+  </si>
+  <si>
+    <t>noisy label+
+value+
+self-correction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +264,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -252,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,8 +351,11 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,20 +369,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,7 +724,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,23 +738,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="22" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -731,7 +776,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -758,7 +803,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -783,7 +828,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -808,7 +853,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -833,7 +878,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -860,7 +905,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -885,7 +930,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -910,7 +955,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -964,7 +1009,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:L14"/>
+      <selection activeCell="H3" sqref="H3:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,20 +1022,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1025,7 +1070,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1063,7 +1108,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1144,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1135,7 +1180,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1171,7 +1216,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1209,7 +1254,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1290,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1281,7 +1326,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1317,7 +1362,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1355,7 +1400,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1436,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1427,7 +1472,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1497,23 +1542,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="22" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1535,7 +1580,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1562,7 +1607,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1587,7 +1632,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1612,7 +1657,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1637,7 +1682,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1664,7 +1709,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1689,7 +1734,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1714,7 +1759,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1781,20 +1826,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1829,7 +1874,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1867,7 +1912,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1903,7 +1948,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1939,7 +1984,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1975,7 +2020,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2023,7 +2068,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2060,7 +2105,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2096,7 +2141,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2132,7 +2177,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2170,7 +2215,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +2251,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2242,7 +2287,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2291,10 +2336,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2304,29 +2349,26 @@
     <col min="4" max="4" width="20.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="12"/>
-    <col min="8" max="8" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="12"/>
+    <col min="7" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2334,474 +2376,486 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="31">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="31">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="26"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28" t="s">
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="31">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="31">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="26"/>
-    </row>
-    <row r="7" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
+      <c r="F6" s="31"/>
+    </row>
+    <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="31">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="F7" s="31"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="29">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="27"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="F8" s="29"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="13" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E12" s="19">
         <v>0.49234278266536302</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F12" s="19">
         <v>0.40795047246660099</v>
       </c>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E13" s="19">
         <v>0.51710654936461298</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F13" s="19">
         <v>0.59237536656891498</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E14" s="19">
         <v>0.54089279895731501</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F14" s="19">
         <v>0.50667970022808695</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E15" s="19">
         <v>0.49201694362984599</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F15" s="19">
         <v>0.46757901596611201</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E16" s="19">
         <v>0.596285434995112</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F16" s="19">
         <v>0.93385467579015902</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="13" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E17" s="19">
         <v>0.55751058976865397</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F17" s="19">
         <v>0.76050830889540499</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="13" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E18" s="19">
         <v>0.55131964809384104</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F18" s="19">
         <v>0.88367546432062505</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="13" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E19" s="19">
         <v>0.47214076246334302</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F19" s="19">
         <v>0.493320299771912</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E20" s="19">
         <v>0.46953405017921102</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F20" s="19">
         <v>0.60182469859889198</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="13" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E21" s="19">
         <v>0.50993809058325101</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F21" s="19">
         <v>0.516780710329097</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="13" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E22" s="19">
         <v>0.50863473444118601</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F22" s="19">
         <v>0.53828608667318301</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E23" s="19">
         <v>0.598892147279244</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F23" s="19">
         <v>0.92049527533398501</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="13" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E24" s="19">
         <v>0.503421309872922</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F24" s="19">
         <v>0.83447376995764</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="13" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E25" s="19">
         <v>0.51482567611599805</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F25" s="19">
         <v>0.916585206907787</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="26" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D26" s="13">
         <v>1</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E26" s="8">
         <v>0.83805799999999997</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F26" s="8">
         <v>0.86933899999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="13">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="13">
         <v>2</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="20"/>
-    </row>
-    <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="13">
-        <v>5</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+    <row r="28" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="13">
+        <v>5</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="13">
         <v>10</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E29" s="8">
         <v>0.92701199999999995</v>
       </c>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="13">
+      <c r="F29" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="13">
         <v>20</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="13"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="13">
-        <v>1</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27" t="s">
+        <v>35</v>
+      </c>
       <c r="D31" s="13">
+        <v>1</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="13">
         <v>2</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="13">
-        <v>3</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="13">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="13">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="27" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="12" t="s">
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="F36" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A12:A25"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:F24 E26:F27 E29:F35 F28">
+  <conditionalFormatting sqref="E3:F25 E27:F28 E30:F36 F29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percentile" val="0"/>
@@ -2815,4 +2869,323 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="21" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="31">
+        <v>0.85728300000000002</v>
+      </c>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="31">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+    </row>
+    <row r="7" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.49234278266536302</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.40795047246660099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.51710654936461298</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.59237536656891498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="22">
+        <v>0.596285434995112</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.93385467579015902</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="40" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="22">
+        <v>0.47214076246334302</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0.493320299771912</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="22">
+        <v>0.46953405017921102</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0.60182469859889198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0.598892147279244</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0.92049527533398501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="40" x14ac:dyDescent="0.2">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22">
+        <v>0.83805799999999997</v>
+      </c>
+      <c r="F17" s="22">
+        <v>0.86933899999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="28"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13">
+        <v>2</v>
+      </c>
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="28"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="13">
+        <v>5</v>
+      </c>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="28"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="13">
+        <v>10</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0.92701199999999995</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="28"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A3:C4"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A5:C6"/>
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B7:C11"/>
+    <mergeCell ref="B12:C16"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added self correction code
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E267BD6-BAD4-0047-8B77-05AB2CCF7DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BABFAC6-F591-CE43-9FB3-568053604B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="10840" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="10840" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="49">
   <si>
     <t>llama</t>
   </si>
@@ -187,13 +187,10 @@
     <t>Model</t>
   </si>
   <si>
-    <t>value+
-self-correction</t>
-  </si>
-  <si>
-    <t>noisy label+
-value+
-self-correction</t>
+    <t>value+sc</t>
+  </si>
+  <si>
+    <t>heuristics</t>
   </si>
 </sst>
 </file>
@@ -342,9 +339,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,6 +380,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,23 +735,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -776,7 +773,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -803,7 +800,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -828,7 +825,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -853,7 +850,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -878,7 +875,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -905,7 +902,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -930,7 +927,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -955,7 +952,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1009,7 +1006,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:L6"/>
+      <selection activeCell="C3" sqref="C3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1022,20 +1019,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1070,7 +1067,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1108,7 +1105,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1141,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1180,7 +1177,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1213,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1254,7 +1251,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1287,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1326,7 +1323,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1362,7 +1359,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1400,7 +1397,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +1433,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1472,7 +1469,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1542,23 +1539,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1580,7 +1577,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1607,7 +1604,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1632,7 +1629,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1657,7 +1654,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1682,7 +1679,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1709,7 +1706,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1734,7 +1731,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1759,7 +1756,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1826,20 +1823,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1874,7 +1871,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1912,7 +1909,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1948,7 +1945,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1984,7 +1981,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2020,7 +2017,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2068,7 +2065,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2105,7 +2102,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2141,7 +2138,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2177,7 +2174,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2215,7 +2212,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2248,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2287,7 +2284,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2338,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2353,22 +2350,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2377,333 +2374,333 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="31"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="31"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="31"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="30">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="31"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="30">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="31"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="30">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <v>0.49234278266536302</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="18">
         <v>0.40795047246660099</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <v>0.51710654936461298</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="18">
         <v>0.59237536656891498</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="18">
         <v>0.54089279895731501</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="18">
         <v>0.50667970022808695</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="18">
         <v>0.49201694362984599</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="18">
         <v>0.46757901596611201</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="18">
         <v>0.596285434995112</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="18">
         <v>0.93385467579015902</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="18">
         <v>0.55751058976865397</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="18">
         <v>0.76050830889540499</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="18">
         <v>0.55131964809384104</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="18">
         <v>0.88367546432062505</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="18">
         <v>0.47214076246334302</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="18">
         <v>0.493320299771912</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="18">
         <v>0.46953405017921102</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="18">
         <v>0.60182469859889198</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="18">
         <v>0.50993809058325101</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="18">
         <v>0.516780710329097</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="18">
         <v>0.50863473444118601</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="18">
         <v>0.53828608667318301</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27" t="s">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <v>0.598892147279244</v>
       </c>
-      <c r="F23" s="19">
-        <v>0.92049527533398501</v>
+      <c r="F23" s="18">
+        <v>0.928641251221896</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="18">
         <v>0.503421309872922</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="18">
         <v>0.83447376995764</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="18">
         <v>0.51482567611599805</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="18">
         <v>0.916585206907787</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="13">
@@ -2717,65 +2714,65 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="13">
         <v>2</v>
       </c>
       <c r="E27" s="16"/>
-      <c r="F27" s="20"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="13">
         <v>5</v>
       </c>
       <c r="E28" s="16"/>
-      <c r="F28" s="20"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="13">
         <v>10</v>
       </c>
       <c r="E29" s="8">
         <v>0.92701199999999995</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="13">
         <v>20</v>
       </c>
       <c r="E30" s="16"/>
-      <c r="F30" s="13"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27" t="s">
+      <c r="A31" s="27"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="13">
         <v>1</v>
       </c>
       <c r="E31" s="16"/>
-      <c r="F31" s="13"/>
+      <c r="F31" s="19"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="13">
         <v>2</v>
       </c>
@@ -2783,9 +2780,9 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="13">
         <v>3</v>
       </c>
@@ -2793,37 +2790,41 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="13">
         <v>4</v>
       </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="13">
         <v>5</v>
       </c>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
-      <c r="B36" s="29" t="s">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="12" t="s">
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="32" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="A37" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="27">
@@ -2855,13 +2856,13 @@
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="C26:C30"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:F25 E27:F28 E30:F36 F29">
+  <conditionalFormatting sqref="E3:F36">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percentile" val="0"/>
-        <cfvo type="percentile" val="65"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color theme="1" tint="0.34998626667073579"/>
+        <color theme="1" tint="0.499984740745262"/>
         <color theme="0" tint="-4.9989318521683403E-2"/>
         <color theme="6"/>
       </colorScale>
@@ -2873,315 +2874,353 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="21" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="13"/>
+    <col min="7" max="9" width="10.83203125" style="13"/>
+    <col min="10" max="11" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="13"/>
+    <col min="13" max="13" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="M2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="31"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="F3" s="30"/>
+      <c r="J3" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="26"/>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.85728300000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="31"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="F4" s="30"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="13">
+        <v>2</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.90257399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="13">
+        <v>5</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.93776499999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-    </row>
-    <row r="7" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="13">
+        <v>10</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.94330400000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>0.49234278266536302</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>0.40795047246660099</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="13">
+        <v>20</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0.93548399999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <v>0.51710654936461298</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="21">
         <v>0.59237536656891498</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <v>0.596285434995112</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="21">
         <v>0.93385467579015902</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="40" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+    <row r="10" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28" t="s">
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="27"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0.47214076246334302</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0.493320299771912</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="22">
-        <v>0.47214076246334302</v>
-      </c>
-      <c r="F12" s="22">
-        <v>0.493320299771912</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0.46953405017921102</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0.60182469859889198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="22">
-        <v>0.46953405017921102</v>
-      </c>
-      <c r="F13" s="22">
-        <v>0.60182469859889198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E13" s="21">
         <v>0.598892147279244</v>
       </c>
-      <c r="F14" s="22">
-        <v>0.92049527533398501</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="40" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="14" t="s">
+      <c r="F13" s="18">
+        <v>0.928641251221896</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1</v>
+      </c>
+      <c r="E15" s="21">
+        <v>0.83805799999999997</v>
+      </c>
+      <c r="F15" s="21">
+        <v>0.86933899999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="13">
+        <v>2</v>
+      </c>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>12</v>
-      </c>
+      <c r="A17" s="27"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="13">
-        <v>1</v>
-      </c>
-      <c r="E17" s="22">
-        <v>0.83805799999999997</v>
-      </c>
-      <c r="F17" s="22">
-        <v>0.86933899999999997</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="13">
-        <v>2</v>
-      </c>
-      <c r="F18" s="20"/>
-    </row>
-    <row r="19" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+        <v>10</v>
+      </c>
+      <c r="E18" s="21">
+        <v>0.92701199999999995</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="27"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="13">
-        <v>5</v>
-      </c>
-      <c r="F19" s="20"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="13">
-        <v>10</v>
-      </c>
-      <c r="E20" s="22">
-        <v>0.92701199999999995</v>
-      </c>
-      <c r="F20" s="20" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="F20" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
+      <c r="A21" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="J3:K7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A3:C4"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="A5:C6"/>
-    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="A7:A14"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B7:C11"/>
-    <mergeCell ref="B12:C16"/>
+    <mergeCell ref="B7:C10"/>
+    <mergeCell ref="B11:C14"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E4:F4"/>

</xml_diff>

<commit_message>
added 4o_mini, degree=10, weak label results
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1277AA8F-5F4E-FD4A-AC82-0031411C0DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5FB47B-D10E-3E48-9DD7-72184E5921DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="13760" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="13760" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -366,19 +366,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2335,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2350,22 +2350,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2374,112 +2374,112 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="31">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="31">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="31">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="31">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="31">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="31">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2494,9 +2494,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2510,9 +2510,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2524,9 +2524,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2538,9 +2538,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2554,9 +2554,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2568,9 +2568,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2582,8 +2582,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2598,9 +2598,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2614,9 +2614,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2628,9 +2628,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2642,9 +2642,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2658,9 +2658,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2672,9 +2672,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2686,13 +2686,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
@@ -2706,9 +2706,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
@@ -2716,9 +2716,9 @@
       <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
@@ -2726,9 +2726,9 @@
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
@@ -2740,9 +2740,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
@@ -2750,9 +2750,9 @@
       <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28" t="s">
+      <c r="A30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2762,9 +2762,9 @@
       <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
@@ -2772,9 +2772,9 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
@@ -2782,9 +2782,9 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
@@ -2792,9 +2792,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
@@ -2802,12 +2802,12 @@
       <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="22" t="s">
         <v>39</v>
       </c>
@@ -2820,11 +2820,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2834,19 +2842,11 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:F35">
     <cfRule type="colorScale" priority="2">
@@ -2868,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2887,22 +2887,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2925,14 +2925,14 @@
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="31">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="J3" s="28" t="s">
+      <c r="F3" s="31"/>
+      <c r="J3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="28"/>
+      <c r="K3" s="27"/>
       <c r="L3" s="13">
         <v>1</v>
       </c>
@@ -2947,12 +2947,12 @@
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="31">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="F4" s="31"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="13">
         <v>2</v>
       </c>
@@ -2964,15 +2964,15 @@
       <c r="A5" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
       <c r="L5" s="13">
         <v>5</v>
       </c>
@@ -2981,16 +2981,16 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
       <c r="L6" s="13">
         <v>10</v>
       </c>
@@ -2999,13 +2999,13 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
@@ -3015,8 +3015,8 @@
       <c r="F7" s="21">
         <v>0.40795047246660099</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="13">
         <v>20</v>
       </c>
@@ -3025,9 +3025,9 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="13" t="s">
         <v>41</v>
       </c>
@@ -3039,9 +3039,9 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="13" t="s">
         <v>42</v>
       </c>
@@ -3053,9 +3053,9 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
@@ -3063,11 +3063,11 @@
       <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
@@ -3079,9 +3079,9 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="13" t="s">
         <v>41</v>
       </c>
@@ -3093,9 +3093,9 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
@@ -3107,9 +3107,9 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
@@ -3122,13 +3122,13 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="13">
@@ -3142,27 +3142,27 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="13">
         <v>2</v>
       </c>
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="13">
         <v>5</v>
       </c>
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="13">
         <v>10</v>
       </c>
@@ -3174,20 +3174,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="13" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added llama3 gt results; good
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5FB47B-D10E-3E48-9DD7-72184E5921DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D99FBF-1593-AB49-B082-FD6C9B403547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="13760" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="49">
   <si>
     <t>llama</t>
   </si>
@@ -268,12 +268,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -288,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,8 +372,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -376,13 +388,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2336,7 +2348,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2350,22 +2362,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2374,112 +2386,112 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="27">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="31"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="27">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="31"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="27">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="31"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="27">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="31"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="27">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="31"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="27">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="31"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2494,9 +2506,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2510,9 +2522,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2524,9 +2536,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2538,9 +2550,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2554,9 +2566,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2568,9 +2580,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2582,8 +2594,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2598,9 +2610,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27" t="s">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2614,9 +2626,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2628,9 +2640,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2642,9 +2654,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27" t="s">
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2658,9 +2670,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2672,9 +2684,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2686,13 +2698,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
@@ -2706,9 +2718,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
@@ -2716,9 +2728,9 @@
       <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
@@ -2726,23 +2738,23 @@
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
       <c r="E28" s="8">
         <v>0.92701199999999995</v>
       </c>
-      <c r="F28" s="19" t="s">
-        <v>39</v>
+      <c r="F28" s="8">
+        <v>0.94069700000000001</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
@@ -2750,9 +2762,9 @@
       <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27" t="s">
+      <c r="A30" s="30"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2762,9 +2774,9 @@
       <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
@@ -2772,9 +2784,9 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
@@ -2782,9 +2794,9 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
@@ -2792,9 +2804,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
@@ -2802,14 +2814,14 @@
       <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29" t="s">
+      <c r="A35" s="30"/>
+      <c r="B35" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="22" t="s">
-        <v>39</v>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="22">
+        <v>0.96579999999999999</v>
       </c>
       <c r="F35" s="22" t="s">
         <v>39</v>
@@ -2820,19 +2832,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2842,14 +2846,22 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:F35">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="E3:F27 E29:F35 E28">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percentile" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2857,6 +2869,18 @@
         <color theme="1" tint="0.499984740745262"/>
         <color theme="0" tint="-4.9989318521683403E-2"/>
         <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -2869,7 +2893,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2887,22 +2911,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2925,20 +2949,21 @@
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="27">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="J3" s="27" t="s">
+      <c r="F3" s="27"/>
+      <c r="J3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="27"/>
+      <c r="K3" s="28"/>
       <c r="L3" s="13">
         <v>1</v>
       </c>
       <c r="M3" s="5">
         <v>0.85728300000000002</v>
       </c>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:19" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="32"/>
@@ -2947,65 +2972,68 @@
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="27">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
       <c r="L4" s="13">
         <v>2</v>
       </c>
       <c r="M4" s="5">
         <v>0.90257399999999999</v>
       </c>
+      <c r="N4" s="34"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
       <c r="L5" s="13">
         <v>5</v>
       </c>
       <c r="M5" s="5">
         <v>0.93776499999999996</v>
       </c>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
       <c r="L6" s="13">
         <v>10</v>
       </c>
       <c r="M6" s="5">
         <v>0.94330400000000003</v>
       </c>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
@@ -3015,19 +3043,20 @@
       <c r="F7" s="21">
         <v>0.40795047246660099</v>
       </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
       <c r="L7" s="13">
         <v>20</v>
       </c>
       <c r="M7" s="5">
         <v>0.93548399999999998</v>
       </c>
+      <c r="N7" s="34"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="13" t="s">
         <v>41</v>
       </c>
@@ -3039,9 +3068,9 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="13" t="s">
         <v>42</v>
       </c>
@@ -3053,21 +3082,21 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
@@ -3079,9 +3108,9 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="13" t="s">
         <v>41</v>
       </c>
@@ -3093,9 +3122,9 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
@@ -3107,14 +3136,14 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -3122,13 +3151,13 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="13">
@@ -3142,54 +3171,54 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="13">
         <v>2</v>
       </c>
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="13">
         <v>5</v>
       </c>
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="13">
         <v>10</v>
       </c>
       <c r="E18" s="21">
         <v>0.92701199999999995</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>39</v>
+      <c r="F18" s="19">
+        <v>0.94099999999999995</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="13" t="s">
-        <v>39</v>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="19">
+        <v>0.96579999999999999</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
added opem model, base with self correction code
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D99FBF-1593-AB49-B082-FD6C9B403547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6A8CD7-68A6-7142-9B4F-79F3DA0EAE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="13760" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -257,12 +257,6 @@
     <font>
       <i/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -354,11 +348,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,14 +366,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -388,12 +376,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,6 +405,185 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF8F9DFE-9B04-E0B6-6B7C-C20164EEDBA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12306300" y="571500"/>
+          <a:ext cx="8204200" cy="5575300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>The</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t> story:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t>1. without ground truth labels, we could use noisy labels under no fine-tuning setting</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>LLMs have the self -correction ability to generate competitive results (to be approved)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Using noisy labels as the initial response, LLMs are critisize and improve the response (to be approved)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- fine-tuning with noisy labels does not work well, because LLMs are powerful enough to learn and memorize the wrong patterns from the noisy labels. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0"/>
+            <a:t>2. with ground truth labels, we could fine-tuning LLMs:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- fine-tuning LLMs outperforms heuristics (yes)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- fine-tuning LLMs outperforms ML/DL methods (to be approved)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- fine-tuning LLMs show cross-data generalization (fine-tuning on different parts of the data; generalize to unseen data paterns)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- fine-tuning LLMs show cross-task generalization (fine-tuning on join task; can perform on union task)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2347,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2362,22 +2535,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2386,112 +2559,112 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="31">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="31">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="31">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="31">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="31">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="31">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2506,9 +2679,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2522,9 +2695,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2536,9 +2709,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2550,9 +2723,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2566,9 +2739,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2580,9 +2753,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2594,8 +2767,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2610,9 +2783,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2626,9 +2799,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2640,9 +2813,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2654,9 +2827,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2670,9 +2843,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2684,9 +2857,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2698,13 +2871,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
@@ -2718,9 +2891,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
@@ -2728,9 +2901,9 @@
       <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
@@ -2738,9 +2911,9 @@
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
@@ -2752,9 +2925,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
@@ -2762,9 +2935,9 @@
       <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28" t="s">
+      <c r="A30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2774,9 +2947,9 @@
       <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
@@ -2784,9 +2957,9 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
@@ -2794,36 +2967,36 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="22">
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="21">
         <v>0.96579999999999999</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="21" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2832,11 +3005,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -2846,19 +3027,11 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:F27 E29:F35 E28">
     <cfRule type="colorScale" priority="3">
@@ -2892,8 +3065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2905,28 +3078,28 @@
     <col min="6" max="6" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.83203125" style="13"/>
     <col min="10" max="11" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="13"/>
+    <col min="12" max="12" width="3.5" style="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2949,21 +3122,21 @@
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="31">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="J3" s="28" t="s">
+      <c r="F3" s="31"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="28"/>
       <c r="L3" s="13">
         <v>1</v>
       </c>
       <c r="M3" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N3" s="34"/>
+      <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:19" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="32"/>
@@ -2972,178 +3145,178 @@
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="31">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="F4" s="31"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="13">
         <v>2</v>
       </c>
       <c r="M4" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N4" s="34"/>
+      <c r="N4" s="22"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="27"/>
       <c r="L5" s="13">
         <v>5</v>
       </c>
       <c r="M5" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N5" s="34"/>
+      <c r="N5" s="22"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="27"/>
       <c r="L6" s="13">
         <v>10</v>
       </c>
       <c r="M6" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N6" s="34"/>
+      <c r="N6" s="22"/>
     </row>
     <row r="7" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>0.49234278266536302</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="19">
         <v>0.40795047246660099</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="13">
         <v>20</v>
       </c>
       <c r="M7" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N7" s="34"/>
+      <c r="N7" s="22"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="19">
         <v>0.51710654936461298</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="19">
         <v>0.59237536656891498</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>0.596285434995112</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="19">
         <v>0.93385467579015902</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <v>0.47214076246334302</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="19">
         <v>0.493320299771912</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="19">
         <v>0.46953405017921102</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="19">
         <v>0.60182469859889198</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="19">
         <v>0.598892147279244</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="21">
         <v>0.928641251221896</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -3151,51 +3324,51 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="13">
         <v>1</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="19">
         <v>0.83805799999999997</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="19">
         <v>0.86933899999999997</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="13">
         <v>2</v>
       </c>
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="13">
         <v>5</v>
       </c>
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="13">
         <v>10</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="19">
         <v>0.92701199999999995</v>
       </c>
       <c r="F18" s="19">
@@ -3203,20 +3376,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="19">
         <v>0.96579999999999999</v>
       </c>
@@ -3229,7 +3402,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J3:K7"/>
+    <mergeCell ref="K3:K7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A3:C4"/>
@@ -3247,5 +3420,6 @@
     <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added gpt gt data geenration code
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6A8CD7-68A6-7142-9B4F-79F3DA0EAE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960BDA5-E25B-5B47-A2DF-EE19D57A5E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
   <si>
     <t>llama</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>heuristics</t>
+  </si>
+  <si>
+    <t>value+ec</t>
   </si>
 </sst>
 </file>
@@ -288,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,6 +357,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -366,8 +375,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -376,19 +391,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,15 +587,52 @@
             <a:t>- fine-tuning LLMs show cross-task generalization (fine-tuning on join task; can perform on union task)</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>4o-mini costs</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- 3.33 for inference (for 14 tasks, 30 mins)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -906,7 +955,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F5" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,23 +969,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -958,7 +1007,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -985,7 +1034,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1010,7 +1059,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1035,7 +1084,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1109,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1087,7 +1136,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1161,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1186,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1204,20 +1253,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1252,7 +1301,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1290,7 +1339,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1326,7 +1375,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1362,7 +1411,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1447,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1436,7 +1485,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1472,7 +1521,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1508,7 +1557,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1544,7 +1593,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1582,7 +1631,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1618,7 +1667,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1654,7 +1703,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1724,23 +1773,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1762,7 +1811,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1789,7 +1838,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1814,7 +1863,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1839,7 +1888,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1864,7 +1913,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1891,7 +1940,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1916,7 +1965,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1941,7 +1990,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2008,20 +2057,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -2056,7 +2105,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2094,7 +2143,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2130,7 +2179,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2215,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2202,7 +2251,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2250,7 +2299,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2287,7 +2336,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2323,7 +2372,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2359,7 +2408,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2397,7 +2446,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2433,7 +2482,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2469,7 +2518,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2518,10 +2567,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2534,137 +2583,146 @@
     <col min="7" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="F1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="G2" s="36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="29">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="31"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+    </row>
+    <row r="4" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="29">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="31"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="29">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="31"/>
-    </row>
-    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="29">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="31"/>
-    </row>
-    <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27" t="s">
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="29">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="31"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="29">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="31"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="30" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15"/>
@@ -2678,10 +2736,10 @@
         <v>0.40795047246660099</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2694,10 +2752,10 @@
         <v>0.59237536656891498</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2708,10 +2766,10 @@
         <v>0.50667970022808695</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
@@ -2722,10 +2780,10 @@
         <v>0.46757901596611201</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -2738,10 +2796,10 @@
         <v>0.93385467579015902</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -2752,10 +2810,10 @@
         <v>0.76050830889540499</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -2766,9 +2824,9 @@
         <v>0.88367546432062505</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="15"/>
@@ -2782,10 +2840,10 @@
         <v>0.493320299771912</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="13" t="s">
@@ -2798,10 +2856,10 @@
         <v>0.60182469859889198</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="13" t="s">
         <v>26</v>
       </c>
@@ -2812,10 +2870,10 @@
         <v>0.516780710329097</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="13" t="s">
         <v>27</v>
       </c>
@@ -2826,10 +2884,10 @@
         <v>0.53828608667318301</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="13" t="s">
@@ -2842,10 +2900,10 @@
         <v>0.928641251221896</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
@@ -2856,10 +2914,10 @@
         <v>0.83447376995764</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2870,14 +2928,14 @@
         <v>0.916585206907787</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13">
@@ -2889,31 +2947,34 @@
       <c r="F25" s="8">
         <v>0.86933899999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="G25" s="37"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="13">
         <v>2</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="19"/>
-    </row>
-    <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="G26" s="37"/>
+    </row>
+    <row r="27" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="13">
         <v>5</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="19"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="13">
         <v>10</v>
       </c>
@@ -2923,21 +2984,23 @@
       <c r="F28" s="8">
         <v>0.94069700000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="G28" s="37"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="13">
         <v>20</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="19"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27" t="s">
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="32"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="13">
@@ -2945,79 +3008,78 @@
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="19"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+      <c r="G30" s="37"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="13">
         <v>2</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+      <c r="G31" s="37"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
       <c r="D32" s="13">
         <v>3</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="G32" s="37"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="13">
         <v>4</v>
       </c>
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
+      <c r="G33" s="37"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="13">
         <v>5</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29" t="s">
+      <c r="G34" s="37"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="21">
         <v>0.96579999999999999</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="37"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A11:A24"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
+  <mergeCells count="28">
+    <mergeCell ref="G25:G35"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -3027,13 +3089,21 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:F27 E29:F35 E28">
+  <conditionalFormatting sqref="E9:F27 E29:F35 E28 E3:E8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percentile" val="0"/>
@@ -3045,7 +3115,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F35">
+  <conditionalFormatting sqref="E9:F35 E3:E8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3065,8 +3135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3076,7 +3146,8 @@
     <col min="4" max="4" width="20.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10.83203125" style="13"/>
+    <col min="7" max="7" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="13"/>
     <col min="10" max="11" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.5" style="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
@@ -3084,50 +3155,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="N1" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="M2" s="13" t="s">
         <v>48</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="29">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="27" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="30" t="s">
         <v>17</v>
       </c>
       <c r="L3" s="13">
@@ -3137,20 +3224,23 @@
         <v>0.85728300000000002</v>
       </c>
       <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
     </row>
     <row r="4" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="29">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="27"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="30"/>
       <c r="L4" s="13">
         <v>2</v>
       </c>
@@ -3158,20 +3248,23 @@
         <v>0.90257399999999999</v>
       </c>
       <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="27"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="30"/>
       <c r="L5" s="13">
         <v>5</v>
       </c>
@@ -3179,18 +3272,21 @@
         <v>0.93776499999999996</v>
       </c>
       <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="27"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="30"/>
       <c r="L6" s="13">
         <v>10</v>
       </c>
@@ -3198,15 +3294,17 @@
         <v>0.94330400000000003</v>
       </c>
       <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
     </row>
     <row r="7" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
@@ -3216,8 +3314,9 @@
       <c r="F7" s="19">
         <v>0.40795047246660099</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="27"/>
+      <c r="G7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="30"/>
       <c r="L7" s="13">
         <v>20</v>
       </c>
@@ -3225,11 +3324,13 @@
         <v>0.93548399999999998</v>
       </c>
       <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="13" t="s">
         <v>41</v>
       </c>
@@ -3239,11 +3340,12 @@
       <c r="F8" s="19">
         <v>0.59237536656891498</v>
       </c>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="13" t="s">
         <v>42</v>
       </c>
@@ -3253,23 +3355,25 @@
       <c r="F9" s="19">
         <v>0.93385467579015902</v>
       </c>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
@@ -3279,11 +3383,12 @@
       <c r="F11" s="19">
         <v>0.493320299771912</v>
       </c>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="13" t="s">
         <v>41</v>
       </c>
@@ -3293,11 +3398,12 @@
       <c r="F12" s="19">
         <v>0.60182469859889198</v>
       </c>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
@@ -3307,16 +3413,18 @@
       <c r="F13" s="21">
         <v>0.928641251221896</v>
       </c>
+      <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="22"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -3324,13 +3432,13 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="13">
@@ -3342,29 +3450,32 @@
       <c r="F15" s="19">
         <v>0.86933899999999997</v>
       </c>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="13">
         <v>2</v>
       </c>
       <c r="F16" s="19"/>
-    </row>
-    <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="32"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="13">
         <v>5</v>
       </c>
       <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="32"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="13">
         <v>10</v>
       </c>
@@ -3374,37 +3485,45 @@
       <c r="F18" s="19">
         <v>0.94099999999999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="G18" s="33"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="32"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="13">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29" t="s">
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="32"/>
+      <c r="B20" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="19">
         <v>0.96579999999999999</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="22" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="G15:G20"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
     <mergeCell ref="K3:K7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="B15:B19"/>
@@ -3415,9 +3534,6 @@
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="B7:C10"/>
     <mergeCell ref="B11:C14"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
visualized ec results; good with degree=1
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCB89C2-076A-6945-B6B1-46F4B1CE1387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0849D22E-D986-4B48-BF1A-13CEF97E4408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
     <author>tc={8EEEE5FB-BB02-E74A-8762-6734D3965F35}</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{8EEEE5FB-BB02-E74A-8762-6734D3965F35}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{8EEEE5FB-BB02-E74A-8762-6734D3965F35}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="49">
   <si>
     <t>llama</t>
   </si>
@@ -223,10 +223,12 @@
     <t>heuristics</t>
   </si>
   <si>
-    <t>value+ec</t>
-  </si>
-  <si>
-    <t>no fine-tuning</t>
+    <t>few_shot_with_
+heur_angle_value</t>
+  </si>
+  <si>
+    <t>zero_shot_with_
+heur_angle_value</t>
   </si>
 </sst>
 </file>
@@ -429,36 +431,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -470,6 +466,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,15 +494,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1104,7 +1106,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A13" dT="2025-02-24T23:09:20.07" personId="{9D9E5CA6-6815-0341-8285-EC861268655E}" id="{8EEEE5FB-BB02-E74A-8762-6734D3965F35}">
+  <threadedComment ref="A12" dT="2025-02-24T23:09:20.07" personId="{9D9E5CA6-6815-0341-8285-EC861268655E}" id="{8EEEE5FB-BB02-E74A-8762-6734D3965F35}">
     <text>Fine-tuning is no longer needed since simple ML method (XGBoost) works very well.</text>
   </threadedComment>
 </ThreadedComments>
@@ -2729,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2740,7 +2742,7 @@
     <col min="4" max="4" width="20.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
@@ -2782,11 +2784,11 @@
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="37">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
@@ -2795,11 +2797,11 @@
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="37">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="39"/>
@@ -2810,11 +2812,11 @@
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="37">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="39"/>
@@ -2823,11 +2825,11 @@
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="37">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="39"/>
@@ -2838,11 +2840,11 @@
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="37">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="39"/>
@@ -2851,11 +2853,11 @@
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="37">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
@@ -2934,6 +2936,9 @@
       <c r="F13" s="17">
         <v>0.93385467579015902</v>
       </c>
+      <c r="G13" s="6">
+        <v>0.94395568589116896</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="39"/>
@@ -2948,6 +2953,7 @@
       <c r="F14" s="17">
         <v>0.76050830889540499</v>
       </c>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="39"/>
@@ -2962,6 +2968,9 @@
       <c r="F15" s="17">
         <v>0.88367546432062505</v>
       </c>
+      <c r="G15" s="6">
+        <v>0.93776474421635703</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="39"/>
@@ -2978,6 +2987,7 @@
       <c r="F16" s="17">
         <v>0.493320299771912</v>
       </c>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
@@ -2994,6 +3004,7 @@
       <c r="F17" s="17">
         <v>0.60182469859889198</v>
       </c>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
@@ -3008,6 +3019,7 @@
       <c r="F18" s="17">
         <v>0.516780710329097</v>
       </c>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="39"/>
@@ -3022,6 +3034,7 @@
       <c r="F19" s="17">
         <v>0.53828608667318301</v>
       </c>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="39"/>
@@ -3037,6 +3050,9 @@
       </c>
       <c r="F20" s="17">
         <v>0.928641251221896</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.92994460736396201</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3052,6 +3068,7 @@
       <c r="F21" s="17">
         <v>0.83447376995764</v>
       </c>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="39"/>
@@ -3066,9 +3083,12 @@
       <c r="F22" s="17">
         <v>0.916585206907787</v>
       </c>
+      <c r="G22" s="6">
+        <v>0.94134897360703795</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="34" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="35"/>
@@ -3076,11 +3096,11 @@
       <c r="D23" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="41">
+      <c r="E23" s="36">
         <v>0.995</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
@@ -3089,12 +3109,12 @@
       <c r="D24" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="35" t="s">
@@ -3112,10 +3132,10 @@
       <c r="F25" s="25">
         <v>0.86933899999999997</v>
       </c>
-      <c r="G25" s="34"/>
+      <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="35"/>
       <c r="C26" s="35"/>
       <c r="D26" s="24">
@@ -3123,10 +3143,10 @@
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="34"/>
+      <c r="G26" s="40"/>
     </row>
     <row r="27" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="35"/>
       <c r="C27" s="35"/>
       <c r="D27" s="24">
@@ -3134,10 +3154,10 @@
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="27"/>
-      <c r="G27" s="34"/>
+      <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
       <c r="D28" s="24">
@@ -3149,10 +3169,10 @@
       <c r="F28" s="25">
         <v>0.94069700000000001</v>
       </c>
-      <c r="G28" s="34"/>
+      <c r="G28" s="40"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
       <c r="D29" s="24">
@@ -3160,10 +3180,10 @@
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="34"/>
+      <c r="G29" s="40"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="35"/>
       <c r="C30" s="35" t="s">
         <v>35</v>
@@ -3173,10 +3193,10 @@
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="34"/>
+      <c r="G30" s="40"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="35"/>
       <c r="C31" s="35"/>
       <c r="D31" s="24">
@@ -3184,10 +3204,10 @@
       </c>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
-      <c r="G31" s="34"/>
+      <c r="G31" s="40"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="35"/>
       <c r="C32" s="35"/>
       <c r="D32" s="24">
@@ -3195,10 +3215,10 @@
       </c>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="34"/>
+      <c r="G32" s="40"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
       <c r="D33" s="24">
@@ -3206,10 +3226,10 @@
       </c>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
-      <c r="G33" s="34"/>
+      <c r="G33" s="40"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="35"/>
       <c r="C34" s="35"/>
       <c r="D34" s="24">
@@ -3217,38 +3237,34 @@
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
-      <c r="G34" s="34"/>
+      <c r="G34" s="40"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37" t="s">
+      <c r="A35" s="34"/>
+      <c r="B35" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
       <c r="E35" s="29">
         <v>0.96579999999999999</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="34"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A23:C24"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="G25:G35"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C25:C29"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C13:C15"/>
@@ -3261,12 +3277,16 @@
     <mergeCell ref="A9:A22"/>
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="B16:B22"/>
-    <mergeCell ref="G25:G35"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A23:C24"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:F22 E3:E8">
     <cfRule type="colorScale" priority="1">
@@ -3297,10 +3317,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3309,353 +3329,319 @@
     <col min="3" max="3" width="4.1640625" style="13" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.83203125" style="13"/>
     <col min="9" max="10" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.5" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.1640625" style="13" customWidth="1"/>
+    <col min="13" max="14" width="17.5" style="13" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="M1" s="42" t="s">
+      <c r="E1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="42"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="16" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="37">
+        <v>0.85728300000000002</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="13">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0.85728300000000002</v>
+      </c>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="37">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="F3" s="37"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="13">
         <v>2</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="40">
-        <v>0.85728300000000002</v>
-      </c>
-      <c r="F3" s="40"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="13">
-        <v>1</v>
-      </c>
       <c r="L3" s="5">
-        <v>0.85728300000000002</v>
-      </c>
-      <c r="M3" s="43">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="N3" s="43"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-    </row>
-    <row r="4" spans="1:19" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="40">
-        <v>0.94330400000000003</v>
-      </c>
-      <c r="F4" s="40"/>
+        <v>0.90257399999999999</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.40795047246660099</v>
+      </c>
+      <c r="F4" s="21"/>
       <c r="I4" s="22"/>
       <c r="J4" s="39"/>
       <c r="K4" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L4" s="5">
-        <v>0.90257399999999999</v>
-      </c>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-    </row>
-    <row r="5" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="46"/>
+        <v>0.93776499999999996</v>
+      </c>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="39"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="13" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E5" s="18">
-        <v>0.40795047246660099</v>
+        <v>0.59237536656891498</v>
       </c>
       <c r="F5" s="21"/>
       <c r="I5" s="22"/>
       <c r="J5" s="39"/>
       <c r="K5" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L5" s="5">
-        <v>0.93776499999999996</v>
-      </c>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="18">
-        <v>0.59237536656891498</v>
-      </c>
-      <c r="F6" s="21"/>
+        <v>0.93385467579015902</v>
+      </c>
+      <c r="F6" s="46">
+        <v>0.94399999999999995</v>
+      </c>
       <c r="I6" s="22"/>
       <c r="J6" s="39"/>
       <c r="K6" s="13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L6" s="5">
-        <v>0.94330400000000003</v>
-      </c>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-    </row>
-    <row r="7" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.93548399999999998</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="1:16" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="39"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="44"/>
       <c r="D7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.493320299771912</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.60182469859889198</v>
+      </c>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="18">
-        <v>0.93385467579015902</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="13">
+      <c r="E9" s="20">
+        <v>0.928641251221896</v>
+      </c>
+      <c r="F9" s="46">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="5">
-        <v>0.93548399999999998</v>
-      </c>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-    </row>
-    <row r="8" spans="1:19" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
-      <c r="B8" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="18">
-        <v>0.493320299771912</v>
-      </c>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="18">
-        <v>0.60182469859889198</v>
-      </c>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="20">
-        <v>0.928641251221896</v>
-      </c>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-    </row>
-    <row r="13" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B12" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C12" s="35" t="s">
         <v>12</v>
       </c>
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.86933899999999997</v>
+      </c>
+      <c r="F12" s="41"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="24">
-        <v>1</v>
-      </c>
-      <c r="E13" s="27">
-        <v>0.86933899999999997</v>
-      </c>
-      <c r="F13" s="37"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="41"/>
+    </row>
+    <row r="14" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
       <c r="B14" s="35"/>
       <c r="C14" s="35"/>
       <c r="D14" s="24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E14" s="27"/>
-      <c r="F14" s="37"/>
-    </row>
-    <row r="15" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
       <c r="D15" s="24">
-        <v>5</v>
-      </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="37"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="36"/>
+        <v>10</v>
+      </c>
+      <c r="E15" s="27">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="24">
-        <v>10</v>
-      </c>
-      <c r="E16" s="27">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="F16" s="37"/>
+        <v>20</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="24">
-        <v>20</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="37"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="41"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="36"/>
-      <c r="B18" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="37"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
+      <c r="A18" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="A11:C12"/>
+  <mergeCells count="16">
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B5:C7"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="B8:C10"/>
-    <mergeCell ref="A3:C4"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="F13:F18"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="B4:C6"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B7:C9"/>
+    <mergeCell ref="A2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
other llms have great performance
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA60012-DDB6-4048-B23A-370948DCCFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C53430-2348-394D-8A1F-96BE99BCAA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -46,25 +46,7 @@
     <author>tc={EED0D08B-EFB4-6449-9728-0EC52AEB9BD2}</author>
   </authors>
   <commentList>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{EED0D08B-EFB4-6449-9728-0EC52AEB9BD2}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Fine-tuning is no longer needed since simple ML method (XGBoost) works very well.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={8EEEE5FB-BB02-E74A-8762-6734D3965F35}</author>
-  </authors>
-  <commentList>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{8EEEE5FB-BB02-E74A-8762-6734D3965F35}">
+    <comment ref="A26" authorId="0" shapeId="0" xr:uid="{EED0D08B-EFB4-6449-9728-0EC52AEB9BD2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -77,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="55">
   <si>
     <t>llama</t>
   </si>
@@ -203,23 +185,6 @@
 Driven</t>
   </si>
   <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Few-
-Shot</t>
-  </si>
-  <si>
-    <t>Zero-
-Shot</t>
-  </si>
-  <si>
-    <t>No Fine-Tuning</t>
-  </si>
-  <si>
     <t>heuristics</t>
   </si>
   <si>
@@ -259,6 +224,12 @@
   </si>
   <si>
     <t>noisy label</t>
+  </si>
+  <si>
+    <t>gemini</t>
+  </si>
+  <si>
+    <t>qwen</t>
   </si>
 </sst>
 </file>
@@ -356,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -404,9 +375,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,24 +390,25 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,58 +442,29 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,291 +481,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF8F9DFE-9B04-E0B6-6B7C-C20164EEDBA2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16268700" y="1231900"/>
-          <a:ext cx="8204200" cy="7581900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600"/>
-            <a:t>The</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t> story:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1600" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>1. without ground truth labels, we could use noisy labels under no fine-tuning setting</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>- </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>LLMs have the self-correction ability to generate competitive results (to be approved)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>- </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Using noisy labels as the initial response, LLMs are critisize and improve the response (to be approved)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- fine-tuning with noisy labels does not work well, because LLMs are powerful enough to learn and memorize the wrong patterns from the noisy labels. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>	- it also does not work well with XGBoost.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1600" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>add vision results</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1600" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>2. with ground truth labels, we could fine-tuning LLMs:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- fine-tuning LLMs outperforms heuristics (yes)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- fine-tuning LLMs outperforms ML/DL methods (to be approved)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>	- no. LLMs do not outperform ML/DL</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- fine-tuning LLMs show cross-data generalization (fine-tuning on different parts of the data; generalize to unseen data paterns)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>	- XGBoost does not have this ability</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- fine-tuning LLMs show cross-task generalization (fine-tuning on join task; can perform on union task)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>	- XGBoost does not have this ability</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- overall, when we have ground truth labels, the results are not in favor of ML methods. XGBoost has an awesome job (even though they do not generalize well cross-data)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>4o-mini costs</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- 3.33 for inference (for 14 tasks, 30 mins)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1151,15 +806,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A25" dT="2025-02-24T23:09:05.30" personId="{9D9E5CA6-6815-0341-8285-EC861268655E}" id="{EED0D08B-EFB4-6449-9728-0EC52AEB9BD2}">
-    <text>Fine-tuning is no longer needed since simple ML method (XGBoost) works very well.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A12" dT="2025-02-24T23:09:20.07" personId="{9D9E5CA6-6815-0341-8285-EC861268655E}" id="{8EEEE5FB-BB02-E74A-8762-6734D3965F35}">
+  <threadedComment ref="A26" dT="2025-02-24T23:09:05.30" personId="{9D9E5CA6-6815-0341-8285-EC861268655E}" id="{EED0D08B-EFB4-6449-9728-0EC52AEB9BD2}">
     <text>Fine-tuning is no longer needed since simple ML method (XGBoost) works very well.</text>
   </threadedComment>
 </ThreadedComments>
@@ -2782,10 +2429,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8E7FE-FAB4-D346-82D0-F2324C6E246F}">
-  <dimension ref="A1:AG36"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2834,6 +2481,12 @@
       <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
@@ -2850,6 +2503,8 @@
         <v>0.85728300000000002</v>
       </c>
       <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
@@ -2865,10 +2520,11 @@
         <v>0.94330400000000003</v>
       </c>
       <c r="F4" s="38"/>
-      <c r="H4" s="47"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
@@ -2883,10 +2539,11 @@
         <v>0.84620399999999996</v>
       </c>
       <c r="F5" s="38"/>
-      <c r="H5" s="47"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="45"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="37"/>
@@ -2899,10 +2556,11 @@
         <v>0.86510299999999996</v>
       </c>
       <c r="F6" s="38"/>
-      <c r="H6" s="47"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="45"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
@@ -2917,10 +2575,11 @@
         <v>0.83699999999999997</v>
       </c>
       <c r="F7" s="38"/>
-      <c r="H7" s="47"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
@@ -2933,10 +2592,11 @@
         <v>0.95099999999999996</v>
       </c>
       <c r="F8" s="38"/>
-      <c r="H8" s="47"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
@@ -2949,32 +2609,38 @@
       <c r="D9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="19">
         <v>0.49234278266536302</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="19">
         <v>0.40795047246660099</v>
       </c>
-      <c r="L9" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="51"/>
-      <c r="N9" s="52" t="s">
+      <c r="G9" s="19">
+        <v>0.64418399999999998</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.603128</v>
+      </c>
+      <c r="L9" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="42"/>
+      <c r="N9" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="52"/>
-      <c r="X9" s="52"/>
-      <c r="Y9" s="52"/>
-      <c r="Z9" s="52"/>
-      <c r="AA9" s="52"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="40"/>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="40"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
@@ -2985,32 +2651,38 @@
       <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="19">
         <v>0.51710654936461298</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="19">
         <v>0.59237536656891498</v>
       </c>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="52" t="s">
+      <c r="G10" s="19">
+        <v>0.64678999999999998</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0.63962200000000002</v>
+      </c>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52" t="s">
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="52"/>
-      <c r="W10" s="52"/>
-      <c r="X10" s="52"/>
-      <c r="Y10" s="52"/>
-      <c r="Z10" s="52"/>
-      <c r="AA10" s="52"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="40"/>
+      <c r="Z10" s="40"/>
+      <c r="AA10" s="40"/>
     </row>
     <row r="11" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
@@ -3019,40 +2691,46 @@
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="19">
         <v>0.54089279895731501</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="19">
         <v>0.50667970022808695</v>
       </c>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="O11" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="V11" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="W11" s="52"/>
-      <c r="X11" s="52"/>
-      <c r="Y11" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z11" s="52"/>
-      <c r="AA11" s="52"/>
+      <c r="G11" s="19">
+        <v>0.727599</v>
+      </c>
+      <c r="H11" s="19">
+        <v>0.60540899999999997</v>
+      </c>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="V11" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="W11" s="40"/>
+      <c r="X11" s="40"/>
+      <c r="Y11" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z11" s="40"/>
+      <c r="AA11" s="40"/>
     </row>
     <row r="12" spans="1:33" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="37"/>
@@ -3061,60 +2739,66 @@
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="19">
         <v>0.49201694362984599</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="19">
         <v>0.46757901596611201</v>
       </c>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="53" t="s">
+      <c r="G12" s="19">
+        <v>0.75920500000000002</v>
+      </c>
+      <c r="H12" s="19">
+        <v>0.65982399999999997</v>
+      </c>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="P12" s="53" t="s">
+      <c r="P12" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="53" t="s">
+      <c r="Q12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="R12" s="53" t="s">
+      <c r="R12" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="S12" s="53" t="s">
+      <c r="S12" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="T12" s="53" t="s">
+      <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="52"/>
-      <c r="V12" s="53" t="s">
+      <c r="U12" s="40"/>
+      <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="W12" s="53" t="s">
+      <c r="W12" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="X12" s="53" t="s">
+      <c r="X12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="Y12" s="53" t="s">
+      <c r="Y12" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="Z12" s="53" t="s">
+      <c r="Z12" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AA12" s="53" t="s">
+      <c r="AA12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AC12" s="50" t="s">
-        <v>57</v>
+      <c r="AC12" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="AD12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="AE12" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="AF12" s="12" t="s">
         <v>36</v>
@@ -3132,25 +2816,31 @@
       <c r="D13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="19">
         <v>0.596285434995112</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="19">
         <v>0.93385467579015902</v>
       </c>
-      <c r="L13" s="28">
+      <c r="G13" s="19">
+        <v>0.79081100000000004</v>
+      </c>
+      <c r="H13" s="19">
+        <v>0.94037099999999996</v>
+      </c>
+      <c r="L13" s="24">
         <v>1</v>
       </c>
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="48">
+      <c r="N13" s="41">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="49">
+      <c r="O13" s="43">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="49">
+      <c r="P13" s="43">
         <v>0.50667970022808695</v>
       </c>
       <c r="Q13" s="38">
@@ -3165,13 +2855,13 @@
       <c r="T13" s="38">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="48">
+      <c r="U13" s="41">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="49">
+      <c r="V13" s="43">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="49">
+      <c r="W13" s="43">
         <v>0.516780710329097</v>
       </c>
       <c r="X13" s="38">
@@ -3186,19 +2876,19 @@
       <c r="AA13" s="38">
         <v>0.916585206907787</v>
       </c>
-      <c r="AC13" s="28">
+      <c r="AC13" s="24">
         <v>1</v>
       </c>
-      <c r="AD13" s="56">
+      <c r="AD13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="AE13" s="45">
+      <c r="AE13" s="25">
         <v>0.85630498533724297</v>
       </c>
-      <c r="AF13" s="58">
+      <c r="AF13" s="28">
         <v>0.83805799999999997</v>
       </c>
-      <c r="AG13" s="58">
+      <c r="AG13" s="28">
         <v>0.86933899999999997</v>
       </c>
     </row>
@@ -3209,45 +2899,51 @@
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="19">
         <v>0.55751058976865397</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="19">
         <v>0.76050830889540499</v>
       </c>
-      <c r="L14" s="28">
+      <c r="G14" s="19">
+        <v>0.70837399999999995</v>
+      </c>
+      <c r="H14" s="19">
+        <v>0.754969</v>
+      </c>
+      <c r="L14" s="24">
         <v>2</v>
       </c>
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="48"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
       <c r="Q14" s="38"/>
       <c r="R14" s="38"/>
       <c r="S14" s="38"/>
       <c r="T14" s="38"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
       <c r="X14" s="38"/>
       <c r="Y14" s="38"/>
       <c r="Z14" s="38"/>
       <c r="AA14" s="38"/>
-      <c r="AC14" s="28">
+      <c r="AC14" s="24">
         <v>10</v>
       </c>
-      <c r="AD14" s="56">
+      <c r="AD14" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="AE14" s="58">
+      <c r="AE14" s="28">
         <v>0.94199999999999995</v>
       </c>
-      <c r="AF14" s="58">
+      <c r="AF14" s="28">
         <v>0.92701199999999995</v>
       </c>
-      <c r="AG14" s="58">
+      <c r="AG14" s="28">
         <v>0.94069700000000001</v>
       </c>
     </row>
@@ -3258,28 +2954,34 @@
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="19">
         <v>0.55131964809384104</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="19">
         <v>0.88367546432062505</v>
       </c>
-      <c r="L15" s="28">
+      <c r="G15" s="19">
+        <v>0.88432699999999997</v>
+      </c>
+      <c r="H15" s="19">
+        <v>0.94884299999999999</v>
+      </c>
+      <c r="L15" s="24">
         <v>5</v>
       </c>
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="48"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
       <c r="S15" s="38"/>
       <c r="T15" s="38"/>
-      <c r="U15" s="48"/>
-      <c r="V15" s="49"/>
-      <c r="W15" s="49"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="43"/>
       <c r="X15" s="38"/>
       <c r="Y15" s="38"/>
       <c r="Z15" s="38"/>
@@ -3294,28 +2996,34 @@
       <c r="D16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="19">
         <v>0.47214076246334302</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="19">
         <v>0.493320299771912</v>
       </c>
-      <c r="L16" s="28">
+      <c r="G16" s="19">
+        <v>0.608016</v>
+      </c>
+      <c r="H16" s="19">
+        <v>0.63245399999999996</v>
+      </c>
+      <c r="L16" s="24">
         <v>10</v>
       </c>
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="48"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
       <c r="Q16" s="38"/>
       <c r="R16" s="38"/>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
-      <c r="U16" s="48"/>
-      <c r="V16" s="49"/>
-      <c r="W16" s="49"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="43"/>
       <c r="X16" s="38"/>
       <c r="Y16" s="38"/>
       <c r="Z16" s="38"/>
@@ -3330,28 +3038,34 @@
       <c r="D17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="19">
         <v>0.46953405017921102</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="19">
         <v>0.60182469859889198</v>
       </c>
-      <c r="L17" s="28">
+      <c r="G17" s="19">
+        <v>0.61551</v>
+      </c>
+      <c r="H17" s="19">
+        <v>0.68589100000000003</v>
+      </c>
+      <c r="L17" s="24">
         <v>20</v>
       </c>
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="48"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
       <c r="S17" s="38"/>
       <c r="T17" s="38"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="49"/>
-      <c r="W17" s="49"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
       <c r="X17" s="38"/>
       <c r="Y17" s="38"/>
       <c r="Z17" s="38"/>
@@ -3364,11 +3078,17 @@
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="19">
         <v>0.50993809058325101</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="19">
         <v>0.516780710329097</v>
+      </c>
+      <c r="G18" s="19">
+        <v>0.62463299999999999</v>
+      </c>
+      <c r="H18" s="19">
+        <v>0.68067800000000001</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
@@ -3378,11 +3098,17 @@
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="19">
         <v>0.50863473444118601</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="19">
         <v>0.53828608667318301</v>
+      </c>
+      <c r="G19" s="19">
+        <v>0.63603799999999999</v>
+      </c>
+      <c r="H19" s="19">
+        <v>0.67513800000000002</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
@@ -3394,18 +3120,18 @@
       <c r="D20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="19">
         <v>0.598892147279244</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="19">
         <v>0.928641251221896</v>
       </c>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="54"/>
-      <c r="Q20" s="54"/>
+      <c r="G20" s="19">
+        <v>0.88139500000000004</v>
+      </c>
+      <c r="H20" s="19">
+        <v>0.93581000000000003</v>
+      </c>
     </row>
     <row r="21" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
@@ -3414,19 +3140,24 @@
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="19">
         <v>0.503421309872922</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="19">
         <v>0.83447376995764</v>
       </c>
-      <c r="L21" s="55"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="57"/>
-      <c r="P21" s="57"/>
-      <c r="Q21" s="54"/>
-      <c r="AC21" s="50"/>
+      <c r="G21" s="19">
+        <v>0.84685600000000005</v>
+      </c>
+      <c r="H21" s="19">
+        <v>0.85695699999999997</v>
+      </c>
+      <c r="L21" s="24"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="AC21" s="26"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
@@ -3435,203 +3166,218 @@
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="19">
         <v>0.51482567611599805</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="19">
         <v>0.916585206907787</v>
       </c>
-      <c r="L22" s="55"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="57"/>
-      <c r="O22" s="57"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="54"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="56"/>
-      <c r="AE22" s="45"/>
-      <c r="AF22" s="58"/>
-      <c r="AG22" s="58"/>
+      <c r="G22" s="19">
+        <v>0.90746199999999999</v>
+      </c>
+      <c r="H22" s="19">
+        <v>0.94525899999999996</v>
+      </c>
+      <c r="L22" s="24"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="AC22" s="24"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="25"/>
+      <c r="AF22" s="28"/>
+      <c r="AG22" s="28"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="AC23" s="24"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="28"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="39">
-        <v>0.995</v>
-      </c>
-      <c r="F23" s="39"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="56"/>
-      <c r="AE23" s="58"/>
-      <c r="AF23" s="58"/>
-      <c r="AG23" s="58"/>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
       <c r="B24" s="33"/>
       <c r="C24" s="33"/>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="39">
+        <v>0.995</v>
+      </c>
+      <c r="F24" s="39"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="5"/>
+      <c r="AC24" s="24"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="28"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="54"/>
-    </row>
-    <row r="25" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+    </row>
+    <row r="26" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B26" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C26" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D26" s="21">
         <v>1</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E26" s="23">
         <v>0.83805799999999997</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F26" s="23">
         <v>0.86933899999999997</v>
       </c>
-      <c r="L25" s="55"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="54"/>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="22">
-        <v>2</v>
-      </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25"/>
-    </row>
-    <row r="27" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="24"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
-      <c r="D27" s="22">
-        <v>5</v>
-      </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="D27" s="21">
+        <v>2</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
-      <c r="D28" s="22">
-        <v>10</v>
-      </c>
-      <c r="E28" s="23">
-        <v>0.92701199999999995</v>
-      </c>
-      <c r="F28" s="23">
-        <v>0.94069700000000001</v>
-      </c>
+      <c r="D28" s="21">
+        <v>5</v>
+      </c>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
-      <c r="D29" s="22">
-        <v>20</v>
-      </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="25"/>
+      <c r="D29" s="21">
+        <v>10</v>
+      </c>
+      <c r="E29" s="23">
+        <v>0.92701199999999995</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.94069700000000001</v>
+      </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
       <c r="B30" s="33"/>
-      <c r="C30" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="22">
-        <v>1</v>
-      </c>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="21">
+        <v>20</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="22">
-        <v>2</v>
-      </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="C31" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="21">
+        <v>1</v>
+      </c>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
-      <c r="D32" s="22">
-        <v>3</v>
-      </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="D32" s="21">
+        <v>2</v>
+      </c>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="34"/>
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
-      <c r="D33" s="22">
-        <v>4</v>
-      </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
+      <c r="D33" s="21">
+        <v>3</v>
+      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="22">
-        <v>5</v>
-      </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
+      <c r="D34" s="21">
+        <v>4</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="21">
+        <v>5</v>
+      </c>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
+      <c r="B36" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="27">
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F36" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="51">
@@ -3659,16 +3405,16 @@
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="O13:O17"/>
     <mergeCell ref="P13:P17"/>
-    <mergeCell ref="A23:C24"/>
-    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="A24:C25"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C13:C15"/>
@@ -3681,36 +3427,14 @@
     <mergeCell ref="A9:A22"/>
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:F22 E3:E8">
+  <conditionalFormatting sqref="M13:AA17">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-        <color theme="6" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="percentile" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M13:AA17">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3721,17 +3445,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E3:H22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
-  <dimension ref="A1:O18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF747009-55C2-AB4E-B479-FDB3F7D0E7C7}">
+  <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3741,330 +3477,629 @@
     <col min="4" max="4" width="20.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.83203125" style="13"/>
-    <col min="8" max="9" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="13"/>
+    <col min="8" max="8" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="4.1640625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+    </row>
+    <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="G2" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+    </row>
+    <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="14" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E3" s="38">
         <v>0.85728300000000002</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="13">
-        <v>1</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.85728300000000002</v>
-      </c>
-      <c r="L2" s="45">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="M2" s="45">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="N2" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="46"/>
-    </row>
-    <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="14" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+    </row>
+    <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E4" s="38">
         <v>0.94330400000000003</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="13">
-        <v>2</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.90257399999999999</v>
-      </c>
-      <c r="L3" s="44">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="M3" s="45">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0.40795047246660099</v>
-      </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="13">
-        <v>5</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.93776499999999996</v>
-      </c>
-      <c r="L4" s="44">
-        <v>0.93840000000000001</v>
-      </c>
-      <c r="M4" s="45">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="37"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37" t="s">
+        <v>26</v>
+      </c>
       <c r="D5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="18">
-        <v>0.59237536656891498</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="13">
-        <v>10</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0.94330400000000003</v>
-      </c>
-      <c r="L5" s="45">
-        <v>0.94200065167807101</v>
-      </c>
-      <c r="M5" s="45">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-    </row>
-    <row r="6" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0.84620399999999996</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+    </row>
+    <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="37"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="18">
-        <v>0.93385467579015902</v>
-      </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="13">
-        <v>20</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0.93548399999999998</v>
-      </c>
-      <c r="L6" s="45">
-        <v>0.93711306614532397</v>
-      </c>
-      <c r="M6" s="45">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-    </row>
-    <row r="7" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="42"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.86510299999999996</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+    </row>
+    <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="15"/>
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="19">
+        <v>0.49234278266536302</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.40795047246660099</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0.64418399999999998</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.603128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0.51710654936461298</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.59237536656891498</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.64678999999999998</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.63962200000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="19">
+        <v>0.54089279895731501</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.50667970022808695</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0.727599</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.60540899999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0.49201694362984599</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.46757901596611201</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0.75920500000000002</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0.65982399999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0.596285434995112</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.93385467579015902</v>
+      </c>
+      <c r="G11" s="19">
+        <v>0.79081100000000004</v>
+      </c>
+      <c r="H11" s="19">
+        <v>0.94037099999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="19">
+        <v>0.55751058976865397</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0.76050830889540499</v>
+      </c>
+      <c r="G12" s="19">
+        <v>0.70837399999999995</v>
+      </c>
+      <c r="H12" s="19">
+        <v>0.754969</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0.55131964809384104</v>
+      </c>
+      <c r="F13" s="19">
+        <v>0.88367546432062505</v>
+      </c>
+      <c r="G13" s="19">
+        <v>0.88432699999999997</v>
+      </c>
+      <c r="H13" s="19">
+        <v>0.94884299999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.47214076246334302</v>
+      </c>
+      <c r="F14" s="19">
         <v>0.493320299771912</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="13" t="s">
+      <c r="G14" s="19">
+        <v>0.608016</v>
+      </c>
+      <c r="H14" s="19">
+        <v>0.63245399999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="19">
+        <v>0.46953405017921102</v>
+      </c>
+      <c r="F15" s="19">
+        <v>0.60182469859889198</v>
+      </c>
+      <c r="G15" s="19">
+        <v>0.61551</v>
+      </c>
+      <c r="H15" s="19">
+        <v>0.68589100000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0.50993809058325101</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0.516780710329097</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0.62463299999999999</v>
+      </c>
+      <c r="H16" s="19">
+        <v>0.68067800000000001</v>
+      </c>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="19">
+        <v>0.50863473444118601</v>
+      </c>
+      <c r="F17" s="19">
+        <v>0.53828608667318301</v>
+      </c>
+      <c r="G17" s="19">
+        <v>0.63603799999999999</v>
+      </c>
+      <c r="H17" s="19">
+        <v>0.67513800000000002</v>
+      </c>
+      <c r="N17" s="37"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="44"/>
+      <c r="T17" s="44"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="19">
+        <v>0.598892147279244</v>
+      </c>
+      <c r="F18" s="19">
+        <v>0.928641251221896</v>
+      </c>
+      <c r="G18" s="19">
+        <v>0.88139500000000004</v>
+      </c>
+      <c r="H18" s="19">
+        <v>0.93581000000000003</v>
+      </c>
+      <c r="N18" s="37"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="19">
+        <v>0.503421309872922</v>
+      </c>
+      <c r="F19" s="19">
+        <v>0.83447376995764</v>
+      </c>
+      <c r="G19" s="19">
+        <v>0.84685600000000005</v>
+      </c>
+      <c r="H19" s="19">
+        <v>0.85695699999999997</v>
+      </c>
+      <c r="N19" s="37"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="19">
+        <v>0.51482567611599805</v>
+      </c>
+      <c r="F20" s="19">
+        <v>0.916585206907787</v>
+      </c>
+      <c r="G20" s="19">
+        <v>0.90746199999999999</v>
+      </c>
+      <c r="H20" s="19">
+        <v>0.94525899999999996</v>
+      </c>
+      <c r="N20" s="37"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="44"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N21" s="37"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+    </row>
+    <row r="27" spans="1:20" ht="80" x14ac:dyDescent="0.2">
+      <c r="P27" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="18">
-        <v>0.60182469859889198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="13" t="s">
+      <c r="Q27" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="R27" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="S27" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="20">
-        <v>0.928641251221896</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="22" t="s">
+      <c r="T27" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N28" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="13">
+        <v>1</v>
+      </c>
+      <c r="P28" s="5">
+        <v>0.85728300000000002</v>
+      </c>
+      <c r="Q28" s="25">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="R28" s="25">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S28" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="T28" s="44"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N29" s="37"/>
+      <c r="O29" s="13">
+        <v>2</v>
+      </c>
+      <c r="P29" s="5">
+        <v>0.90257399999999999</v>
+      </c>
+      <c r="Q29" s="17">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="R29" s="25">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S29" s="44"/>
+      <c r="T29" s="44"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N30" s="37"/>
+      <c r="O30" s="13">
+        <v>5</v>
+      </c>
+      <c r="P30" s="5">
+        <v>0.93776499999999996</v>
+      </c>
+      <c r="Q30" s="17">
+        <v>0.93840000000000001</v>
+      </c>
+      <c r="R30" s="25">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S30" s="44"/>
+      <c r="T30" s="44"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N31" s="37"/>
+      <c r="O31" s="13">
+        <v>10</v>
+      </c>
+      <c r="P31" s="5">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="Q31" s="25">
+        <v>0.94200065167807101</v>
+      </c>
+      <c r="R31" s="25">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S31" s="44"/>
+      <c r="T31" s="44"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N32" s="37"/>
+      <c r="O32" s="13">
         <v>20</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="22">
-        <v>1</v>
-      </c>
-      <c r="E12" s="25">
-        <v>0.86933899999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="22">
-        <v>2</v>
-      </c>
-      <c r="E13" s="25"/>
-    </row>
-    <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="22">
-        <v>5</v>
-      </c>
-      <c r="E14" s="25"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="22">
-        <v>10</v>
-      </c>
-      <c r="E15" s="25">
-        <v>0.94099999999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="22">
-        <v>20</v>
-      </c>
-      <c r="E16" s="22"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+      <c r="P32" s="5">
+        <v>0.93548399999999998</v>
+      </c>
+      <c r="Q32" s="25">
+        <v>0.93711306614532397</v>
+      </c>
+      <c r="R32" s="25">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S32" s="44"/>
+      <c r="T32" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="N2:O6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="B4:C6"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B7:C9"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="B17:D17"/>
+  <mergeCells count="20">
+    <mergeCell ref="N28:N32"/>
+    <mergeCell ref="S28:T32"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="N17:N21"/>
+    <mergeCell ref="S17:T21"/>
+    <mergeCell ref="A3:B6"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:M6">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="P17:R21">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4075,8 +4110,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E3:H20">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added gemini and qwen external correction code
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C53430-2348-394D-8A1F-96BE99BCAA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AA355E-BDFE-8540-96A5-B4CDF0B52C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="56">
   <si>
     <t>llama</t>
   </si>
@@ -185,28 +185,6 @@
 Driven</t>
   </si>
   <si>
-    <t>heuristics</t>
-  </si>
-  <si>
-    <t>zero_shot_with_
-heur_value_comb</t>
-  </si>
-  <si>
-    <t>few_shot_with_
-heur_value_comb</t>
-  </si>
-  <si>
-    <t>few_shot_with_
-heur_value_angle</t>
-  </si>
-  <si>
-    <t>zero_shot_with_
-heur_value_angle</t>
-  </si>
-  <si>
-    <t>tonight</t>
-  </si>
-  <si>
     <t>Heuristic Hint</t>
   </si>
   <si>
@@ -230,6 +208,27 @@
   </si>
   <si>
     <t>qwen</t>
+  </si>
+  <si>
+    <t>zs-angle</t>
+  </si>
+  <si>
+    <t>fs-angle</t>
+  </si>
+  <si>
+    <t>zs-comb</t>
+  </si>
+  <si>
+    <t>fs-comb</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>min_angle threshold</t>
+  </si>
+  <si>
+    <t>models</t>
   </si>
 </sst>
 </file>
@@ -327,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -409,6 +408,12 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,50 +426,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,23 +833,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -869,7 +871,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -896,7 +898,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -921,7 +923,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -946,7 +948,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -971,7 +973,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -998,7 +1000,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1023,7 +1025,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1048,7 +1050,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1115,20 +1117,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1163,7 +1165,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1201,7 +1203,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1239,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1273,7 +1275,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1309,7 +1311,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1347,7 +1349,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1385,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1419,7 +1421,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1455,7 +1457,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1493,7 +1495,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1531,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1565,7 +1567,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1635,23 +1637,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1673,7 +1675,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1700,7 +1702,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1725,7 +1727,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1750,7 +1752,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +1777,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1802,7 +1804,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1827,7 +1829,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1852,7 +1854,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1919,20 +1921,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1967,7 +1969,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2005,7 +2007,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2043,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2077,7 +2079,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2113,7 +2115,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2161,7 +2163,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +2200,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2234,7 +2236,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2270,7 +2272,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2308,7 +2310,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2344,7 +2346,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2380,7 +2382,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2432,7 +2434,7 @@
   <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2459,150 +2461,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="36"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="46" t="s">
-        <v>54</v>
+      <c r="G2" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="37">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="37">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
       <c r="J4" s="5"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="37">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
       <c r="J5" s="5"/>
       <c r="K5" s="17"/>
       <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="37">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="37">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
       <c r="J7" s="5"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="37">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
       <c r="J8" s="5"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="44" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
@@ -2621,31 +2623,31 @@
       <c r="H9" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L9" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="M9" s="42"/>
-      <c r="N9" s="40" t="s">
+      <c r="L9" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="36"/>
+      <c r="N9" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="40"/>
-      <c r="Y9" s="40"/>
-      <c r="Z9" s="40"/>
-      <c r="AA9" s="40"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="35"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37" t="s">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -2663,31 +2665,31 @@
       <c r="H10" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="40" t="s">
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="40"/>
-      <c r="T10" s="40"/>
-      <c r="U10" s="40" t="s">
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="40"/>
-      <c r="W10" s="40"/>
-      <c r="X10" s="40"/>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="40"/>
-      <c r="AA10" s="40"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="35"/>
+      <c r="AA10" s="35"/>
     </row>
     <row r="11" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
@@ -2703,39 +2705,39 @@
       <c r="H11" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="O11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="S11" s="40"/>
-      <c r="T11" s="40"/>
-      <c r="U11" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="V11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="W11" s="40"/>
-      <c r="X11" s="40"/>
-      <c r="Y11" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z11" s="40"/>
-      <c r="AA11" s="40"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="V11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="W11" s="35"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z11" s="35"/>
+      <c r="AA11" s="35"/>
     </row>
     <row r="12" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
@@ -2751,9 +2753,9 @@
       <c r="H12" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="40"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="35"/>
       <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
@@ -2772,7 +2774,7 @@
       <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="40"/>
+      <c r="U12" s="35"/>
       <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
@@ -2792,13 +2794,13 @@
         <v>27</v>
       </c>
       <c r="AC12" s="26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AD12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="AE12" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AF12" s="12" t="s">
         <v>36</v>
@@ -2808,9 +2810,9 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37" t="s">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -2834,46 +2836,46 @@
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="41">
+      <c r="N13" s="38">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="43">
+      <c r="O13" s="39">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="43">
+      <c r="P13" s="39">
         <v>0.50667970022808695</v>
       </c>
-      <c r="Q13" s="38">
+      <c r="Q13" s="37">
         <v>0.46757901596611201</v>
       </c>
-      <c r="R13" s="38">
+      <c r="R13" s="37">
         <v>0.93385467579015902</v>
       </c>
-      <c r="S13" s="38">
+      <c r="S13" s="37">
         <v>0.76050830889540499</v>
       </c>
-      <c r="T13" s="38">
+      <c r="T13" s="37">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="41">
+      <c r="U13" s="38">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="43">
+      <c r="V13" s="39">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="43">
+      <c r="W13" s="39">
         <v>0.516780710329097</v>
       </c>
-      <c r="X13" s="38">
+      <c r="X13" s="37">
         <v>0.53828608667318301</v>
       </c>
-      <c r="Y13" s="38">
+      <c r="Y13" s="37">
         <v>0.928641251221896</v>
       </c>
-      <c r="Z13" s="38">
+      <c r="Z13" s="37">
         <v>0.83447376995764</v>
       </c>
-      <c r="AA13" s="38">
+      <c r="AA13" s="37">
         <v>0.916585206907787</v>
       </c>
       <c r="AC13" s="24">
@@ -2893,9 +2895,9 @@
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -2917,20 +2919,20 @@
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="41"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="43"/>
-      <c r="W14" s="43"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="37"/>
+      <c r="AA14" s="37"/>
       <c r="AC14" s="24">
         <v>10</v>
       </c>
@@ -2948,9 +2950,9 @@
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -2972,24 +2974,24 @@
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="41"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="38"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="43"/>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="38"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="39"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+      <c r="Z15" s="37"/>
+      <c r="AA15" s="37"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="15"/>
@@ -3014,25 +3016,25 @@
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="41"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="43"/>
-      <c r="W16" s="43"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="38"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="38"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="37"/>
+      <c r="Z16" s="37"/>
+      <c r="AA16" s="37"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37" t="s">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3056,25 +3058,25 @@
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="43"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="37"/>
+      <c r="Z17" s="37"/>
+      <c r="AA17" s="37"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
@@ -3092,9 +3094,9 @@
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3112,9 +3114,9 @@
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -3134,9 +3136,9 @@
       </c>
     </row>
     <row r="21" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
@@ -3160,9 +3162,9 @@
       <c r="AC21" s="26"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
@@ -3210,18 +3212,18 @@
       <c r="AG23" s="28"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="39">
+      <c r="E24" s="42">
         <v>0.995</v>
       </c>
-      <c r="F24" s="39"/>
+      <c r="F24" s="42"/>
       <c r="L24" s="24"/>
       <c r="M24" s="5"/>
       <c r="AC24" s="24"/>
@@ -3231,27 +3233,27 @@
       <c r="AG24" s="28"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
       <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
       <c r="L25" s="24"/>
       <c r="M25" s="5"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="41" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="21">
@@ -3267,9 +3269,9 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
       <c r="D27" s="21">
         <v>2</v>
       </c>
@@ -3277,9 +3279,9 @@
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
       <c r="D28" s="21">
         <v>5</v>
       </c>
@@ -3287,9 +3289,9 @@
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
       <c r="D29" s="21">
         <v>10</v>
       </c>
@@ -3301,9 +3303,9 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
       <c r="D30" s="21">
         <v>20</v>
       </c>
@@ -3311,9 +3313,9 @@
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33" t="s">
+      <c r="A31" s="40"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="21">
@@ -3323,9 +3325,9 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
       <c r="D32" s="21">
         <v>2</v>
       </c>
@@ -3333,9 +3335,9 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
       <c r="D33" s="21">
         <v>3</v>
       </c>
@@ -3343,9 +3345,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
       <c r="D34" s="21">
         <v>4</v>
       </c>
@@ -3353,9 +3355,9 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
       <c r="D35" s="21">
         <v>5</v>
       </c>
@@ -3363,12 +3365,12 @@
       <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
-      <c r="B36" s="35" t="s">
+      <c r="A36" s="40"/>
+      <c r="B36" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
@@ -3381,6 +3383,41 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A9:A22"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="AA13:AA17"/>
+    <mergeCell ref="N10:T10"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="P13:P17"/>
     <mergeCell ref="N9:AA9"/>
     <mergeCell ref="L9:M12"/>
     <mergeCell ref="Q13:Q17"/>
@@ -3397,42 +3434,19 @@
     <mergeCell ref="X13:X17"/>
     <mergeCell ref="Y13:Y17"/>
     <mergeCell ref="Z13:Z17"/>
-    <mergeCell ref="AA13:AA17"/>
-    <mergeCell ref="N10:T10"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="P13:P17"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A9:A22"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="C26:C30"/>
   </mergeCells>
+  <conditionalFormatting sqref="E3:H22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color theme="6" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M13:AA17">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -3442,18 +3456,6 @@
         <color theme="1" tint="0.499984740745262"/>
         <color theme="0" tint="-4.9989318521683403E-2"/>
         <color theme="6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:H22">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <color theme="6" tint="-0.249977111117893"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3467,7 +3469,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3480,170 +3482,232 @@
     <col min="8" max="8" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="4.1640625" style="13" customWidth="1"/>
     <col min="12" max="12" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="17.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="13"/>
+    <col min="13" max="13" width="3.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="48" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="46" t="s">
-        <v>54</v>
+      <c r="G2" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
+      <c r="L2" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="46">
+        <v>1</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="37">
+        <v>0.85728300000000002</v>
+      </c>
+      <c r="P2" s="17">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="Q2" s="17">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="R2" s="17">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S2" s="17">
+        <v>0.94525904203323496</v>
+      </c>
+      <c r="T2" s="17">
+        <v>0.94819159335288306</v>
+      </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="37">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="37"/>
+      <c r="P3" s="17">
+        <v>0.90700000000000003</v>
+      </c>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="37">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="37"/>
+      <c r="P4" s="17">
+        <v>0.94899999999999995</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="37">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="46">
+        <v>2</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="37">
+        <v>0.90257399999999999</v>
+      </c>
+      <c r="P5" s="17">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="R5" s="17">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S5" s="17">
+        <v>0.94558488106875205</v>
+      </c>
+      <c r="T5" s="17">
+        <v>0.94688823721081705</v>
+      </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="37">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="37"/>
+      <c r="P6" s="17">
+        <v>0.90700000000000003</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="44" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="15"/>
@@ -3662,11 +3726,20 @@
       <c r="H7" s="19">
         <v>0.603128</v>
       </c>
+      <c r="L7" s="44"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="37"/>
+      <c r="P7" s="17">
+        <v>0.94899999999999995</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37" t="s">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -3684,11 +3757,36 @@
       <c r="H8" s="19">
         <v>0.63962200000000002</v>
       </c>
+      <c r="L8" s="44"/>
+      <c r="M8" s="46">
+        <v>5</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="37">
+        <v>0.93776499999999996</v>
+      </c>
+      <c r="P8" s="17">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>0.93840000000000001</v>
+      </c>
+      <c r="R8" s="17">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S8" s="17">
+        <v>0.94656239817530097</v>
+      </c>
+      <c r="T8" s="17">
+        <v>0.94623655913978499</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
@@ -3704,11 +3802,20 @@
       <c r="H9" s="19">
         <v>0.60540899999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="37"/>
+      <c r="P9" s="17">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -3724,11 +3831,20 @@
       <c r="H10" s="19">
         <v>0.65982399999999997</v>
       </c>
+      <c r="L10" s="44"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="37"/>
+      <c r="P10" s="17">
+        <v>0.94899999999999995</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -3746,11 +3862,34 @@
       <c r="H11" s="19">
         <v>0.94037099999999996</v>
       </c>
+      <c r="L11" s="44"/>
+      <c r="M11" s="46">
+        <v>10</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="37">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="P11" s="17">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>0.94200065167807101</v>
+      </c>
+      <c r="R11" s="17">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S11" s="17">
+        <v>0.94851743238840003</v>
+      </c>
+      <c r="T11" s="17"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
@@ -3766,11 +3905,20 @@
       <c r="H12" s="19">
         <v>0.754969</v>
       </c>
+      <c r="L12" s="44"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="37"/>
+      <c r="P12" s="17">
+        <v>0.90700000000000003</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
@@ -3786,10 +3934,19 @@
       <c r="H13" s="19">
         <v>0.94884299999999999</v>
       </c>
+      <c r="L13" s="44"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="37"/>
+      <c r="P13" s="17">
+        <v>0.94899999999999995</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="15"/>
@@ -3808,11 +3965,34 @@
       <c r="H14" s="19">
         <v>0.63245399999999996</v>
       </c>
+      <c r="L14" s="44"/>
+      <c r="M14" s="46">
+        <v>20</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="37">
+        <v>0.93548399999999998</v>
+      </c>
+      <c r="P14" s="17">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>0.93711306614532397</v>
+      </c>
+      <c r="R14" s="17">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="S14" s="17">
+        <v>0.94428152492668604</v>
+      </c>
+      <c r="T14" s="17"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -3830,11 +4010,20 @@
       <c r="H15" s="19">
         <v>0.68589100000000003</v>
       </c>
+      <c r="L15" s="44"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="37"/>
+      <c r="P15" s="17">
+        <v>0.90700000000000003</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -3850,15 +4039,20 @@
       <c r="H16" s="19">
         <v>0.68067800000000001</v>
       </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16" s="37"/>
+      <c r="P16" s="17">
+        <v>0.94899999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -3874,17 +4068,13 @@
       <c r="H17" s="19">
         <v>0.67513800000000002</v>
       </c>
-      <c r="N17" s="37"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37" t="s">
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -3902,17 +4092,17 @@
       <c r="H18" s="19">
         <v>0.93581000000000003</v>
       </c>
-      <c r="N18" s="37"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="17"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
-      <c r="S18" s="44"/>
-      <c r="T18" s="44"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
@@ -3928,17 +4118,13 @@
       <c r="H19" s="19">
         <v>0.85695699999999997</v>
       </c>
-      <c r="N19" s="37"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
@@ -3954,134 +4140,107 @@
       <c r="H20" s="19">
         <v>0.94525899999999996</v>
       </c>
-      <c r="N20" s="37"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="44"/>
-      <c r="T20" s="44"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N21" s="37"/>
-      <c r="P21" s="5"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M21" s="5"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
-      <c r="S21" s="44"/>
-      <c r="T21" s="44"/>
-    </row>
-    <row r="27" spans="1:20" ht="80" x14ac:dyDescent="0.2">
-      <c r="P27" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q27" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="R27" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="S27" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="T27" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N28" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="O28" s="13">
-        <v>1</v>
-      </c>
-      <c r="P28" s="5">
-        <v>0.85728300000000002</v>
-      </c>
-      <c r="Q28" s="25">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="R28" s="25">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="S28" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="T28" s="44"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N29" s="37"/>
-      <c r="O29" s="13">
-        <v>2</v>
-      </c>
-      <c r="P29" s="5">
-        <v>0.90257399999999999</v>
-      </c>
-      <c r="Q29" s="17">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="R29" s="25">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="S29" s="44"/>
-      <c r="T29" s="44"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N30" s="37"/>
-      <c r="O30" s="13">
-        <v>5</v>
-      </c>
-      <c r="P30" s="5">
-        <v>0.93776499999999996</v>
-      </c>
-      <c r="Q30" s="17">
-        <v>0.93840000000000001</v>
-      </c>
-      <c r="R30" s="25">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="S30" s="44"/>
-      <c r="T30" s="44"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N31" s="37"/>
-      <c r="O31" s="13">
-        <v>10</v>
-      </c>
-      <c r="P31" s="5">
-        <v>0.94330400000000003</v>
-      </c>
-      <c r="Q31" s="25">
-        <v>0.94200065167807101</v>
-      </c>
-      <c r="R31" s="25">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="S31" s="44"/>
-      <c r="T31" s="44"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N32" s="37"/>
-      <c r="O32" s="13">
-        <v>20</v>
-      </c>
-      <c r="P32" s="5">
-        <v>0.93548399999999998</v>
-      </c>
-      <c r="Q32" s="25">
-        <v>0.93711306614532397</v>
-      </c>
-      <c r="R32" s="25">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="S32" s="44"/>
-      <c r="T32" s="44"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M24" s="5"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L27" s="30"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L28" s="5"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L29" s="5"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L30" s="5"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="25"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L31" s="5"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="17"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L32" s="5"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="N28:N32"/>
-    <mergeCell ref="S28:T32"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="N17:N21"/>
-    <mergeCell ref="S17:T21"/>
+  <mergeCells count="28">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="M28:M32"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
     <mergeCell ref="A3:B6"/>
     <mergeCell ref="A7:A20"/>
     <mergeCell ref="B7:B13"/>
@@ -4090,26 +4249,15 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="O2:O4"/>
   </mergeCells>
-  <conditionalFormatting sqref="P17:R21">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E3:H20">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
modified qwen ec evaluation code; evaluate on a subset of 1000 pairs.
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD9EE14-9B6A-4A40-8C59-4D17CA9A64FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCD9FD8-5963-FD46-B6F5-B94503972F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -426,6 +426,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,47 +441,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,23 +845,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -910,7 +910,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -935,7 +935,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -985,7 +985,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1012,7 +1012,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1062,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1129,20 +1129,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1177,7 +1177,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1215,7 +1215,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1287,7 +1287,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1323,7 +1323,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1361,7 +1361,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1397,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1507,7 +1507,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1649,23 +1649,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1687,7 +1687,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1714,7 +1714,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1739,7 +1739,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1764,7 +1764,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1789,7 +1789,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1816,7 +1816,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1841,7 +1841,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1866,7 +1866,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1933,20 +1933,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1981,7 +1981,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2019,7 +2019,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2055,7 +2055,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2091,7 +2091,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2127,7 +2127,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2175,7 +2175,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2248,7 +2248,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2284,7 +2284,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2322,7 +2322,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2358,7 +2358,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2394,7 +2394,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2473,24 +2473,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -2505,120 +2505,120 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="40">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="40">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
       <c r="J4" s="5"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="40">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
       <c r="J5" s="5"/>
       <c r="K5" s="17"/>
       <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="40">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41" t="s">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="40">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
       <c r="J7" s="5"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="40">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
       <c r="J8" s="5"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
@@ -2637,31 +2637,31 @@
       <c r="H9" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L9" s="46" t="s">
+      <c r="L9" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="46"/>
-      <c r="N9" s="44" t="s">
+      <c r="M9" s="39"/>
+      <c r="N9" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="44"/>
-      <c r="Z9" s="44"/>
-      <c r="AA9" s="44"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41" t="s">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -2679,31 +2679,31 @@
       <c r="H10" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="44" t="s">
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="44"/>
-      <c r="U10" s="44" t="s">
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="44"/>
-      <c r="W10" s="44"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="44"/>
-      <c r="AA10" s="44"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
     </row>
     <row r="11" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
@@ -2719,39 +2719,39 @@
       <c r="H11" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46" t="s">
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="44" t="s">
+      <c r="O11" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44" t="s">
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="44"/>
-      <c r="T11" s="44"/>
-      <c r="U11" s="46" t="s">
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="44" t="s">
+      <c r="V11" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="W11" s="44"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="44" t="s">
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="Z11" s="44"/>
-      <c r="AA11" s="44"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
     </row>
     <row r="12" spans="1:33" ht="20" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
@@ -2767,9 +2767,9 @@
       <c r="H12" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="44"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="38"/>
       <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
@@ -2788,7 +2788,7 @@
       <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="44"/>
+      <c r="U12" s="38"/>
       <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
@@ -2824,9 +2824,9 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41" t="s">
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -2850,46 +2850,46 @@
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="45">
+      <c r="N13" s="41">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="42">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="47">
+      <c r="P13" s="42">
         <v>0.50667970022808695</v>
       </c>
-      <c r="Q13" s="42">
+      <c r="Q13" s="40">
         <v>0.46757901596611201</v>
       </c>
-      <c r="R13" s="42">
+      <c r="R13" s="40">
         <v>0.93385467579015902</v>
       </c>
-      <c r="S13" s="42">
+      <c r="S13" s="40">
         <v>0.76050830889540499</v>
       </c>
-      <c r="T13" s="42">
+      <c r="T13" s="40">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="45">
+      <c r="U13" s="41">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="47">
+      <c r="V13" s="42">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="47">
+      <c r="W13" s="42">
         <v>0.516780710329097</v>
       </c>
-      <c r="X13" s="42">
+      <c r="X13" s="40">
         <v>0.53828608667318301</v>
       </c>
-      <c r="Y13" s="42">
+      <c r="Y13" s="40">
         <v>0.928641251221896</v>
       </c>
-      <c r="Z13" s="42">
+      <c r="Z13" s="40">
         <v>0.83447376995764</v>
       </c>
-      <c r="AA13" s="42">
+      <c r="AA13" s="40">
         <v>0.916585206907787</v>
       </c>
       <c r="AC13" s="24">
@@ -2909,9 +2909,9 @@
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -2933,20 +2933,20 @@
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="45"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="42"/>
-      <c r="Y14" s="42"/>
-      <c r="Z14" s="42"/>
-      <c r="AA14" s="42"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="42"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="40"/>
+      <c r="Z14" s="40"/>
+      <c r="AA14" s="40"/>
       <c r="AC14" s="24">
         <v>10</v>
       </c>
@@ -2964,9 +2964,9 @@
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -2988,24 +2988,24 @@
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="45"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="47"/>
-      <c r="X15" s="42"/>
-      <c r="Y15" s="42"/>
-      <c r="Z15" s="42"/>
-      <c r="AA15" s="42"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="42"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="40"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41" t="s">
+      <c r="A16" s="47"/>
+      <c r="B16" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="15"/>
@@ -3030,25 +3030,25 @@
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="45"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="47"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="42"/>
-      <c r="Z16" s="42"/>
-      <c r="AA16" s="42"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="42"/>
+      <c r="W16" s="42"/>
+      <c r="X16" s="40"/>
+      <c r="Y16" s="40"/>
+      <c r="Z16" s="40"/>
+      <c r="AA16" s="40"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41" t="s">
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3072,25 +3072,25 @@
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="45"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="42"/>
-      <c r="Y17" s="42"/>
-      <c r="Z17" s="42"/>
-      <c r="AA17" s="42"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="42"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="40"/>
+      <c r="Z17" s="40"/>
+      <c r="AA17" s="40"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
@@ -3108,9 +3108,9 @@
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3128,9 +3128,9 @@
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41" t="s">
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -3150,9 +3150,9 @@
       </c>
     </row>
     <row r="21" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
@@ -3176,9 +3176,9 @@
       <c r="AC21" s="26"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
@@ -3226,18 +3226,18 @@
       <c r="AG23" s="28"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="45">
         <v>0.995</v>
       </c>
-      <c r="F24" s="43"/>
+      <c r="F24" s="45"/>
       <c r="L24" s="24"/>
       <c r="M24" s="5"/>
       <c r="AC24" s="24"/>
@@ -3247,27 +3247,27 @@
       <c r="AG24" s="28"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
       <c r="L25" s="24"/>
       <c r="M25" s="5"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="44" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="21">
@@ -3283,9 +3283,9 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="21">
         <v>2</v>
       </c>
@@ -3293,9 +3293,9 @@
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="21">
         <v>5</v>
       </c>
@@ -3303,9 +3303,9 @@
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="21">
         <v>10</v>
       </c>
@@ -3317,9 +3317,9 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="21">
         <v>20</v>
       </c>
@@ -3327,9 +3327,9 @@
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37" t="s">
+      <c r="A31" s="43"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="21">
@@ -3339,9 +3339,9 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="21">
         <v>2</v>
       </c>
@@ -3349,9 +3349,9 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
       <c r="D33" s="21">
         <v>3</v>
       </c>
@@ -3359,9 +3359,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
       <c r="D34" s="21">
         <v>4</v>
       </c>
@@ -3369,9 +3369,9 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="21">
         <v>5</v>
       </c>
@@ -3379,12 +3379,12 @@
       <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
-      <c r="B36" s="39" t="s">
+      <c r="A36" s="43"/>
+      <c r="B36" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
@@ -3397,6 +3397,41 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A9:A22"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="AA13:AA17"/>
+    <mergeCell ref="N10:T10"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="P13:P17"/>
     <mergeCell ref="N9:AA9"/>
     <mergeCell ref="L9:M12"/>
     <mergeCell ref="Q13:Q17"/>
@@ -3413,41 +3448,6 @@
     <mergeCell ref="X13:X17"/>
     <mergeCell ref="Y13:Y17"/>
     <mergeCell ref="Z13:Z17"/>
-    <mergeCell ref="AA13:AA17"/>
-    <mergeCell ref="N10:T10"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="P13:P17"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A9:A22"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="C26:C30"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H22">
     <cfRule type="colorScale" priority="1">
@@ -3483,7 +3483,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3509,18 +3509,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="M1" s="14"/>
       <c r="N1" s="24" t="s">
         <v>55</v>
@@ -3545,10 +3545,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -3564,7 +3564,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="47" t="s">
         <v>54</v>
       </c>
       <c r="M2" s="49">
@@ -3573,7 +3573,7 @@
       <c r="N2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="42">
+      <c r="O2" s="40">
         <v>0.85728300000000002</v>
       </c>
       <c r="P2" s="17">
@@ -3593,91 +3593,91 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="40">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="41"/>
+      <c r="L3" s="47"/>
       <c r="M3" s="49"/>
       <c r="N3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="42"/>
+      <c r="O3" s="40"/>
       <c r="P3" s="17">
         <v>0.90700000000000003</v>
       </c>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="40">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="41"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="49"/>
       <c r="N4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="42"/>
+      <c r="O4" s="40"/>
       <c r="P4" s="17">
         <v>0.94899999999999995</v>
       </c>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="40">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="41"/>
+      <c r="L5" s="47"/>
       <c r="M5" s="49">
         <v>2</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="42">
+      <c r="O5" s="40">
         <v>0.90257399999999999</v>
       </c>
       <c r="P5" s="17">
@@ -3697,38 +3697,38 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="40">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="41"/>
+      <c r="L6" s="47"/>
       <c r="M6" s="49"/>
       <c r="N6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="42"/>
+      <c r="O6" s="40"/>
       <c r="P6" s="17">
         <v>0.90700000000000003</v>
       </c>
-      <c r="S6" s="50"/>
-      <c r="T6" s="50"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="15"/>
@@ -3747,22 +3747,22 @@
       <c r="H7" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L7" s="41"/>
+      <c r="L7" s="47"/>
       <c r="M7" s="49"/>
       <c r="N7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="42"/>
+      <c r="O7" s="40"/>
       <c r="P7" s="17">
         <v>0.94899999999999995</v>
       </c>
-      <c r="S7" s="50"/>
-      <c r="T7" s="50"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41" t="s">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -3780,14 +3780,14 @@
       <c r="H8" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L8" s="41"/>
+      <c r="L8" s="47"/>
       <c r="M8" s="49">
         <v>5</v>
       </c>
       <c r="N8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="42">
+      <c r="O8" s="40">
         <v>0.93776499999999996</v>
       </c>
       <c r="P8" s="17">
@@ -3807,9 +3807,9 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
@@ -3825,22 +3825,22 @@
       <c r="H9" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L9" s="41"/>
+      <c r="L9" s="47"/>
       <c r="M9" s="49"/>
       <c r="N9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="42"/>
+      <c r="O9" s="40"/>
       <c r="P9" s="17">
         <v>0.90700000000000003</v>
       </c>
-      <c r="S9" s="50"/>
-      <c r="T9" s="50"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
     </row>
     <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -3856,22 +3856,22 @@
       <c r="H10" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L10" s="41"/>
+      <c r="L10" s="47"/>
       <c r="M10" s="49"/>
       <c r="N10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="42"/>
+      <c r="O10" s="40"/>
       <c r="P10" s="17">
         <v>0.94899999999999995</v>
       </c>
-      <c r="S10" s="50"/>
-      <c r="T10" s="50"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -3889,14 +3889,14 @@
       <c r="H11" s="19">
         <v>0.94037099999999996</v>
       </c>
-      <c r="L11" s="41"/>
+      <c r="L11" s="47"/>
       <c r="M11" s="49">
         <v>10</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="42">
+      <c r="O11" s="40">
         <v>0.94330400000000003</v>
       </c>
       <c r="P11" s="17">
@@ -3916,9 +3916,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
@@ -3934,22 +3934,22 @@
       <c r="H12" s="19">
         <v>0.754969</v>
       </c>
-      <c r="L12" s="41"/>
+      <c r="L12" s="47"/>
       <c r="M12" s="49"/>
       <c r="N12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="42"/>
+      <c r="O12" s="40"/>
       <c r="P12" s="17">
         <v>0.90700000000000003</v>
       </c>
-      <c r="S12" s="50"/>
-      <c r="T12" s="50"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
@@ -3965,21 +3965,21 @@
       <c r="H13" s="19">
         <v>0.94884299999999999</v>
       </c>
-      <c r="L13" s="41"/>
+      <c r="L13" s="47"/>
       <c r="M13" s="49"/>
       <c r="N13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="42"/>
+      <c r="O13" s="40"/>
       <c r="P13" s="17">
         <v>0.94899999999999995</v>
       </c>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41" t="s">
+      <c r="A14" s="47"/>
+      <c r="B14" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="15"/>
@@ -3998,14 +3998,14 @@
       <c r="H14" s="19">
         <v>0.63245399999999996</v>
       </c>
-      <c r="L14" s="41"/>
+      <c r="L14" s="47"/>
       <c r="M14" s="49">
         <v>20</v>
       </c>
       <c r="N14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="42">
+      <c r="O14" s="40">
         <v>0.93548399999999998</v>
       </c>
       <c r="P14" s="17">
@@ -4025,9 +4025,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41" t="s">
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -4045,22 +4045,22 @@
       <c r="H15" s="19">
         <v>0.68589100000000003</v>
       </c>
-      <c r="L15" s="41"/>
+      <c r="L15" s="47"/>
       <c r="M15" s="49"/>
       <c r="N15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="42"/>
+      <c r="O15" s="40"/>
       <c r="P15" s="17">
         <v>0.90700000000000003</v>
       </c>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -4076,22 +4076,22 @@
       <c r="H16" s="19">
         <v>0.68067800000000001</v>
       </c>
-      <c r="L16" s="41"/>
+      <c r="L16" s="47"/>
       <c r="M16" s="49"/>
       <c r="N16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="42"/>
+      <c r="O16" s="40"/>
       <c r="P16" s="17">
         <v>0.94899999999999995</v>
       </c>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -4111,9 +4111,9 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41" t="s">
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -4139,9 +4139,9 @@
       <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
@@ -4161,9 +4161,9 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
@@ -4223,7 +4223,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L28" s="5"/>
-      <c r="M28" s="45"/>
+      <c r="M28" s="41"/>
       <c r="N28" s="5"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L29" s="5"/>
-      <c r="M29" s="45"/>
+      <c r="M29" s="41"/>
       <c r="N29" s="5"/>
       <c r="O29" s="17"/>
       <c r="P29" s="25"/>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L30" s="5"/>
-      <c r="M30" s="45"/>
+      <c r="M30" s="41"/>
       <c r="N30" s="5"/>
       <c r="O30" s="17"/>
       <c r="P30" s="25"/>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L31" s="5"/>
-      <c r="M31" s="45"/>
+      <c r="M31" s="41"/>
       <c r="N31" s="5"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
@@ -4259,7 +4259,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L32" s="5"/>
-      <c r="M32" s="45"/>
+      <c r="M32" s="41"/>
       <c r="N32" s="5"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -4268,18 +4268,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="L2:L16"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="O14:O16"/>
     <mergeCell ref="M28:M32"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C3:C4"/>
@@ -4296,6 +4284,18 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H6 E7:F20 H7:H20">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
added qwen base ec results
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C364C272-C6F6-0F41-BBB7-F08F5A84D7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D102C3E5-8A05-7F4B-8560-80B8B418B10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="68">
   <si>
     <t>llama</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>noisy finetuning results</t>
+  </si>
+  <si>
+    <t>worst</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>avg</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -544,173 +553,192 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -718,49 +746,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1128,23 +1113,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1166,7 +1151,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="67" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1193,7 +1178,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1218,7 +1203,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1243,7 +1228,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1268,7 +1253,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="67" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1295,7 +1280,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1320,7 +1305,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1345,7 +1330,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1412,20 +1397,20 @@
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -1460,7 +1445,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="68" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1498,7 +1483,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1534,7 +1519,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1570,7 +1555,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1606,7 +1591,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1644,7 +1629,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1680,7 +1665,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1716,7 +1701,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1752,7 +1737,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="68" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1790,7 +1775,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1811,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1862,7 +1847,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1932,23 +1917,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1970,7 +1955,7 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="67" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1997,7 +1982,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2022,7 +2007,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -2047,7 +2032,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2072,7 +2057,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="67" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2099,7 +2084,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
@@ -2124,7 +2109,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -2149,7 +2134,7 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2216,20 +2201,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
     </row>
     <row r="2" spans="1:24" ht="19" x14ac:dyDescent="0.2">
       <c r="C2" s="3">
@@ -2264,7 +2249,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="68" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2302,7 +2287,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2323,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2374,7 +2359,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2410,7 +2395,7 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2458,7 +2443,7 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2480,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2531,7 +2516,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="68"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2567,7 +2552,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="68" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2605,7 +2590,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2641,7 +2626,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
@@ -2677,7 +2662,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2752,24 +2737,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -2784,120 +2769,120 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="J4" s="5"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="J5" s="5"/>
       <c r="K5" s="17"/>
       <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46" t="s">
+      <c r="A7" s="78"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="71">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
       <c r="J7" s="5"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
       <c r="J8" s="5"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="78" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
@@ -2916,31 +2901,31 @@
       <c r="H9" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="38"/>
-      <c r="N9" s="37" t="s">
+      <c r="M9" s="70"/>
+      <c r="N9" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="37"/>
-      <c r="Z9" s="37"/>
-      <c r="AA9" s="37"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
+      <c r="W9" s="69"/>
+      <c r="X9" s="69"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46" t="s">
+      <c r="A10" s="78"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -2958,31 +2943,31 @@
       <c r="H10" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="37" t="s">
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="37" t="s">
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="37"/>
-      <c r="W10" s="37"/>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="37"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="37"/>
+      <c r="V10" s="69"/>
+      <c r="W10" s="69"/>
+      <c r="X10" s="69"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
     </row>
     <row r="11" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
@@ -2998,39 +2983,39 @@
       <c r="H11" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38" t="s">
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="37" t="s">
+      <c r="O11" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37" t="s">
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="37"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="38" t="s">
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="37" t="s">
+      <c r="V11" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="W11" s="37"/>
-      <c r="X11" s="37"/>
-      <c r="Y11" s="37" t="s">
+      <c r="W11" s="69"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="Z11" s="37"/>
-      <c r="AA11" s="37"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
@@ -3046,9 +3031,9 @@
       <c r="H12" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="37"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="69"/>
       <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3067,7 +3052,7 @@
       <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="37"/>
+      <c r="U12" s="69"/>
       <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3088,9 +3073,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46" t="s">
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -3114,53 +3099,53 @@
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="40">
+      <c r="N13" s="72">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="41">
+      <c r="O13" s="73">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="41">
+      <c r="P13" s="73">
         <v>0.50667970022808695</v>
       </c>
-      <c r="Q13" s="39">
+      <c r="Q13" s="71">
         <v>0.46757901596611201</v>
       </c>
-      <c r="R13" s="39">
+      <c r="R13" s="71">
         <v>0.93385467579015902</v>
       </c>
-      <c r="S13" s="39">
+      <c r="S13" s="71">
         <v>0.76050830889540499</v>
       </c>
-      <c r="T13" s="39">
+      <c r="T13" s="71">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="40">
+      <c r="U13" s="72">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="41">
+      <c r="V13" s="73">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="41">
+      <c r="W13" s="73">
         <v>0.516780710329097</v>
       </c>
-      <c r="X13" s="39">
+      <c r="X13" s="71">
         <v>0.53828608667318301</v>
       </c>
-      <c r="Y13" s="39">
+      <c r="Y13" s="71">
         <v>0.928641251221896</v>
       </c>
-      <c r="Z13" s="39">
+      <c r="Z13" s="71">
         <v>0.83447376995764</v>
       </c>
-      <c r="AA13" s="39">
+      <c r="AA13" s="71">
         <v>0.916585206907787</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -3182,25 +3167,25 @@
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="40"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="40"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="39"/>
-      <c r="Y14" s="39"/>
-      <c r="Z14" s="39"/>
-      <c r="AA14" s="39"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="72"/>
+      <c r="V14" s="73"/>
+      <c r="W14" s="73"/>
+      <c r="X14" s="71"/>
+      <c r="Y14" s="71"/>
+      <c r="Z14" s="71"/>
+      <c r="AA14" s="71"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -3222,24 +3207,24 @@
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="40"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="39"/>
-      <c r="U15" s="40"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="39"/>
-      <c r="Y15" s="39"/>
-      <c r="Z15" s="39"/>
-      <c r="AA15" s="39"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="73"/>
+      <c r="W15" s="73"/>
+      <c r="X15" s="71"/>
+      <c r="Y15" s="71"/>
+      <c r="Z15" s="71"/>
+      <c r="AA15" s="71"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46" t="s">
+      <c r="A16" s="78"/>
+      <c r="B16" s="78" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="15"/>
@@ -3264,25 +3249,25 @@
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="40"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="40"/>
-      <c r="V16" s="41"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="39"/>
-      <c r="Y16" s="39"/>
-      <c r="Z16" s="39"/>
-      <c r="AA16" s="39"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="72"/>
+      <c r="V16" s="73"/>
+      <c r="W16" s="73"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46" t="s">
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3306,25 +3291,25 @@
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="40"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="39"/>
-      <c r="Y17" s="39"/>
-      <c r="Z17" s="39"/>
-      <c r="AA17" s="39"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="72"/>
+      <c r="V17" s="73"/>
+      <c r="W17" s="73"/>
+      <c r="X17" s="71"/>
+      <c r="Y17" s="71"/>
+      <c r="Z17" s="71"/>
+      <c r="AA17" s="71"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
@@ -3342,9 +3327,9 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3362,9 +3347,9 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46" t="s">
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -3384,9 +3369,9 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
@@ -3419,9 +3404,9 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
@@ -3479,43 +3464,43 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="44">
+      <c r="E24" s="76">
         <v>0.995</v>
       </c>
-      <c r="F24" s="44"/>
+      <c r="F24" s="76"/>
       <c r="L24" s="24"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
       <c r="L25" s="24"/>
       <c r="M25" s="5"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="75" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="21">
@@ -3531,9 +3516,9 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
+      <c r="A27" s="74"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
       <c r="D27" s="21">
         <v>2</v>
       </c>
@@ -3541,9 +3526,9 @@
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="21">
         <v>5</v>
       </c>
@@ -3551,9 +3536,9 @@
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
       <c r="D29" s="21">
         <v>10</v>
       </c>
@@ -3565,9 +3550,9 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
+      <c r="A30" s="74"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
       <c r="D30" s="21">
         <v>20</v>
       </c>
@@ -3575,9 +3560,9 @@
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43" t="s">
+      <c r="A31" s="74"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="21">
@@ -3587,9 +3572,9 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
+      <c r="A32" s="74"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
       <c r="D32" s="21">
         <v>2</v>
       </c>
@@ -3597,9 +3582,9 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
       <c r="D33" s="21">
         <v>3</v>
       </c>
@@ -3607,9 +3592,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
+      <c r="A34" s="74"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
       <c r="D34" s="21">
         <v>4</v>
       </c>
@@ -3617,9 +3602,9 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
+      <c r="A35" s="74"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
       <c r="D35" s="21">
         <v>5</v>
       </c>
@@ -3627,12 +3612,12 @@
       <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="47" t="s">
+      <c r="A36" s="74"/>
+      <c r="B36" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
       <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
@@ -3757,18 +3742,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
       <c r="M1" s="14"/>
       <c r="N1" s="24" t="s">
         <v>55</v>
@@ -3793,10 +3778,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -3812,16 +3797,16 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="46" t="s">
+      <c r="L2" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="48">
+      <c r="M2" s="80">
         <v>1</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="39">
+      <c r="O2" s="71">
         <v>0.85728300000000002</v>
       </c>
       <c r="P2" s="17">
@@ -3841,31 +3826,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="48"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="80"/>
       <c r="N3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="39"/>
+      <c r="O3" s="71"/>
       <c r="P3" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -3877,27 +3862,27 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="48"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="80"/>
       <c r="N4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="39"/>
+      <c r="O4" s="71"/>
       <c r="P4" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -3911,31 +3896,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="48">
+      <c r="L5" s="78"/>
+      <c r="M5" s="80">
         <v>2</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="39">
+      <c r="O5" s="71">
         <v>0.90257399999999999</v>
       </c>
       <c r="P5" s="17">
@@ -3955,27 +3940,27 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="48"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="80"/>
       <c r="N6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="39"/>
+      <c r="O6" s="71"/>
       <c r="P6" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -3987,10 +3972,10 @@
       <c r="T6" s="17"/>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="78" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="15"/>
@@ -4009,12 +3994,12 @@
       <c r="H7" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L7" s="46"/>
-      <c r="M7" s="48"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="80"/>
       <c r="N7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="39"/>
+      <c r="O7" s="71"/>
       <c r="P7" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4028,9 +4013,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46" t="s">
+      <c r="A8" s="78"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -4048,14 +4033,14 @@
       <c r="H8" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L8" s="46"/>
-      <c r="M8" s="48">
+      <c r="L8" s="78"/>
+      <c r="M8" s="80">
         <v>5</v>
       </c>
       <c r="N8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="39">
+      <c r="O8" s="71">
         <v>0.93776499999999996</v>
       </c>
       <c r="P8" s="17">
@@ -4075,9 +4060,9 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
@@ -4093,12 +4078,12 @@
       <c r="H9" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L9" s="46"/>
-      <c r="M9" s="48"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="80"/>
       <c r="N9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="39"/>
+      <c r="O9" s="71"/>
       <c r="P9" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4110,9 +4095,9 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -4128,12 +4113,12 @@
       <c r="H10" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L10" s="46"/>
-      <c r="M10" s="48"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="80"/>
       <c r="N10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="39"/>
+      <c r="O10" s="71"/>
       <c r="P10" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4147,9 +4132,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46" t="s">
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -4167,14 +4152,14 @@
       <c r="H11" s="19">
         <v>0.94037099999999996</v>
       </c>
-      <c r="L11" s="46"/>
-      <c r="M11" s="48">
+      <c r="L11" s="78"/>
+      <c r="M11" s="80">
         <v>10</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="39">
+      <c r="O11" s="71">
         <v>0.94330400000000003</v>
       </c>
       <c r="P11" s="17">
@@ -4194,9 +4179,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
@@ -4212,12 +4197,12 @@
       <c r="H12" s="19">
         <v>0.754969</v>
       </c>
-      <c r="L12" s="46"/>
-      <c r="M12" s="48"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="80"/>
       <c r="N12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="39"/>
+      <c r="O12" s="71"/>
       <c r="P12" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4229,9 +4214,9 @@
       <c r="T12" s="17"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
@@ -4247,12 +4232,12 @@
       <c r="H13" s="19">
         <v>0.94884299999999999</v>
       </c>
-      <c r="L13" s="46"/>
-      <c r="M13" s="48"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="80"/>
       <c r="N13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="39"/>
+      <c r="O13" s="71"/>
       <c r="P13" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4266,8 +4251,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46" t="s">
+      <c r="A14" s="78"/>
+      <c r="B14" s="78" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="15"/>
@@ -4286,14 +4271,14 @@
       <c r="H14" s="19">
         <v>0.63245399999999996</v>
       </c>
-      <c r="L14" s="46"/>
-      <c r="M14" s="48">
+      <c r="L14" s="78"/>
+      <c r="M14" s="80">
         <v>20</v>
       </c>
       <c r="N14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="39">
+      <c r="O14" s="71">
         <v>0.93548399999999998</v>
       </c>
       <c r="P14" s="17">
@@ -4313,9 +4298,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46" t="s">
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -4333,12 +4318,12 @@
       <c r="H15" s="19">
         <v>0.68589100000000003</v>
       </c>
-      <c r="L15" s="46"/>
-      <c r="M15" s="48"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="80"/>
       <c r="N15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="39"/>
+      <c r="O15" s="71"/>
       <c r="P15" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4350,9 +4335,9 @@
       <c r="T15" s="17"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -4368,12 +4353,12 @@
       <c r="H16" s="19">
         <v>0.68067800000000001</v>
       </c>
-      <c r="L16" s="46"/>
-      <c r="M16" s="48"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="80"/>
       <c r="N16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="39"/>
+      <c r="O16" s="71"/>
       <c r="P16" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4387,9 +4372,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -4409,9 +4394,9 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46" t="s">
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -4437,9 +4422,9 @@
       <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
@@ -4459,9 +4444,9 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
       <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
@@ -4521,7 +4506,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L28" s="5"/>
-      <c r="M28" s="40"/>
+      <c r="M28" s="72"/>
       <c r="N28" s="5"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -4530,7 +4515,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L29" s="5"/>
-      <c r="M29" s="40"/>
+      <c r="M29" s="72"/>
       <c r="N29" s="5"/>
       <c r="O29" s="17"/>
       <c r="P29" s="25"/>
@@ -4539,7 +4524,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L30" s="5"/>
-      <c r="M30" s="40"/>
+      <c r="M30" s="72"/>
       <c r="N30" s="5"/>
       <c r="O30" s="17"/>
       <c r="P30" s="25"/>
@@ -4548,7 +4533,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L31" s="5"/>
-      <c r="M31" s="40"/>
+      <c r="M31" s="72"/>
       <c r="N31" s="5"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
@@ -4557,7 +4542,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L32" s="5"/>
-      <c r="M32" s="40"/>
+      <c r="M32" s="72"/>
       <c r="N32" s="5"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -4625,10 +4610,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
-  <dimension ref="B2:AN49"/>
+  <dimension ref="B2:AK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4637,930 +4622,915 @@
     <col min="2" max="2" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="6.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="13"/>
-    <col min="11" max="11" width="8.1640625" style="13" customWidth="1"/>
-    <col min="12" max="13" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.1640625" style="13" customWidth="1"/>
-    <col min="15" max="15" width="20.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="4.1640625" style="13" customWidth="1"/>
-    <col min="23" max="23" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="13" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="6.5" style="13" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="13"/>
+    <col min="16" max="17" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.1640625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="20.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.1640625" style="13" customWidth="1"/>
+    <col min="25" max="25" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" style="13" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9" style="13" customWidth="1"/>
-    <col min="34" max="34" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.83203125" style="13"/>
-    <col min="36" max="36" width="11" style="13" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="10.83203125" style="13"/>
+    <col min="32" max="32" width="9" style="13" customWidth="1"/>
+    <col min="33" max="33" width="11" style="13" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:40" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+    <row r="2" spans="2:37" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="L2" s="85" t="s">
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="P2" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="X2" s="85" t="s">
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+      <c r="Z2" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="Y2" s="85"/>
-      <c r="Z2" s="85"/>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="85"/>
-      <c r="AC2" s="85"/>
-      <c r="AD2" s="85"/>
-      <c r="AE2" s="85"/>
-      <c r="AJ2" s="85" t="s">
+      <c r="AA2" s="91"/>
+      <c r="AB2" s="91"/>
+      <c r="AC2" s="91"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
+      <c r="AG2" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="AK2" s="85"/>
-      <c r="AL2" s="85"/>
-      <c r="AM2" s="85"/>
-      <c r="AN2" s="85"/>
-    </row>
-    <row r="3" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="92"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93" t="s">
+      <c r="AH2" s="91"/>
+      <c r="AI2" s="91"/>
+      <c r="AJ2" s="91"/>
+      <c r="AK2" s="91"/>
+    </row>
+    <row r="3" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
-      <c r="L3" s="53" t="s">
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="96"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54" t="s">
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="55"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="79"/>
-      <c r="Z3" s="80" t="s">
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="88"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="80" t="s">
+      <c r="AC3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC3" s="80" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD3" s="80" t="s">
+      <c r="AD3" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="AE3" s="81" t="s">
+      <c r="AE3" s="36" t="s">
         <v>52</v>
       </c>
       <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
-      <c r="AJ3" s="101" t="s">
+      <c r="AG3" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="AK3" s="102" t="s">
+      <c r="AH3" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="AL3" s="102" t="s">
+      <c r="AI3" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="AM3" s="102" t="s">
+      <c r="AJ3" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="AN3" s="103" t="s">
+      <c r="AK3" s="60" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:40" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:37" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="95"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="67" t="s">
+      <c r="C4" s="80"/>
+      <c r="D4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="67">
+      <c r="E4" s="13">
         <v>1</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="13">
         <v>2</v>
       </c>
-      <c r="G4" s="67">
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="13">
         <v>4</v>
       </c>
-      <c r="I4" s="96">
+      <c r="I4" s="53">
         <v>5</v>
       </c>
-      <c r="L4" s="56"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="58" t="s">
+      <c r="K4" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="54">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="M4" s="54">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="N4" s="55">
+        <f>AVERAGE(D6:D10)</f>
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="58" t="s">
+      <c r="U4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="59" t="s">
+      <c r="V4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="60" t="s">
+      <c r="W4" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="66" t="s">
+      <c r="X4" s="20"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="Y4" s="82">
+      <c r="AA4" s="80">
         <v>1</v>
       </c>
-      <c r="Z4" s="58" t="s">
+      <c r="AB4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AA4" s="64">
+      <c r="AC4" s="71">
         <v>0.86699999999999999</v>
       </c>
-      <c r="AB4" s="83">
+      <c r="AD4" s="17">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AE4" s="39">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="17">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="AI4" s="17">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="AJ4" s="61">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="AK4" s="39">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:37" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="97" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="F5" s="54">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="G5" s="54">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="H5" s="54">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I5" s="55">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="J5" s="54"/>
+      <c r="K5" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="54">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="M5" s="54">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="N5" s="55">
+        <f>AVERAGE(E5:I5)</f>
+        <v>0.84460000000000002</v>
+      </c>
+      <c r="P5" s="89" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="71">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="U5" s="71"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="90"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="30"/>
+      <c r="Z5" s="82"/>
+      <c r="AA5" s="80"/>
+      <c r="AB5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="17">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="AE5" s="39"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="62">
+        <v>10</v>
+      </c>
+      <c r="AH5" s="49">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AI5" s="49">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AJ5" s="49">
+        <v>0.92</v>
+      </c>
+      <c r="AK5" s="50">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="2:37" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="97"/>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="54">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="E6" s="54">
+        <v>0.85923753665689095</v>
+      </c>
+      <c r="F6" s="54">
+        <v>0.85988921472792401</v>
+      </c>
+      <c r="G6" s="54">
+        <v>0.85858585858585801</v>
+      </c>
+      <c r="H6" s="54">
+        <v>0.85337243401759499</v>
+      </c>
+      <c r="I6" s="55">
+        <v>0.83740632127728898</v>
+      </c>
+      <c r="J6" s="54"/>
+      <c r="K6" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="56">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="M6" s="56">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="N6" s="57">
+        <f>AVERAGE(E6:I10)</f>
+        <v>0.91474745461062212</v>
+      </c>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" s="71">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="90"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="80"/>
+      <c r="AB6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC6" s="71"/>
+      <c r="AD6" s="17">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="AE6" s="39">
+        <v>0.95</v>
+      </c>
+      <c r="AF6" s="33"/>
+    </row>
+    <row r="7" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="97"/>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="54">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="E7" s="54">
+        <v>0.90648399999999996</v>
+      </c>
+      <c r="F7" s="54">
+        <v>0.90713600000000005</v>
+      </c>
+      <c r="G7" s="54">
+        <v>0.90550699999999995</v>
+      </c>
+      <c r="H7" s="54">
+        <v>0.89996699999999996</v>
+      </c>
+      <c r="I7" s="55">
+        <v>0.88302400000000003</v>
+      </c>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="T7" s="71">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="90"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="82"/>
+      <c r="AA7" s="80">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="71">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="AD7" s="17">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AE7" s="39">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AF7" s="17"/>
+    </row>
+    <row r="8" spans="2:37" ht="20" x14ac:dyDescent="0.2">
+      <c r="B8" s="97"/>
+      <c r="C8" s="13">
+        <v>5</v>
+      </c>
+      <c r="D8" s="54">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="E8" s="54">
+        <v>0.942326</v>
+      </c>
+      <c r="F8" s="54">
+        <v>0.94330400000000003</v>
+      </c>
+      <c r="G8" s="54">
+        <v>0.94167500000000004</v>
+      </c>
+      <c r="H8" s="54">
+        <v>0.93548399999999998</v>
+      </c>
+      <c r="I8" s="55">
+        <v>0.91756300000000002</v>
+      </c>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="T8" s="71">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="90"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="82"/>
+      <c r="AA8" s="80"/>
+      <c r="AB8" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC8" s="71"/>
+      <c r="AD8" s="17">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="17"/>
+    </row>
+    <row r="9" spans="2:37" ht="20" x14ac:dyDescent="0.25">
+      <c r="B9" s="97"/>
+      <c r="C9" s="13">
+        <v>10</v>
+      </c>
+      <c r="D9" s="54">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="E9" s="54">
+        <v>0.95047199999999998</v>
+      </c>
+      <c r="F9" s="54">
+        <v>0.95145000000000002</v>
+      </c>
+      <c r="G9" s="54">
+        <v>0.94982100000000003</v>
+      </c>
+      <c r="H9" s="54">
+        <v>0.94362999999999997</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0.92538299999999996</v>
+      </c>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="71">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="90"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="82"/>
+      <c r="AA9" s="80"/>
+      <c r="AB9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC9" s="71"/>
+      <c r="AD9" s="17">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="AE9" s="39">
+        <v>0.95</v>
+      </c>
+      <c r="AF9" s="33"/>
+    </row>
+    <row r="10" spans="2:37" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="98"/>
+      <c r="C10" s="41">
+        <v>20</v>
+      </c>
+      <c r="D10" s="56">
         <v>0.93400000000000005</v>
       </c>
-      <c r="AC4" s="83">
+      <c r="E10" s="56">
+        <v>0.94525899999999996</v>
+      </c>
+      <c r="F10" s="56">
+        <v>0.94688799999999995</v>
+      </c>
+      <c r="G10" s="56">
+        <v>0.94525899999999996</v>
+      </c>
+      <c r="H10" s="56">
+        <v>0.93906800000000001</v>
+      </c>
+      <c r="I10" s="57">
+        <v>0.92049499999999995</v>
+      </c>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" s="71">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="90"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="80">
+        <v>5</v>
+      </c>
+      <c r="AB10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="71">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AD10" s="17">
         <v>0.94799999999999995</v>
       </c>
-      <c r="AD4" s="83">
+      <c r="AE10" s="39">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AF10" s="17"/>
+    </row>
+    <row r="11" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="P11" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q11" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="15"/>
+      <c r="S11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" s="19">
+        <v>0.52</v>
+      </c>
+      <c r="U11" s="19">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="V11" s="19">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="W11" s="40">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="82"/>
+      <c r="AA11" s="80"/>
+      <c r="AB11" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC11" s="71"/>
+      <c r="AD11" s="17">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="17"/>
+    </row>
+    <row r="12" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="82"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T12" s="19">
+        <v>0.52</v>
+      </c>
+      <c r="U12" s="19">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="V12" s="19">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="W12" s="40">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="82"/>
+      <c r="AA12" s="80"/>
+      <c r="AB12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC12" s="71"/>
+      <c r="AD12" s="17">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="AE12" s="39">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="AF12" s="33"/>
+    </row>
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="P13" s="82"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="19">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="U13" s="19">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="V13" s="19">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="W13" s="40">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="82"/>
+      <c r="AA13" s="80">
+        <v>10</v>
+      </c>
+      <c r="AB13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="71">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AD13" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AE13" s="39">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AF13" s="17"/>
+    </row>
+    <row r="14" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="82"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T14" s="19">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="U14" s="19">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="V14" s="19">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="W14" s="40">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="82"/>
+      <c r="AA14" s="80"/>
+      <c r="AB14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC14" s="71"/>
+      <c r="AD14" s="17">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AE14" s="39"/>
+      <c r="AF14" s="17"/>
+    </row>
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="P15" s="82"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="S15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T15" s="19">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="U15" s="19">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="V15" s="19">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="W15" s="40">
         <v>0.94599999999999995</v>
       </c>
-      <c r="AE4" s="84">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-      <c r="AJ4" s="104">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="83">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="AL4" s="83">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="AM4" s="105">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="AN4" s="84">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="5" spans="2:40" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97">
-        <v>0.83799999999999997</v>
-      </c>
-      <c r="F5" s="97">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="G5" s="97">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="H5" s="97">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="I5" s="98">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="L5" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62" t="s">
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="82"/>
+      <c r="AA15" s="80"/>
+      <c r="AB15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC15" s="71"/>
+      <c r="AD15" s="17">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AE15" s="39">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="AF15" s="33"/>
+    </row>
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="P16" s="82"/>
+      <c r="Q16" s="78"/>
+      <c r="R16" s="78"/>
+      <c r="S16" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T16" s="19">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="U16" s="19">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="V16" s="19">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="W16" s="40">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="82"/>
+      <c r="AA16" s="80">
+        <v>20</v>
+      </c>
+      <c r="AB16" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="71">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="AD16" s="17">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AE16" s="39">
+        <v>0.94</v>
+      </c>
+      <c r="AF16" s="17"/>
+    </row>
+    <row r="17" spans="16:32" x14ac:dyDescent="0.25">
+      <c r="P17" s="82"/>
+      <c r="Q17" s="78"/>
+      <c r="R17" s="78"/>
+      <c r="S17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T17" s="19">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="U17" s="19">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="V17" s="19">
+        <v>0.877</v>
+      </c>
+      <c r="W17" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="82"/>
+      <c r="AA17" s="80"/>
+      <c r="AB17" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC17" s="71"/>
+      <c r="AD17" s="17">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="AE17" s="39"/>
+      <c r="AF17" s="17"/>
+    </row>
+    <row r="18" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="82"/>
+      <c r="Q18" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="R18" s="15"/>
+      <c r="S18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="T18" s="19">
+        <v>0.495</v>
+      </c>
+      <c r="U18" s="19">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="V18" s="19">
+        <v>0.495</v>
+      </c>
+      <c r="W18" s="40">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="83"/>
+      <c r="AA18" s="91"/>
+      <c r="AB18" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC18" s="92"/>
+      <c r="AD18" s="49">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AE18" s="50">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AF18" s="33"/>
+    </row>
+    <row r="19" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="82"/>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="S19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="64">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA5" s="64"/>
-      <c r="AB5" s="83"/>
-      <c r="AC5" s="83"/>
-      <c r="AD5" s="83">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="AE5" s="84"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="17"/>
-      <c r="AJ5" s="106">
-        <v>10</v>
-      </c>
-      <c r="AK5" s="88">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AL5" s="88">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="AM5" s="88">
-        <v>0.92</v>
-      </c>
-      <c r="AN5" s="89">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="90"/>
-      <c r="C6" s="67">
-        <v>1</v>
-      </c>
-      <c r="D6" s="97">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="E6" s="97">
-        <v>0.85923753665689095</v>
-      </c>
-      <c r="F6" s="97">
-        <v>0.85988921472792401</v>
-      </c>
-      <c r="G6" s="97">
-        <v>0.85858585858585801</v>
-      </c>
-      <c r="H6" s="97">
-        <v>0.85337243401759499</v>
-      </c>
-      <c r="I6" s="98">
-        <v>0.83740632127728898</v>
-      </c>
-      <c r="L6" s="66"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="64">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="64"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="82"/>
-      <c r="Z6" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA6" s="64"/>
-      <c r="AB6" s="83"/>
-      <c r="AC6" s="83"/>
-      <c r="AD6" s="83">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="AE6" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-    </row>
-    <row r="7" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="90"/>
-      <c r="C7" s="67">
-        <v>2</v>
-      </c>
-      <c r="D7" s="97">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="E7" s="97">
-        <v>0.90648399999999996</v>
-      </c>
-      <c r="F7" s="97">
-        <v>0.90713600000000005</v>
-      </c>
-      <c r="G7" s="97">
-        <v>0.90550699999999995</v>
-      </c>
-      <c r="H7" s="97">
-        <v>0.89996699999999996</v>
-      </c>
-      <c r="I7" s="98">
-        <v>0.88302400000000003</v>
-      </c>
-      <c r="L7" s="66"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" s="67" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" s="64">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="82">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA7" s="64">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="AB7" s="83">
-        <v>0.94</v>
-      </c>
-      <c r="AC7" s="83">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AD7" s="83">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AE7" s="84">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="17"/>
-    </row>
-    <row r="8" spans="2:40" ht="20" x14ac:dyDescent="0.2">
-      <c r="B8" s="90"/>
-      <c r="C8" s="67">
-        <v>5</v>
-      </c>
-      <c r="D8" s="97">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="E8" s="97">
-        <v>0.942326</v>
-      </c>
-      <c r="F8" s="97">
-        <v>0.94330400000000003</v>
-      </c>
-      <c r="G8" s="97">
-        <v>0.94167500000000004</v>
-      </c>
-      <c r="H8" s="97">
-        <v>0.93548399999999998</v>
-      </c>
-      <c r="I8" s="98">
-        <v>0.91756300000000002</v>
-      </c>
-      <c r="L8" s="66"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="P8" s="64">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="30"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="82"/>
-      <c r="Z8" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA8" s="64"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="AE8" s="84"/>
-      <c r="AF8" s="17"/>
-      <c r="AG8" s="17"/>
-    </row>
-    <row r="9" spans="2:40" ht="20" x14ac:dyDescent="0.25">
-      <c r="B9" s="90"/>
-      <c r="C9" s="67">
-        <v>10</v>
-      </c>
-      <c r="D9" s="97">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="E9" s="97">
-        <v>0.95047199999999998</v>
-      </c>
-      <c r="F9" s="97">
-        <v>0.95145000000000002</v>
-      </c>
-      <c r="G9" s="97">
-        <v>0.94982100000000003</v>
-      </c>
-      <c r="H9" s="97">
-        <v>0.94362999999999997</v>
-      </c>
-      <c r="I9" s="98">
-        <v>0.92538299999999996</v>
-      </c>
-      <c r="L9" s="66"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="P9" s="64">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="82"/>
-      <c r="Z9" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="83"/>
-      <c r="AC9" s="83"/>
-      <c r="AD9" s="83">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="AE9" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="AF9" s="51"/>
-      <c r="AG9" s="51"/>
-    </row>
-    <row r="10" spans="2:40" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="91"/>
-      <c r="C10" s="73">
-        <v>20</v>
-      </c>
-      <c r="D10" s="99">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="E10" s="99">
-        <v>0.94525899999999996</v>
-      </c>
-      <c r="F10" s="99">
-        <v>0.94688799999999995</v>
-      </c>
-      <c r="G10" s="99">
-        <v>0.94525899999999996</v>
-      </c>
-      <c r="H10" s="99">
-        <v>0.93906800000000001</v>
-      </c>
-      <c r="I10" s="100">
-        <v>0.92049499999999995</v>
-      </c>
-      <c r="L10" s="66"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="P10" s="64">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="82">
-        <v>5</v>
-      </c>
-      <c r="Z10" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA10" s="64">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AB10" s="83">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="AC10" s="83">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AD10" s="83">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AE10" s="84">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AF10" s="17"/>
-      <c r="AG10" s="17"/>
-    </row>
-    <row r="11" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L11" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="N11" s="68"/>
-      <c r="O11" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="P11" s="69">
-        <v>0.52</v>
-      </c>
-      <c r="Q11" s="69">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="R11" s="69">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="S11" s="70">
-        <v>0.60299999999999998</v>
-      </c>
-      <c r="W11" s="30"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="82"/>
-      <c r="Z11" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA11" s="64"/>
-      <c r="AB11" s="83"/>
-      <c r="AC11" s="83"/>
-      <c r="AD11" s="83">
-        <v>0.94</v>
-      </c>
-      <c r="AE11" s="84"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="17"/>
-    </row>
-    <row r="12" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L12" s="66"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="69">
-        <v>0.52</v>
-      </c>
-      <c r="Q12" s="69">
-        <v>0.65900000000000003</v>
-      </c>
-      <c r="R12" s="69">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="S12" s="70">
-        <v>0.64500000000000002</v>
-      </c>
-      <c r="W12" s="30"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="82"/>
-      <c r="Z12" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA12" s="64"/>
-      <c r="AB12" s="83"/>
-      <c r="AC12" s="83"/>
-      <c r="AD12" s="83">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="AE12" s="84">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="AF12" s="51"/>
-      <c r="AG12" s="51"/>
-    </row>
-    <row r="13" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="L13" s="66"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="69">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="Q13" s="69">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="R13" s="69">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="S13" s="70">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="W13" s="30"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="82">
-        <v>10</v>
-      </c>
-      <c r="Z13" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA13" s="64">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AB13" s="83">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="AC13" s="83">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AD13" s="83">
-        <v>0.95</v>
-      </c>
-      <c r="AE13" s="84">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AF13" s="17"/>
-      <c r="AG13" s="17"/>
-    </row>
-    <row r="14" spans="2:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L14" s="66"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="62"/>
-      <c r="O14" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="P14" s="69">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="Q14" s="69">
-        <v>0.76500000000000001</v>
-      </c>
-      <c r="R14" s="69">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="S14" s="70">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="W14" s="30"/>
-      <c r="X14" s="66"/>
-      <c r="Y14" s="82"/>
-      <c r="Z14" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA14" s="64"/>
-      <c r="AB14" s="83"/>
-      <c r="AC14" s="83"/>
-      <c r="AD14" s="83">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AE14" s="84"/>
-      <c r="AF14" s="17"/>
-      <c r="AG14" s="17"/>
-    </row>
-    <row r="15" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="L15" s="66"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="O15" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="69">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="Q15" s="69">
-        <v>0.80200000000000005</v>
-      </c>
-      <c r="R15" s="69">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="S15" s="70">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="W15" s="30"/>
-      <c r="X15" s="66"/>
-      <c r="Y15" s="82"/>
-      <c r="Z15" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA15" s="64"/>
-      <c r="AB15" s="83"/>
-      <c r="AC15" s="83"/>
-      <c r="AD15" s="83">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="AE15" s="84">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="AF15" s="51"/>
-      <c r="AG15" s="51"/>
-    </row>
-    <row r="16" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="L16" s="66"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="69">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="Q16" s="69">
-        <v>0.68700000000000006</v>
-      </c>
-      <c r="R16" s="69">
-        <v>0.74199999999999999</v>
-      </c>
-      <c r="S16" s="70">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="W16" s="30"/>
-      <c r="X16" s="66"/>
-      <c r="Y16" s="82">
-        <v>20</v>
-      </c>
-      <c r="Z16" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA16" s="64">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="AB16" s="83">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="AC16" s="83">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="AD16" s="83">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="AE16" s="84">
-        <v>0.4</v>
-      </c>
-      <c r="AF16" s="17"/>
-      <c r="AG16" s="17"/>
-    </row>
-    <row r="17" spans="12:34" x14ac:dyDescent="0.25">
-      <c r="L17" s="66"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" s="69">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="Q17" s="69">
-        <v>0.88300000000000001</v>
-      </c>
-      <c r="R17" s="69">
-        <v>0.877</v>
-      </c>
-      <c r="S17" s="70">
-        <v>0.95</v>
-      </c>
-      <c r="W17" s="30"/>
-      <c r="X17" s="66"/>
-      <c r="Y17" s="82"/>
-      <c r="Z17" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA17" s="64"/>
-      <c r="AB17" s="83"/>
-      <c r="AC17" s="83"/>
-      <c r="AD17" s="83">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="AE17" s="84"/>
-      <c r="AF17" s="17"/>
-      <c r="AG17" s="17"/>
-    </row>
-    <row r="18" spans="12:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L18" s="66"/>
-      <c r="M18" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="N18" s="68"/>
-      <c r="O18" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="P18" s="69">
-        <v>0.495</v>
-      </c>
-      <c r="Q18" s="69">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="R18" s="69">
-        <v>0.495</v>
-      </c>
-      <c r="S18" s="70">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="W18" s="30"/>
-      <c r="X18" s="71"/>
-      <c r="Y18" s="85"/>
-      <c r="Z18" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA18" s="87"/>
-      <c r="AB18" s="88"/>
-      <c r="AC18" s="88"/>
-      <c r="AD18" s="88">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="AE18" s="89">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="AF18" s="51"/>
-      <c r="AG18" s="51"/>
-    </row>
-    <row r="19" spans="12:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L19" s="66"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="O19" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="P19" s="69">
+      <c r="T19" s="19">
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q19" s="69">
+      <c r="U19" s="19">
         <v>0.628</v>
       </c>
-      <c r="R19" s="69">
+      <c r="V19" s="19">
         <v>0.58899999999999997</v>
       </c>
-      <c r="S19" s="70">
+      <c r="W19" s="40">
         <v>0.68200000000000005</v>
       </c>
-      <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
       <c r="Y19" s="30"/>
       <c r="Z19" s="30"/>
       <c r="AA19" s="30"/>
@@ -5569,444 +5539,398 @@
       <c r="AD19" s="30"/>
       <c r="AE19" s="30"/>
       <c r="AF19" s="30"/>
-      <c r="AG19" s="30"/>
-      <c r="AH19" s="30"/>
-    </row>
-    <row r="20" spans="12:34" x14ac:dyDescent="0.25">
-      <c r="L20" s="66"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="67" t="s">
+    </row>
+    <row r="20" spans="16:32" x14ac:dyDescent="0.25">
+      <c r="P20" s="82"/>
+      <c r="Q20" s="78"/>
+      <c r="R20" s="78"/>
+      <c r="S20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="69">
+      <c r="T20" s="19">
         <v>0.52600000000000002</v>
       </c>
-      <c r="Q20" s="69">
+      <c r="U20" s="19">
         <v>0.627</v>
       </c>
-      <c r="R20" s="69">
+      <c r="V20" s="19">
         <v>0.51200000000000001</v>
       </c>
-      <c r="S20" s="70">
+      <c r="W20" s="40">
         <v>0.67900000000000005</v>
       </c>
-      <c r="W20" s="30"/>
-      <c r="X20" s="92"/>
-      <c r="Y20" s="93"/>
-      <c r="Z20" s="80" t="s">
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="93"/>
+      <c r="AA20" s="94"/>
+      <c r="AB20" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="AA20" s="80" t="s">
+      <c r="AC20" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="AB20" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC20" s="80" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD20" s="80" t="s">
+      <c r="AD20" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="AE20" s="81" t="s">
+      <c r="AE20" s="36" t="s">
         <v>52</v>
       </c>
       <c r="AF20" s="30"/>
-      <c r="AG20" s="30"/>
-      <c r="AH20" s="30"/>
-    </row>
-    <row r="21" spans="12:34" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L21" s="66"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="62"/>
-      <c r="O21" s="67" t="s">
+    </row>
+    <row r="21" spans="16:32" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="82"/>
+      <c r="Q21" s="78"/>
+      <c r="R21" s="78"/>
+      <c r="S21" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="69">
+      <c r="T21" s="19">
         <v>0.51600000000000001</v>
       </c>
-      <c r="Q21" s="69">
+      <c r="U21" s="19">
         <v>0.64</v>
       </c>
-      <c r="R21" s="69">
+      <c r="V21" s="19">
         <v>0.54800000000000004</v>
       </c>
-      <c r="S21" s="70">
+      <c r="W21" s="40">
         <v>0.66300000000000003</v>
       </c>
-      <c r="W21" s="30"/>
-      <c r="X21" s="61" t="s">
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="Y21" s="62"/>
-      <c r="Z21" s="58" t="s">
+      <c r="AA21" s="78"/>
+      <c r="AB21" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AA21" s="64">
+      <c r="AC21" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="AB21" s="83"/>
-      <c r="AC21" s="83"/>
-      <c r="AD21" s="83"/>
-      <c r="AE21" s="84"/>
+      <c r="AD21" s="17"/>
+      <c r="AE21" s="39"/>
       <c r="AF21" s="30"/>
-      <c r="AG21" s="30"/>
-      <c r="AH21" s="30"/>
-    </row>
-    <row r="22" spans="12:34" x14ac:dyDescent="0.25">
-      <c r="L22" s="66"/>
-      <c r="M22" s="62"/>
-      <c r="N22" s="62" t="s">
+    </row>
+    <row r="22" spans="16:32" x14ac:dyDescent="0.25">
+      <c r="P22" s="82"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="O22" s="67" t="s">
+      <c r="S22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="P22" s="69">
+      <c r="T22" s="19">
         <v>0.60599999999999998</v>
       </c>
-      <c r="Q22" s="69">
+      <c r="U22" s="19">
         <v>0.872</v>
       </c>
-      <c r="R22" s="69">
+      <c r="V22" s="19">
         <v>0.92900000000000005</v>
       </c>
-      <c r="S22" s="70">
+      <c r="W22" s="40">
         <v>0.93600000000000005</v>
       </c>
-      <c r="W22" s="30"/>
-      <c r="X22" s="66"/>
-      <c r="Y22" s="62"/>
-      <c r="Z22" s="58" t="s">
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="82"/>
+      <c r="AA22" s="78"/>
+      <c r="AB22" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AA22" s="64"/>
-      <c r="AB22" s="83"/>
-      <c r="AC22" s="83"/>
-      <c r="AD22" s="83"/>
-      <c r="AE22" s="84"/>
+      <c r="AC22" s="71"/>
+      <c r="AD22" s="17"/>
+      <c r="AE22" s="39"/>
       <c r="AF22" s="30"/>
-      <c r="AG22" s="30"/>
-      <c r="AH22" s="30"/>
-    </row>
-    <row r="23" spans="12:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L23" s="66"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="67" t="s">
+    </row>
+    <row r="23" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P23" s="82"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="P23" s="69">
+      <c r="T23" s="19">
         <v>0.48499999999999999</v>
       </c>
-      <c r="Q23" s="69">
+      <c r="U23" s="19">
         <v>0.83799999999999997</v>
       </c>
-      <c r="R23" s="69">
+      <c r="V23" s="19">
         <v>0.82199999999999995</v>
       </c>
-      <c r="S23" s="70">
+      <c r="W23" s="40">
         <v>0.94499999999999995</v>
       </c>
-      <c r="W23" s="30"/>
-      <c r="X23" s="71"/>
-      <c r="Y23" s="72"/>
-      <c r="Z23" s="86" t="s">
+      <c r="Y23" s="30"/>
+      <c r="Z23" s="83"/>
+      <c r="AA23" s="84"/>
+      <c r="AB23" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="AA23" s="87"/>
-      <c r="AB23" s="88"/>
-      <c r="AC23" s="88"/>
-      <c r="AD23" s="88"/>
-      <c r="AE23" s="89"/>
+      <c r="AC23" s="92"/>
+      <c r="AD23" s="49"/>
+      <c r="AE23" s="50"/>
       <c r="AF23" s="30"/>
-      <c r="AG23" s="30"/>
-      <c r="AH23" s="30"/>
-    </row>
-    <row r="24" spans="12:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L24" s="71"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="73" t="s">
+    </row>
+    <row r="24" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P24" s="83"/>
+      <c r="Q24" s="84"/>
+      <c r="R24" s="84"/>
+      <c r="S24" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="P24" s="74">
+      <c r="T24" s="42">
         <v>0.51700000000000002</v>
       </c>
-      <c r="Q24" s="74">
+      <c r="U24" s="42">
         <v>0.89300000000000002</v>
       </c>
-      <c r="R24" s="74">
+      <c r="V24" s="42">
         <v>0.91600000000000004</v>
       </c>
-      <c r="S24" s="75">
+      <c r="W24" s="43">
         <v>0.94099999999999995</v>
       </c>
-      <c r="X24" s="76"/>
-      <c r="Y24" s="76"/>
-    </row>
-    <row r="25" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="X25" s="77"/>
-      <c r="Y25" s="76"/>
-      <c r="Z25" s="32"/>
-      <c r="AA25" s="32"/>
+      <c r="Z24" s="44"/>
+      <c r="AA24" s="44"/>
+    </row>
+    <row r="25" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Z25" s="45"/>
+      <c r="AA25" s="44"/>
       <c r="AB25" s="32"/>
-    </row>
-    <row r="26" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="X26" s="76"/>
-      <c r="Y26" s="76"/>
-    </row>
-    <row r="27" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="X27" s="76"/>
-      <c r="Y27" s="76"/>
-    </row>
-    <row r="28" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="X28" s="77"/>
-      <c r="Y28" s="76"/>
-      <c r="Z28" s="32"/>
-      <c r="AA28" s="32"/>
+      <c r="AC25" s="32"/>
+    </row>
+    <row r="26" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Z26" s="44"/>
+      <c r="AA26" s="44"/>
+    </row>
+    <row r="27" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Z27" s="44"/>
+      <c r="AA27" s="44"/>
+    </row>
+    <row r="28" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Z28" s="45"/>
+      <c r="AA28" s="44"/>
       <c r="AB28" s="32"/>
-    </row>
-    <row r="29" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="X29" s="76"/>
-      <c r="Y29" s="76"/>
-    </row>
-    <row r="30" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="X30" s="76"/>
-      <c r="Y30" s="76"/>
-    </row>
-    <row r="31" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="X31" s="14"/>
-      <c r="Y31" s="24"/>
-      <c r="Z31" s="24"/>
+      <c r="AC28" s="32"/>
+    </row>
+    <row r="29" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Z29" s="44"/>
+      <c r="AA29" s="44"/>
+    </row>
+    <row r="30" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Z30" s="44"/>
+      <c r="AA30" s="44"/>
+    </row>
+    <row r="31" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Z31" s="14"/>
       <c r="AA31" s="24"/>
-      <c r="AB31" s="31"/>
-      <c r="AC31" s="31"/>
+      <c r="AB31" s="24"/>
+      <c r="AC31" s="24"/>
       <c r="AD31" s="31"/>
-      <c r="AH31" s="30"/>
-    </row>
-    <row r="32" spans="12:34" x14ac:dyDescent="0.2">
-      <c r="W32" s="20"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="16"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="17"/>
-      <c r="AB32" s="17"/>
+    </row>
+    <row r="32" spans="16:32" x14ac:dyDescent="0.2">
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="30"/>
+      <c r="AA32" s="16"/>
+      <c r="AB32" s="34"/>
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
-      <c r="AH32" s="30"/>
-    </row>
-    <row r="33" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W33" s="20"/>
-      <c r="X33" s="30"/>
-      <c r="Y33" s="16"/>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="17"/>
-      <c r="AB33" s="17"/>
+    </row>
+    <row r="33" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="30"/>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="34"/>
       <c r="AC33" s="17"/>
       <c r="AD33" s="17"/>
-      <c r="AH33" s="50"/>
-    </row>
-    <row r="34" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W34" s="20"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="16"/>
-      <c r="Z34" s="52"/>
-      <c r="AA34" s="17"/>
-      <c r="AB34" s="17"/>
+    </row>
+    <row r="34" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y34" s="20"/>
+      <c r="Z34" s="30"/>
+      <c r="AA34" s="16"/>
+      <c r="AB34" s="34"/>
       <c r="AC34" s="17"/>
       <c r="AD34" s="17"/>
-      <c r="AH34" s="50"/>
-    </row>
-    <row r="35" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W35" s="20"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="16"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="17"/>
+    </row>
+    <row r="35" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="30"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="34"/>
       <c r="AC35" s="17"/>
       <c r="AD35" s="17"/>
-      <c r="AH35" s="50"/>
-    </row>
-    <row r="36" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W36" s="20"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="16"/>
-      <c r="Z36" s="52"/>
-      <c r="AA36" s="17"/>
-      <c r="AB36" s="17"/>
+    </row>
+    <row r="36" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="30"/>
+      <c r="AA36" s="16"/>
+      <c r="AB36" s="34"/>
       <c r="AC36" s="17"/>
       <c r="AD36" s="17"/>
-      <c r="AH36" s="50"/>
-    </row>
-    <row r="37" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W37" s="20"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="16"/>
-      <c r="Z37" s="52"/>
-      <c r="AA37" s="17"/>
-      <c r="AB37" s="17"/>
+    </row>
+    <row r="37" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="30"/>
+      <c r="AA37" s="16"/>
+      <c r="AB37" s="34"/>
       <c r="AC37" s="17"/>
       <c r="AD37" s="17"/>
-      <c r="AH37" s="50"/>
-    </row>
-    <row r="38" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W38" s="20"/>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="16"/>
-      <c r="Z38" s="52"/>
-      <c r="AA38" s="17"/>
-      <c r="AB38" s="17"/>
+    </row>
+    <row r="38" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="30"/>
+      <c r="AA38" s="16"/>
+      <c r="AB38" s="34"/>
       <c r="AC38" s="17"/>
       <c r="AD38" s="17"/>
-      <c r="AH38" s="50"/>
-    </row>
-    <row r="39" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W39" s="20"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="16"/>
-      <c r="Z39" s="52"/>
-      <c r="AA39" s="17"/>
-      <c r="AB39" s="17"/>
+    </row>
+    <row r="39" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="16"/>
+      <c r="AB39" s="34"/>
       <c r="AC39" s="17"/>
       <c r="AD39" s="17"/>
     </row>
-    <row r="40" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W40" s="20"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="16"/>
-      <c r="Z40" s="52"/>
-      <c r="AA40" s="17"/>
-      <c r="AB40" s="17"/>
+    <row r="40" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="16"/>
+      <c r="AB40" s="34"/>
       <c r="AC40" s="17"/>
       <c r="AD40" s="17"/>
     </row>
-    <row r="41" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W41" s="20"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="16"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="17"/>
-      <c r="AB41" s="17"/>
+    <row r="41" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y41" s="20"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="34"/>
       <c r="AC41" s="17"/>
       <c r="AD41" s="32"/>
     </row>
-    <row r="42" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W42" s="20"/>
-      <c r="X42" s="30"/>
-      <c r="Y42" s="16"/>
-      <c r="Z42" s="52"/>
-      <c r="AA42" s="17"/>
-      <c r="AB42" s="17"/>
+    <row r="42" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="30"/>
+      <c r="AA42" s="16"/>
+      <c r="AB42" s="34"/>
       <c r="AC42" s="17"/>
       <c r="AD42" s="17"/>
     </row>
-    <row r="43" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W43" s="20"/>
-      <c r="X43" s="30"/>
-      <c r="Y43" s="16"/>
-      <c r="Z43" s="52"/>
-      <c r="AA43" s="17"/>
-      <c r="AB43" s="17"/>
+    <row r="43" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="30"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="34"/>
       <c r="AC43" s="17"/>
       <c r="AD43" s="17"/>
     </row>
-    <row r="44" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W44" s="20"/>
-      <c r="X44" s="30"/>
-      <c r="Y44" s="16"/>
-      <c r="Z44" s="52"/>
-      <c r="AA44" s="17"/>
-      <c r="AB44" s="17"/>
+    <row r="44" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="30"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="34"/>
       <c r="AC44" s="17"/>
       <c r="AD44" s="32"/>
     </row>
-    <row r="45" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W45" s="20"/>
-      <c r="X45" s="30"/>
-      <c r="Y45" s="16"/>
-      <c r="Z45" s="52"/>
-      <c r="AA45" s="17"/>
-      <c r="AB45" s="17"/>
+    <row r="45" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="30"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="34"/>
       <c r="AC45" s="17"/>
       <c r="AD45" s="17"/>
-      <c r="AH45" s="50"/>
-    </row>
-    <row r="46" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="W46" s="20"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="16"/>
-      <c r="Z46" s="52"/>
-      <c r="AA46" s="17"/>
-      <c r="AB46" s="17"/>
+    </row>
+    <row r="46" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Y46" s="20"/>
+      <c r="Z46" s="30"/>
+      <c r="AA46" s="16"/>
+      <c r="AB46" s="34"/>
       <c r="AC46" s="17"/>
       <c r="AD46" s="17"/>
-      <c r="AH46" s="50"/>
-    </row>
-    <row r="47" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="X47" s="76"/>
-      <c r="Y47" s="76"/>
-      <c r="AH47" s="50"/>
-    </row>
-    <row r="48" spans="23:34" x14ac:dyDescent="0.2">
-      <c r="X48" s="77"/>
-      <c r="Y48" s="76"/>
-      <c r="Z48" s="17"/>
-      <c r="AA48" s="32"/>
-      <c r="AB48" s="32"/>
-      <c r="AH48" s="50"/>
-    </row>
-    <row r="49" spans="24:34" x14ac:dyDescent="0.2">
-      <c r="X49" s="76"/>
-      <c r="Y49" s="76"/>
-      <c r="AH49" s="50"/>
+    </row>
+    <row r="47" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Z47" s="44"/>
+      <c r="AA47" s="44"/>
+    </row>
+    <row r="48" spans="25:30" x14ac:dyDescent="0.2">
+      <c r="Z48" s="45"/>
+      <c r="AA48" s="44"/>
+      <c r="AB48" s="17"/>
+      <c r="AC48" s="32"/>
+    </row>
+    <row r="49" spans="26:27" x14ac:dyDescent="0.2">
+      <c r="Z49" s="44"/>
+      <c r="AA49" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="40">
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="L2:S2"/>
-    <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="AA21:AA23"/>
-    <mergeCell ref="X21:Y23"/>
-    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="P2:W2"/>
+    <mergeCell ref="Z2:AE2"/>
+    <mergeCell ref="AG2:AK2"/>
+    <mergeCell ref="AC21:AC23"/>
+    <mergeCell ref="Z21:AA23"/>
+    <mergeCell ref="Z20:AA20"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="B5:B10"/>
+    <mergeCell ref="AC10:AC12"/>
+    <mergeCell ref="AA13:AA15"/>
+    <mergeCell ref="AC13:AC15"/>
+    <mergeCell ref="AA16:AA18"/>
+    <mergeCell ref="AC16:AC18"/>
+    <mergeCell ref="Z4:Z18"/>
+    <mergeCell ref="AA4:AA6"/>
+    <mergeCell ref="AC4:AC6"/>
+    <mergeCell ref="AA7:AA9"/>
+    <mergeCell ref="AC7:AC9"/>
     <mergeCell ref="AA10:AA12"/>
-    <mergeCell ref="Y13:Y15"/>
-    <mergeCell ref="AA13:AA15"/>
-    <mergeCell ref="Y16:Y18"/>
-    <mergeCell ref="AA16:AA18"/>
-    <mergeCell ref="X4:X18"/>
-    <mergeCell ref="Y4:Y6"/>
-    <mergeCell ref="AA4:AA6"/>
-    <mergeCell ref="Y7:Y9"/>
-    <mergeCell ref="AA7:AA9"/>
-    <mergeCell ref="Y10:Y12"/>
-    <mergeCell ref="L3:O4"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="L5:M10"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="L11:L24"/>
-    <mergeCell ref="M11:M17"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="M18:M24"/>
-    <mergeCell ref="N19:N21"/>
-    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="P3:S4"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="P5:Q10"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="P11:P24"/>
+    <mergeCell ref="Q11:Q17"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="Q18:Q24"/>
+    <mergeCell ref="R19:R21"/>
+    <mergeCell ref="R22:R24"/>
   </mergeCells>
-  <conditionalFormatting sqref="P5:S7 P11:Q24 S11:S24 P8:P10">
+  <conditionalFormatting sqref="K5:K6 D8:N10 D5:I5 D6:K7">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T5:W7 T11:U24 W11:W24 T8:T10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V11:V24">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -6018,30 +5942,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R11:R24">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FFFCFCFF"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:I10">
+  <conditionalFormatting sqref="AC4:AE18">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFFF0000"/>
-        <color rgb="FFFCFCFF"/>
+        <color theme="2"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
gemini, degree=1,2, fs-comb ec results added
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969CC8F3-A649-FC4C-9016-B7F385C8AF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B54E0D-C333-2249-B8FE-9FA8E4635876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="13760" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -657,43 +657,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -702,18 +729,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -731,21 +746,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2737,24 +2737,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -2769,120 +2769,120 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="74">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="J4" s="5"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73" t="s">
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="J5" s="5"/>
       <c r="K5" s="17"/>
       <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73" t="s">
+      <c r="A7" s="78"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="74">
+      <c r="E7" s="71">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
       <c r="J7" s="5"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
       <c r="J8" s="5"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="78" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
@@ -2901,31 +2901,31 @@
       <c r="H9" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L9" s="78" t="s">
+      <c r="L9" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="78"/>
-      <c r="N9" s="76" t="s">
+      <c r="M9" s="70"/>
+      <c r="N9" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
-      <c r="S9" s="76"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="76"/>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="76"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
+      <c r="W9" s="69"/>
+      <c r="X9" s="69"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73" t="s">
+      <c r="A10" s="78"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -2943,31 +2943,31 @@
       <c r="H10" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="76" t="s">
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="76"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="76" t="s">
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="76"/>
-      <c r="W10" s="76"/>
-      <c r="X10" s="76"/>
-      <c r="Y10" s="76"/>
-      <c r="Z10" s="76"/>
-      <c r="AA10" s="76"/>
+      <c r="V10" s="69"/>
+      <c r="W10" s="69"/>
+      <c r="X10" s="69"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
     </row>
     <row r="11" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
@@ -2983,39 +2983,39 @@
       <c r="H11" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78" t="s">
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="76" t="s">
+      <c r="O11" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="76" t="s">
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="76"/>
-      <c r="T11" s="76"/>
-      <c r="U11" s="78" t="s">
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="76" t="s">
+      <c r="V11" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="W11" s="76"/>
-      <c r="X11" s="76"/>
-      <c r="Y11" s="76" t="s">
+      <c r="W11" s="69"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="Z11" s="76"/>
-      <c r="AA11" s="76"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
@@ -3031,9 +3031,9 @@
       <c r="H12" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="76"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="69"/>
       <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3052,7 +3052,7 @@
       <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="76"/>
+      <c r="U12" s="69"/>
       <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3073,9 +3073,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73" t="s">
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -3099,53 +3099,53 @@
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="77">
+      <c r="N13" s="72">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="79">
+      <c r="O13" s="73">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="79">
+      <c r="P13" s="73">
         <v>0.50667970022808695</v>
       </c>
-      <c r="Q13" s="74">
+      <c r="Q13" s="71">
         <v>0.46757901596611201</v>
       </c>
-      <c r="R13" s="74">
+      <c r="R13" s="71">
         <v>0.93385467579015902</v>
       </c>
-      <c r="S13" s="74">
+      <c r="S13" s="71">
         <v>0.76050830889540499</v>
       </c>
-      <c r="T13" s="74">
+      <c r="T13" s="71">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="77">
+      <c r="U13" s="72">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="79">
+      <c r="V13" s="73">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="79">
+      <c r="W13" s="73">
         <v>0.516780710329097</v>
       </c>
-      <c r="X13" s="74">
+      <c r="X13" s="71">
         <v>0.53828608667318301</v>
       </c>
-      <c r="Y13" s="74">
+      <c r="Y13" s="71">
         <v>0.928641251221896</v>
       </c>
-      <c r="Z13" s="74">
+      <c r="Z13" s="71">
         <v>0.83447376995764</v>
       </c>
-      <c r="AA13" s="74">
+      <c r="AA13" s="71">
         <v>0.916585206907787</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -3167,25 +3167,25 @@
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="77"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="74"/>
-      <c r="T14" s="74"/>
-      <c r="U14" s="77"/>
-      <c r="V14" s="79"/>
-      <c r="W14" s="79"/>
-      <c r="X14" s="74"/>
-      <c r="Y14" s="74"/>
-      <c r="Z14" s="74"/>
-      <c r="AA14" s="74"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="72"/>
+      <c r="V14" s="73"/>
+      <c r="W14" s="73"/>
+      <c r="X14" s="71"/>
+      <c r="Y14" s="71"/>
+      <c r="Z14" s="71"/>
+      <c r="AA14" s="71"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -3207,24 +3207,24 @@
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="77"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="74"/>
-      <c r="T15" s="74"/>
-      <c r="U15" s="77"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="79"/>
-      <c r="X15" s="74"/>
-      <c r="Y15" s="74"/>
-      <c r="Z15" s="74"/>
-      <c r="AA15" s="74"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="73"/>
+      <c r="W15" s="73"/>
+      <c r="X15" s="71"/>
+      <c r="Y15" s="71"/>
+      <c r="Z15" s="71"/>
+      <c r="AA15" s="71"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73" t="s">
+      <c r="A16" s="78"/>
+      <c r="B16" s="78" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="15"/>
@@ -3249,25 +3249,25 @@
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="77"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="74"/>
-      <c r="T16" s="74"/>
-      <c r="U16" s="77"/>
-      <c r="V16" s="79"/>
-      <c r="W16" s="79"/>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
-      <c r="Z16" s="74"/>
-      <c r="AA16" s="74"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="72"/>
+      <c r="V16" s="73"/>
+      <c r="W16" s="73"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="73"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73" t="s">
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3291,25 +3291,25 @@
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="77"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="74"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="77"/>
-      <c r="V17" s="79"/>
-      <c r="W17" s="79"/>
-      <c r="X17" s="74"/>
-      <c r="Y17" s="74"/>
-      <c r="Z17" s="74"/>
-      <c r="AA17" s="74"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="72"/>
+      <c r="V17" s="73"/>
+      <c r="W17" s="73"/>
+      <c r="X17" s="71"/>
+      <c r="Y17" s="71"/>
+      <c r="Z17" s="71"/>
+      <c r="AA17" s="71"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
@@ -3327,9 +3327,9 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3347,9 +3347,9 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73" t="s">
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -3369,9 +3369,9 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
@@ -3404,9 +3404,9 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
@@ -3464,43 +3464,43 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="75">
+      <c r="E24" s="76">
         <v>0.995</v>
       </c>
-      <c r="F24" s="75"/>
+      <c r="F24" s="76"/>
       <c r="L24" s="24"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
       <c r="L25" s="24"/>
       <c r="M25" s="5"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="75" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="21">
@@ -3516,9 +3516,9 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="70"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
+      <c r="A27" s="74"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
       <c r="D27" s="21">
         <v>2</v>
       </c>
@@ -3526,9 +3526,9 @@
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="21">
         <v>5</v>
       </c>
@@ -3536,9 +3536,9 @@
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="70"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
       <c r="D29" s="21">
         <v>10</v>
       </c>
@@ -3550,9 +3550,9 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="70"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
+      <c r="A30" s="74"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
       <c r="D30" s="21">
         <v>20</v>
       </c>
@@ -3560,9 +3560,9 @@
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="70"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69" t="s">
+      <c r="A31" s="74"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="21">
@@ -3572,9 +3572,9 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
+      <c r="A32" s="74"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
       <c r="D32" s="21">
         <v>2</v>
       </c>
@@ -3582,9 +3582,9 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="70"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
       <c r="D33" s="21">
         <v>3</v>
       </c>
@@ -3592,9 +3592,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="70"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
+      <c r="A34" s="74"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
       <c r="D34" s="21">
         <v>4</v>
       </c>
@@ -3602,9 +3602,9 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="70"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
+      <c r="A35" s="74"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
       <c r="D35" s="21">
         <v>5</v>
       </c>
@@ -3612,12 +3612,12 @@
       <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" s="71" t="s">
+      <c r="A36" s="74"/>
+      <c r="B36" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
       <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
@@ -3630,6 +3630,41 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A9:A22"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="AA13:AA17"/>
+    <mergeCell ref="N10:T10"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="P13:P17"/>
     <mergeCell ref="N9:AA9"/>
     <mergeCell ref="L9:M12"/>
     <mergeCell ref="Q13:Q17"/>
@@ -3646,41 +3681,6 @@
     <mergeCell ref="X13:X17"/>
     <mergeCell ref="Y13:Y17"/>
     <mergeCell ref="Z13:Z17"/>
-    <mergeCell ref="AA13:AA17"/>
-    <mergeCell ref="N10:T10"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="P13:P17"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A9:A22"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="C26:C30"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H22">
     <cfRule type="colorScale" priority="1">
@@ -3742,18 +3742,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
       <c r="M1" s="14"/>
       <c r="N1" s="24" t="s">
         <v>55</v>
@@ -3778,10 +3778,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -3797,16 +3797,16 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="73" t="s">
+      <c r="L2" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="81">
+      <c r="M2" s="80">
         <v>1</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="74">
+      <c r="O2" s="71">
         <v>0.85728300000000002</v>
       </c>
       <c r="P2" s="17">
@@ -3826,31 +3826,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="74">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="81"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="80"/>
       <c r="N3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="74"/>
+      <c r="O3" s="71"/>
       <c r="P3" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -3862,27 +3862,27 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="81"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="80"/>
       <c r="N4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="74"/>
+      <c r="O4" s="71"/>
       <c r="P4" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -3896,31 +3896,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73" t="s">
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="81">
+      <c r="L5" s="78"/>
+      <c r="M5" s="80">
         <v>2</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="74">
+      <c r="O5" s="71">
         <v>0.90257399999999999</v>
       </c>
       <c r="P5" s="17">
@@ -3940,27 +3940,27 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="81"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="80"/>
       <c r="N6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="74"/>
+      <c r="O6" s="71"/>
       <c r="P6" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -3972,10 +3972,10 @@
       <c r="T6" s="17"/>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="78" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="15"/>
@@ -3994,12 +3994,12 @@
       <c r="H7" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L7" s="73"/>
-      <c r="M7" s="81"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="80"/>
       <c r="N7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="74"/>
+      <c r="O7" s="71"/>
       <c r="P7" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4013,9 +4013,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73" t="s">
+      <c r="A8" s="78"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -4033,14 +4033,14 @@
       <c r="H8" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L8" s="73"/>
-      <c r="M8" s="81">
+      <c r="L8" s="78"/>
+      <c r="M8" s="80">
         <v>5</v>
       </c>
       <c r="N8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="74">
+      <c r="O8" s="71">
         <v>0.93776499999999996</v>
       </c>
       <c r="P8" s="17">
@@ -4060,9 +4060,9 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
@@ -4078,12 +4078,12 @@
       <c r="H9" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L9" s="73"/>
-      <c r="M9" s="81"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="80"/>
       <c r="N9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="74"/>
+      <c r="O9" s="71"/>
       <c r="P9" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4095,9 +4095,9 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -4113,12 +4113,12 @@
       <c r="H10" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L10" s="73"/>
-      <c r="M10" s="81"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="80"/>
       <c r="N10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="74"/>
+      <c r="O10" s="71"/>
       <c r="P10" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4132,9 +4132,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73" t="s">
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -4152,14 +4152,14 @@
       <c r="H11" s="19">
         <v>0.94037099999999996</v>
       </c>
-      <c r="L11" s="73"/>
-      <c r="M11" s="81">
+      <c r="L11" s="78"/>
+      <c r="M11" s="80">
         <v>10</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="74">
+      <c r="O11" s="71">
         <v>0.94330400000000003</v>
       </c>
       <c r="P11" s="17">
@@ -4179,9 +4179,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
@@ -4197,12 +4197,12 @@
       <c r="H12" s="19">
         <v>0.754969</v>
       </c>
-      <c r="L12" s="73"/>
-      <c r="M12" s="81"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="80"/>
       <c r="N12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="74"/>
+      <c r="O12" s="71"/>
       <c r="P12" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4214,9 +4214,9 @@
       <c r="T12" s="17"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
@@ -4232,12 +4232,12 @@
       <c r="H13" s="19">
         <v>0.94884299999999999</v>
       </c>
-      <c r="L13" s="73"/>
-      <c r="M13" s="81"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="80"/>
       <c r="N13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="74"/>
+      <c r="O13" s="71"/>
       <c r="P13" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4251,8 +4251,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73" t="s">
+      <c r="A14" s="78"/>
+      <c r="B14" s="78" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="15"/>
@@ -4271,14 +4271,14 @@
       <c r="H14" s="19">
         <v>0.63245399999999996</v>
       </c>
-      <c r="L14" s="73"/>
-      <c r="M14" s="81">
+      <c r="L14" s="78"/>
+      <c r="M14" s="80">
         <v>20</v>
       </c>
       <c r="N14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="74">
+      <c r="O14" s="71">
         <v>0.93548399999999998</v>
       </c>
       <c r="P14" s="17">
@@ -4298,9 +4298,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73" t="s">
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -4318,12 +4318,12 @@
       <c r="H15" s="19">
         <v>0.68589100000000003</v>
       </c>
-      <c r="L15" s="73"/>
-      <c r="M15" s="81"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="80"/>
       <c r="N15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="74"/>
+      <c r="O15" s="71"/>
       <c r="P15" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4335,9 +4335,9 @@
       <c r="T15" s="17"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -4353,12 +4353,12 @@
       <c r="H16" s="19">
         <v>0.68067800000000001</v>
       </c>
-      <c r="L16" s="73"/>
-      <c r="M16" s="81"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="80"/>
       <c r="N16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="74"/>
+      <c r="O16" s="71"/>
       <c r="P16" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4372,9 +4372,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="73"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -4394,9 +4394,9 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73" t="s">
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -4422,9 +4422,9 @@
       <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
@@ -4444,9 +4444,9 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
       <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L28" s="5"/>
-      <c r="M28" s="77"/>
+      <c r="M28" s="72"/>
       <c r="N28" s="5"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L29" s="5"/>
-      <c r="M29" s="77"/>
+      <c r="M29" s="72"/>
       <c r="N29" s="5"/>
       <c r="O29" s="17"/>
       <c r="P29" s="25"/>
@@ -4524,7 +4524,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L30" s="5"/>
-      <c r="M30" s="77"/>
+      <c r="M30" s="72"/>
       <c r="N30" s="5"/>
       <c r="O30" s="17"/>
       <c r="P30" s="25"/>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L31" s="5"/>
-      <c r="M31" s="77"/>
+      <c r="M31" s="72"/>
       <c r="N31" s="5"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L32" s="5"/>
-      <c r="M32" s="77"/>
+      <c r="M32" s="72"/>
       <c r="N32" s="5"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -4551,18 +4551,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="L2:L16"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="O14:O16"/>
     <mergeCell ref="M28:M32"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C3:C4"/>
@@ -4579,6 +4567,18 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H6 E7:F20 H7:H20">
     <cfRule type="colorScale" priority="4">
@@ -4612,8 +4612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
   <dimension ref="B2:AK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4651,53 +4651,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:37" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="P2" s="82" t="s">
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="P2" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82"/>
-      <c r="Z2" s="82" t="s">
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+      <c r="Z2" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="AA2" s="82"/>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82"/>
-      <c r="AG2" s="82" t="s">
+      <c r="AA2" s="91"/>
+      <c r="AB2" s="91"/>
+      <c r="AC2" s="91"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
+      <c r="AG2" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82"/>
-      <c r="AJ2" s="82"/>
-      <c r="AK2" s="82"/>
+      <c r="AH2" s="91"/>
+      <c r="AI2" s="91"/>
+      <c r="AJ2" s="91"/>
+      <c r="AK2" s="91"/>
     </row>
     <row r="3" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="91"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="96"/>
       <c r="K3" s="46"/>
       <c r="L3" s="51" t="s">
         <v>65</v>
@@ -4708,18 +4708,18 @@
       <c r="N3" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="94" t="s">
+      <c r="P3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95" t="s">
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="97"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="88"/>
       <c r="Y3" s="30"/>
       <c r="Z3" s="46"/>
       <c r="AA3" s="47"/>
@@ -4753,8 +4753,8 @@
       </c>
     </row>
     <row r="4" spans="2:37" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="90"/>
-      <c r="C4" s="81"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="13" t="s">
         <v>56</v>
       </c>
@@ -4786,10 +4786,10 @@
         <f>AVERAGE(D6:D10)</f>
         <v>0.92059999999999997</v>
       </c>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
       <c r="T4" s="16" t="s">
         <v>36</v>
       </c>
@@ -4804,16 +4804,16 @@
       </c>
       <c r="X4" s="20"/>
       <c r="Y4" s="30"/>
-      <c r="Z4" s="85" t="s">
+      <c r="Z4" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="AA4" s="81">
+      <c r="AA4" s="80">
         <v>1</v>
       </c>
       <c r="AB4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AC4" s="74">
+      <c r="AC4" s="71">
         <v>0.86699999999999999</v>
       </c>
       <c r="AD4" s="17">
@@ -4840,7 +4840,7 @@
       </c>
     </row>
     <row r="5" spans="2:37" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="97" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -4876,34 +4876,36 @@
         <f>AVERAGE(E5:I5)</f>
         <v>0.84460000000000002</v>
       </c>
-      <c r="P5" s="84" t="s">
+      <c r="P5" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73" t="s">
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78" t="s">
         <v>25</v>
       </c>
       <c r="S5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="74">
+      <c r="T5" s="71">
         <v>0.86699999999999999</v>
       </c>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="98"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="90"/>
       <c r="X5" s="20"/>
       <c r="Y5" s="30"/>
-      <c r="Z5" s="85"/>
-      <c r="AA5" s="81"/>
+      <c r="Z5" s="82"/>
+      <c r="AA5" s="80"/>
       <c r="AB5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AC5" s="74"/>
+      <c r="AC5" s="71"/>
       <c r="AD5" s="17">
         <v>0.91500000000000004</v>
       </c>
-      <c r="AE5" s="39"/>
+      <c r="AE5" s="39">
+        <v>0.93700000000000006</v>
+      </c>
       <c r="AF5" s="17"/>
       <c r="AG5" s="62">
         <v>10</v>
@@ -4922,7 +4924,7 @@
       </c>
     </row>
     <row r="6" spans="2:37" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="92"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="13">
         <v>1</v>
       </c>
@@ -4958,26 +4960,26 @@
         <f>AVERAGE(E6:I10)</f>
         <v>0.91474745461062212</v>
       </c>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
       <c r="S6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="74">
+      <c r="T6" s="71">
         <v>0.94799999999999995</v>
       </c>
-      <c r="U6" s="74"/>
-      <c r="V6" s="74"/>
-      <c r="W6" s="98"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="90"/>
       <c r="X6" s="20"/>
       <c r="Y6" s="30"/>
-      <c r="Z6" s="85"/>
-      <c r="AA6" s="81"/>
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="80"/>
       <c r="AB6" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AC6" s="74"/>
+      <c r="AC6" s="71"/>
       <c r="AD6" s="17"/>
       <c r="AE6" s="39">
         <v>0.95</v>
@@ -4985,7 +4987,7 @@
       <c r="AF6" s="33"/>
     </row>
     <row r="7" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="92"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="13">
         <v>2</v>
       </c>
@@ -5012,30 +5014,30 @@
       <c r="L7" s="54"/>
       <c r="M7" s="54"/>
       <c r="N7" s="54"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73" t="s">
+      <c r="P7" s="82"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78" t="s">
         <v>26</v>
       </c>
       <c r="S7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="T7" s="74">
+      <c r="T7" s="71">
         <v>0.83499999999999996</v>
       </c>
-      <c r="U7" s="74"/>
-      <c r="V7" s="74"/>
-      <c r="W7" s="98"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="90"/>
       <c r="X7" s="20"/>
       <c r="Y7" s="30"/>
-      <c r="Z7" s="85"/>
-      <c r="AA7" s="81">
+      <c r="Z7" s="82"/>
+      <c r="AA7" s="80">
         <v>2</v>
       </c>
       <c r="AB7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AC7" s="74">
+      <c r="AC7" s="71">
         <v>0.90800000000000003</v>
       </c>
       <c r="AD7" s="17">
@@ -5047,7 +5049,7 @@
       <c r="AF7" s="17"/>
     </row>
     <row r="8" spans="2:37" ht="20" x14ac:dyDescent="0.2">
-      <c r="B8" s="92"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="13">
         <v>5</v>
       </c>
@@ -5074,34 +5076,36 @@
       <c r="L8" s="54"/>
       <c r="M8" s="54"/>
       <c r="N8" s="54"/>
-      <c r="P8" s="85"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
       <c r="S8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="T8" s="74">
+      <c r="T8" s="71">
         <v>0.85199999999999998</v>
       </c>
-      <c r="U8" s="74"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="98"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="90"/>
       <c r="X8" s="20"/>
       <c r="Y8" s="30"/>
-      <c r="Z8" s="85"/>
-      <c r="AA8" s="81"/>
+      <c r="Z8" s="82"/>
+      <c r="AA8" s="80"/>
       <c r="AB8" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AC8" s="74"/>
+      <c r="AC8" s="71"/>
       <c r="AD8" s="17">
         <v>0.93200000000000005</v>
       </c>
-      <c r="AE8" s="39"/>
+      <c r="AE8" s="39">
+        <v>0.93700000000000006</v>
+      </c>
       <c r="AF8" s="17"/>
     </row>
     <row r="9" spans="2:37" ht="20" x14ac:dyDescent="0.25">
-      <c r="B9" s="92"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="13">
         <v>10</v>
       </c>
@@ -5128,28 +5132,28 @@
       <c r="L9" s="54"/>
       <c r="M9" s="54"/>
       <c r="N9" s="54"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73" t="s">
+      <c r="P9" s="82"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78" t="s">
         <v>27</v>
       </c>
       <c r="S9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="T9" s="74">
+      <c r="T9" s="71">
         <v>0.83699999999999997</v>
       </c>
-      <c r="U9" s="74"/>
-      <c r="V9" s="74"/>
-      <c r="W9" s="98"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="90"/>
       <c r="X9" s="20"/>
       <c r="Y9" s="30"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="81"/>
+      <c r="Z9" s="82"/>
+      <c r="AA9" s="80"/>
       <c r="AB9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AC9" s="74"/>
+      <c r="AC9" s="71"/>
       <c r="AD9" s="17"/>
       <c r="AE9" s="39">
         <v>0.95</v>
@@ -5157,7 +5161,7 @@
       <c r="AF9" s="33"/>
     </row>
     <row r="10" spans="2:37" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="93"/>
+      <c r="B10" s="98"/>
       <c r="C10" s="41">
         <v>20</v>
       </c>
@@ -5184,28 +5188,28 @@
       <c r="L10" s="54"/>
       <c r="M10" s="54"/>
       <c r="N10" s="54"/>
-      <c r="P10" s="85"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
       <c r="S10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T10" s="74">
+      <c r="T10" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="U10" s="74"/>
-      <c r="V10" s="74"/>
-      <c r="W10" s="98"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="90"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="30"/>
-      <c r="Z10" s="85"/>
-      <c r="AA10" s="81">
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="80">
         <v>5</v>
       </c>
       <c r="AB10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AC10" s="74">
+      <c r="AC10" s="71">
         <v>0.94599999999999995</v>
       </c>
       <c r="AD10" s="17">
@@ -5223,10 +5227,10 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
-      <c r="P11" s="85" t="s">
+      <c r="P11" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="73" t="s">
+      <c r="Q11" s="78" t="s">
         <v>6</v>
       </c>
       <c r="R11" s="15"/>
@@ -5246,12 +5250,12 @@
         <v>0.60299999999999998</v>
       </c>
       <c r="Y11" s="30"/>
-      <c r="Z11" s="85"/>
-      <c r="AA11" s="81"/>
+      <c r="Z11" s="82"/>
+      <c r="AA11" s="80"/>
       <c r="AB11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AC11" s="74"/>
+      <c r="AC11" s="71"/>
       <c r="AD11" s="17">
         <v>0.94799999999999995</v>
       </c>
@@ -5259,9 +5263,9 @@
       <c r="AF11" s="17"/>
     </row>
     <row r="12" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="85"/>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="73" t="s">
+      <c r="P12" s="82"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="78" t="s">
         <v>23</v>
       </c>
       <c r="S12" s="13" t="s">
@@ -5280,12 +5284,12 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="Y12" s="30"/>
-      <c r="Z12" s="85"/>
-      <c r="AA12" s="81"/>
+      <c r="Z12" s="82"/>
+      <c r="AA12" s="80"/>
       <c r="AB12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AC12" s="74"/>
+      <c r="AC12" s="71"/>
       <c r="AD12" s="17"/>
       <c r="AE12" s="39">
         <v>0.95199999999999996</v>
@@ -5293,9 +5297,9 @@
       <c r="AF12" s="33"/>
     </row>
     <row r="13" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P13" s="85"/>
-      <c r="Q13" s="73"/>
-      <c r="R13" s="73"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
       <c r="S13" s="13" t="s">
         <v>26</v>
       </c>
@@ -5312,14 +5316,14 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="Y13" s="30"/>
-      <c r="Z13" s="85"/>
-      <c r="AA13" s="81">
+      <c r="Z13" s="82"/>
+      <c r="AA13" s="80">
         <v>10</v>
       </c>
       <c r="AB13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AC13" s="74">
+      <c r="AC13" s="71">
         <v>0.94799999999999995</v>
       </c>
       <c r="AD13" s="17">
@@ -5331,9 +5335,9 @@
       <c r="AF13" s="17"/>
     </row>
     <row r="14" spans="2:37" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P14" s="85"/>
-      <c r="Q14" s="73"/>
-      <c r="R14" s="73"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
       <c r="S14" s="13" t="s">
         <v>27</v>
       </c>
@@ -5350,12 +5354,12 @@
         <v>0.67600000000000005</v>
       </c>
       <c r="Y14" s="30"/>
-      <c r="Z14" s="85"/>
-      <c r="AA14" s="81"/>
+      <c r="Z14" s="82"/>
+      <c r="AA14" s="80"/>
       <c r="AB14" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AC14" s="74"/>
+      <c r="AC14" s="71"/>
       <c r="AD14" s="17">
         <v>0.94799999999999995</v>
       </c>
@@ -5363,9 +5367,9 @@
       <c r="AF14" s="17"/>
     </row>
     <row r="15" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P15" s="85"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="73" t="s">
+      <c r="P15" s="82"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="78" t="s">
         <v>24</v>
       </c>
       <c r="S15" s="13" t="s">
@@ -5384,12 +5388,12 @@
         <v>0.94599999999999995</v>
       </c>
       <c r="Y15" s="30"/>
-      <c r="Z15" s="85"/>
-      <c r="AA15" s="81"/>
+      <c r="Z15" s="82"/>
+      <c r="AA15" s="80"/>
       <c r="AB15" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AC15" s="74"/>
+      <c r="AC15" s="71"/>
       <c r="AD15" s="17"/>
       <c r="AE15" s="39">
         <v>0.95199999999999996</v>
@@ -5397,9 +5401,9 @@
       <c r="AF15" s="33"/>
     </row>
     <row r="16" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="P16" s="85"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="78"/>
+      <c r="R16" s="78"/>
       <c r="S16" s="13" t="s">
         <v>26</v>
       </c>
@@ -5416,14 +5420,14 @@
         <v>0.73199999999999998</v>
       </c>
       <c r="Y16" s="30"/>
-      <c r="Z16" s="85"/>
-      <c r="AA16" s="81">
+      <c r="Z16" s="82"/>
+      <c r="AA16" s="80">
         <v>20</v>
       </c>
       <c r="AB16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AC16" s="74">
+      <c r="AC16" s="71">
         <v>0.93400000000000005</v>
       </c>
       <c r="AD16" s="17">
@@ -5435,9 +5439,9 @@
       <c r="AF16" s="17"/>
     </row>
     <row r="17" spans="16:32" x14ac:dyDescent="0.25">
-      <c r="P17" s="85"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="73"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="78"/>
+      <c r="R17" s="78"/>
       <c r="S17" s="13" t="s">
         <v>27</v>
       </c>
@@ -5454,12 +5458,12 @@
         <v>0.95</v>
       </c>
       <c r="Y17" s="30"/>
-      <c r="Z17" s="85"/>
-      <c r="AA17" s="81"/>
+      <c r="Z17" s="82"/>
+      <c r="AA17" s="80"/>
       <c r="AB17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AC17" s="74"/>
+      <c r="AC17" s="71"/>
       <c r="AD17" s="17">
         <v>0.93700000000000006</v>
       </c>
@@ -5467,8 +5471,8 @@
       <c r="AF17" s="17"/>
     </row>
     <row r="18" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P18" s="85"/>
-      <c r="Q18" s="73" t="s">
+      <c r="P18" s="82"/>
+      <c r="Q18" s="78" t="s">
         <v>7</v>
       </c>
       <c r="R18" s="15"/>
@@ -5488,12 +5492,12 @@
         <v>0.63300000000000001</v>
       </c>
       <c r="Y18" s="30"/>
-      <c r="Z18" s="86"/>
-      <c r="AA18" s="82"/>
+      <c r="Z18" s="83"/>
+      <c r="AA18" s="91"/>
       <c r="AB18" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="AC18" s="83"/>
+      <c r="AC18" s="92"/>
       <c r="AD18" s="49"/>
       <c r="AE18" s="50">
         <v>0.94699999999999995</v>
@@ -5501,9 +5505,9 @@
       <c r="AF18" s="33"/>
     </row>
     <row r="19" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P19" s="85"/>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="73" t="s">
+      <c r="P19" s="82"/>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="78" t="s">
         <v>23</v>
       </c>
       <c r="S19" s="13" t="s">
@@ -5531,9 +5535,9 @@
       <c r="AF19" s="30"/>
     </row>
     <row r="20" spans="16:32" x14ac:dyDescent="0.25">
-      <c r="P20" s="85"/>
-      <c r="Q20" s="73"/>
-      <c r="R20" s="73"/>
+      <c r="P20" s="82"/>
+      <c r="Q20" s="78"/>
+      <c r="R20" s="78"/>
       <c r="S20" s="13" t="s">
         <v>26</v>
       </c>
@@ -5550,8 +5554,8 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="Y20" s="30"/>
-      <c r="Z20" s="88"/>
-      <c r="AA20" s="89"/>
+      <c r="Z20" s="93"/>
+      <c r="AA20" s="94"/>
       <c r="AB20" s="35" t="s">
         <v>55</v>
       </c>
@@ -5567,9 +5571,9 @@
       <c r="AF20" s="30"/>
     </row>
     <row r="21" spans="16:32" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P21" s="85"/>
-      <c r="Q21" s="73"/>
-      <c r="R21" s="73"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="78"/>
+      <c r="R21" s="78"/>
       <c r="S21" s="13" t="s">
         <v>27</v>
       </c>
@@ -5586,14 +5590,14 @@
         <v>0.66300000000000003</v>
       </c>
       <c r="Y21" s="30"/>
-      <c r="Z21" s="84" t="s">
+      <c r="Z21" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="AA21" s="73"/>
+      <c r="AA21" s="78"/>
       <c r="AB21" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AC21" s="74">
+      <c r="AC21" s="71">
         <v>0.95099999999999996</v>
       </c>
       <c r="AD21" s="17"/>
@@ -5601,9 +5605,9 @@
       <c r="AF21" s="30"/>
     </row>
     <row r="22" spans="16:32" x14ac:dyDescent="0.25">
-      <c r="P22" s="85"/>
-      <c r="Q22" s="73"/>
-      <c r="R22" s="73" t="s">
+      <c r="P22" s="82"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78" t="s">
         <v>24</v>
       </c>
       <c r="S22" s="13" t="s">
@@ -5622,20 +5626,20 @@
         <v>0.93600000000000005</v>
       </c>
       <c r="Y22" s="30"/>
-      <c r="Z22" s="85"/>
-      <c r="AA22" s="73"/>
+      <c r="Z22" s="82"/>
+      <c r="AA22" s="78"/>
       <c r="AB22" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AC22" s="74"/>
+      <c r="AC22" s="71"/>
       <c r="AD22" s="17"/>
       <c r="AE22" s="39"/>
       <c r="AF22" s="30"/>
     </row>
     <row r="23" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P23" s="85"/>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="73"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
       <c r="S23" s="13" t="s">
         <v>26</v>
       </c>
@@ -5652,20 +5656,20 @@
         <v>0.94499999999999995</v>
       </c>
       <c r="Y23" s="30"/>
-      <c r="Z23" s="86"/>
-      <c r="AA23" s="87"/>
+      <c r="Z23" s="83"/>
+      <c r="AA23" s="84"/>
       <c r="AB23" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="AC23" s="83"/>
+      <c r="AC23" s="92"/>
       <c r="AD23" s="49"/>
       <c r="AE23" s="50"/>
       <c r="AF23" s="30"/>
     </row>
     <row r="24" spans="16:32" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P24" s="86"/>
-      <c r="Q24" s="87"/>
-      <c r="R24" s="87"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="84"/>
+      <c r="R24" s="84"/>
       <c r="S24" s="41" t="s">
         <v>27</v>
       </c>
@@ -5855,30 +5859,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="P11:P24"/>
-    <mergeCell ref="Q11:Q17"/>
-    <mergeCell ref="R12:R14"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="Q18:Q24"/>
-    <mergeCell ref="R19:R21"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="P3:S4"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="P5:Q10"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="AA4:AA6"/>
-    <mergeCell ref="AC4:AC6"/>
-    <mergeCell ref="AA7:AA9"/>
-    <mergeCell ref="AC7:AC9"/>
-    <mergeCell ref="AA10:AA12"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="P2:W2"/>
     <mergeCell ref="Z2:AE2"/>
@@ -5895,6 +5875,30 @@
     <mergeCell ref="AA16:AA18"/>
     <mergeCell ref="AC16:AC18"/>
     <mergeCell ref="Z4:Z18"/>
+    <mergeCell ref="AA4:AA6"/>
+    <mergeCell ref="AC4:AC6"/>
+    <mergeCell ref="AA7:AA9"/>
+    <mergeCell ref="AC7:AC9"/>
+    <mergeCell ref="AA10:AA12"/>
+    <mergeCell ref="P3:S4"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="P5:Q10"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="P11:P24"/>
+    <mergeCell ref="Q11:Q17"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="Q18:Q24"/>
+    <mergeCell ref="R19:R21"/>
+    <mergeCell ref="R22:R24"/>
   </mergeCells>
   <conditionalFormatting sqref="K5:K6 D8:N10 D5:I5 D6:K7">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
test gpt comb ec results
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21B310B-7176-014B-9776-C4CC9BFD5084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0763E680-6413-0C49-94D7-D933C195F982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="13760" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -687,104 +687,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2776,24 +2776,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -2808,120 +2808,120 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="J4" s="5"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75" t="s">
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="J5" s="5"/>
       <c r="K5" s="17"/>
       <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="75"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="71">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
       <c r="J7" s="5"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
       <c r="J8" s="5"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="70" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
@@ -2940,31 +2940,31 @@
       <c r="H9" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L9" s="67" t="s">
+      <c r="L9" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="67"/>
-      <c r="N9" s="66" t="s">
+      <c r="M9" s="75"/>
+      <c r="N9" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="66"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="66"/>
-      <c r="U9" s="66"/>
-      <c r="V9" s="66"/>
-      <c r="W9" s="66"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="73"/>
+      <c r="V9" s="73"/>
+      <c r="W9" s="73"/>
+      <c r="X9" s="73"/>
+      <c r="Y9" s="73"/>
+      <c r="Z9" s="73"/>
+      <c r="AA9" s="73"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75" t="s">
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -2982,31 +2982,31 @@
       <c r="H10" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="66" t="s">
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
-      <c r="U10" s="66" t="s">
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="66"/>
-      <c r="W10" s="66"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="66"/>
+      <c r="V10" s="73"/>
+      <c r="W10" s="73"/>
+      <c r="X10" s="73"/>
+      <c r="Y10" s="73"/>
+      <c r="Z10" s="73"/>
+      <c r="AA10" s="73"/>
     </row>
     <row r="11" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
@@ -3022,39 +3022,39 @@
       <c r="H11" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67" t="s">
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="66" t="s">
+      <c r="O11" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66" t="s">
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="67" t="s">
+      <c r="S11" s="73"/>
+      <c r="T11" s="73"/>
+      <c r="U11" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="66" t="s">
+      <c r="V11" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="W11" s="66"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="66" t="s">
+      <c r="W11" s="73"/>
+      <c r="X11" s="73"/>
+      <c r="Y11" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
+      <c r="Z11" s="73"/>
+      <c r="AA11" s="73"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
@@ -3070,9 +3070,9 @@
       <c r="H12" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="66"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="66"/>
+      <c r="U12" s="73"/>
       <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3112,9 +3112,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75" t="s">
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -3138,53 +3138,53 @@
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="69">
+      <c r="N13" s="74">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="70">
+      <c r="O13" s="76">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="70">
+      <c r="P13" s="76">
         <v>0.50667970022808695</v>
       </c>
-      <c r="Q13" s="68">
+      <c r="Q13" s="71">
         <v>0.46757901596611201</v>
       </c>
-      <c r="R13" s="68">
+      <c r="R13" s="71">
         <v>0.93385467579015902</v>
       </c>
-      <c r="S13" s="68">
+      <c r="S13" s="71">
         <v>0.76050830889540499</v>
       </c>
-      <c r="T13" s="68">
+      <c r="T13" s="71">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="69">
+      <c r="U13" s="74">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="70">
+      <c r="V13" s="76">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="70">
+      <c r="W13" s="76">
         <v>0.516780710329097</v>
       </c>
-      <c r="X13" s="68">
+      <c r="X13" s="71">
         <v>0.53828608667318301</v>
       </c>
-      <c r="Y13" s="68">
+      <c r="Y13" s="71">
         <v>0.928641251221896</v>
       </c>
-      <c r="Z13" s="68">
+      <c r="Z13" s="71">
         <v>0.83447376995764</v>
       </c>
-      <c r="AA13" s="68">
+      <c r="AA13" s="71">
         <v>0.916585206907787</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -3206,25 +3206,25 @@
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="69"/>
-      <c r="O14" s="70"/>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="68"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="68"/>
-      <c r="T14" s="68"/>
-      <c r="U14" s="69"/>
-      <c r="V14" s="70"/>
-      <c r="W14" s="70"/>
-      <c r="X14" s="68"/>
-      <c r="Y14" s="68"/>
-      <c r="Z14" s="68"/>
-      <c r="AA14" s="68"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="76"/>
+      <c r="P14" s="76"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="76"/>
+      <c r="W14" s="76"/>
+      <c r="X14" s="71"/>
+      <c r="Y14" s="71"/>
+      <c r="Z14" s="71"/>
+      <c r="AA14" s="71"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -3246,24 +3246,24 @@
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="69"/>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="68"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="68"/>
-      <c r="T15" s="68"/>
-      <c r="U15" s="69"/>
-      <c r="V15" s="70"/>
-      <c r="W15" s="70"/>
-      <c r="X15" s="68"/>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="68"/>
-      <c r="AA15" s="68"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="74"/>
+      <c r="V15" s="76"/>
+      <c r="W15" s="76"/>
+      <c r="X15" s="71"/>
+      <c r="Y15" s="71"/>
+      <c r="Z15" s="71"/>
+      <c r="AA15" s="71"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
-      <c r="B16" s="75" t="s">
+      <c r="A16" s="70"/>
+      <c r="B16" s="70" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="15"/>
@@ -3288,25 +3288,25 @@
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="69"/>
-      <c r="O16" s="70"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="68"/>
-      <c r="R16" s="68"/>
-      <c r="S16" s="68"/>
-      <c r="T16" s="68"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="70"/>
-      <c r="W16" s="70"/>
-      <c r="X16" s="68"/>
-      <c r="Y16" s="68"/>
-      <c r="Z16" s="68"/>
-      <c r="AA16" s="68"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="76"/>
+      <c r="P16" s="76"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="76"/>
+      <c r="W16" s="76"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75" t="s">
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3330,25 +3330,25 @@
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="69"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="68"/>
-      <c r="R17" s="68"/>
-      <c r="S17" s="68"/>
-      <c r="T17" s="68"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="70"/>
-      <c r="W17" s="70"/>
-      <c r="X17" s="68"/>
-      <c r="Y17" s="68"/>
-      <c r="Z17" s="68"/>
-      <c r="AA17" s="68"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="76"/>
+      <c r="P17" s="76"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="76"/>
+      <c r="W17" s="76"/>
+      <c r="X17" s="71"/>
+      <c r="Y17" s="71"/>
+      <c r="Z17" s="71"/>
+      <c r="AA17" s="71"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
@@ -3366,9 +3366,9 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="75"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3386,9 +3386,9 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75" t="s">
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -3408,9 +3408,9 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
@@ -3443,9 +3443,9 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="75"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
@@ -3503,43 +3503,43 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="73">
+      <c r="E24" s="72">
         <v>0.995</v>
       </c>
-      <c r="F24" s="73"/>
+      <c r="F24" s="72"/>
       <c r="L24" s="24"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
       <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
       <c r="L25" s="24"/>
       <c r="M25" s="5"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="66" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="21">
@@ -3555,9 +3555,9 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
       <c r="D27" s="21">
         <v>2</v>
       </c>
@@ -3565,9 +3565,9 @@
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="71"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
       <c r="D28" s="21">
         <v>5</v>
       </c>
@@ -3575,9 +3575,9 @@
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="71"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
       <c r="D29" s="21">
         <v>10</v>
       </c>
@@ -3589,9 +3589,9 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="71"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
       <c r="D30" s="21">
         <v>20</v>
       </c>
@@ -3599,9 +3599,9 @@
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="71"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72" t="s">
+      <c r="A31" s="67"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="21">
@@ -3611,9 +3611,9 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="71"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="21">
         <v>2</v>
       </c>
@@ -3621,9 +3621,9 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="71"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
       <c r="D33" s="21">
         <v>3</v>
       </c>
@@ -3631,9 +3631,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="71"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
       <c r="D34" s="21">
         <v>4</v>
       </c>
@@ -3641,9 +3641,9 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="71"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="21">
         <v>5</v>
       </c>
@@ -3651,12 +3651,12 @@
       <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
-      <c r="B36" s="76" t="s">
+      <c r="A36" s="67"/>
+      <c r="B36" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
       <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
@@ -3669,41 +3669,6 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A9:A22"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="AA13:AA17"/>
-    <mergeCell ref="N10:T10"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="P13:P17"/>
     <mergeCell ref="N9:AA9"/>
     <mergeCell ref="L9:M12"/>
     <mergeCell ref="Q13:Q17"/>
@@ -3720,6 +3685,41 @@
     <mergeCell ref="X13:X17"/>
     <mergeCell ref="Y13:Y17"/>
     <mergeCell ref="Z13:Z17"/>
+    <mergeCell ref="AA13:AA17"/>
+    <mergeCell ref="N10:T10"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="P13:P17"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A9:A22"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H22">
     <cfRule type="colorScale" priority="1">
@@ -3781,18 +3781,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
       <c r="M1" s="14"/>
       <c r="N1" s="24" t="s">
         <v>55</v>
@@ -3817,10 +3817,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -3836,16 +3836,16 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="75" t="s">
+      <c r="L2" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="77">
+      <c r="M2" s="78">
         <v>1</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="68">
+      <c r="O2" s="71">
         <v>0.85728300000000002</v>
       </c>
       <c r="P2" s="17">
@@ -3865,31 +3865,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="77"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="78"/>
       <c r="N3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="68"/>
+      <c r="O3" s="71"/>
       <c r="P3" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -3901,27 +3901,27 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="77"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="78"/>
       <c r="N4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="68"/>
+      <c r="O4" s="71"/>
       <c r="P4" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -3935,31 +3935,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75" t="s">
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="77">
+      <c r="L5" s="70"/>
+      <c r="M5" s="78">
         <v>2</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="68">
+      <c r="O5" s="71">
         <v>0.90257399999999999</v>
       </c>
       <c r="P5" s="17">
@@ -3979,27 +3979,27 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="75"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="78"/>
       <c r="N6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="68"/>
+      <c r="O6" s="71"/>
       <c r="P6" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4011,10 +4011,10 @@
       <c r="T6" s="17"/>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="70" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="15"/>
@@ -4033,12 +4033,12 @@
       <c r="H7" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L7" s="75"/>
-      <c r="M7" s="77"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="78"/>
       <c r="N7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="68"/>
+      <c r="O7" s="71"/>
       <c r="P7" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4052,9 +4052,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75" t="s">
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -4072,14 +4072,14 @@
       <c r="H8" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L8" s="75"/>
-      <c r="M8" s="77">
+      <c r="L8" s="70"/>
+      <c r="M8" s="78">
         <v>5</v>
       </c>
       <c r="N8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="68">
+      <c r="O8" s="71">
         <v>0.93776499999999996</v>
       </c>
       <c r="P8" s="17">
@@ -4099,9 +4099,9 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="75"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
@@ -4117,12 +4117,12 @@
       <c r="H9" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L9" s="75"/>
-      <c r="M9" s="77"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="78"/>
       <c r="N9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="68"/>
+      <c r="O9" s="71"/>
       <c r="P9" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4134,9 +4134,9 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -4152,12 +4152,12 @@
       <c r="H10" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L10" s="75"/>
-      <c r="M10" s="77"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="78"/>
       <c r="N10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="68"/>
+      <c r="O10" s="71"/>
       <c r="P10" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4171,9 +4171,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75" t="s">
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -4191,14 +4191,14 @@
       <c r="H11" s="19">
         <v>0.94037099999999996</v>
       </c>
-      <c r="L11" s="75"/>
-      <c r="M11" s="77">
+      <c r="L11" s="70"/>
+      <c r="M11" s="78">
         <v>10</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="68">
+      <c r="O11" s="71">
         <v>0.94330400000000003</v>
       </c>
       <c r="P11" s="17">
@@ -4218,9 +4218,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
@@ -4236,12 +4236,12 @@
       <c r="H12" s="19">
         <v>0.754969</v>
       </c>
-      <c r="L12" s="75"/>
-      <c r="M12" s="77"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="78"/>
       <c r="N12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="68"/>
+      <c r="O12" s="71"/>
       <c r="P12" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4253,9 +4253,9 @@
       <c r="T12" s="17"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
@@ -4271,12 +4271,12 @@
       <c r="H13" s="19">
         <v>0.94884299999999999</v>
       </c>
-      <c r="L13" s="75"/>
-      <c r="M13" s="77"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="78"/>
       <c r="N13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="68"/>
+      <c r="O13" s="71"/>
       <c r="P13" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4290,8 +4290,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="75" t="s">
+      <c r="A14" s="70"/>
+      <c r="B14" s="70" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="15"/>
@@ -4310,14 +4310,14 @@
       <c r="H14" s="19">
         <v>0.63245399999999996</v>
       </c>
-      <c r="L14" s="75"/>
-      <c r="M14" s="77">
+      <c r="L14" s="70"/>
+      <c r="M14" s="78">
         <v>20</v>
       </c>
       <c r="N14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="68">
+      <c r="O14" s="71">
         <v>0.93548399999999998</v>
       </c>
       <c r="P14" s="17">
@@ -4337,9 +4337,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75" t="s">
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -4357,12 +4357,12 @@
       <c r="H15" s="19">
         <v>0.68589100000000003</v>
       </c>
-      <c r="L15" s="75"/>
-      <c r="M15" s="77"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="78"/>
       <c r="N15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="68"/>
+      <c r="O15" s="71"/>
       <c r="P15" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4374,9 +4374,9 @@
       <c r="T15" s="17"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -4392,12 +4392,12 @@
       <c r="H16" s="19">
         <v>0.68067800000000001</v>
       </c>
-      <c r="L16" s="75"/>
-      <c r="M16" s="77"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="78"/>
       <c r="N16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="68"/>
+      <c r="O16" s="71"/>
       <c r="P16" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4411,9 +4411,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -4433,9 +4433,9 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75" t="s">
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -4461,9 +4461,9 @@
       <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="75"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
@@ -4483,9 +4483,9 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
       <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L28" s="5"/>
-      <c r="M28" s="69"/>
+      <c r="M28" s="74"/>
       <c r="N28" s="5"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L29" s="5"/>
-      <c r="M29" s="69"/>
+      <c r="M29" s="74"/>
       <c r="N29" s="5"/>
       <c r="O29" s="17"/>
       <c r="P29" s="25"/>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L30" s="5"/>
-      <c r="M30" s="69"/>
+      <c r="M30" s="74"/>
       <c r="N30" s="5"/>
       <c r="O30" s="17"/>
       <c r="P30" s="25"/>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L31" s="5"/>
-      <c r="M31" s="69"/>
+      <c r="M31" s="74"/>
       <c r="N31" s="5"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L32" s="5"/>
-      <c r="M32" s="69"/>
+      <c r="M32" s="74"/>
       <c r="N32" s="5"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -4590,6 +4590,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
     <mergeCell ref="M28:M32"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C3:C4"/>
@@ -4606,18 +4618,6 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="L2:L16"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="O14:O16"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H6 E7:F20 H7:H20">
     <cfRule type="colorScale" priority="4">
@@ -4651,8 +4651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
   <dimension ref="B1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4689,52 +4689,52 @@
   <sheetData>
     <row r="1" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="94"/>
-      <c r="P2" s="92" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="83"/>
+      <c r="P2" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="94"/>
-      <c r="Y2" s="92" t="s">
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="83"/>
+      <c r="Y2" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="Z2" s="93"/>
-      <c r="AA2" s="93"/>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="93"/>
-      <c r="AD2" s="94"/>
-      <c r="AF2" s="92" t="s">
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="83"/>
+      <c r="AF2" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="93"/>
-      <c r="AH2" s="93"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="94"/>
+      <c r="AG2" s="82"/>
+      <c r="AH2" s="82"/>
+      <c r="AI2" s="82"/>
+      <c r="AJ2" s="83"/>
     </row>
     <row r="3" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="83"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="96"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="87"/>
       <c r="K3" s="45"/>
       <c r="L3" s="50" t="s">
         <v>65</v>
@@ -4745,17 +4745,17 @@
       <c r="N3" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="87" t="s">
+      <c r="P3" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="88"/>
-      <c r="R3" s="88"/>
-      <c r="S3" s="88"/>
-      <c r="T3" s="88" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="89"/>
+      <c r="T3" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="88"/>
-      <c r="V3" s="90"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="91"/>
       <c r="X3" s="30"/>
       <c r="Y3" s="45"/>
       <c r="Z3" s="46"/>
@@ -4789,8 +4789,8 @@
       </c>
     </row>
     <row r="4" spans="2:36" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="95"/>
-      <c r="C4" s="77"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="13" t="s">
         <v>56</v>
       </c>
@@ -4822,10 +4822,10 @@
         <f>AVERAGE(D6:D10)</f>
         <v>0.92059999999999997</v>
       </c>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
       <c r="T4" s="16" t="s">
         <v>36</v>
       </c>
@@ -4837,16 +4837,16 @@
       </c>
       <c r="W4" s="20"/>
       <c r="X4" s="30"/>
-      <c r="Y4" s="80" t="s">
+      <c r="Y4" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="Z4" s="77">
+      <c r="Z4" s="78">
         <v>1</v>
       </c>
       <c r="AA4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB4" s="68">
+      <c r="AB4" s="71">
         <v>0.86699999999999999</v>
       </c>
       <c r="AC4" s="17">
@@ -4873,7 +4873,7 @@
       </c>
     </row>
     <row r="5" spans="2:36" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="79" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -4909,30 +4909,32 @@
         <f>AVERAGE(E5:I5)</f>
         <v>0.84460000000000002</v>
       </c>
-      <c r="P5" s="85" t="s">
+      <c r="P5" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75" t="s">
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70" t="s">
         <v>25</v>
       </c>
       <c r="S5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="68">
+      <c r="T5" s="71">
         <v>0.86699999999999999</v>
       </c>
-      <c r="U5" s="68"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="94"/>
       <c r="W5" s="20"/>
       <c r="X5" s="30"/>
-      <c r="Y5" s="80"/>
-      <c r="Z5" s="77"/>
+      <c r="Y5" s="93"/>
+      <c r="Z5" s="78"/>
       <c r="AA5" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="17"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="17">
+        <v>0.91300000000000003</v>
+      </c>
       <c r="AD5" s="38">
         <v>0.95</v>
       </c>
@@ -4954,7 +4956,7 @@
       </c>
     </row>
     <row r="6" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="97"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="13">
         <v>1</v>
       </c>
@@ -4990,27 +4992,27 @@
         <f>AVERAGE(E6:I10)</f>
         <v>0.91474745461062212</v>
       </c>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="75"/>
+      <c r="P6" s="93"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
       <c r="S6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="68">
+      <c r="T6" s="71">
         <v>0.94799999999999995</v>
       </c>
-      <c r="U6" s="68"/>
-      <c r="V6" s="91"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="94"/>
       <c r="W6" s="20"/>
       <c r="X6" s="30"/>
-      <c r="Y6" s="80"/>
-      <c r="Z6" s="77">
+      <c r="Y6" s="93"/>
+      <c r="Z6" s="78">
         <v>2</v>
       </c>
       <c r="AA6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB6" s="68">
+      <c r="AB6" s="71">
         <v>0.90800000000000003</v>
       </c>
       <c r="AC6" s="17">
@@ -5022,7 +5024,7 @@
       <c r="AE6" s="60"/>
     </row>
     <row r="7" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="97"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="13">
         <v>2</v>
       </c>
@@ -5049,35 +5051,37 @@
       <c r="L7" s="53"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="75" t="s">
+      <c r="P7" s="93"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70" t="s">
         <v>26</v>
       </c>
       <c r="S7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="T7" s="68">
+      <c r="T7" s="71">
         <v>0.83499999999999996</v>
       </c>
-      <c r="U7" s="68"/>
-      <c r="V7" s="91"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="94"/>
       <c r="W7" s="20"/>
       <c r="X7" s="30"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="77"/>
+      <c r="Y7" s="93"/>
+      <c r="Z7" s="78"/>
       <c r="AA7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB7" s="68"/>
-      <c r="AC7" s="17"/>
+      <c r="AB7" s="71"/>
+      <c r="AC7" s="17">
+        <v>0.91400000000000003</v>
+      </c>
       <c r="AD7" s="38">
         <v>0.95</v>
       </c>
       <c r="AE7" s="17"/>
     </row>
     <row r="8" spans="2:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="B8" s="97"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="13">
         <v>5</v>
       </c>
@@ -5104,27 +5108,27 @@
       <c r="L8" s="53"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
-      <c r="P8" s="80"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
       <c r="S8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="T8" s="68">
+      <c r="T8" s="71">
         <v>0.85199999999999998</v>
       </c>
-      <c r="U8" s="68"/>
-      <c r="V8" s="91"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="94"/>
       <c r="W8" s="20"/>
       <c r="X8" s="30"/>
-      <c r="Y8" s="80"/>
-      <c r="Z8" s="77">
+      <c r="Y8" s="93"/>
+      <c r="Z8" s="78">
         <v>5</v>
       </c>
       <c r="AA8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB8" s="68">
+      <c r="AB8" s="71">
         <v>0.94599999999999995</v>
       </c>
       <c r="AC8" s="17">
@@ -5136,7 +5140,7 @@
       <c r="AE8" s="17"/>
     </row>
     <row r="9" spans="2:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="B9" s="97"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="13">
         <v>10</v>
       </c>
@@ -5163,27 +5167,27 @@
       <c r="L9" s="53"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75" t="s">
+      <c r="P9" s="93"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70" t="s">
         <v>27</v>
       </c>
       <c r="S9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="T9" s="68">
+      <c r="T9" s="71">
         <v>0.83699999999999997</v>
       </c>
-      <c r="U9" s="68"/>
-      <c r="V9" s="91"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="94"/>
       <c r="W9" s="20"/>
       <c r="X9" s="30"/>
-      <c r="Y9" s="80"/>
-      <c r="Z9" s="77"/>
+      <c r="Y9" s="93"/>
+      <c r="Z9" s="78"/>
       <c r="AA9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB9" s="68"/>
+      <c r="AB9" s="71"/>
       <c r="AC9" s="17"/>
       <c r="AD9" s="38">
         <v>0.95199999999999996</v>
@@ -5191,7 +5195,7 @@
       <c r="AE9" s="60"/>
     </row>
     <row r="10" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="98"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="40">
         <v>20</v>
       </c>
@@ -5218,27 +5222,27 @@
       <c r="L10" s="53"/>
       <c r="M10" s="53"/>
       <c r="N10" s="53"/>
-      <c r="P10" s="80"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="75"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
       <c r="S10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T10" s="68">
+      <c r="T10" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="U10" s="68"/>
-      <c r="V10" s="91"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="94"/>
       <c r="W10" s="20"/>
       <c r="X10" s="30"/>
-      <c r="Y10" s="80"/>
-      <c r="Z10" s="77">
+      <c r="Y10" s="93"/>
+      <c r="Z10" s="78">
         <v>10</v>
       </c>
       <c r="AA10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB10" s="68">
+      <c r="AB10" s="71">
         <v>0.94799999999999995</v>
       </c>
       <c r="AC10" s="17">
@@ -5256,10 +5260,10 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
-      <c r="P11" s="80" t="s">
+      <c r="P11" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="75" t="s">
+      <c r="Q11" s="70" t="s">
         <v>6</v>
       </c>
       <c r="R11" s="15"/>
@@ -5276,12 +5280,12 @@
         <v>0.60299999999999998</v>
       </c>
       <c r="X11" s="30"/>
-      <c r="Y11" s="80"/>
-      <c r="Z11" s="77"/>
+      <c r="Y11" s="93"/>
+      <c r="Z11" s="78"/>
       <c r="AA11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB11" s="68"/>
+      <c r="AB11" s="71"/>
       <c r="AC11" s="17"/>
       <c r="AD11" s="38">
         <v>0.95199999999999996</v>
@@ -5289,9 +5293,9 @@
       <c r="AE11" s="17"/>
     </row>
     <row r="12" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="80"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75" t="s">
+      <c r="P12" s="93"/>
+      <c r="Q12" s="70"/>
+      <c r="R12" s="70" t="s">
         <v>23</v>
       </c>
       <c r="S12" s="13" t="s">
@@ -5307,14 +5311,14 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="X12" s="30"/>
-      <c r="Y12" s="80"/>
-      <c r="Z12" s="77">
+      <c r="Y12" s="93"/>
+      <c r="Z12" s="78">
         <v>20</v>
       </c>
       <c r="AA12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB12" s="68">
+      <c r="AB12" s="71">
         <v>0.93400000000000005</v>
       </c>
       <c r="AC12" s="17">
@@ -5326,9 +5330,9 @@
       <c r="AE12" s="60"/>
     </row>
     <row r="13" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P13" s="80"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="70"/>
       <c r="S13" s="13" t="s">
         <v>26</v>
       </c>
@@ -5342,12 +5346,12 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="X13" s="30"/>
-      <c r="Y13" s="81"/>
-      <c r="Z13" s="82"/>
+      <c r="Y13" s="95"/>
+      <c r="Z13" s="98"/>
       <c r="AA13" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AB13" s="79"/>
+      <c r="AB13" s="97"/>
       <c r="AC13" s="48"/>
       <c r="AD13" s="49">
         <v>0.94699999999999995</v>
@@ -5355,9 +5359,9 @@
       <c r="AE13" s="17"/>
     </row>
     <row r="14" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P14" s="80"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="75"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="70"/>
+      <c r="R14" s="70"/>
       <c r="S14" s="13" t="s">
         <v>27</v>
       </c>
@@ -5380,9 +5384,9 @@
       <c r="AE14" s="17"/>
     </row>
     <row r="15" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="P15" s="80"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="75" t="s">
+      <c r="P15" s="93"/>
+      <c r="Q15" s="70"/>
+      <c r="R15" s="70" t="s">
         <v>24</v>
       </c>
       <c r="S15" s="13" t="s">
@@ -5398,8 +5402,8 @@
         <v>0.94599999999999995</v>
       </c>
       <c r="X15" s="30"/>
-      <c r="Y15" s="83"/>
-      <c r="Z15" s="84"/>
+      <c r="Y15" s="84"/>
+      <c r="Z15" s="85"/>
       <c r="AA15" s="34" t="s">
         <v>55</v>
       </c>
@@ -5415,9 +5419,9 @@
       <c r="AE15" s="60"/>
     </row>
     <row r="16" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="P16" s="80"/>
-      <c r="Q16" s="75"/>
-      <c r="R16" s="75"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
       <c r="S16" s="13" t="s">
         <v>26</v>
       </c>
@@ -5431,24 +5435,28 @@
         <v>0.73199999999999998</v>
       </c>
       <c r="X16" s="30"/>
-      <c r="Y16" s="85" t="s">
+      <c r="Y16" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="Z16" s="75"/>
+      <c r="Z16" s="70"/>
       <c r="AA16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB16" s="68">
+      <c r="AB16" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="AC16" s="17"/>
-      <c r="AD16" s="38"/>
+      <c r="AC16" s="17">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AD16" s="38">
+        <v>0.94899999999999995</v>
+      </c>
       <c r="AE16" s="17"/>
     </row>
     <row r="17" spans="16:38" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P17" s="80"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="70"/>
+      <c r="R17" s="70"/>
       <c r="S17" s="13" t="s">
         <v>27</v>
       </c>
@@ -5462,19 +5470,19 @@
         <v>0.95</v>
       </c>
       <c r="X17" s="30"/>
-      <c r="Y17" s="81"/>
-      <c r="Z17" s="86"/>
+      <c r="Y17" s="95"/>
+      <c r="Z17" s="96"/>
       <c r="AA17" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AB17" s="79"/>
+      <c r="AB17" s="97"/>
       <c r="AC17" s="48"/>
       <c r="AD17" s="49"/>
       <c r="AE17" s="17"/>
     </row>
     <row r="18" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P18" s="80"/>
-      <c r="Q18" s="75" t="s">
+      <c r="P18" s="93"/>
+      <c r="Q18" s="70" t="s">
         <v>7</v>
       </c>
       <c r="R18" s="15"/>
@@ -5500,9 +5508,9 @@
       <c r="AE18" s="60"/>
     </row>
     <row r="19" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P19" s="80"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75" t="s">
+      <c r="P19" s="93"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70" t="s">
         <v>23</v>
       </c>
       <c r="S19" s="13" t="s">
@@ -5527,9 +5535,9 @@
       <c r="AE19" s="30"/>
     </row>
     <row r="20" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P20" s="80"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="70"/>
       <c r="S20" s="13" t="s">
         <v>26</v>
       </c>
@@ -5552,9 +5560,9 @@
       <c r="AE20" s="30"/>
     </row>
     <row r="21" spans="16:38" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P21" s="80"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
       <c r="S21" s="13" t="s">
         <v>27</v>
       </c>
@@ -5577,9 +5585,9 @@
       <c r="AE21" s="30"/>
     </row>
     <row r="22" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P22" s="80"/>
-      <c r="Q22" s="75"/>
-      <c r="R22" s="75" t="s">
+      <c r="P22" s="93"/>
+      <c r="Q22" s="70"/>
+      <c r="R22" s="70" t="s">
         <v>24</v>
       </c>
       <c r="S22" s="13" t="s">
@@ -5604,9 +5612,9 @@
       <c r="AE22" s="30"/>
     </row>
     <row r="23" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P23" s="80"/>
-      <c r="Q23" s="75"/>
-      <c r="R23" s="75"/>
+      <c r="P23" s="93"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70"/>
       <c r="S23" s="13" t="s">
         <v>26</v>
       </c>
@@ -5635,9 +5643,9 @@
       <c r="AL23" s="30"/>
     </row>
     <row r="24" spans="16:38" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P24" s="81"/>
-      <c r="Q24" s="86"/>
-      <c r="R24" s="86"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="96"/>
+      <c r="R24" s="96"/>
       <c r="S24" s="40" t="s">
         <v>27</v>
       </c>
@@ -5873,6 +5881,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="Y4:Y13"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="AB4:AB5"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="AB12:AB13"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z17"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="P11:P24"/>
+    <mergeCell ref="Q11:Q17"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="Q18:Q24"/>
+    <mergeCell ref="R19:R21"/>
+    <mergeCell ref="R22:R24"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="P2:V2"/>
@@ -5889,30 +5921,6 @@
     <mergeCell ref="R7:R8"/>
     <mergeCell ref="R9:R10"/>
     <mergeCell ref="T8:V8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="P11:P24"/>
-    <mergeCell ref="Q11:Q17"/>
-    <mergeCell ref="R12:R14"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="Q18:Q24"/>
-    <mergeCell ref="R19:R21"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="Y4:Y13"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="AB12:AB13"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z17"/>
   </mergeCells>
   <conditionalFormatting sqref="K5:K6 D8:N10 D5:I5 D6:K7">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
qwen comb, zeroshot results added
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0763E680-6413-0C49-94D7-D933C195F982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897C5243-CABF-2341-BE0D-73B874BFF7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -687,43 +687,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -741,12 +768,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -763,27 +784,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2776,24 +2776,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -2808,120 +2808,120 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="68">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="71">
+      <c r="E4" s="68">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
       <c r="J4" s="5"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70" t="s">
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="71">
+      <c r="E5" s="68">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
       <c r="J5" s="5"/>
       <c r="K5" s="17"/>
       <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="71">
+      <c r="E6" s="68">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70" t="s">
+      <c r="A7" s="75"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="71">
+      <c r="E7" s="68">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
       <c r="J7" s="5"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="70"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="71">
+      <c r="E8" s="68">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
       <c r="J8" s="5"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
@@ -2940,31 +2940,31 @@
       <c r="H9" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L9" s="75" t="s">
+      <c r="L9" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="75"/>
-      <c r="N9" s="73" t="s">
+      <c r="M9" s="67"/>
+      <c r="N9" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
-      <c r="U9" s="73"/>
-      <c r="V9" s="73"/>
-      <c r="W9" s="73"/>
-      <c r="X9" s="73"/>
-      <c r="Y9" s="73"/>
-      <c r="Z9" s="73"/>
-      <c r="AA9" s="73"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="66"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70" t="s">
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -2982,31 +2982,31 @@
       <c r="H10" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="73" t="s">
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73"/>
-      <c r="T10" s="73"/>
-      <c r="U10" s="73" t="s">
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
+      <c r="U10" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="73"/>
-      <c r="W10" s="73"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-      <c r="Z10" s="73"/>
-      <c r="AA10" s="73"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
+      <c r="Z10" s="66"/>
+      <c r="AA10" s="66"/>
     </row>
     <row r="11" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
@@ -3022,39 +3022,39 @@
       <c r="H11" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75" t="s">
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="73" t="s">
+      <c r="O11" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73" t="s">
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="75" t="s">
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="73" t="s">
+      <c r="V11" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="W11" s="73"/>
-      <c r="X11" s="73"/>
-      <c r="Y11" s="73" t="s">
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="Z11" s="73"/>
-      <c r="AA11" s="73"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="66"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="70"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
@@ -3070,9 +3070,9 @@
       <c r="H12" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="73"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="66"/>
       <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="73"/>
+      <c r="U12" s="66"/>
       <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3112,9 +3112,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70" t="s">
+      <c r="A13" s="75"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -3138,53 +3138,53 @@
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="74">
+      <c r="N13" s="69">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="76">
+      <c r="O13" s="70">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="76">
+      <c r="P13" s="70">
         <v>0.50667970022808695</v>
       </c>
-      <c r="Q13" s="71">
+      <c r="Q13" s="68">
         <v>0.46757901596611201</v>
       </c>
-      <c r="R13" s="71">
+      <c r="R13" s="68">
         <v>0.93385467579015902</v>
       </c>
-      <c r="S13" s="71">
+      <c r="S13" s="68">
         <v>0.76050830889540499</v>
       </c>
-      <c r="T13" s="71">
+      <c r="T13" s="68">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="74">
+      <c r="U13" s="69">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="76">
+      <c r="V13" s="70">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="76">
+      <c r="W13" s="70">
         <v>0.516780710329097</v>
       </c>
-      <c r="X13" s="71">
+      <c r="X13" s="68">
         <v>0.53828608667318301</v>
       </c>
-      <c r="Y13" s="71">
+      <c r="Y13" s="68">
         <v>0.928641251221896</v>
       </c>
-      <c r="Z13" s="71">
+      <c r="Z13" s="68">
         <v>0.83447376995764</v>
       </c>
-      <c r="AA13" s="71">
+      <c r="AA13" s="68">
         <v>0.916585206907787</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -3206,25 +3206,25 @@
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="74"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="71"/>
-      <c r="R14" s="71"/>
-      <c r="S14" s="71"/>
-      <c r="T14" s="71"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="76"/>
-      <c r="W14" s="76"/>
-      <c r="X14" s="71"/>
-      <c r="Y14" s="71"/>
-      <c r="Z14" s="71"/>
-      <c r="AA14" s="71"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="70"/>
+      <c r="P14" s="70"/>
+      <c r="Q14" s="68"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="68"/>
+      <c r="T14" s="68"/>
+      <c r="U14" s="69"/>
+      <c r="V14" s="70"/>
+      <c r="W14" s="70"/>
+      <c r="X14" s="68"/>
+      <c r="Y14" s="68"/>
+      <c r="Z14" s="68"/>
+      <c r="AA14" s="68"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -3246,24 +3246,24 @@
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="74"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="71"/>
-      <c r="S15" s="71"/>
-      <c r="T15" s="71"/>
-      <c r="U15" s="74"/>
-      <c r="V15" s="76"/>
-      <c r="W15" s="76"/>
-      <c r="X15" s="71"/>
-      <c r="Y15" s="71"/>
-      <c r="Z15" s="71"/>
-      <c r="AA15" s="71"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="70"/>
+      <c r="P15" s="70"/>
+      <c r="Q15" s="68"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="70"/>
+      <c r="W15" s="70"/>
+      <c r="X15" s="68"/>
+      <c r="Y15" s="68"/>
+      <c r="Z15" s="68"/>
+      <c r="AA15" s="68"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
-      <c r="B16" s="70" t="s">
+      <c r="A16" s="75"/>
+      <c r="B16" s="75" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="15"/>
@@ -3288,25 +3288,25 @@
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="74"/>
-      <c r="O16" s="76"/>
-      <c r="P16" s="76"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="71"/>
-      <c r="S16" s="71"/>
-      <c r="T16" s="71"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="76"/>
-      <c r="W16" s="76"/>
-      <c r="X16" s="71"/>
-      <c r="Y16" s="71"/>
-      <c r="Z16" s="71"/>
-      <c r="AA16" s="71"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="68"/>
+      <c r="R16" s="68"/>
+      <c r="S16" s="68"/>
+      <c r="T16" s="68"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="70"/>
+      <c r="W16" s="70"/>
+      <c r="X16" s="68"/>
+      <c r="Y16" s="68"/>
+      <c r="Z16" s="68"/>
+      <c r="AA16" s="68"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70" t="s">
+      <c r="A17" s="75"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3330,25 +3330,25 @@
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="74"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="71"/>
-      <c r="S17" s="71"/>
-      <c r="T17" s="71"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="71"/>
-      <c r="Y17" s="71"/>
-      <c r="Z17" s="71"/>
-      <c r="AA17" s="71"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
+      <c r="Q17" s="68"/>
+      <c r="R17" s="68"/>
+      <c r="S17" s="68"/>
+      <c r="T17" s="68"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="70"/>
+      <c r="W17" s="70"/>
+      <c r="X17" s="68"/>
+      <c r="Y17" s="68"/>
+      <c r="Z17" s="68"/>
+      <c r="AA17" s="68"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
@@ -3366,9 +3366,9 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="70"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3386,9 +3386,9 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70" t="s">
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -3408,9 +3408,9 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
@@ -3443,9 +3443,9 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="70"/>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
@@ -3503,43 +3503,43 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="72">
+      <c r="E24" s="73">
         <v>0.995</v>
       </c>
-      <c r="F24" s="72"/>
+      <c r="F24" s="73"/>
       <c r="L24" s="24"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
       <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
       <c r="L25" s="24"/>
       <c r="M25" s="5"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="72" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="21">
@@ -3555,9 +3555,9 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="67"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
       <c r="D27" s="21">
         <v>2</v>
       </c>
@@ -3565,9 +3565,9 @@
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="67"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
       <c r="D28" s="21">
         <v>5</v>
       </c>
@@ -3575,9 +3575,9 @@
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="67"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="21">
         <v>10</v>
       </c>
@@ -3589,9 +3589,9 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="67"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
+      <c r="A30" s="71"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="21">
         <v>20</v>
       </c>
@@ -3599,9 +3599,9 @@
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="67"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66" t="s">
+      <c r="A31" s="71"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="21">
@@ -3611,9 +3611,9 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="67"/>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
+      <c r="A32" s="71"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
       <c r="D32" s="21">
         <v>2</v>
       </c>
@@ -3621,9 +3621,9 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="67"/>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
       <c r="D33" s="21">
         <v>3</v>
       </c>
@@ -3631,9 +3631,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="67"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
+      <c r="A34" s="71"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
       <c r="D34" s="21">
         <v>4</v>
       </c>
@@ -3641,9 +3641,9 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="67"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="66"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="21">
         <v>5</v>
       </c>
@@ -3651,12 +3651,12 @@
       <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="67"/>
-      <c r="B36" s="68" t="s">
+      <c r="A36" s="71"/>
+      <c r="B36" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
       <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
@@ -3669,6 +3669,41 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A9:A22"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="AA13:AA17"/>
+    <mergeCell ref="N10:T10"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="P13:P17"/>
     <mergeCell ref="N9:AA9"/>
     <mergeCell ref="L9:M12"/>
     <mergeCell ref="Q13:Q17"/>
@@ -3685,41 +3720,6 @@
     <mergeCell ref="X13:X17"/>
     <mergeCell ref="Y13:Y17"/>
     <mergeCell ref="Z13:Z17"/>
-    <mergeCell ref="AA13:AA17"/>
-    <mergeCell ref="N10:T10"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="P13:P17"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A9:A22"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="C26:C30"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H22">
     <cfRule type="colorScale" priority="1">
@@ -3755,7 +3755,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="S16" activeCellId="2" sqref="S10 S13 S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3781,18 +3781,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
       <c r="M1" s="14"/>
       <c r="N1" s="24" t="s">
         <v>55</v>
@@ -3817,10 +3817,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -3836,16 +3836,16 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="70" t="s">
+      <c r="L2" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="78">
+      <c r="M2" s="77">
         <v>1</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="71">
+      <c r="O2" s="68">
         <v>0.85728300000000002</v>
       </c>
       <c r="P2" s="17">
@@ -3865,31 +3865,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="68">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="78"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="71"/>
+      <c r="O3" s="68"/>
       <c r="P3" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -3901,27 +3901,27 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="70"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="71">
+      <c r="E4" s="68">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="78"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="77"/>
       <c r="N4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="71"/>
+      <c r="O4" s="68"/>
       <c r="P4" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -3935,31 +3935,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="70"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70" t="s">
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="71">
+      <c r="E5" s="68">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="78">
+      <c r="L5" s="75"/>
+      <c r="M5" s="77">
         <v>2</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="71">
+      <c r="O5" s="68">
         <v>0.90257399999999999</v>
       </c>
       <c r="P5" s="17">
@@ -3979,27 +3979,27 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="70"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="71">
+      <c r="E6" s="68">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="78"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="77"/>
       <c r="N6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="71"/>
+      <c r="O6" s="68"/>
       <c r="P6" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4011,10 +4011,10 @@
       <c r="T6" s="17"/>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="15"/>
@@ -4033,12 +4033,12 @@
       <c r="H7" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L7" s="70"/>
-      <c r="M7" s="78"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="77"/>
       <c r="N7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="71"/>
+      <c r="O7" s="68"/>
       <c r="P7" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4052,9 +4052,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="70"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70" t="s">
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -4072,14 +4072,14 @@
       <c r="H8" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L8" s="70"/>
-      <c r="M8" s="78">
+      <c r="L8" s="75"/>
+      <c r="M8" s="77">
         <v>5</v>
       </c>
       <c r="N8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="71">
+      <c r="O8" s="68">
         <v>0.93776499999999996</v>
       </c>
       <c r="P8" s="17">
@@ -4099,9 +4099,9 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="70"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
       <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
@@ -4117,12 +4117,12 @@
       <c r="H9" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="78"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="77"/>
       <c r="N9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="71"/>
+      <c r="O9" s="68"/>
       <c r="P9" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4134,9 +4134,9 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -4152,12 +4152,12 @@
       <c r="H10" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L10" s="70"/>
-      <c r="M10" s="78"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="77"/>
       <c r="N10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="71"/>
+      <c r="O10" s="68"/>
       <c r="P10" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4171,9 +4171,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70" t="s">
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -4191,14 +4191,14 @@
       <c r="H11" s="19">
         <v>0.94037099999999996</v>
       </c>
-      <c r="L11" s="70"/>
-      <c r="M11" s="78">
+      <c r="L11" s="75"/>
+      <c r="M11" s="77">
         <v>10</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="71">
+      <c r="O11" s="68">
         <v>0.94330400000000003</v>
       </c>
       <c r="P11" s="17">
@@ -4218,9 +4218,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="70"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
@@ -4236,12 +4236,12 @@
       <c r="H12" s="19">
         <v>0.754969</v>
       </c>
-      <c r="L12" s="70"/>
-      <c r="M12" s="78"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="77"/>
       <c r="N12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="71"/>
+      <c r="O12" s="68"/>
       <c r="P12" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4253,9 +4253,9 @@
       <c r="T12" s="17"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
@@ -4271,12 +4271,12 @@
       <c r="H13" s="19">
         <v>0.94884299999999999</v>
       </c>
-      <c r="L13" s="70"/>
-      <c r="M13" s="78"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="77"/>
       <c r="N13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="71"/>
+      <c r="O13" s="68"/>
       <c r="P13" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4290,8 +4290,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
-      <c r="B14" s="70" t="s">
+      <c r="A14" s="75"/>
+      <c r="B14" s="75" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="15"/>
@@ -4310,14 +4310,14 @@
       <c r="H14" s="19">
         <v>0.63245399999999996</v>
       </c>
-      <c r="L14" s="70"/>
-      <c r="M14" s="78">
+      <c r="L14" s="75"/>
+      <c r="M14" s="77">
         <v>20</v>
       </c>
       <c r="N14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="71">
+      <c r="O14" s="68">
         <v>0.93548399999999998</v>
       </c>
       <c r="P14" s="17">
@@ -4337,9 +4337,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70" t="s">
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -4357,12 +4357,12 @@
       <c r="H15" s="19">
         <v>0.68589100000000003</v>
       </c>
-      <c r="L15" s="70"/>
-      <c r="M15" s="78"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="77"/>
       <c r="N15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="71"/>
+      <c r="O15" s="68"/>
       <c r="P15" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4374,9 +4374,9 @@
       <c r="T15" s="17"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -4392,12 +4392,12 @@
       <c r="H16" s="19">
         <v>0.68067800000000001</v>
       </c>
-      <c r="L16" s="70"/>
-      <c r="M16" s="78"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="77"/>
       <c r="N16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="71"/>
+      <c r="O16" s="68"/>
       <c r="P16" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4411,9 +4411,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -4433,9 +4433,9 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70" t="s">
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -4461,9 +4461,9 @@
       <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="70"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
@@ -4483,9 +4483,9 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
       <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L28" s="5"/>
-      <c r="M28" s="74"/>
+      <c r="M28" s="69"/>
       <c r="N28" s="5"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L29" s="5"/>
-      <c r="M29" s="74"/>
+      <c r="M29" s="69"/>
       <c r="N29" s="5"/>
       <c r="O29" s="17"/>
       <c r="P29" s="25"/>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L30" s="5"/>
-      <c r="M30" s="74"/>
+      <c r="M30" s="69"/>
       <c r="N30" s="5"/>
       <c r="O30" s="17"/>
       <c r="P30" s="25"/>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L31" s="5"/>
-      <c r="M31" s="74"/>
+      <c r="M31" s="69"/>
       <c r="N31" s="5"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L32" s="5"/>
-      <c r="M32" s="74"/>
+      <c r="M32" s="69"/>
       <c r="N32" s="5"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -4590,18 +4590,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="L2:L16"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="O14:O16"/>
     <mergeCell ref="M28:M32"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C3:C4"/>
@@ -4618,6 +4606,18 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H6 E7:F20 H7:H20">
     <cfRule type="colorScale" priority="4">
@@ -4651,8 +4651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
   <dimension ref="B1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4689,52 +4689,52 @@
   <sheetData>
     <row r="1" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="83"/>
-      <c r="P2" s="81" t="s">
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="92"/>
+      <c r="P2" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="83"/>
-      <c r="Y2" s="81" t="s">
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="92"/>
+      <c r="Y2" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="82"/>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="83"/>
-      <c r="AF2" s="81" t="s">
+      <c r="Z2" s="91"/>
+      <c r="AA2" s="91"/>
+      <c r="AB2" s="91"/>
+      <c r="AC2" s="91"/>
+      <c r="AD2" s="92"/>
+      <c r="AF2" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="82"/>
-      <c r="AH2" s="82"/>
-      <c r="AI2" s="82"/>
-      <c r="AJ2" s="83"/>
+      <c r="AG2" s="91"/>
+      <c r="AH2" s="91"/>
+      <c r="AI2" s="91"/>
+      <c r="AJ2" s="92"/>
     </row>
     <row r="3" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85" t="s">
+      <c r="B3" s="83"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="87"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="94"/>
       <c r="K3" s="45"/>
       <c r="L3" s="50" t="s">
         <v>65</v>
@@ -4745,17 +4745,17 @@
       <c r="N3" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="88" t="s">
+      <c r="P3" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89" t="s">
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="89"/>
-      <c r="V3" s="91"/>
+      <c r="U3" s="96"/>
+      <c r="V3" s="98"/>
       <c r="X3" s="30"/>
       <c r="Y3" s="45"/>
       <c r="Z3" s="46"/>
@@ -4789,8 +4789,8 @@
       </c>
     </row>
     <row r="4" spans="2:36" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="86"/>
-      <c r="C4" s="78"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="77"/>
       <c r="D4" s="13" t="s">
         <v>56</v>
       </c>
@@ -4822,10 +4822,10 @@
         <f>AVERAGE(D6:D10)</f>
         <v>0.92059999999999997</v>
       </c>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
       <c r="T4" s="16" t="s">
         <v>36</v>
       </c>
@@ -4837,16 +4837,16 @@
       </c>
       <c r="W4" s="20"/>
       <c r="X4" s="30"/>
-      <c r="Y4" s="93" t="s">
+      <c r="Y4" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="Z4" s="78">
+      <c r="Z4" s="77">
         <v>1</v>
       </c>
       <c r="AA4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB4" s="71">
+      <c r="AB4" s="68">
         <v>0.86699999999999999</v>
       </c>
       <c r="AC4" s="17">
@@ -4873,7 +4873,7 @@
       </c>
     </row>
     <row r="5" spans="2:36" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="88" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -4909,29 +4909,29 @@
         <f>AVERAGE(E5:I5)</f>
         <v>0.84460000000000002</v>
       </c>
-      <c r="P5" s="92" t="s">
+      <c r="P5" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70" t="s">
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75" t="s">
         <v>25</v>
       </c>
       <c r="S5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="71">
+      <c r="T5" s="68">
         <v>0.86699999999999999</v>
       </c>
-      <c r="U5" s="71"/>
-      <c r="V5" s="94"/>
+      <c r="U5" s="68"/>
+      <c r="V5" s="87"/>
       <c r="W5" s="20"/>
       <c r="X5" s="30"/>
-      <c r="Y5" s="93"/>
-      <c r="Z5" s="78"/>
+      <c r="Y5" s="80"/>
+      <c r="Z5" s="77"/>
       <c r="AA5" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" s="71"/>
+      <c r="AB5" s="68"/>
       <c r="AC5" s="17">
         <v>0.91300000000000003</v>
       </c>
@@ -4956,7 +4956,7 @@
       </c>
     </row>
     <row r="6" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="79"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="13">
         <v>1</v>
       </c>
@@ -4992,27 +4992,27 @@
         <f>AVERAGE(E6:I10)</f>
         <v>0.91474745461062212</v>
       </c>
-      <c r="P6" s="93"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="75"/>
       <c r="S6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="71">
+      <c r="T6" s="68">
         <v>0.94799999999999995</v>
       </c>
-      <c r="U6" s="71"/>
-      <c r="V6" s="94"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="87"/>
       <c r="W6" s="20"/>
       <c r="X6" s="30"/>
-      <c r="Y6" s="93"/>
-      <c r="Z6" s="78">
+      <c r="Y6" s="80"/>
+      <c r="Z6" s="77">
         <v>2</v>
       </c>
       <c r="AA6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB6" s="71">
+      <c r="AB6" s="68">
         <v>0.90800000000000003</v>
       </c>
       <c r="AC6" s="17">
@@ -5024,7 +5024,7 @@
       <c r="AE6" s="60"/>
     </row>
     <row r="7" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="79"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="13">
         <v>2</v>
       </c>
@@ -5051,27 +5051,27 @@
       <c r="L7" s="53"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
-      <c r="P7" s="93"/>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="70" t="s">
+      <c r="P7" s="80"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="75" t="s">
         <v>26</v>
       </c>
       <c r="S7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="T7" s="71">
+      <c r="T7" s="68">
         <v>0.83499999999999996</v>
       </c>
-      <c r="U7" s="71"/>
-      <c r="V7" s="94"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="87"/>
       <c r="W7" s="20"/>
       <c r="X7" s="30"/>
-      <c r="Y7" s="93"/>
-      <c r="Z7" s="78"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="77"/>
       <c r="AA7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB7" s="71"/>
+      <c r="AB7" s="68"/>
       <c r="AC7" s="17">
         <v>0.91400000000000003</v>
       </c>
@@ -5081,7 +5081,7 @@
       <c r="AE7" s="17"/>
     </row>
     <row r="8" spans="2:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="B8" s="79"/>
+      <c r="B8" s="88"/>
       <c r="C8" s="13">
         <v>5</v>
       </c>
@@ -5108,27 +5108,27 @@
       <c r="L8" s="53"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
       <c r="S8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="T8" s="71">
+      <c r="T8" s="68">
         <v>0.85199999999999998</v>
       </c>
-      <c r="U8" s="71"/>
-      <c r="V8" s="94"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="87"/>
       <c r="W8" s="20"/>
       <c r="X8" s="30"/>
-      <c r="Y8" s="93"/>
-      <c r="Z8" s="78">
+      <c r="Y8" s="80"/>
+      <c r="Z8" s="77">
         <v>5</v>
       </c>
       <c r="AA8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB8" s="71">
+      <c r="AB8" s="68">
         <v>0.94599999999999995</v>
       </c>
       <c r="AC8" s="17">
@@ -5140,7 +5140,7 @@
       <c r="AE8" s="17"/>
     </row>
     <row r="9" spans="2:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="B9" s="79"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="13">
         <v>10</v>
       </c>
@@ -5167,35 +5167,37 @@
       <c r="L9" s="53"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
-      <c r="P9" s="93"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70" t="s">
+      <c r="P9" s="80"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75" t="s">
         <v>27</v>
       </c>
       <c r="S9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="T9" s="71">
+      <c r="T9" s="68">
         <v>0.83699999999999997</v>
       </c>
-      <c r="U9" s="71"/>
-      <c r="V9" s="94"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="87"/>
       <c r="W9" s="20"/>
       <c r="X9" s="30"/>
-      <c r="Y9" s="93"/>
-      <c r="Z9" s="78"/>
+      <c r="Y9" s="80"/>
+      <c r="Z9" s="77"/>
       <c r="AA9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB9" s="71"/>
-      <c r="AC9" s="17"/>
+      <c r="AB9" s="68"/>
+      <c r="AC9" s="17">
+        <v>0.92400000000000004</v>
+      </c>
       <c r="AD9" s="38">
         <v>0.95199999999999996</v>
       </c>
       <c r="AE9" s="60"/>
     </row>
     <row r="10" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="80"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="40">
         <v>20</v>
       </c>
@@ -5222,27 +5224,27 @@
       <c r="L10" s="53"/>
       <c r="M10" s="53"/>
       <c r="N10" s="53"/>
-      <c r="P10" s="93"/>
-      <c r="Q10" s="70"/>
-      <c r="R10" s="70"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
       <c r="S10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T10" s="71">
+      <c r="T10" s="68">
         <v>0.95099999999999996</v>
       </c>
-      <c r="U10" s="71"/>
-      <c r="V10" s="94"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="87"/>
       <c r="W10" s="20"/>
       <c r="X10" s="30"/>
-      <c r="Y10" s="93"/>
-      <c r="Z10" s="78">
+      <c r="Y10" s="80"/>
+      <c r="Z10" s="77">
         <v>10</v>
       </c>
       <c r="AA10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB10" s="71">
+      <c r="AB10" s="68">
         <v>0.94799999999999995</v>
       </c>
       <c r="AC10" s="17">
@@ -5260,10 +5262,10 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
-      <c r="P11" s="93" t="s">
+      <c r="P11" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="70" t="s">
+      <c r="Q11" s="75" t="s">
         <v>6</v>
       </c>
       <c r="R11" s="15"/>
@@ -5280,22 +5282,24 @@
         <v>0.60299999999999998</v>
       </c>
       <c r="X11" s="30"/>
-      <c r="Y11" s="93"/>
-      <c r="Z11" s="78"/>
+      <c r="Y11" s="80"/>
+      <c r="Z11" s="77"/>
       <c r="AA11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB11" s="71"/>
-      <c r="AC11" s="17"/>
+      <c r="AB11" s="68"/>
+      <c r="AC11" s="17">
+        <v>0.91200000000000003</v>
+      </c>
       <c r="AD11" s="38">
         <v>0.95199999999999996</v>
       </c>
       <c r="AE11" s="17"/>
     </row>
     <row r="12" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="93"/>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="70" t="s">
+      <c r="P12" s="80"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="75" t="s">
         <v>23</v>
       </c>
       <c r="S12" s="13" t="s">
@@ -5311,14 +5315,14 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="X12" s="30"/>
-      <c r="Y12" s="93"/>
-      <c r="Z12" s="78">
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="77">
         <v>20</v>
       </c>
       <c r="AA12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB12" s="71">
+      <c r="AB12" s="68">
         <v>0.93400000000000005</v>
       </c>
       <c r="AC12" s="17">
@@ -5330,9 +5334,9 @@
       <c r="AE12" s="60"/>
     </row>
     <row r="13" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P13" s="93"/>
-      <c r="Q13" s="70"/>
-      <c r="R13" s="70"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
       <c r="S13" s="13" t="s">
         <v>26</v>
       </c>
@@ -5346,22 +5350,24 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="X13" s="30"/>
-      <c r="Y13" s="95"/>
-      <c r="Z13" s="98"/>
+      <c r="Y13" s="81"/>
+      <c r="Z13" s="82"/>
       <c r="AA13" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AB13" s="97"/>
-      <c r="AC13" s="48"/>
+      <c r="AB13" s="79"/>
+      <c r="AC13" s="48">
+        <v>0.91200000000000003</v>
+      </c>
       <c r="AD13" s="49">
         <v>0.94699999999999995</v>
       </c>
       <c r="AE13" s="17"/>
     </row>
     <row r="14" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P14" s="93"/>
-      <c r="Q14" s="70"/>
-      <c r="R14" s="70"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="75"/>
       <c r="S14" s="13" t="s">
         <v>27</v>
       </c>
@@ -5384,9 +5390,9 @@
       <c r="AE14" s="17"/>
     </row>
     <row r="15" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="P15" s="93"/>
-      <c r="Q15" s="70"/>
-      <c r="R15" s="70" t="s">
+      <c r="P15" s="80"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75" t="s">
         <v>24</v>
       </c>
       <c r="S15" s="13" t="s">
@@ -5402,8 +5408,8 @@
         <v>0.94599999999999995</v>
       </c>
       <c r="X15" s="30"/>
-      <c r="Y15" s="84"/>
-      <c r="Z15" s="85"/>
+      <c r="Y15" s="83"/>
+      <c r="Z15" s="84"/>
       <c r="AA15" s="34" t="s">
         <v>55</v>
       </c>
@@ -5419,9 +5425,9 @@
       <c r="AE15" s="60"/>
     </row>
     <row r="16" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="P16" s="93"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="70"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75"/>
       <c r="S16" s="13" t="s">
         <v>26</v>
       </c>
@@ -5435,14 +5441,14 @@
         <v>0.73199999999999998</v>
       </c>
       <c r="X16" s="30"/>
-      <c r="Y16" s="92" t="s">
+      <c r="Y16" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="Z16" s="70"/>
+      <c r="Z16" s="75"/>
       <c r="AA16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB16" s="71">
+      <c r="AB16" s="68">
         <v>0.95099999999999996</v>
       </c>
       <c r="AC16" s="17">
@@ -5454,9 +5460,9 @@
       <c r="AE16" s="17"/>
     </row>
     <row r="17" spans="16:38" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P17" s="93"/>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="70"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
       <c r="S17" s="13" t="s">
         <v>27</v>
       </c>
@@ -5470,19 +5476,19 @@
         <v>0.95</v>
       </c>
       <c r="X17" s="30"/>
-      <c r="Y17" s="95"/>
-      <c r="Z17" s="96"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="86"/>
       <c r="AA17" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AB17" s="97"/>
+      <c r="AB17" s="79"/>
       <c r="AC17" s="48"/>
       <c r="AD17" s="49"/>
       <c r="AE17" s="17"/>
     </row>
     <row r="18" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P18" s="93"/>
-      <c r="Q18" s="70" t="s">
+      <c r="P18" s="80"/>
+      <c r="Q18" s="75" t="s">
         <v>7</v>
       </c>
       <c r="R18" s="15"/>
@@ -5508,9 +5514,9 @@
       <c r="AE18" s="60"/>
     </row>
     <row r="19" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P19" s="93"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="70" t="s">
+      <c r="P19" s="80"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="75" t="s">
         <v>23</v>
       </c>
       <c r="S19" s="13" t="s">
@@ -5535,9 +5541,9 @@
       <c r="AE19" s="30"/>
     </row>
     <row r="20" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P20" s="93"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
       <c r="S20" s="13" t="s">
         <v>26</v>
       </c>
@@ -5560,9 +5566,9 @@
       <c r="AE20" s="30"/>
     </row>
     <row r="21" spans="16:38" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P21" s="93"/>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="70"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
       <c r="S21" s="13" t="s">
         <v>27</v>
       </c>
@@ -5585,9 +5591,9 @@
       <c r="AE21" s="30"/>
     </row>
     <row r="22" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P22" s="93"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="70" t="s">
+      <c r="P22" s="80"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75" t="s">
         <v>24</v>
       </c>
       <c r="S22" s="13" t="s">
@@ -5612,9 +5618,9 @@
       <c r="AE22" s="30"/>
     </row>
     <row r="23" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P23" s="93"/>
-      <c r="Q23" s="70"/>
-      <c r="R23" s="70"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
       <c r="S23" s="13" t="s">
         <v>26</v>
       </c>
@@ -5643,9 +5649,9 @@
       <c r="AL23" s="30"/>
     </row>
     <row r="24" spans="16:38" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P24" s="95"/>
-      <c r="Q24" s="96"/>
-      <c r="R24" s="96"/>
+      <c r="P24" s="81"/>
+      <c r="Q24" s="86"/>
+      <c r="R24" s="86"/>
       <c r="S24" s="40" t="s">
         <v>27</v>
       </c>
@@ -5881,30 +5887,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="Y4:Y13"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="AB12:AB13"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z17"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="P11:P24"/>
-    <mergeCell ref="Q11:Q17"/>
-    <mergeCell ref="R12:R14"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="Q18:Q24"/>
-    <mergeCell ref="R19:R21"/>
-    <mergeCell ref="R22:R24"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="P2:V2"/>
@@ -5921,6 +5903,30 @@
     <mergeCell ref="R7:R8"/>
     <mergeCell ref="R9:R10"/>
     <mergeCell ref="T8:V8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="P11:P24"/>
+    <mergeCell ref="Q11:Q17"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="Q18:Q24"/>
+    <mergeCell ref="R19:R21"/>
+    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="Y4:Y13"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="AB4:AB5"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="AB12:AB13"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z17"/>
   </mergeCells>
   <conditionalFormatting sqref="K5:K6 D8:N10 D5:I5 D6:K7">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
added qwen degree 5 ec results
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897C5243-CABF-2341-BE0D-73B874BFF7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1D27D3-7C93-E247-8451-53B095B59AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="13260" windowWidth="38400" windowHeight="21600" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="13760" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -687,103 +687,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2776,24 +2776,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -2808,120 +2808,120 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="J4" s="5"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75" t="s">
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="J5" s="5"/>
       <c r="K5" s="17"/>
       <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="75"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:27" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="71">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
       <c r="J7" s="5"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
       <c r="J8" s="5"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="70" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
@@ -2940,31 +2940,31 @@
       <c r="H9" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L9" s="67" t="s">
+      <c r="L9" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="67"/>
-      <c r="N9" s="66" t="s">
+      <c r="M9" s="75"/>
+      <c r="N9" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="66"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="66"/>
-      <c r="U9" s="66"/>
-      <c r="V9" s="66"/>
-      <c r="W9" s="66"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="73"/>
+      <c r="V9" s="73"/>
+      <c r="W9" s="73"/>
+      <c r="X9" s="73"/>
+      <c r="Y9" s="73"/>
+      <c r="Z9" s="73"/>
+      <c r="AA9" s="73"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75" t="s">
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -2982,31 +2982,31 @@
       <c r="H10" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="66" t="s">
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
-      <c r="U10" s="66" t="s">
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="66"/>
-      <c r="W10" s="66"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="66"/>
+      <c r="V10" s="73"/>
+      <c r="W10" s="73"/>
+      <c r="X10" s="73"/>
+      <c r="Y10" s="73"/>
+      <c r="Z10" s="73"/>
+      <c r="AA10" s="73"/>
     </row>
     <row r="11" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
@@ -3022,39 +3022,39 @@
       <c r="H11" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67" t="s">
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="66" t="s">
+      <c r="O11" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66" t="s">
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="67" t="s">
+      <c r="S11" s="73"/>
+      <c r="T11" s="73"/>
+      <c r="U11" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="66" t="s">
+      <c r="V11" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="W11" s="66"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="66" t="s">
+      <c r="W11" s="73"/>
+      <c r="X11" s="73"/>
+      <c r="Y11" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
+      <c r="Z11" s="73"/>
+      <c r="AA11" s="73"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
@@ -3070,9 +3070,9 @@
       <c r="H12" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="66"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="T12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="66"/>
+      <c r="U12" s="73"/>
       <c r="V12" s="27" t="s">
         <v>25</v>
       </c>
@@ -3112,9 +3112,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75" t="s">
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -3138,53 +3138,53 @@
       <c r="M13" s="5">
         <v>0.85728300000000002</v>
       </c>
-      <c r="N13" s="69">
+      <c r="N13" s="74">
         <v>0.40795047246660099</v>
       </c>
-      <c r="O13" s="70">
+      <c r="O13" s="76">
         <v>0.59237536656891498</v>
       </c>
-      <c r="P13" s="70">
+      <c r="P13" s="76">
         <v>0.50667970022808695</v>
       </c>
-      <c r="Q13" s="68">
+      <c r="Q13" s="71">
         <v>0.46757901596611201</v>
       </c>
-      <c r="R13" s="68">
+      <c r="R13" s="71">
         <v>0.93385467579015902</v>
       </c>
-      <c r="S13" s="68">
+      <c r="S13" s="71">
         <v>0.76050830889540499</v>
       </c>
-      <c r="T13" s="68">
+      <c r="T13" s="71">
         <v>0.88367546432062505</v>
       </c>
-      <c r="U13" s="69">
+      <c r="U13" s="74">
         <v>0.493320299771912</v>
       </c>
-      <c r="V13" s="70">
+      <c r="V13" s="76">
         <v>0.60182469859889198</v>
       </c>
-      <c r="W13" s="70">
+      <c r="W13" s="76">
         <v>0.516780710329097</v>
       </c>
-      <c r="X13" s="68">
+      <c r="X13" s="71">
         <v>0.53828608667318301</v>
       </c>
-      <c r="Y13" s="68">
+      <c r="Y13" s="71">
         <v>0.928641251221896</v>
       </c>
-      <c r="Z13" s="68">
+      <c r="Z13" s="71">
         <v>0.83447376995764</v>
       </c>
-      <c r="AA13" s="68">
+      <c r="AA13" s="71">
         <v>0.916585206907787</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -3206,25 +3206,25 @@
       <c r="M14" s="5">
         <v>0.90257399999999999</v>
       </c>
-      <c r="N14" s="69"/>
-      <c r="O14" s="70"/>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="68"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="68"/>
-      <c r="T14" s="68"/>
-      <c r="U14" s="69"/>
-      <c r="V14" s="70"/>
-      <c r="W14" s="70"/>
-      <c r="X14" s="68"/>
-      <c r="Y14" s="68"/>
-      <c r="Z14" s="68"/>
-      <c r="AA14" s="68"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="76"/>
+      <c r="P14" s="76"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="76"/>
+      <c r="W14" s="76"/>
+      <c r="X14" s="71"/>
+      <c r="Y14" s="71"/>
+      <c r="Z14" s="71"/>
+      <c r="AA14" s="71"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -3246,24 +3246,24 @@
       <c r="M15" s="5">
         <v>0.93776499999999996</v>
       </c>
-      <c r="N15" s="69"/>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="68"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="68"/>
-      <c r="T15" s="68"/>
-      <c r="U15" s="69"/>
-      <c r="V15" s="70"/>
-      <c r="W15" s="70"/>
-      <c r="X15" s="68"/>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="68"/>
-      <c r="AA15" s="68"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="74"/>
+      <c r="V15" s="76"/>
+      <c r="W15" s="76"/>
+      <c r="X15" s="71"/>
+      <c r="Y15" s="71"/>
+      <c r="Z15" s="71"/>
+      <c r="AA15" s="71"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
-      <c r="B16" s="75" t="s">
+      <c r="A16" s="70"/>
+      <c r="B16" s="70" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="15"/>
@@ -3288,25 +3288,25 @@
       <c r="M16" s="5">
         <v>0.94330400000000003</v>
       </c>
-      <c r="N16" s="69"/>
-      <c r="O16" s="70"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="68"/>
-      <c r="R16" s="68"/>
-      <c r="S16" s="68"/>
-      <c r="T16" s="68"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="70"/>
-      <c r="W16" s="70"/>
-      <c r="X16" s="68"/>
-      <c r="Y16" s="68"/>
-      <c r="Z16" s="68"/>
-      <c r="AA16" s="68"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="76"/>
+      <c r="P16" s="76"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="76"/>
+      <c r="W16" s="76"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75" t="s">
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -3330,25 +3330,25 @@
       <c r="M17" s="5">
         <v>0.93548399999999998</v>
       </c>
-      <c r="N17" s="69"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="68"/>
-      <c r="R17" s="68"/>
-      <c r="S17" s="68"/>
-      <c r="T17" s="68"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="70"/>
-      <c r="W17" s="70"/>
-      <c r="X17" s="68"/>
-      <c r="Y17" s="68"/>
-      <c r="Z17" s="68"/>
-      <c r="AA17" s="68"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="76"/>
+      <c r="P17" s="76"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="76"/>
+      <c r="W17" s="76"/>
+      <c r="X17" s="71"/>
+      <c r="Y17" s="71"/>
+      <c r="Z17" s="71"/>
+      <c r="AA17" s="71"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="13" t="s">
         <v>26</v>
       </c>
@@ -3366,9 +3366,9 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="75"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3386,9 +3386,9 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75" t="s">
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="13" t="s">
@@ -3408,9 +3408,9 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="13" t="s">
         <v>26</v>
       </c>
@@ -3443,9 +3443,9 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="75"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="13" t="s">
         <v>27</v>
       </c>
@@ -3503,43 +3503,43 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="73">
+      <c r="E24" s="72">
         <v>0.995</v>
       </c>
-      <c r="F24" s="73"/>
+      <c r="F24" s="72"/>
       <c r="L24" s="24"/>
       <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
       <c r="D25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
       <c r="L25" s="24"/>
       <c r="M25" s="5"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="66" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="21">
@@ -3555,9 +3555,9 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
       <c r="D27" s="21">
         <v>2</v>
       </c>
@@ -3565,9 +3565,9 @@
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:27" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="71"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
       <c r="D28" s="21">
         <v>5</v>
       </c>
@@ -3575,9 +3575,9 @@
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="71"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
       <c r="D29" s="21">
         <v>10</v>
       </c>
@@ -3589,9 +3589,9 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="71"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
       <c r="D30" s="21">
         <v>20</v>
       </c>
@@ -3599,9 +3599,9 @@
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="71"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72" t="s">
+      <c r="A31" s="67"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="21">
@@ -3611,9 +3611,9 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="71"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="21">
         <v>2</v>
       </c>
@@ -3621,9 +3621,9 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="71"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
       <c r="D33" s="21">
         <v>3</v>
       </c>
@@ -3631,9 +3631,9 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="71"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
       <c r="D34" s="21">
         <v>4</v>
       </c>
@@ -3641,9 +3641,9 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="71"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="21">
         <v>5</v>
       </c>
@@ -3651,12 +3651,12 @@
       <c r="F35" s="23"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
-      <c r="B36" s="76" t="s">
+      <c r="A36" s="67"/>
+      <c r="B36" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
       <c r="E36" s="23">
         <v>0.96579999999999999</v>
       </c>
@@ -3669,41 +3669,6 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="A26:A36"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A3:B8"/>
-    <mergeCell ref="A9:A22"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="AA13:AA17"/>
-    <mergeCell ref="N10:T10"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="P13:P17"/>
     <mergeCell ref="N9:AA9"/>
     <mergeCell ref="L9:M12"/>
     <mergeCell ref="Q13:Q17"/>
@@ -3720,6 +3685,41 @@
     <mergeCell ref="X13:X17"/>
     <mergeCell ref="Y13:Y17"/>
     <mergeCell ref="Z13:Z17"/>
+    <mergeCell ref="AA13:AA17"/>
+    <mergeCell ref="N10:T10"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="P13:P17"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A3:B8"/>
+    <mergeCell ref="A9:A22"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="A26:A36"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="C26:C30"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H22">
     <cfRule type="colorScale" priority="1">
@@ -3781,18 +3781,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
       <c r="M1" s="14"/>
       <c r="N1" s="24" t="s">
         <v>55</v>
@@ -3817,10 +3817,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -3836,16 +3836,16 @@
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="75" t="s">
+      <c r="L2" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="77">
+      <c r="M2" s="78">
         <v>1</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="68">
+      <c r="O2" s="71">
         <v>0.85728300000000002</v>
       </c>
       <c r="P2" s="17">
@@ -3865,31 +3865,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="71">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="77"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="78"/>
       <c r="N3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="68"/>
+      <c r="O3" s="71"/>
       <c r="P3" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -3901,27 +3901,27 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="71">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="77"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="78"/>
       <c r="N4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="68"/>
+      <c r="O4" s="71"/>
       <c r="P4" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -3935,31 +3935,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75" t="s">
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="71">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="77">
+      <c r="L5" s="70"/>
+      <c r="M5" s="78">
         <v>2</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="68">
+      <c r="O5" s="71">
         <v>0.90257399999999999</v>
       </c>
       <c r="P5" s="17">
@@ -3979,27 +3979,27 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="75"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="71">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="77"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="78"/>
       <c r="N6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="68"/>
+      <c r="O6" s="71"/>
       <c r="P6" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4011,10 +4011,10 @@
       <c r="T6" s="17"/>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="70" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="15"/>
@@ -4033,12 +4033,12 @@
       <c r="H7" s="19">
         <v>0.603128</v>
       </c>
-      <c r="L7" s="75"/>
-      <c r="M7" s="77"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="78"/>
       <c r="N7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="68"/>
+      <c r="O7" s="71"/>
       <c r="P7" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4052,9 +4052,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75" t="s">
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -4072,14 +4072,14 @@
       <c r="H8" s="19">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L8" s="75"/>
-      <c r="M8" s="77">
+      <c r="L8" s="70"/>
+      <c r="M8" s="78">
         <v>5</v>
       </c>
       <c r="N8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="68">
+      <c r="O8" s="71">
         <v>0.93776499999999996</v>
       </c>
       <c r="P8" s="17">
@@ -4099,9 +4099,9 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="75"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
@@ -4117,12 +4117,12 @@
       <c r="H9" s="19">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L9" s="75"/>
-      <c r="M9" s="77"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="78"/>
       <c r="N9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="68"/>
+      <c r="O9" s="71"/>
       <c r="P9" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4134,9 +4134,9 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -4152,12 +4152,12 @@
       <c r="H10" s="19">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L10" s="75"/>
-      <c r="M10" s="77"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="78"/>
       <c r="N10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="68"/>
+      <c r="O10" s="71"/>
       <c r="P10" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4171,9 +4171,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75" t="s">
+      <c r="A11" s="70"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -4191,14 +4191,14 @@
       <c r="H11" s="19">
         <v>0.94037099999999996</v>
       </c>
-      <c r="L11" s="75"/>
-      <c r="M11" s="77">
+      <c r="L11" s="70"/>
+      <c r="M11" s="78">
         <v>10</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="68">
+      <c r="O11" s="71">
         <v>0.94330400000000003</v>
       </c>
       <c r="P11" s="17">
@@ -4218,9 +4218,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="13" t="s">
         <v>26</v>
       </c>
@@ -4236,12 +4236,12 @@
       <c r="H12" s="19">
         <v>0.754969</v>
       </c>
-      <c r="L12" s="75"/>
-      <c r="M12" s="77"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="78"/>
       <c r="N12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="68"/>
+      <c r="O12" s="71"/>
       <c r="P12" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4253,9 +4253,9 @@
       <c r="T12" s="17"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
@@ -4271,12 +4271,12 @@
       <c r="H13" s="19">
         <v>0.94884299999999999</v>
       </c>
-      <c r="L13" s="75"/>
-      <c r="M13" s="77"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="78"/>
       <c r="N13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="68"/>
+      <c r="O13" s="71"/>
       <c r="P13" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4290,8 +4290,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="75" t="s">
+      <c r="A14" s="70"/>
+      <c r="B14" s="70" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="15"/>
@@ -4310,14 +4310,14 @@
       <c r="H14" s="19">
         <v>0.63245399999999996</v>
       </c>
-      <c r="L14" s="75"/>
-      <c r="M14" s="77">
+      <c r="L14" s="70"/>
+      <c r="M14" s="78">
         <v>20</v>
       </c>
       <c r="N14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="68">
+      <c r="O14" s="71">
         <v>0.93548399999999998</v>
       </c>
       <c r="P14" s="17">
@@ -4337,9 +4337,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75" t="s">
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="13" t="s">
@@ -4357,12 +4357,12 @@
       <c r="H15" s="19">
         <v>0.68589100000000003</v>
       </c>
-      <c r="L15" s="75"/>
-      <c r="M15" s="77"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="78"/>
       <c r="N15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="68"/>
+      <c r="O15" s="71"/>
       <c r="P15" s="17">
         <v>0.90700000000000003</v>
       </c>
@@ -4374,9 +4374,9 @@
       <c r="T15" s="17"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="13" t="s">
         <v>26</v>
       </c>
@@ -4392,12 +4392,12 @@
       <c r="H16" s="19">
         <v>0.68067800000000001</v>
       </c>
-      <c r="L16" s="75"/>
-      <c r="M16" s="77"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="78"/>
       <c r="N16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="68"/>
+      <c r="O16" s="71"/>
       <c r="P16" s="17">
         <v>0.94899999999999995</v>
       </c>
@@ -4411,9 +4411,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
@@ -4433,9 +4433,9 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75" t="s">
+      <c r="A18" s="70"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -4461,9 +4461,9 @@
       <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="75"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
@@ -4483,9 +4483,9 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="75"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
       <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L28" s="5"/>
-      <c r="M28" s="69"/>
+      <c r="M28" s="74"/>
       <c r="N28" s="5"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L29" s="5"/>
-      <c r="M29" s="69"/>
+      <c r="M29" s="74"/>
       <c r="N29" s="5"/>
       <c r="O29" s="17"/>
       <c r="P29" s="25"/>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L30" s="5"/>
-      <c r="M30" s="69"/>
+      <c r="M30" s="74"/>
       <c r="N30" s="5"/>
       <c r="O30" s="17"/>
       <c r="P30" s="25"/>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L31" s="5"/>
-      <c r="M31" s="69"/>
+      <c r="M31" s="74"/>
       <c r="N31" s="5"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L32" s="5"/>
-      <c r="M32" s="69"/>
+      <c r="M32" s="74"/>
       <c r="N32" s="5"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -4590,6 +4590,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
     <mergeCell ref="M28:M32"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C3:C4"/>
@@ -4606,18 +4618,6 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="L2:L16"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="O14:O16"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H6 E7:F20 H7:H20">
     <cfRule type="colorScale" priority="4">
@@ -4652,7 +4652,7 @@
   <dimension ref="B1:AL43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+      <selection activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -4689,52 +4689,52 @@
   <sheetData>
     <row r="1" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92"/>
-      <c r="P2" s="90" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="83"/>
+      <c r="P2" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="91"/>
-      <c r="V2" s="92"/>
-      <c r="Y2" s="90" t="s">
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="83"/>
+      <c r="Y2" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="Z2" s="91"/>
-      <c r="AA2" s="91"/>
-      <c r="AB2" s="91"/>
-      <c r="AC2" s="91"/>
-      <c r="AD2" s="92"/>
-      <c r="AF2" s="90" t="s">
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="83"/>
+      <c r="AF2" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="91"/>
-      <c r="AH2" s="91"/>
-      <c r="AI2" s="91"/>
-      <c r="AJ2" s="92"/>
+      <c r="AG2" s="82"/>
+      <c r="AH2" s="82"/>
+      <c r="AI2" s="82"/>
+      <c r="AJ2" s="83"/>
     </row>
     <row r="3" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="83"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="94"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="87"/>
       <c r="K3" s="45"/>
       <c r="L3" s="50" t="s">
         <v>65</v>
@@ -4745,17 +4745,17 @@
       <c r="N3" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="95" t="s">
+      <c r="P3" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="96"/>
-      <c r="R3" s="96"/>
-      <c r="S3" s="96"/>
-      <c r="T3" s="96" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="89"/>
+      <c r="T3" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="96"/>
-      <c r="V3" s="98"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="91"/>
       <c r="X3" s="30"/>
       <c r="Y3" s="45"/>
       <c r="Z3" s="46"/>
@@ -4789,8 +4789,8 @@
       </c>
     </row>
     <row r="4" spans="2:36" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="93"/>
-      <c r="C4" s="77"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="13" t="s">
         <v>56</v>
       </c>
@@ -4822,10 +4822,10 @@
         <f>AVERAGE(D6:D10)</f>
         <v>0.92059999999999997</v>
       </c>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
       <c r="T4" s="16" t="s">
         <v>36</v>
       </c>
@@ -4837,16 +4837,16 @@
       </c>
       <c r="W4" s="20"/>
       <c r="X4" s="30"/>
-      <c r="Y4" s="80" t="s">
+      <c r="Y4" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="Z4" s="77">
+      <c r="Z4" s="78">
         <v>1</v>
       </c>
       <c r="AA4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB4" s="68">
+      <c r="AB4" s="71">
         <v>0.86699999999999999</v>
       </c>
       <c r="AC4" s="17">
@@ -4873,7 +4873,7 @@
       </c>
     </row>
     <row r="5" spans="2:36" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="79" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -4909,29 +4909,29 @@
         <f>AVERAGE(E5:I5)</f>
         <v>0.84460000000000002</v>
       </c>
-      <c r="P5" s="85" t="s">
+      <c r="P5" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75" t="s">
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70" t="s">
         <v>25</v>
       </c>
       <c r="S5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="68">
+      <c r="T5" s="71">
         <v>0.86699999999999999</v>
       </c>
-      <c r="U5" s="68"/>
-      <c r="V5" s="87"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="94"/>
       <c r="W5" s="20"/>
       <c r="X5" s="30"/>
-      <c r="Y5" s="80"/>
-      <c r="Z5" s="77"/>
+      <c r="Y5" s="93"/>
+      <c r="Z5" s="78"/>
       <c r="AA5" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" s="68"/>
+      <c r="AB5" s="71"/>
       <c r="AC5" s="17">
         <v>0.91300000000000003</v>
       </c>
@@ -4956,7 +4956,7 @@
       </c>
     </row>
     <row r="6" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="88"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="13">
         <v>1</v>
       </c>
@@ -4992,27 +4992,27 @@
         <f>AVERAGE(E6:I10)</f>
         <v>0.91474745461062212</v>
       </c>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="75"/>
+      <c r="P6" s="93"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
       <c r="S6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="68">
+      <c r="T6" s="71">
         <v>0.94799999999999995</v>
       </c>
-      <c r="U6" s="68"/>
-      <c r="V6" s="87"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="94"/>
       <c r="W6" s="20"/>
       <c r="X6" s="30"/>
-      <c r="Y6" s="80"/>
-      <c r="Z6" s="77">
+      <c r="Y6" s="93"/>
+      <c r="Z6" s="78">
         <v>2</v>
       </c>
       <c r="AA6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB6" s="68">
+      <c r="AB6" s="71">
         <v>0.90800000000000003</v>
       </c>
       <c r="AC6" s="17">
@@ -5024,7 +5024,7 @@
       <c r="AE6" s="60"/>
     </row>
     <row r="7" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="88"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="13">
         <v>2</v>
       </c>
@@ -5051,27 +5051,27 @@
       <c r="L7" s="53"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="75" t="s">
+      <c r="P7" s="93"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70" t="s">
         <v>26</v>
       </c>
       <c r="S7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="T7" s="68">
+      <c r="T7" s="71">
         <v>0.83499999999999996</v>
       </c>
-      <c r="U7" s="68"/>
-      <c r="V7" s="87"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="94"/>
       <c r="W7" s="20"/>
       <c r="X7" s="30"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="77"/>
+      <c r="Y7" s="93"/>
+      <c r="Z7" s="78"/>
       <c r="AA7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB7" s="68"/>
+      <c r="AB7" s="71"/>
       <c r="AC7" s="17">
         <v>0.91400000000000003</v>
       </c>
@@ -5081,7 +5081,7 @@
       <c r="AE7" s="17"/>
     </row>
     <row r="8" spans="2:36" ht="20" x14ac:dyDescent="0.2">
-      <c r="B8" s="88"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="13">
         <v>5</v>
       </c>
@@ -5108,27 +5108,27 @@
       <c r="L8" s="53"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
-      <c r="P8" s="80"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
       <c r="S8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="T8" s="68">
+      <c r="T8" s="71">
         <v>0.85199999999999998</v>
       </c>
-      <c r="U8" s="68"/>
-      <c r="V8" s="87"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="94"/>
       <c r="W8" s="20"/>
       <c r="X8" s="30"/>
-      <c r="Y8" s="80"/>
-      <c r="Z8" s="77">
+      <c r="Y8" s="93"/>
+      <c r="Z8" s="78">
         <v>5</v>
       </c>
       <c r="AA8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB8" s="68">
+      <c r="AB8" s="71">
         <v>0.94599999999999995</v>
       </c>
       <c r="AC8" s="17">
@@ -5140,7 +5140,7 @@
       <c r="AE8" s="17"/>
     </row>
     <row r="9" spans="2:36" ht="20" x14ac:dyDescent="0.25">
-      <c r="B9" s="88"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="13">
         <v>10</v>
       </c>
@@ -5167,29 +5167,29 @@
       <c r="L9" s="53"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75" t="s">
+      <c r="P9" s="93"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70" t="s">
         <v>27</v>
       </c>
       <c r="S9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="T9" s="68">
+      <c r="T9" s="71">
         <v>0.83699999999999997</v>
       </c>
-      <c r="U9" s="68"/>
-      <c r="V9" s="87"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="94"/>
       <c r="W9" s="20"/>
       <c r="X9" s="30"/>
-      <c r="Y9" s="80"/>
-      <c r="Z9" s="77"/>
+      <c r="Y9" s="93"/>
+      <c r="Z9" s="78"/>
       <c r="AA9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB9" s="68"/>
+      <c r="AB9" s="71"/>
       <c r="AC9" s="17">
-        <v>0.92400000000000004</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="AD9" s="38">
         <v>0.95199999999999996</v>
@@ -5197,7 +5197,7 @@
       <c r="AE9" s="60"/>
     </row>
     <row r="10" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="89"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="40">
         <v>20</v>
       </c>
@@ -5224,27 +5224,27 @@
       <c r="L10" s="53"/>
       <c r="M10" s="53"/>
       <c r="N10" s="53"/>
-      <c r="P10" s="80"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="75"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
       <c r="S10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T10" s="68">
+      <c r="T10" s="71">
         <v>0.95099999999999996</v>
       </c>
-      <c r="U10" s="68"/>
-      <c r="V10" s="87"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="94"/>
       <c r="W10" s="20"/>
       <c r="X10" s="30"/>
-      <c r="Y10" s="80"/>
-      <c r="Z10" s="77">
+      <c r="Y10" s="93"/>
+      <c r="Z10" s="78">
         <v>10</v>
       </c>
       <c r="AA10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB10" s="68">
+      <c r="AB10" s="71">
         <v>0.94799999999999995</v>
       </c>
       <c r="AC10" s="17">
@@ -5262,10 +5262,10 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
-      <c r="P11" s="80" t="s">
+      <c r="P11" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="75" t="s">
+      <c r="Q11" s="70" t="s">
         <v>6</v>
       </c>
       <c r="R11" s="15"/>
@@ -5282,12 +5282,12 @@
         <v>0.60299999999999998</v>
       </c>
       <c r="X11" s="30"/>
-      <c r="Y11" s="80"/>
-      <c r="Z11" s="77"/>
+      <c r="Y11" s="93"/>
+      <c r="Z11" s="78"/>
       <c r="AA11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB11" s="68"/>
+      <c r="AB11" s="71"/>
       <c r="AC11" s="17">
         <v>0.91200000000000003</v>
       </c>
@@ -5297,9 +5297,9 @@
       <c r="AE11" s="17"/>
     </row>
     <row r="12" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="80"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75" t="s">
+      <c r="P12" s="93"/>
+      <c r="Q12" s="70"/>
+      <c r="R12" s="70" t="s">
         <v>23</v>
       </c>
       <c r="S12" s="13" t="s">
@@ -5315,14 +5315,14 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="X12" s="30"/>
-      <c r="Y12" s="80"/>
-      <c r="Z12" s="77">
+      <c r="Y12" s="93"/>
+      <c r="Z12" s="78">
         <v>20</v>
       </c>
       <c r="AA12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB12" s="68">
+      <c r="AB12" s="71">
         <v>0.93400000000000005</v>
       </c>
       <c r="AC12" s="17">
@@ -5334,9 +5334,9 @@
       <c r="AE12" s="60"/>
     </row>
     <row r="13" spans="2:36" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P13" s="80"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="70"/>
       <c r="S13" s="13" t="s">
         <v>26</v>
       </c>
@@ -5350,12 +5350,12 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="X13" s="30"/>
-      <c r="Y13" s="81"/>
-      <c r="Z13" s="82"/>
+      <c r="Y13" s="95"/>
+      <c r="Z13" s="98"/>
       <c r="AA13" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AB13" s="79"/>
+      <c r="AB13" s="97"/>
       <c r="AC13" s="48">
         <v>0.91200000000000003</v>
       </c>
@@ -5365,9 +5365,9 @@
       <c r="AE13" s="17"/>
     </row>
     <row r="14" spans="2:36" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P14" s="80"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="75"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="70"/>
+      <c r="R14" s="70"/>
       <c r="S14" s="13" t="s">
         <v>27</v>
       </c>
@@ -5390,9 +5390,9 @@
       <c r="AE14" s="17"/>
     </row>
     <row r="15" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="P15" s="80"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="75" t="s">
+      <c r="P15" s="93"/>
+      <c r="Q15" s="70"/>
+      <c r="R15" s="70" t="s">
         <v>24</v>
       </c>
       <c r="S15" s="13" t="s">
@@ -5408,8 +5408,8 @@
         <v>0.94599999999999995</v>
       </c>
       <c r="X15" s="30"/>
-      <c r="Y15" s="83"/>
-      <c r="Z15" s="84"/>
+      <c r="Y15" s="84"/>
+      <c r="Z15" s="85"/>
       <c r="AA15" s="34" t="s">
         <v>55</v>
       </c>
@@ -5425,9 +5425,9 @@
       <c r="AE15" s="60"/>
     </row>
     <row r="16" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="P16" s="80"/>
-      <c r="Q16" s="75"/>
-      <c r="R16" s="75"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
       <c r="S16" s="13" t="s">
         <v>26</v>
       </c>
@@ -5441,14 +5441,14 @@
         <v>0.73199999999999998</v>
       </c>
       <c r="X16" s="30"/>
-      <c r="Y16" s="85" t="s">
+      <c r="Y16" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="Z16" s="75"/>
+      <c r="Z16" s="70"/>
       <c r="AA16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AB16" s="68">
+      <c r="AB16" s="71">
         <v>0.95099999999999996</v>
       </c>
       <c r="AC16" s="17">
@@ -5460,9 +5460,9 @@
       <c r="AE16" s="17"/>
     </row>
     <row r="17" spans="16:38" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P17" s="80"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="70"/>
+      <c r="R17" s="70"/>
       <c r="S17" s="13" t="s">
         <v>27</v>
       </c>
@@ -5476,19 +5476,19 @@
         <v>0.95</v>
       </c>
       <c r="X17" s="30"/>
-      <c r="Y17" s="81"/>
-      <c r="Z17" s="86"/>
+      <c r="Y17" s="95"/>
+      <c r="Z17" s="96"/>
       <c r="AA17" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AB17" s="79"/>
+      <c r="AB17" s="97"/>
       <c r="AC17" s="48"/>
       <c r="AD17" s="49"/>
       <c r="AE17" s="17"/>
     </row>
     <row r="18" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P18" s="80"/>
-      <c r="Q18" s="75" t="s">
+      <c r="P18" s="93"/>
+      <c r="Q18" s="70" t="s">
         <v>7</v>
       </c>
       <c r="R18" s="15"/>
@@ -5514,9 +5514,9 @@
       <c r="AE18" s="60"/>
     </row>
     <row r="19" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P19" s="80"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75" t="s">
+      <c r="P19" s="93"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70" t="s">
         <v>23</v>
       </c>
       <c r="S19" s="13" t="s">
@@ -5541,9 +5541,9 @@
       <c r="AE19" s="30"/>
     </row>
     <row r="20" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P20" s="80"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="70"/>
       <c r="S20" s="13" t="s">
         <v>26</v>
       </c>
@@ -5566,9 +5566,9 @@
       <c r="AE20" s="30"/>
     </row>
     <row r="21" spans="16:38" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P21" s="80"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
       <c r="S21" s="13" t="s">
         <v>27</v>
       </c>
@@ -5591,9 +5591,9 @@
       <c r="AE21" s="30"/>
     </row>
     <row r="22" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P22" s="80"/>
-      <c r="Q22" s="75"/>
-      <c r="R22" s="75" t="s">
+      <c r="P22" s="93"/>
+      <c r="Q22" s="70"/>
+      <c r="R22" s="70" t="s">
         <v>24</v>
       </c>
       <c r="S22" s="13" t="s">
@@ -5618,9 +5618,9 @@
       <c r="AE22" s="30"/>
     </row>
     <row r="23" spans="16:38" x14ac:dyDescent="0.25">
-      <c r="P23" s="80"/>
-      <c r="Q23" s="75"/>
-      <c r="R23" s="75"/>
+      <c r="P23" s="93"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70"/>
       <c r="S23" s="13" t="s">
         <v>26</v>
       </c>
@@ -5649,9 +5649,9 @@
       <c r="AL23" s="30"/>
     </row>
     <row r="24" spans="16:38" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P24" s="81"/>
-      <c r="Q24" s="86"/>
-      <c r="R24" s="86"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="96"/>
+      <c r="R24" s="96"/>
       <c r="S24" s="40" t="s">
         <v>27</v>
       </c>
@@ -5887,6 +5887,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="Y4:Y13"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="AB4:AB5"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="AB12:AB13"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z17"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="P11:P24"/>
+    <mergeCell ref="Q11:Q17"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="Q18:Q24"/>
+    <mergeCell ref="R19:R21"/>
+    <mergeCell ref="R22:R24"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="P2:V2"/>
@@ -5903,30 +5927,6 @@
     <mergeCell ref="R7:R8"/>
     <mergeCell ref="R9:R10"/>
     <mergeCell ref="T8:V8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="P11:P24"/>
-    <mergeCell ref="Q11:Q17"/>
-    <mergeCell ref="R12:R14"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="Q18:Q24"/>
-    <mergeCell ref="R19:R21"/>
-    <mergeCell ref="R22:R24"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="Y4:Y13"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="AB12:AB13"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z17"/>
   </mergeCells>
   <conditionalFormatting sqref="K5:K6 D8:N10 D5:I5 D6:K7">
     <cfRule type="colorScale" priority="4">

</xml_diff>

<commit_message>
added area heuristic code
</commit_message>
<xml_diff>
--- a/misc/results.xlsx
+++ b/misc/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA9782D-381F-9A49-B5AE-C0670B4333E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18A6ED3-8F47-9947-9D41-BB669F47B1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="8740" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="10960" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="join-no-learning" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="64">
   <si>
     <t>llama</t>
   </si>
@@ -216,6 +216,24 @@
   </si>
   <si>
     <t>fs</t>
+  </si>
+  <si>
+    <t>0..509</t>
+  </si>
+  <si>
+    <t>zs-all</t>
+  </si>
+  <si>
+    <t>fs-all</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>worst (max_area=0.1)</t>
+  </si>
+  <si>
+    <t>best (max_areat=0.4)</t>
   </si>
 </sst>
 </file>
@@ -309,7 +327,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -434,12 +452,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -553,9 +707,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -596,8 +747,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -611,9 +765,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -623,14 +774,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -638,7 +792,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -646,125 +812,172 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -781,10 +994,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2748,18 +2957,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="M1" s="13"/>
       <c r="N1" s="19" t="s">
         <v>43</v>
@@ -2784,10 +2993,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="15" t="s">
         <v>29</v>
       </c>
@@ -2803,16 +3012,16 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
-      <c r="L2" s="62" t="s">
+      <c r="L2" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="63">
+      <c r="M2" s="64">
         <v>1</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="59">
+      <c r="O2" s="62">
         <v>0.85728300000000002</v>
       </c>
       <c r="P2" s="16">
@@ -2832,31 +3041,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="62">
         <v>0.85728300000000002</v>
       </c>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="64"/>
       <c r="N3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="59"/>
+      <c r="O3" s="62"/>
       <c r="P3" s="16">
         <v>0.90700000000000003</v>
       </c>
@@ -2868,27 +3077,27 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="62">
         <v>0.94330400000000003</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="63"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="64"/>
       <c r="N4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="59"/>
+      <c r="O4" s="62"/>
       <c r="P4" s="16">
         <v>0.94899999999999995</v>
       </c>
@@ -2902,31 +3111,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="59">
+      <c r="E5" s="62">
         <v>0.84620399999999996</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63">
+      <c r="L5" s="61"/>
+      <c r="M5" s="64">
         <v>2</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="59">
+      <c r="O5" s="62">
         <v>0.90257399999999999</v>
       </c>
       <c r="P5" s="16">
@@ -2946,27 +3155,27 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="62">
         <v>0.86510299999999996</v>
       </c>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="63"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="64"/>
       <c r="N6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="59"/>
+      <c r="O6" s="62"/>
       <c r="P6" s="16">
         <v>0.90700000000000003</v>
       </c>
@@ -2978,10 +3187,10 @@
       <c r="T6" s="16"/>
     </row>
     <row r="7" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="61" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="14"/>
@@ -3000,12 +3209,12 @@
       <c r="H7" s="17">
         <v>0.603128</v>
       </c>
-      <c r="L7" s="62"/>
-      <c r="M7" s="63"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="64"/>
       <c r="N7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="59"/>
+      <c r="O7" s="62"/>
       <c r="P7" s="16">
         <v>0.94899999999999995</v>
       </c>
@@ -3019,9 +3228,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62" t="s">
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -3039,14 +3248,14 @@
       <c r="H8" s="17">
         <v>0.63962200000000002</v>
       </c>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63">
+      <c r="L8" s="61"/>
+      <c r="M8" s="64">
         <v>5</v>
       </c>
       <c r="N8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="59">
+      <c r="O8" s="62">
         <v>0.93776499999999996</v>
       </c>
       <c r="P8" s="16">
@@ -3066,9 +3275,9 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
@@ -3084,12 +3293,12 @@
       <c r="H9" s="17">
         <v>0.60540899999999997</v>
       </c>
-      <c r="L9" s="62"/>
-      <c r="M9" s="63"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="64"/>
       <c r="N9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="59"/>
+      <c r="O9" s="62"/>
       <c r="P9" s="16">
         <v>0.90700000000000003</v>
       </c>
@@ -3101,9 +3310,9 @@
       <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
@@ -3119,12 +3328,12 @@
       <c r="H10" s="17">
         <v>0.65982399999999997</v>
       </c>
-      <c r="L10" s="62"/>
-      <c r="M10" s="63"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="64"/>
       <c r="N10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="59"/>
+      <c r="O10" s="62"/>
       <c r="P10" s="16">
         <v>0.94899999999999995</v>
       </c>
@@ -3138,9 +3347,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="12" t="s">
@@ -3158,14 +3367,14 @@
       <c r="H11" s="17">
         <v>0.94037099999999996</v>
       </c>
-      <c r="L11" s="62"/>
-      <c r="M11" s="63">
+      <c r="L11" s="61"/>
+      <c r="M11" s="64">
         <v>10</v>
       </c>
       <c r="N11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="59">
+      <c r="O11" s="62">
         <v>0.94330400000000003</v>
       </c>
       <c r="P11" s="16">
@@ -3185,9 +3394,9 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="12" t="s">
         <v>21</v>
       </c>
@@ -3203,12 +3412,12 @@
       <c r="H12" s="17">
         <v>0.754969</v>
       </c>
-      <c r="L12" s="62"/>
-      <c r="M12" s="63"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="64"/>
       <c r="N12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="59"/>
+      <c r="O12" s="62"/>
       <c r="P12" s="16">
         <v>0.90700000000000003</v>
       </c>
@@ -3220,9 +3429,9 @@
       <c r="T12" s="16"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="12" t="s">
         <v>22</v>
       </c>
@@ -3238,12 +3447,12 @@
       <c r="H13" s="17">
         <v>0.94884299999999999</v>
       </c>
-      <c r="L13" s="62"/>
-      <c r="M13" s="63"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="64"/>
       <c r="N13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="59"/>
+      <c r="O13" s="62"/>
       <c r="P13" s="16">
         <v>0.94899999999999995</v>
       </c>
@@ -3257,8 +3466,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="B14" s="62" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="61" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="14"/>
@@ -3277,14 +3486,14 @@
       <c r="H14" s="17">
         <v>0.63245399999999996</v>
       </c>
-      <c r="L14" s="62"/>
-      <c r="M14" s="63">
+      <c r="L14" s="61"/>
+      <c r="M14" s="64">
         <v>20</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="59">
+      <c r="O14" s="62">
         <v>0.93548399999999998</v>
       </c>
       <c r="P14" s="16">
@@ -3304,9 +3513,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -3324,12 +3533,12 @@
       <c r="H15" s="17">
         <v>0.68589100000000003</v>
       </c>
-      <c r="L15" s="62"/>
-      <c r="M15" s="63"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="64"/>
       <c r="N15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="59"/>
+      <c r="O15" s="62"/>
       <c r="P15" s="16">
         <v>0.90700000000000003</v>
       </c>
@@ -3341,9 +3550,9 @@
       <c r="T15" s="16"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="12" t="s">
         <v>21</v>
       </c>
@@ -3359,12 +3568,12 @@
       <c r="H16" s="17">
         <v>0.68067800000000001</v>
       </c>
-      <c r="L16" s="62"/>
-      <c r="M16" s="63"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="64"/>
       <c r="N16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="O16" s="59"/>
+      <c r="O16" s="62"/>
       <c r="P16" s="16">
         <v>0.94899999999999995</v>
       </c>
@@ -3378,9 +3587,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="12" t="s">
         <v>22</v>
       </c>
@@ -3400,9 +3609,9 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="12" t="s">
@@ -3428,9 +3637,9 @@
       <c r="R18" s="20"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="12" t="s">
         <v>21</v>
       </c>
@@ -3450,9 +3659,9 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="12" t="s">
         <v>22</v>
       </c>
@@ -3512,7 +3721,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L28" s="5"/>
-      <c r="M28" s="60"/>
+      <c r="M28" s="59"/>
       <c r="N28" s="5"/>
       <c r="O28" s="20"/>
       <c r="P28" s="20"/>
@@ -3521,7 +3730,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L29" s="5"/>
-      <c r="M29" s="60"/>
+      <c r="M29" s="59"/>
       <c r="N29" s="5"/>
       <c r="O29" s="16"/>
       <c r="P29" s="20"/>
@@ -3530,7 +3739,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L30" s="5"/>
-      <c r="M30" s="60"/>
+      <c r="M30" s="59"/>
       <c r="N30" s="5"/>
       <c r="O30" s="16"/>
       <c r="P30" s="20"/>
@@ -3539,7 +3748,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L31" s="5"/>
-      <c r="M31" s="60"/>
+      <c r="M31" s="59"/>
       <c r="N31" s="5"/>
       <c r="O31" s="20"/>
       <c r="P31" s="20"/>
@@ -3548,7 +3757,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L32" s="5"/>
-      <c r="M32" s="60"/>
+      <c r="M32" s="59"/>
       <c r="N32" s="5"/>
       <c r="O32" s="20"/>
       <c r="P32" s="20"/>
@@ -3557,6 +3766,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
     <mergeCell ref="M28:M32"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="C3:C4"/>
@@ -3573,18 +3794,6 @@
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="L2:L16"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="O8:O10"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="O14:O16"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:H6 E7:F20 H7:H20">
     <cfRule type="colorScale" priority="4">
@@ -3616,10 +3825,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D01CA2-3159-F448-9006-FF836418E31D}">
-  <dimension ref="B1:AR53"/>
+  <dimension ref="B1:AS54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH22" sqref="AH22"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -3634,7 +3843,7 @@
     <col min="15" max="15" width="10.83203125" style="12"/>
     <col min="16" max="17" width="4.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.1640625" style="12" customWidth="1"/>
-    <col min="19" max="19" width="20.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" style="12" customWidth="1"/>
     <col min="20" max="20" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7" style="12" bestFit="1" customWidth="1"/>
@@ -3647,130 +3856,116 @@
     <col min="30" max="30" width="2.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="36" width="9" style="12" customWidth="1"/>
-    <col min="37" max="37" width="11" style="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="10.83203125" style="12"/>
+    <col min="33" max="33" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="38" width="9" style="12" customWidth="1"/>
+    <col min="39" max="39" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:41" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:41" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+    <row r="1" spans="2:43" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:43" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76"/>
-      <c r="P2" s="74" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="76"/>
-      <c r="Y2" s="74" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
-      <c r="AC2" s="75"/>
-      <c r="AD2" s="75"/>
-      <c r="AE2" s="75"/>
-      <c r="AF2" s="76"/>
-      <c r="AK2" s="74" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="72"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="92"/>
+      <c r="AA2" s="92"/>
+      <c r="AB2" s="92"/>
+      <c r="AC2" s="92"/>
+      <c r="AD2" s="92"/>
+      <c r="AE2" s="92"/>
+      <c r="AF2" s="92"/>
+      <c r="AG2" s="92"/>
+      <c r="AH2" s="92"/>
+      <c r="AM2" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="76"/>
-    </row>
-    <row r="3" spans="2:41" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70" t="s">
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="72"/>
+    </row>
+    <row r="3" spans="2:43" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="78"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="76"/>
       <c r="K3" s="37"/>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
-      <c r="T3" s="80" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="80"/>
-      <c r="V3" s="82"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="105"/>
       <c r="X3" s="22"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB3" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC3" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD3" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE3" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF3" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
+      <c r="Y3" s="96"/>
+      <c r="Z3" s="89"/>
+      <c r="AA3" s="90"/>
+      <c r="AB3" s="90"/>
+      <c r="AC3" s="90"/>
+      <c r="AD3" s="90"/>
+      <c r="AE3" s="90"/>
+      <c r="AF3" s="90"/>
+      <c r="AG3" s="90"/>
+      <c r="AH3" s="90"/>
       <c r="AI3" s="19"/>
       <c r="AJ3" s="19"/>
-      <c r="AK3" s="37" t="s">
+      <c r="AK3" s="19"/>
+      <c r="AL3" s="19"/>
+      <c r="AM3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AL3" s="42" t="s">
+      <c r="AN3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="AM3" s="42" t="s">
+      <c r="AO3" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="AN3" s="42" t="s">
+      <c r="AP3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="AO3" s="43" t="s">
+      <c r="AQ3" s="42" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:41" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="77"/>
-      <c r="C4" s="63"/>
+    <row r="4" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="75"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="12" t="s">
         <v>44</v>
       </c>
@@ -3786,864 +3981,734 @@
       <c r="H4" s="12">
         <v>4</v>
       </c>
-      <c r="I4" s="44">
+      <c r="I4" s="43">
         <v>5</v>
       </c>
-      <c r="K4" s="50" t="s">
+      <c r="K4" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="45">
+      <c r="L4" s="44">
         <v>0.86699999999999999</v>
       </c>
-      <c r="M4" s="45">
+      <c r="M4" s="44">
         <v>0.94799999999999995</v>
       </c>
-      <c r="N4" s="46">
+      <c r="N4" s="45">
         <f>AVERAGE(D6:D10)</f>
         <v>0.92059999999999997</v>
       </c>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" s="91" t="s">
-        <v>2</v>
-      </c>
-      <c r="V4" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="P4" s="105"/>
+      <c r="Q4" s="105"/>
+      <c r="R4" s="105"/>
+      <c r="S4" s="105"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="106"/>
+      <c r="V4" s="106"/>
       <c r="W4" s="18"/>
       <c r="X4" s="22"/>
-      <c r="Y4" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z4" s="63">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB4" s="59">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AF4" s="30">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="95"/>
       <c r="AI4" s="16"/>
       <c r="AJ4" s="16"/>
-      <c r="AK4" s="28">
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="28">
         <v>1</v>
       </c>
-      <c r="AL4" s="16">
+      <c r="AN4" s="16">
         <v>0.86699999999999999</v>
       </c>
-      <c r="AM4" s="16">
+      <c r="AO4" s="16">
         <v>0.86299999999999999</v>
       </c>
-      <c r="AN4" s="12">
+      <c r="AP4" s="12">
         <v>0.85099999999999998</v>
       </c>
-      <c r="AO4" s="30">
+      <c r="AQ4" s="30">
         <v>0.87</v>
       </c>
     </row>
-    <row r="5" spans="2:41" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="72" t="s">
+    <row r="5" spans="2:43" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="68" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45">
+      <c r="D5" s="44"/>
+      <c r="E5" s="44">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="44">
         <v>0.84699999999999998</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="44">
         <v>0.85099999999999998</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="44">
         <v>0.85199999999999998</v>
       </c>
-      <c r="I5" s="46">
+      <c r="I5" s="45">
         <v>0.83499999999999996</v>
       </c>
-      <c r="J5" s="45"/>
-      <c r="K5" s="50" t="s">
+      <c r="J5" s="44"/>
+      <c r="K5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="44">
         <v>0.83499999999999996</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="44">
         <v>0.85199999999999998</v>
       </c>
-      <c r="N5" s="46">
+      <c r="N5" s="45">
         <f>AVERAGE(E5:I5)</f>
         <v>0.84460000000000002</v>
       </c>
-      <c r="P5" s="98" t="s">
-        <v>32</v>
-      </c>
+      <c r="P5" s="100"/>
       <c r="Q5" s="99"/>
-      <c r="R5" s="103" t="s">
-        <v>20</v>
-      </c>
-      <c r="S5" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5" s="100">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="U5" s="100"/>
-      <c r="V5" s="101"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="89"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
       <c r="W5" s="18"/>
       <c r="X5" s="22"/>
-      <c r="Y5" s="66"/>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB5" s="59"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="16"/>
-      <c r="AE5" s="16">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="AF5" s="30">
-        <v>0.95</v>
-      </c>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
+      <c r="Y5" s="99"/>
+      <c r="Z5" s="92"/>
+      <c r="AA5" s="93"/>
+      <c r="AB5" s="94"/>
+      <c r="AC5" s="95"/>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
       <c r="AI5" s="16"/>
       <c r="AJ5" s="16"/>
-      <c r="AK5" s="49">
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="48">
         <v>10</v>
       </c>
-      <c r="AL5" s="40">
+      <c r="AN5" s="39">
         <v>0.94799999999999995</v>
       </c>
-      <c r="AM5" s="40">
+      <c r="AO5" s="39">
         <v>0.94699999999999995</v>
       </c>
-      <c r="AN5" s="40">
+      <c r="AP5" s="39">
         <v>0.92</v>
       </c>
-      <c r="AO5" s="41">
+      <c r="AQ5" s="40">
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="6" spans="2:41" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="72"/>
+    <row r="6" spans="2:43" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
       <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <v>0.86699999999999999</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="44">
         <v>0.85923753665689095</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="44">
         <v>0.85988921472792401</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="44">
         <v>0.85858585858585801</v>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="44">
         <v>0.85337243401759499</v>
       </c>
-      <c r="I6" s="46">
+      <c r="I6" s="45">
         <v>0.83740632127728898</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="51" t="s">
+      <c r="J6" s="44"/>
+      <c r="K6" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="46">
         <v>0.83699999999999997</v>
       </c>
-      <c r="M6" s="47">
+      <c r="M6" s="46">
         <v>0.95099999999999996</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="47">
         <f>AVERAGE(E6:I10)</f>
         <v>0.91474745461062212</v>
       </c>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="97"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="106" t="s">
-        <v>24</v>
-      </c>
-      <c r="T6" s="65">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="U6" s="65"/>
-      <c r="V6" s="102"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="94"/>
+      <c r="U6" s="94"/>
+      <c r="V6" s="94"/>
       <c r="W6" s="18"/>
       <c r="X6" s="22"/>
-      <c r="Y6" s="66"/>
-      <c r="Z6" s="63">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB6" s="59">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AF6" s="30">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AG6" s="52"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="52"/>
-      <c r="AJ6" s="52"/>
-    </row>
-    <row r="7" spans="2:41" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="72"/>
+      <c r="Y6" s="99"/>
+      <c r="Z6" s="92"/>
+      <c r="AA6" s="93"/>
+      <c r="AB6" s="94"/>
+      <c r="AC6" s="95"/>
+      <c r="AD6" s="95"/>
+      <c r="AE6" s="95"/>
+      <c r="AF6" s="95"/>
+      <c r="AG6" s="95"/>
+      <c r="AH6" s="95"/>
+      <c r="AI6" s="51"/>
+      <c r="AJ6" s="51"/>
+      <c r="AK6" s="51"/>
+      <c r="AL6" s="51"/>
+    </row>
+    <row r="7" spans="2:43" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="68"/>
       <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="44">
         <v>0.90800000000000003</v>
       </c>
-      <c r="E7" s="45">
+      <c r="E7" s="44">
         <v>0.90648399999999996</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <v>0.90713600000000005</v>
       </c>
-      <c r="G7" s="45">
+      <c r="G7" s="44">
         <v>0.90550699999999995</v>
       </c>
-      <c r="H7" s="45">
+      <c r="H7" s="44">
         <v>0.89996699999999996</v>
       </c>
-      <c r="I7" s="46">
+      <c r="I7" s="45">
         <v>0.88302400000000003</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="103" t="s">
-        <v>21</v>
-      </c>
-      <c r="S7" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="T7" s="100">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="U7" s="100"/>
-      <c r="V7" s="101"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="99"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="94"/>
+      <c r="U7" s="94"/>
+      <c r="V7" s="94"/>
       <c r="W7" s="18"/>
       <c r="X7" s="22"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="63"/>
-      <c r="AA7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB7" s="59"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16">
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="AF7" s="30">
-        <v>0.95</v>
-      </c>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="16"/>
+      <c r="Y7" s="99"/>
+      <c r="Z7" s="92"/>
+      <c r="AA7" s="93"/>
+      <c r="AB7" s="94"/>
+      <c r="AC7" s="95"/>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="95"/>
+      <c r="AG7" s="95"/>
+      <c r="AH7" s="95"/>
       <c r="AI7" s="16"/>
       <c r="AJ7" s="16"/>
-    </row>
-    <row r="8" spans="2:41" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="72"/>
+      <c r="AK7" s="16"/>
+      <c r="AL7" s="16"/>
+    </row>
+    <row r="8" spans="2:43" x14ac:dyDescent="0.2">
+      <c r="B8" s="68"/>
       <c r="C8" s="12">
         <v>5</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="44">
         <v>0.94599999999999995</v>
       </c>
-      <c r="E8" s="45">
+      <c r="E8" s="44">
         <v>0.942326</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="44">
         <v>0.94330400000000003</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="44">
         <v>0.94167500000000004</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="44">
         <v>0.93548399999999998</v>
       </c>
-      <c r="I8" s="46">
+      <c r="I8" s="45">
         <v>0.91756300000000002</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="97"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="106" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" s="65">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="U8" s="65"/>
-      <c r="V8" s="102"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="99"/>
+      <c r="R8" s="99"/>
+      <c r="S8" s="89"/>
+      <c r="T8" s="94"/>
+      <c r="U8" s="94"/>
+      <c r="V8" s="94"/>
       <c r="W8" s="18"/>
       <c r="X8" s="22"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="63">
-        <v>5</v>
-      </c>
-      <c r="AA8" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB8" s="59">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="16">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AF8" s="30">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
+      <c r="Y8" s="99"/>
+      <c r="Z8" s="92"/>
+      <c r="AA8" s="93"/>
+      <c r="AB8" s="94"/>
+      <c r="AC8" s="95"/>
+      <c r="AD8" s="95"/>
+      <c r="AE8" s="95"/>
+      <c r="AF8" s="95"/>
+      <c r="AG8" s="95"/>
+      <c r="AH8" s="95"/>
       <c r="AI8" s="16"/>
       <c r="AJ8" s="16"/>
-    </row>
-    <row r="9" spans="2:41" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="72"/>
+      <c r="AK8" s="16"/>
+      <c r="AL8" s="16"/>
+    </row>
+    <row r="9" spans="2:43" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="68"/>
       <c r="C9" s="12">
         <v>10</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="44">
         <v>0.94799999999999995</v>
       </c>
-      <c r="E9" s="45">
+      <c r="E9" s="44">
         <v>0.95047199999999998</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="44">
         <v>0.95145000000000002</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G9" s="44">
         <v>0.94982100000000003</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="44">
         <v>0.94362999999999997</v>
       </c>
-      <c r="I9" s="46">
+      <c r="I9" s="45">
         <v>0.92538299999999996</v>
       </c>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="103" t="s">
-        <v>22</v>
-      </c>
-      <c r="S9" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="T9" s="100">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="U9" s="100"/>
-      <c r="V9" s="101"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="P9" s="99"/>
+      <c r="Q9" s="99"/>
+      <c r="R9" s="99"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="94"/>
+      <c r="U9" s="94"/>
+      <c r="V9" s="94"/>
       <c r="W9" s="18"/>
       <c r="X9" s="22"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="63"/>
-      <c r="AA9" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB9" s="59"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="AF9" s="30">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="AG9" s="52"/>
-      <c r="AH9" s="52"/>
-      <c r="AI9" s="52"/>
-      <c r="AJ9" s="52"/>
-    </row>
-    <row r="10" spans="2:41" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="73"/>
+      <c r="Y9" s="99"/>
+      <c r="Z9" s="92"/>
+      <c r="AA9" s="93"/>
+      <c r="AB9" s="94"/>
+      <c r="AC9" s="95"/>
+      <c r="AD9" s="95"/>
+      <c r="AE9" s="95"/>
+      <c r="AF9" s="95"/>
+      <c r="AG9" s="95"/>
+      <c r="AH9" s="95"/>
+      <c r="AI9" s="51"/>
+      <c r="AJ9" s="51"/>
+      <c r="AK9" s="51"/>
+      <c r="AL9" s="51"/>
+    </row>
+    <row r="10" spans="2:43" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="69"/>
       <c r="C10" s="32">
         <v>20</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="46">
         <v>0.93400000000000005</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="46">
         <v>0.94525899999999996</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="46">
         <v>0.94688799999999995</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="46">
         <v>0.94525899999999996</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H10" s="46">
         <v>0.93906800000000001</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="47">
         <v>0.92049499999999995</v>
       </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="T10" s="65">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="U10" s="65"/>
-      <c r="V10" s="102"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="P10" s="99"/>
+      <c r="Q10" s="99"/>
+      <c r="R10" s="99"/>
+      <c r="S10" s="96"/>
+      <c r="T10" s="94"/>
+      <c r="U10" s="94"/>
+      <c r="V10" s="94"/>
       <c r="W10" s="18"/>
       <c r="X10" s="22"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="63">
-        <v>10</v>
-      </c>
-      <c r="AA10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB10" s="59">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="16">
-        <v>0.95</v>
-      </c>
-      <c r="AF10" s="30">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="AG10" s="16"/>
-      <c r="AH10" s="16"/>
+      <c r="Y10" s="99"/>
+      <c r="Z10" s="92"/>
+      <c r="AA10" s="93"/>
+      <c r="AB10" s="94"/>
+      <c r="AC10" s="95"/>
+      <c r="AD10" s="95"/>
+      <c r="AE10" s="95"/>
+      <c r="AF10" s="95"/>
+      <c r="AG10" s="95"/>
+      <c r="AH10" s="95"/>
       <c r="AI10" s="16"/>
       <c r="AJ10" s="16"/>
-    </row>
-    <row r="11" spans="2:41" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK10" s="16"/>
+      <c r="AL10" s="16"/>
+    </row>
+    <row r="11" spans="2:43" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
-      <c r="P11" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q11" s="103" t="s">
-        <v>6</v>
-      </c>
-      <c r="R11" s="107"/>
-      <c r="S11" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="T11" s="108">
-        <v>0.52</v>
-      </c>
-      <c r="U11" s="108">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="V11" s="109">
-        <v>0.60299999999999998</v>
-      </c>
+      <c r="P11" s="99"/>
+      <c r="Q11" s="99"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="96"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="107"/>
       <c r="X11" s="22"/>
-      <c r="Y11" s="66"/>
-      <c r="Z11" s="63"/>
-      <c r="AA11" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB11" s="59"/>
-      <c r="AC11" s="16"/>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="16">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="AF11" s="30">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="16"/>
+      <c r="Y11" s="99"/>
+      <c r="Z11" s="92"/>
+      <c r="AA11" s="93"/>
+      <c r="AB11" s="94"/>
+      <c r="AC11" s="95"/>
+      <c r="AD11" s="95"/>
+      <c r="AE11" s="95"/>
+      <c r="AF11" s="95"/>
+      <c r="AG11" s="95"/>
+      <c r="AH11" s="95"/>
       <c r="AI11" s="16"/>
       <c r="AJ11" s="16"/>
-    </row>
-    <row r="12" spans="2:41" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="103" t="s">
-        <v>18</v>
-      </c>
-      <c r="S12" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="T12" s="104">
-        <v>0.52</v>
-      </c>
-      <c r="U12" s="104">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="V12" s="105">
-        <v>0.64500000000000002</v>
-      </c>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="16"/>
+    </row>
+    <row r="12" spans="2:43" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="99"/>
+      <c r="Q12" s="99"/>
+      <c r="R12" s="99"/>
+      <c r="S12" s="96"/>
+      <c r="T12" s="107"/>
+      <c r="U12" s="107"/>
+      <c r="V12" s="107"/>
       <c r="X12" s="22"/>
-      <c r="Y12" s="66"/>
-      <c r="Z12" s="63">
-        <v>20</v>
-      </c>
-      <c r="AA12" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB12" s="59">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="16">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="AF12" s="30">
-        <v>0.94</v>
-      </c>
-      <c r="AG12" s="52"/>
-      <c r="AH12" s="52"/>
-      <c r="AI12" s="52"/>
-      <c r="AJ12" s="52"/>
-    </row>
-    <row r="13" spans="2:41" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="83" t="s">
-        <v>21</v>
-      </c>
-      <c r="T13" s="84">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="U13" s="84">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="V13" s="31">
-        <v>0.60899999999999999</v>
-      </c>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="22"/>
+      <c r="AH12" s="22"/>
+      <c r="AI12" s="16"/>
+      <c r="AJ12" s="16"/>
+      <c r="AK12" s="16"/>
+      <c r="AL12" s="16"/>
+    </row>
+    <row r="13" spans="2:43" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P13" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q13" s="71"/>
+      <c r="R13" s="71"/>
+      <c r="S13" s="71"/>
+      <c r="T13" s="71"/>
+      <c r="U13" s="71"/>
+      <c r="V13" s="72"/>
       <c r="X13" s="22"/>
-      <c r="Y13" s="67"/>
-      <c r="Z13" s="68"/>
-      <c r="AA13" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB13" s="65"/>
-      <c r="AC13" s="40"/>
-      <c r="AD13" s="40"/>
-      <c r="AE13" s="40">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="AF13" s="41">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="AG13" s="16"/>
-      <c r="AH13" s="16"/>
-      <c r="AI13" s="16"/>
-      <c r="AJ13" s="16"/>
-    </row>
-    <row r="14" spans="2:41" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P14" s="66"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="66"/>
-      <c r="S14" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="T14" s="84">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="U14" s="84">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="V14" s="31">
-        <v>0.67600000000000005</v>
-      </c>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="22"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+      <c r="AG13" s="19"/>
+      <c r="AH13" s="19"/>
+      <c r="AI13" s="51"/>
+      <c r="AJ13" s="51"/>
+      <c r="AK13" s="51"/>
+      <c r="AL13" s="51"/>
+    </row>
+    <row r="14" spans="2:43" x14ac:dyDescent="0.2">
+      <c r="P14" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="78"/>
+      <c r="T14" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="U14" s="78"/>
+      <c r="V14" s="80"/>
       <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="22"/>
-      <c r="AA14" s="22"/>
-      <c r="AB14" s="22"/>
-      <c r="AC14" s="22"/>
-      <c r="AD14" s="22"/>
-      <c r="AE14" s="22"/>
-      <c r="AF14" s="22"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="25"/>
+      <c r="AD14" s="25"/>
+      <c r="AE14" s="25"/>
+      <c r="AF14" s="25"/>
       <c r="AG14" s="16"/>
       <c r="AH14" s="16"/>
       <c r="AI14" s="16"/>
       <c r="AJ14" s="16"/>
-    </row>
-    <row r="15" spans="2:41" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P15" s="66"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="67"/>
-      <c r="S15" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="34"/>
-      <c r="X15" s="86"/>
-      <c r="Y15" s="86"/>
-      <c r="Z15" s="86"/>
-      <c r="AA15" s="88"/>
-      <c r="AB15" s="88"/>
-      <c r="AC15" s="88"/>
-      <c r="AD15" s="88"/>
-      <c r="AE15" s="88"/>
-      <c r="AF15" s="88"/>
-      <c r="AG15" s="110"/>
-      <c r="AH15" s="52"/>
-      <c r="AI15" s="52"/>
-      <c r="AJ15" s="52"/>
-    </row>
-    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="103" t="s">
-        <v>19</v>
-      </c>
-      <c r="S16" s="42" t="s">
+      <c r="AK14" s="16"/>
+      <c r="AL14" s="16"/>
+    </row>
+    <row r="15" spans="2:43" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="79"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="U15" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="V15" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="25"/>
+      <c r="AD15" s="25"/>
+      <c r="AE15" s="25"/>
+      <c r="AF15" s="25"/>
+      <c r="AG15" s="16"/>
+      <c r="AH15" s="16"/>
+      <c r="AI15" s="16"/>
+      <c r="AJ15" s="16"/>
+      <c r="AK15" s="16"/>
+      <c r="AL15" s="16"/>
+    </row>
+    <row r="16" spans="2:43" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="T16" s="104">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="U16" s="104">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="V16" s="105">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="X16" s="86"/>
-      <c r="Y16" s="92"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="90"/>
-      <c r="AB16" s="94"/>
-      <c r="AC16" s="94"/>
-      <c r="AD16" s="94"/>
-      <c r="AE16" s="85"/>
-      <c r="AF16" s="85"/>
-      <c r="AG16" s="85"/>
+      <c r="S16" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="T16" s="84">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="U16" s="84"/>
+      <c r="V16" s="85"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="25"/>
+      <c r="AC16" s="25"/>
+      <c r="AD16" s="25"/>
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="25"/>
+      <c r="AG16" s="16"/>
       <c r="AH16" s="16"/>
-      <c r="AI16" s="16"/>
-      <c r="AJ16" s="16"/>
-    </row>
-    <row r="17" spans="16:44" x14ac:dyDescent="0.25">
+      <c r="AI16" s="51"/>
+      <c r="AJ16" s="51"/>
+      <c r="AK16" s="51"/>
+      <c r="AL16" s="51"/>
+    </row>
+    <row r="17" spans="16:45" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P17" s="66"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="66"/>
-      <c r="S17" s="83" t="s">
+      <c r="Q17" s="61"/>
+      <c r="R17" s="109"/>
+      <c r="S17" s="110" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17" s="111">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="U17" s="111"/>
+      <c r="V17" s="112"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="22"/>
+      <c r="AI17" s="22"/>
+      <c r="AJ17" s="22"/>
+      <c r="AK17" s="22"/>
+      <c r="AL17" s="22"/>
+    </row>
+    <row r="18" spans="16:45" x14ac:dyDescent="0.2">
+      <c r="P18" s="66"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="T17" s="84">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="U17" s="84">
-        <v>0.74199999999999999</v>
-      </c>
-      <c r="V17" s="31">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="X17" s="86"/>
-      <c r="Y17" s="93"/>
-      <c r="Z17" s="93"/>
-      <c r="AA17" s="90"/>
-      <c r="AB17" s="94"/>
-      <c r="AC17" s="94"/>
-      <c r="AD17" s="94"/>
-      <c r="AE17" s="85"/>
-      <c r="AF17" s="85"/>
-      <c r="AG17" s="85"/>
-      <c r="AH17" s="16"/>
-      <c r="AI17" s="16"/>
-      <c r="AJ17" s="16"/>
-    </row>
-    <row r="18" spans="16:44" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P18" s="66"/>
-      <c r="Q18" s="66"/>
-      <c r="R18" s="66"/>
-      <c r="S18" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="T18" s="84">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="U18" s="84">
-        <v>0.877</v>
-      </c>
-      <c r="V18" s="31">
-        <v>0.95</v>
-      </c>
-      <c r="X18" s="86"/>
-      <c r="Y18" s="93"/>
-      <c r="Z18" s="86"/>
-      <c r="AA18" s="90"/>
-      <c r="AB18" s="94"/>
-      <c r="AC18" s="94"/>
-      <c r="AD18" s="94"/>
-      <c r="AE18" s="85"/>
-      <c r="AF18" s="85"/>
-      <c r="AG18" s="110"/>
-      <c r="AH18" s="52"/>
-      <c r="AI18" s="52"/>
-      <c r="AJ18" s="52"/>
-    </row>
-    <row r="19" spans="16:44" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S18" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="T18" s="115">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="U18" s="115"/>
+      <c r="V18" s="116"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
+      <c r="AG18" s="19"/>
+      <c r="AH18" s="19"/>
+      <c r="AI18" s="22"/>
+      <c r="AJ18" s="22"/>
+      <c r="AK18" s="22"/>
+      <c r="AL18" s="22"/>
+    </row>
+    <row r="19" spans="16:45" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P19" s="66"/>
-      <c r="Q19" s="67"/>
-      <c r="R19" s="67"/>
-      <c r="S19" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="T19" s="33"/>
-      <c r="U19" s="33"/>
-      <c r="V19" s="34"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="109"/>
+      <c r="S19" s="110" t="s">
+        <v>45</v>
+      </c>
+      <c r="T19" s="111">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="U19" s="111"/>
+      <c r="V19" s="112"/>
       <c r="X19" s="22"/>
-      <c r="Y19" s="22"/>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="22"/>
-      <c r="AB19" s="22"/>
-      <c r="AC19" s="22"/>
-      <c r="AD19" s="22"/>
-      <c r="AE19" s="22"/>
-      <c r="AF19" s="22"/>
-      <c r="AG19" s="22"/>
-      <c r="AH19" s="22"/>
+      <c r="Y19" s="52"/>
+      <c r="Z19" s="18"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="25"/>
+      <c r="AC19" s="25"/>
+      <c r="AD19" s="25"/>
+      <c r="AE19" s="25"/>
+      <c r="AF19" s="25"/>
+      <c r="AG19" s="16"/>
+      <c r="AH19" s="16"/>
       <c r="AI19" s="22"/>
       <c r="AJ19" s="22"/>
-    </row>
-    <row r="20" spans="16:44" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK19" s="22"/>
+      <c r="AL19" s="22"/>
+    </row>
+    <row r="20" spans="16:45" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P20" s="66"/>
-      <c r="Q20" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="R20" s="107"/>
-      <c r="S20" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="T20" s="108">
-        <v>0.495</v>
-      </c>
-      <c r="U20" s="108">
-        <v>0.495</v>
-      </c>
-      <c r="V20" s="109">
-        <v>0.63300000000000001</v>
-      </c>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="113" t="s">
+        <v>61</v>
+      </c>
+      <c r="S20" s="114" t="s">
+        <v>62</v>
+      </c>
+      <c r="T20" s="115">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="U20" s="115"/>
+      <c r="V20" s="116"/>
       <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="19"/>
-      <c r="AB20" s="19"/>
-      <c r="AC20" s="19"/>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="19"/>
-      <c r="AF20" s="19"/>
-      <c r="AG20" s="22"/>
-      <c r="AH20" s="22"/>
+      <c r="Y20" s="52"/>
+      <c r="Z20" s="18"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="25"/>
+      <c r="AD20" s="25"/>
+      <c r="AE20" s="25"/>
+      <c r="AF20" s="25"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="16"/>
       <c r="AI20" s="22"/>
       <c r="AJ20" s="22"/>
-    </row>
-    <row r="21" spans="16:44" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK20" s="22"/>
+      <c r="AL20" s="22"/>
+    </row>
+    <row r="21" spans="16:45" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P21" s="66"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="103" t="s">
-        <v>18</v>
-      </c>
-      <c r="S21" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="T21" s="104">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="U21" s="104">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="V21" s="105">
-        <v>0.68200000000000005</v>
-      </c>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="109"/>
+      <c r="S21" s="110" t="s">
+        <v>63</v>
+      </c>
+      <c r="T21" s="111">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="U21" s="111"/>
+      <c r="V21" s="112"/>
       <c r="X21" s="22"/>
-      <c r="Y21" s="53"/>
+      <c r="Y21" s="52"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="15"/>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
       <c r="AD21" s="25"/>
-      <c r="AE21" s="16"/>
-      <c r="AF21" s="16"/>
-      <c r="AG21" s="22"/>
-      <c r="AH21" s="22"/>
+      <c r="AE21" s="25"/>
+      <c r="AF21" s="25"/>
+      <c r="AG21" s="16"/>
+      <c r="AH21" s="16"/>
       <c r="AI21" s="22"/>
       <c r="AJ21" s="22"/>
-    </row>
-    <row r="22" spans="16:44" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK21" s="22"/>
+      <c r="AL21" s="22"/>
+    </row>
+    <row r="22" spans="16:45" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
-      <c r="S22" s="83" t="s">
-        <v>21</v>
-      </c>
-      <c r="T22" s="84">
-        <v>0.52600000000000002</v>
-      </c>
-      <c r="U22" s="84">
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="V22" s="31">
-        <v>0.67900000000000005</v>
-      </c>
+      <c r="Q22" s="61"/>
+      <c r="R22" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="89" t="s">
+        <v>30</v>
+      </c>
+      <c r="T22" s="97">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="U22" s="97"/>
+      <c r="V22" s="108"/>
       <c r="X22" s="22"/>
       <c r="Y22" s="18"/>
       <c r="Z22" s="18"/>
@@ -4651,29 +4716,27 @@
       <c r="AB22" s="25"/>
       <c r="AC22" s="25"/>
       <c r="AD22" s="25"/>
-      <c r="AE22" s="16"/>
-      <c r="AF22" s="16"/>
-      <c r="AG22" s="22"/>
-      <c r="AH22" s="22"/>
+      <c r="AE22" s="25"/>
+      <c r="AF22" s="25"/>
+      <c r="AG22" s="16"/>
+      <c r="AH22" s="16"/>
       <c r="AI22" s="22"/>
       <c r="AJ22" s="22"/>
-    </row>
-    <row r="23" spans="16:44" x14ac:dyDescent="0.25">
-      <c r="P23" s="66"/>
-      <c r="Q23" s="66"/>
-      <c r="R23" s="66"/>
-      <c r="S23" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="T23" s="84">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="U23" s="84">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="V23" s="31">
-        <v>0.66300000000000003</v>
-      </c>
+      <c r="AK22" s="22"/>
+      <c r="AL22" s="22"/>
+    </row>
+    <row r="23" spans="16:45" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="67"/>
+      <c r="Q23" s="83"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="T23" s="86">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="U23" s="86"/>
+      <c r="V23" s="87"/>
       <c r="X23" s="22"/>
       <c r="Y23" s="18"/>
       <c r="Z23" s="18"/>
@@ -4681,64 +4744,66 @@
       <c r="AB23" s="25"/>
       <c r="AC23" s="25"/>
       <c r="AD23" s="25"/>
-      <c r="AE23" s="16"/>
-      <c r="AF23" s="85"/>
-      <c r="AG23" s="86"/>
-      <c r="AH23" s="86"/>
-      <c r="AI23" s="86"/>
-      <c r="AJ23" s="86"/>
-      <c r="AK23" s="83"/>
-      <c r="AL23" s="86"/>
-      <c r="AM23" s="86"/>
-      <c r="AN23" s="86"/>
-      <c r="AO23" s="86"/>
-      <c r="AP23" s="86"/>
-      <c r="AQ23" s="86"/>
-      <c r="AR23" s="83"/>
-    </row>
-    <row r="24" spans="16:44" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P24" s="66"/>
-      <c r="Q24" s="66"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="34"/>
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="25"/>
+      <c r="AG23" s="16"/>
+      <c r="AH23" s="16"/>
+      <c r="AI23" s="22"/>
+      <c r="AJ23" s="22"/>
+      <c r="AK23" s="22"/>
+      <c r="AL23" s="22"/>
+      <c r="AN23" s="22"/>
+      <c r="AO23" s="22"/>
+      <c r="AP23" s="22"/>
+      <c r="AQ23" s="22"/>
+      <c r="AR23" s="22"/>
+      <c r="AS23" s="22"/>
+    </row>
+    <row r="24" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P24" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="R24" s="117"/>
+      <c r="S24" s="118" t="s">
+        <v>15</v>
+      </c>
+      <c r="T24" s="119">
+        <v>0.52</v>
+      </c>
+      <c r="U24" s="119">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="V24" s="120">
+        <v>0.60299999999999998</v>
+      </c>
       <c r="Y24" s="35"/>
       <c r="Z24" s="35"/>
-      <c r="AF24" s="83"/>
-      <c r="AG24" s="83"/>
-      <c r="AH24" s="83"/>
-      <c r="AI24" s="83"/>
-      <c r="AJ24" s="83"/>
-      <c r="AK24" s="83"/>
-      <c r="AL24" s="83"/>
-      <c r="AM24" s="87"/>
-      <c r="AN24" s="88"/>
-      <c r="AO24" s="88"/>
-      <c r="AP24" s="88"/>
-      <c r="AQ24" s="88"/>
-      <c r="AR24" s="83"/>
-    </row>
-    <row r="25" spans="16:44" x14ac:dyDescent="0.25">
+      <c r="AO24" s="13"/>
+      <c r="AP24" s="19"/>
+      <c r="AQ24" s="19"/>
+      <c r="AR24" s="19"/>
+      <c r="AS24" s="19"/>
+    </row>
+    <row r="25" spans="16:45" x14ac:dyDescent="0.25">
       <c r="P25" s="66"/>
       <c r="Q25" s="66"/>
-      <c r="R25" s="103" t="s">
-        <v>19</v>
-      </c>
-      <c r="S25" s="42" t="s">
+      <c r="R25" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="S25" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="T25" s="104">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="U25" s="104">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="V25" s="105">
-        <v>0.93600000000000005</v>
+      <c r="T25" s="121">
+        <v>0.52</v>
+      </c>
+      <c r="U25" s="121">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="V25" s="122">
+        <v>0.64500000000000002</v>
       </c>
       <c r="Y25" s="36"/>
       <c r="Z25" s="35"/>
@@ -4746,67 +4811,70 @@
       <c r="AB25" s="24"/>
       <c r="AC25" s="24"/>
       <c r="AD25" s="24"/>
-      <c r="AF25" s="83"/>
-      <c r="AG25" s="83"/>
-      <c r="AH25" s="83"/>
-      <c r="AI25" s="83"/>
-      <c r="AJ25" s="83"/>
-      <c r="AK25" s="86"/>
-      <c r="AL25" s="86"/>
-      <c r="AM25" s="86"/>
-      <c r="AN25" s="86"/>
-      <c r="AO25" s="86"/>
-      <c r="AP25" s="86"/>
-      <c r="AQ25" s="86"/>
-      <c r="AR25" s="83"/>
-    </row>
-    <row r="26" spans="16:44" x14ac:dyDescent="0.25">
+      <c r="AE25" s="24"/>
+      <c r="AF25" s="92"/>
+      <c r="AG25" s="92"/>
+      <c r="AH25" s="92"/>
+      <c r="AI25" s="92"/>
+      <c r="AJ25" s="92"/>
+      <c r="AK25" s="92"/>
+      <c r="AL25" s="92"/>
+      <c r="AM25" s="22"/>
+      <c r="AN25" s="22"/>
+      <c r="AO25" s="22"/>
+      <c r="AP25" s="22"/>
+      <c r="AQ25" s="22"/>
+      <c r="AR25" s="22"/>
+      <c r="AS25" s="22"/>
+    </row>
+    <row r="26" spans="16:45" x14ac:dyDescent="0.25">
       <c r="P26" s="66"/>
       <c r="Q26" s="66"/>
       <c r="R26" s="66"/>
-      <c r="S26" s="83" t="s">
+      <c r="S26" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="84">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="U26" s="84">
-        <v>0.82199999999999995</v>
+      <c r="T26" s="107">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="U26" s="107">
+        <v>0.51600000000000001</v>
       </c>
       <c r="V26" s="31">
-        <v>0.94499999999999995</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="Y26" s="35"/>
       <c r="Z26" s="35"/>
-      <c r="AF26" s="83"/>
-      <c r="AG26" s="83"/>
-      <c r="AH26" s="83"/>
-      <c r="AI26" s="83"/>
-      <c r="AJ26" s="83"/>
-      <c r="AK26" s="89"/>
-      <c r="AL26" s="89"/>
-      <c r="AM26" s="89"/>
-      <c r="AN26" s="89"/>
-      <c r="AO26" s="89"/>
-      <c r="AP26" s="89"/>
-      <c r="AQ26" s="89"/>
-      <c r="AR26" s="83"/>
-    </row>
-    <row r="27" spans="16:44" x14ac:dyDescent="0.25">
+      <c r="AF26" s="105"/>
+      <c r="AG26" s="105"/>
+      <c r="AH26" s="105"/>
+      <c r="AI26" s="105"/>
+      <c r="AJ26" s="105"/>
+      <c r="AK26" s="105"/>
+      <c r="AL26" s="105"/>
+      <c r="AM26" s="54"/>
+      <c r="AN26" s="54"/>
+      <c r="AO26" s="54"/>
+      <c r="AP26" s="54"/>
+      <c r="AQ26" s="54"/>
+      <c r="AR26" s="54"/>
+      <c r="AS26" s="54"/>
+    </row>
+    <row r="27" spans="16:45" x14ac:dyDescent="0.25">
       <c r="P27" s="66"/>
       <c r="Q27" s="66"/>
       <c r="R27" s="66"/>
-      <c r="S27" s="83" t="s">
+      <c r="S27" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="84">
-        <v>0.51700000000000002</v>
-      </c>
-      <c r="U27" s="84">
-        <v>0.91600000000000004</v>
+      <c r="T27" s="107">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="U27" s="107">
+        <v>0.47899999999999998</v>
       </c>
       <c r="V27" s="31">
-        <v>0.94099999999999995</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="Y27" s="36"/>
       <c r="Z27" s="35"/>
@@ -4814,69 +4882,111 @@
       <c r="AB27" s="24"/>
       <c r="AC27" s="24"/>
       <c r="AD27" s="24"/>
-      <c r="AF27" s="83"/>
-      <c r="AG27" s="83"/>
-      <c r="AH27" s="83"/>
-      <c r="AI27" s="83"/>
-      <c r="AJ27" s="83"/>
-      <c r="AK27" s="89"/>
-      <c r="AL27" s="89"/>
-      <c r="AM27" s="89"/>
-      <c r="AN27" s="89"/>
-      <c r="AO27" s="90"/>
-      <c r="AP27" s="91"/>
-      <c r="AQ27" s="91"/>
-      <c r="AR27" s="83"/>
-    </row>
-    <row r="28" spans="16:44" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P28" s="67"/>
-      <c r="Q28" s="67"/>
-      <c r="R28" s="67"/>
-      <c r="S28" s="32" t="s">
+      <c r="AE27" s="24"/>
+      <c r="AF27" s="105"/>
+      <c r="AG27" s="105"/>
+      <c r="AH27" s="105"/>
+      <c r="AI27" s="105"/>
+      <c r="AJ27" s="93"/>
+      <c r="AK27" s="106"/>
+      <c r="AL27" s="106"/>
+      <c r="AM27" s="54"/>
+      <c r="AN27" s="54"/>
+      <c r="AO27" s="54"/>
+      <c r="AP27" s="54"/>
+      <c r="AQ27" s="15"/>
+      <c r="AR27" s="21"/>
+      <c r="AS27" s="21"/>
+    </row>
+    <row r="28" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="109"/>
+      <c r="S28" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="T28" s="33"/>
-      <c r="U28" s="33"/>
-      <c r="V28" s="34"/>
+      <c r="T28" s="124">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="U28" s="124">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="V28" s="125">
+        <v>0.69599999999999995</v>
+      </c>
       <c r="Y28" s="35"/>
       <c r="Z28" s="35"/>
-      <c r="AF28" s="83"/>
-      <c r="AG28" s="83"/>
-      <c r="AH28" s="83"/>
-      <c r="AI28" s="83"/>
-      <c r="AJ28" s="83"/>
-      <c r="AK28" s="92"/>
-      <c r="AL28" s="93"/>
-      <c r="AM28" s="93"/>
-      <c r="AN28" s="87"/>
-      <c r="AO28" s="94"/>
-      <c r="AP28" s="94"/>
-      <c r="AQ28" s="94"/>
-      <c r="AR28" s="83"/>
-    </row>
-    <row r="29" spans="16:44" x14ac:dyDescent="0.2">
+      <c r="AF28" s="100"/>
+      <c r="AG28" s="99"/>
+      <c r="AH28" s="99"/>
+      <c r="AI28" s="89"/>
+      <c r="AJ28" s="94"/>
+      <c r="AK28" s="94"/>
+      <c r="AL28" s="94"/>
+      <c r="AM28" s="52"/>
+      <c r="AN28" s="18"/>
+      <c r="AO28" s="18"/>
+      <c r="AP28" s="13"/>
+      <c r="AQ28" s="25"/>
+      <c r="AR28" s="25"/>
+      <c r="AS28" s="25"/>
+    </row>
+    <row r="29" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="113" t="s">
+        <v>19</v>
+      </c>
+      <c r="S29" s="114" t="s">
+        <v>20</v>
+      </c>
+      <c r="T29" s="121">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="U29" s="121">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="V29" s="122">
+        <v>0.94599999999999995</v>
+      </c>
       <c r="Y29" s="13"/>
       <c r="Z29" s="19"/>
       <c r="AA29" s="19"/>
       <c r="AB29" s="19"/>
       <c r="AC29" s="19"/>
       <c r="AD29" s="19"/>
-      <c r="AE29" s="23"/>
-      <c r="AF29" s="83"/>
-      <c r="AG29" s="83"/>
-      <c r="AH29" s="83"/>
-      <c r="AI29" s="83"/>
-      <c r="AJ29" s="83"/>
-      <c r="AK29" s="93"/>
-      <c r="AL29" s="93"/>
-      <c r="AM29" s="93"/>
-      <c r="AN29" s="87"/>
-      <c r="AO29" s="94"/>
-      <c r="AP29" s="94"/>
-      <c r="AQ29" s="94"/>
-      <c r="AR29" s="83"/>
-    </row>
-    <row r="30" spans="16:44" x14ac:dyDescent="0.2">
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="99"/>
+      <c r="AG29" s="99"/>
+      <c r="AH29" s="99"/>
+      <c r="AI29" s="89"/>
+      <c r="AJ29" s="94"/>
+      <c r="AK29" s="94"/>
+      <c r="AL29" s="94"/>
+      <c r="AM29" s="18"/>
+      <c r="AN29" s="18"/>
+      <c r="AO29" s="18"/>
+      <c r="AP29" s="13"/>
+      <c r="AQ29" s="25"/>
+      <c r="AR29" s="25"/>
+      <c r="AS29" s="25"/>
+    </row>
+    <row r="30" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="T30" s="107">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="U30" s="107">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="V30" s="31">
+        <v>0.73199999999999998</v>
+      </c>
       <c r="X30" s="18"/>
       <c r="Y30" s="22"/>
       <c r="Z30" s="15"/>
@@ -4885,515 +4995,870 @@
       <c r="AC30" s="16"/>
       <c r="AD30" s="16"/>
       <c r="AE30" s="16"/>
-      <c r="AF30" s="83"/>
-      <c r="AG30" s="83"/>
-      <c r="AH30" s="83"/>
-      <c r="AI30" s="83"/>
-      <c r="AJ30" s="83"/>
-      <c r="AK30" s="93"/>
-      <c r="AL30" s="93"/>
-      <c r="AM30" s="93"/>
-      <c r="AN30" s="83"/>
-      <c r="AO30" s="94"/>
-      <c r="AP30" s="94"/>
-      <c r="AQ30" s="94"/>
-      <c r="AR30" s="83"/>
-    </row>
-    <row r="31" spans="16:44" x14ac:dyDescent="0.2">
+      <c r="AF30" s="99"/>
+      <c r="AG30" s="99"/>
+      <c r="AH30" s="99"/>
+      <c r="AI30" s="96"/>
+      <c r="AJ30" s="94"/>
+      <c r="AK30" s="94"/>
+      <c r="AL30" s="94"/>
+      <c r="AM30" s="18"/>
+      <c r="AN30" s="18"/>
+      <c r="AO30" s="18"/>
+      <c r="AQ30" s="25"/>
+      <c r="AR30" s="25"/>
+      <c r="AS30" s="25"/>
+    </row>
+    <row r="31" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="66"/>
+      <c r="S31" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="T31" s="107">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="U31" s="107">
+        <v>0.877</v>
+      </c>
+      <c r="V31" s="31">
+        <v>0.95</v>
+      </c>
       <c r="X31" s="18"/>
-      <c r="Y31" s="22"/>
-      <c r="Z31" s="15"/>
-      <c r="AA31" s="25"/>
-      <c r="AB31" s="16"/>
-      <c r="AC31" s="16"/>
-      <c r="AD31" s="16"/>
-      <c r="AE31" s="16"/>
-      <c r="AF31" s="83"/>
-      <c r="AG31" s="83"/>
-      <c r="AH31" s="83"/>
-      <c r="AI31" s="83"/>
-      <c r="AJ31" s="83"/>
-      <c r="AK31" s="93"/>
-      <c r="AL31" s="93"/>
-      <c r="AM31" s="93"/>
-      <c r="AN31" s="87"/>
-      <c r="AO31" s="94"/>
-      <c r="AP31" s="94"/>
-      <c r="AQ31" s="94"/>
-      <c r="AR31" s="83"/>
-    </row>
-    <row r="32" spans="16:44" x14ac:dyDescent="0.2">
+      <c r="Y31" s="92"/>
+      <c r="Z31" s="93"/>
+      <c r="AA31" s="94"/>
+      <c r="AB31" s="95"/>
+      <c r="AC31" s="95"/>
+      <c r="AD31" s="95"/>
+      <c r="AE31" s="95"/>
+      <c r="AF31" s="99"/>
+      <c r="AG31" s="99"/>
+      <c r="AH31" s="99"/>
+      <c r="AI31" s="89"/>
+      <c r="AJ31" s="94"/>
+      <c r="AK31" s="94"/>
+      <c r="AL31" s="94"/>
+      <c r="AM31" s="18"/>
+      <c r="AN31" s="18"/>
+      <c r="AO31" s="18"/>
+      <c r="AP31" s="13"/>
+      <c r="AQ31" s="25"/>
+      <c r="AR31" s="25"/>
+      <c r="AS31" s="25"/>
+    </row>
+    <row r="32" spans="16:45" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P32" s="66"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="109"/>
+      <c r="S32" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="T32" s="124">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="U32" s="124">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="V32" s="125">
+        <v>0.94799999999999995</v>
+      </c>
       <c r="X32" s="18"/>
-      <c r="Y32" s="22"/>
-      <c r="Z32" s="15"/>
-      <c r="AA32" s="25"/>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="16"/>
-      <c r="AD32" s="16"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="83"/>
-      <c r="AG32" s="83"/>
-      <c r="AH32" s="83"/>
-      <c r="AI32" s="83"/>
-      <c r="AJ32" s="83"/>
-      <c r="AK32" s="93"/>
-      <c r="AL32" s="93"/>
-      <c r="AM32" s="93"/>
-      <c r="AN32" s="87"/>
-      <c r="AO32" s="94"/>
-      <c r="AP32" s="94"/>
-      <c r="AQ32" s="94"/>
-      <c r="AR32" s="83"/>
-    </row>
-    <row r="33" spans="24:44" x14ac:dyDescent="0.2">
+      <c r="Y32" s="92"/>
+      <c r="Z32" s="92"/>
+      <c r="AA32" s="92"/>
+      <c r="AB32" s="92"/>
+      <c r="AC32" s="92"/>
+      <c r="AD32" s="92"/>
+      <c r="AE32" s="92"/>
+      <c r="AF32" s="99"/>
+      <c r="AG32" s="99"/>
+      <c r="AH32" s="99"/>
+      <c r="AI32" s="89"/>
+      <c r="AJ32" s="94"/>
+      <c r="AK32" s="94"/>
+      <c r="AL32" s="94"/>
+      <c r="AM32" s="18"/>
+      <c r="AN32" s="18"/>
+      <c r="AO32" s="18"/>
+      <c r="AP32" s="13"/>
+      <c r="AQ32" s="25"/>
+      <c r="AR32" s="25"/>
+      <c r="AS32" s="25"/>
+    </row>
+    <row r="33" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P33" s="66"/>
+      <c r="Q33" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="R33" s="126"/>
+      <c r="S33" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="T33" s="128">
+        <v>0.495</v>
+      </c>
+      <c r="U33" s="128">
+        <v>0.495</v>
+      </c>
+      <c r="V33" s="129">
+        <v>0.63300000000000001</v>
+      </c>
       <c r="X33" s="18"/>
-      <c r="Y33" s="22"/>
-      <c r="Z33" s="15"/>
-      <c r="AA33" s="25"/>
-      <c r="AB33" s="16"/>
-      <c r="AC33" s="16"/>
-      <c r="AD33" s="16"/>
-      <c r="AE33" s="16"/>
-      <c r="AF33" s="83"/>
-      <c r="AG33" s="83"/>
-      <c r="AH33" s="83"/>
-      <c r="AI33" s="83"/>
-      <c r="AJ33" s="83"/>
-      <c r="AK33" s="93"/>
-      <c r="AL33" s="93"/>
-      <c r="AM33" s="93"/>
-      <c r="AN33" s="83"/>
-      <c r="AO33" s="94"/>
-      <c r="AP33" s="94"/>
-      <c r="AQ33" s="94"/>
-      <c r="AR33" s="83"/>
-    </row>
-    <row r="34" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y33" s="96"/>
+      <c r="Z33" s="89"/>
+      <c r="AA33" s="90"/>
+      <c r="AB33" s="90"/>
+      <c r="AC33" s="90"/>
+      <c r="AD33" s="90"/>
+      <c r="AE33" s="90"/>
+      <c r="AF33" s="99"/>
+      <c r="AG33" s="99"/>
+      <c r="AH33" s="99"/>
+      <c r="AI33" s="96"/>
+      <c r="AJ33" s="94"/>
+      <c r="AK33" s="94"/>
+      <c r="AL33" s="94"/>
+      <c r="AM33" s="18"/>
+      <c r="AN33" s="18"/>
+      <c r="AO33" s="18"/>
+      <c r="AQ33" s="25"/>
+      <c r="AR33" s="25"/>
+      <c r="AS33" s="25"/>
+    </row>
+    <row r="34" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P34" s="66"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="S34" s="114" t="s">
+        <v>20</v>
+      </c>
+      <c r="T34" s="121">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="U34" s="121">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="V34" s="122">
+        <v>0.68200000000000005</v>
+      </c>
       <c r="X34" s="18"/>
-      <c r="Y34" s="22"/>
-      <c r="Z34" s="15"/>
-      <c r="AA34" s="25"/>
-      <c r="AB34" s="16"/>
-      <c r="AC34" s="16"/>
-      <c r="AD34" s="16"/>
-      <c r="AE34" s="16"/>
-      <c r="AF34" s="83"/>
-      <c r="AG34" s="83"/>
-      <c r="AH34" s="83"/>
-      <c r="AI34" s="83"/>
-      <c r="AJ34" s="83"/>
-      <c r="AK34" s="93"/>
-      <c r="AL34" s="93"/>
-      <c r="AM34" s="95"/>
-      <c r="AN34" s="83"/>
-      <c r="AO34" s="84"/>
-      <c r="AP34" s="84"/>
-      <c r="AQ34" s="84"/>
-      <c r="AR34" s="83"/>
-    </row>
-    <row r="35" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y34" s="100"/>
+      <c r="Z34" s="99"/>
+      <c r="AA34" s="93"/>
+      <c r="AB34" s="90"/>
+      <c r="AC34" s="90"/>
+      <c r="AD34" s="90"/>
+      <c r="AE34" s="90"/>
+      <c r="AF34" s="99"/>
+      <c r="AG34" s="99"/>
+      <c r="AH34" s="98"/>
+      <c r="AI34" s="96"/>
+      <c r="AJ34" s="107"/>
+      <c r="AK34" s="107"/>
+      <c r="AL34" s="107"/>
+      <c r="AM34" s="18"/>
+      <c r="AN34" s="18"/>
+      <c r="AO34" s="18"/>
+      <c r="AQ34" s="25"/>
+      <c r="AR34" s="25"/>
+      <c r="AS34" s="25"/>
+    </row>
+    <row r="35" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="66"/>
+      <c r="S35" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="T35" s="107">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="U35" s="107">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="V35" s="31">
+        <v>0.67900000000000005</v>
+      </c>
       <c r="X35" s="18"/>
-      <c r="Y35" s="22"/>
-      <c r="Z35" s="15"/>
-      <c r="AA35" s="25"/>
-      <c r="AB35" s="16"/>
-      <c r="AC35" s="16"/>
-      <c r="AD35" s="16"/>
-      <c r="AE35" s="16"/>
-      <c r="AF35" s="83"/>
-      <c r="AG35" s="83"/>
-      <c r="AH35" s="83"/>
-      <c r="AI35" s="83"/>
-      <c r="AJ35" s="83"/>
-      <c r="AK35" s="93"/>
-      <c r="AL35" s="93"/>
-      <c r="AM35" s="93"/>
-      <c r="AN35" s="83"/>
-      <c r="AO35" s="84"/>
-      <c r="AP35" s="84"/>
-      <c r="AQ35" s="84"/>
-      <c r="AR35" s="83"/>
-    </row>
-    <row r="36" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y35" s="99"/>
+      <c r="Z35" s="99"/>
+      <c r="AA35" s="93"/>
+      <c r="AB35" s="90"/>
+      <c r="AC35" s="90"/>
+      <c r="AD35" s="90"/>
+      <c r="AE35" s="90"/>
+      <c r="AF35" s="99"/>
+      <c r="AG35" s="99"/>
+      <c r="AH35" s="99"/>
+      <c r="AI35" s="96"/>
+      <c r="AJ35" s="107"/>
+      <c r="AK35" s="107"/>
+      <c r="AL35" s="107"/>
+      <c r="AM35" s="18"/>
+      <c r="AN35" s="18"/>
+      <c r="AO35" s="18"/>
+      <c r="AQ35" s="25"/>
+      <c r="AR35" s="25"/>
+      <c r="AS35" s="25"/>
+    </row>
+    <row r="36" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P36" s="66"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="66"/>
+      <c r="S36" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="T36" s="107">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="U36" s="107">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="V36" s="31">
+        <v>0.66300000000000003</v>
+      </c>
       <c r="X36" s="18"/>
-      <c r="Y36" s="22"/>
-      <c r="Z36" s="15"/>
-      <c r="AA36" s="25"/>
-      <c r="AB36" s="16"/>
-      <c r="AC36" s="16"/>
-      <c r="AD36" s="16"/>
-      <c r="AE36" s="24"/>
-      <c r="AF36" s="83"/>
-      <c r="AG36" s="83"/>
-      <c r="AH36" s="83"/>
-      <c r="AI36" s="83"/>
-      <c r="AJ36" s="83"/>
-      <c r="AK36" s="93"/>
-      <c r="AL36" s="93"/>
-      <c r="AM36" s="93"/>
-      <c r="AN36" s="83"/>
-      <c r="AO36" s="84"/>
-      <c r="AP36" s="84"/>
-      <c r="AQ36" s="84"/>
-      <c r="AR36" s="83"/>
-    </row>
-    <row r="37" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y36" s="99"/>
+      <c r="Z36" s="92"/>
+      <c r="AA36" s="93"/>
+      <c r="AB36" s="94"/>
+      <c r="AC36" s="95"/>
+      <c r="AD36" s="95"/>
+      <c r="AE36" s="95"/>
+      <c r="AF36" s="99"/>
+      <c r="AG36" s="99"/>
+      <c r="AH36" s="99"/>
+      <c r="AI36" s="96"/>
+      <c r="AJ36" s="107"/>
+      <c r="AK36" s="107"/>
+      <c r="AL36" s="107"/>
+      <c r="AM36" s="18"/>
+      <c r="AN36" s="18"/>
+      <c r="AO36" s="14"/>
+      <c r="AQ36" s="17"/>
+      <c r="AR36" s="17"/>
+      <c r="AS36" s="17"/>
+    </row>
+    <row r="37" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P37" s="66"/>
+      <c r="Q37" s="66"/>
+      <c r="R37" s="109"/>
+      <c r="S37" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="T37" s="124" t="s">
+        <v>58</v>
+      </c>
+      <c r="U37" s="124">
+        <v>0.52</v>
+      </c>
+      <c r="V37" s="125">
+        <v>0.66300000000000003</v>
+      </c>
       <c r="X37" s="18"/>
-      <c r="Y37" s="22"/>
-      <c r="Z37" s="15"/>
-      <c r="AA37" s="25"/>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="16"/>
-      <c r="AD37" s="16"/>
-      <c r="AE37" s="24"/>
-      <c r="AF37" s="83"/>
-      <c r="AG37" s="83"/>
-      <c r="AH37" s="83"/>
-      <c r="AI37" s="83"/>
-      <c r="AJ37" s="83"/>
-      <c r="AK37" s="93"/>
-      <c r="AL37" s="93"/>
-      <c r="AM37" s="93"/>
-      <c r="AN37" s="83"/>
-      <c r="AO37" s="84"/>
-      <c r="AP37" s="84"/>
-      <c r="AQ37" s="84"/>
-      <c r="AR37" s="83"/>
-    </row>
-    <row r="38" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y37" s="99"/>
+      <c r="Z37" s="92"/>
+      <c r="AA37" s="93"/>
+      <c r="AB37" s="94"/>
+      <c r="AC37" s="95"/>
+      <c r="AD37" s="95"/>
+      <c r="AE37" s="95"/>
+      <c r="AF37" s="99"/>
+      <c r="AG37" s="99"/>
+      <c r="AH37" s="99"/>
+      <c r="AI37" s="96"/>
+      <c r="AJ37" s="107"/>
+      <c r="AK37" s="107"/>
+      <c r="AL37" s="107"/>
+      <c r="AM37" s="18"/>
+      <c r="AN37" s="18"/>
+      <c r="AO37" s="18"/>
+      <c r="AQ37" s="17"/>
+      <c r="AR37" s="17"/>
+      <c r="AS37" s="17"/>
+    </row>
+    <row r="38" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P38" s="66"/>
+      <c r="Q38" s="66"/>
+      <c r="R38" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="S38" s="96" t="s">
+        <v>20</v>
+      </c>
+      <c r="T38" s="107">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="U38" s="107">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="V38" s="31">
+        <v>0.93600000000000005</v>
+      </c>
       <c r="X38" s="18"/>
-      <c r="Y38" s="22"/>
-      <c r="Z38" s="15"/>
-      <c r="AA38" s="25"/>
-      <c r="AB38" s="16"/>
-      <c r="AC38" s="16"/>
-      <c r="AD38" s="16"/>
-      <c r="AE38" s="16"/>
-      <c r="AF38" s="83"/>
-      <c r="AG38" s="83"/>
-      <c r="AH38" s="83"/>
-      <c r="AI38" s="83"/>
-      <c r="AJ38" s="83"/>
-      <c r="AK38" s="93"/>
-      <c r="AL38" s="93"/>
-      <c r="AM38" s="93"/>
-      <c r="AN38" s="83"/>
-      <c r="AO38" s="84"/>
-      <c r="AP38" s="84"/>
-      <c r="AQ38" s="84"/>
-      <c r="AR38" s="83"/>
-    </row>
-    <row r="39" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y38" s="99"/>
+      <c r="Z38" s="92"/>
+      <c r="AA38" s="93"/>
+      <c r="AB38" s="94"/>
+      <c r="AC38" s="95"/>
+      <c r="AD38" s="95"/>
+      <c r="AE38" s="95"/>
+      <c r="AF38" s="99"/>
+      <c r="AG38" s="99"/>
+      <c r="AH38" s="99"/>
+      <c r="AI38" s="96"/>
+      <c r="AJ38" s="107"/>
+      <c r="AK38" s="107"/>
+      <c r="AL38" s="107"/>
+      <c r="AM38" s="18"/>
+      <c r="AN38" s="18"/>
+      <c r="AO38" s="18"/>
+      <c r="AQ38" s="17"/>
+      <c r="AR38" s="17"/>
+      <c r="AS38" s="17"/>
+    </row>
+    <row r="39" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P39" s="66"/>
+      <c r="Q39" s="66"/>
+      <c r="R39" s="66"/>
+      <c r="S39" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T39" s="17">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="U39" s="17">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="V39" s="31">
+        <v>0.94499999999999995</v>
+      </c>
       <c r="X39" s="18"/>
-      <c r="Y39" s="22"/>
-      <c r="Z39" s="15"/>
-      <c r="AA39" s="25"/>
-      <c r="AB39" s="16"/>
-      <c r="AC39" s="16"/>
-      <c r="AD39" s="16"/>
-      <c r="AE39" s="24"/>
-      <c r="AF39" s="83"/>
-      <c r="AG39" s="83"/>
-      <c r="AH39" s="83"/>
-      <c r="AI39" s="83"/>
-      <c r="AJ39" s="83"/>
-      <c r="AK39" s="93"/>
-      <c r="AL39" s="93"/>
-      <c r="AM39" s="93"/>
-      <c r="AN39" s="83"/>
-      <c r="AO39" s="84"/>
-      <c r="AP39" s="84"/>
-      <c r="AQ39" s="84"/>
-      <c r="AR39" s="83"/>
-    </row>
-    <row r="40" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y39" s="99"/>
+      <c r="Z39" s="92"/>
+      <c r="AA39" s="93"/>
+      <c r="AB39" s="94"/>
+      <c r="AC39" s="95"/>
+      <c r="AD39" s="95"/>
+      <c r="AE39" s="95"/>
+      <c r="AF39" s="99"/>
+      <c r="AG39" s="99"/>
+      <c r="AH39" s="99"/>
+      <c r="AI39" s="96"/>
+      <c r="AJ39" s="107"/>
+      <c r="AK39" s="107"/>
+      <c r="AL39" s="107"/>
+      <c r="AM39" s="18"/>
+      <c r="AN39" s="18"/>
+      <c r="AO39" s="18"/>
+      <c r="AQ39" s="17"/>
+      <c r="AR39" s="17"/>
+      <c r="AS39" s="17"/>
+    </row>
+    <row r="40" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="P40" s="66"/>
+      <c r="Q40" s="66"/>
+      <c r="R40" s="66"/>
+      <c r="S40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T40" s="17">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="U40" s="17">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="V40" s="31">
+        <v>0.94099999999999995</v>
+      </c>
       <c r="X40" s="18"/>
-      <c r="Y40" s="22"/>
-      <c r="Z40" s="15"/>
-      <c r="AA40" s="25"/>
-      <c r="AB40" s="16"/>
-      <c r="AC40" s="16"/>
-      <c r="AD40" s="16"/>
-      <c r="AE40" s="16"/>
-      <c r="AF40" s="83"/>
-      <c r="AG40" s="83"/>
-      <c r="AH40" s="83"/>
-      <c r="AI40" s="83"/>
-      <c r="AJ40" s="83"/>
-      <c r="AK40" s="93"/>
-      <c r="AL40" s="93"/>
-      <c r="AM40" s="93"/>
-      <c r="AN40" s="83"/>
-      <c r="AO40" s="84"/>
-      <c r="AP40" s="84"/>
-      <c r="AQ40" s="84"/>
-      <c r="AR40" s="83"/>
-    </row>
-    <row r="41" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y40" s="99"/>
+      <c r="Z40" s="92"/>
+      <c r="AA40" s="93"/>
+      <c r="AB40" s="94"/>
+      <c r="AC40" s="95"/>
+      <c r="AD40" s="95"/>
+      <c r="AE40" s="95"/>
+      <c r="AF40" s="99"/>
+      <c r="AG40" s="99"/>
+      <c r="AH40" s="99"/>
+      <c r="AI40" s="96"/>
+      <c r="AJ40" s="107"/>
+      <c r="AK40" s="107"/>
+      <c r="AL40" s="107"/>
+      <c r="AM40" s="18"/>
+      <c r="AN40" s="18"/>
+      <c r="AO40" s="18"/>
+      <c r="AQ40" s="17"/>
+      <c r="AR40" s="17"/>
+      <c r="AS40" s="17"/>
+    </row>
+    <row r="41" spans="16:45" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P41" s="67"/>
+      <c r="Q41" s="67"/>
+      <c r="R41" s="67"/>
+      <c r="S41" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="T41" s="33">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="U41" s="33">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="V41" s="34">
+        <v>0.94499999999999995</v>
+      </c>
       <c r="X41" s="18"/>
-      <c r="Y41" s="22"/>
-      <c r="Z41" s="15"/>
-      <c r="AA41" s="25"/>
-      <c r="AB41" s="16"/>
-      <c r="AC41" s="16"/>
-      <c r="AD41" s="16"/>
-      <c r="AE41" s="16"/>
-      <c r="AF41" s="83"/>
-      <c r="AG41" s="83"/>
-      <c r="AH41" s="83"/>
-      <c r="AI41" s="83"/>
-      <c r="AJ41" s="83"/>
-      <c r="AK41" s="93"/>
-      <c r="AL41" s="93"/>
-      <c r="AM41" s="93"/>
-      <c r="AN41" s="83"/>
-      <c r="AO41" s="84"/>
-      <c r="AP41" s="84"/>
-      <c r="AQ41" s="84"/>
-      <c r="AR41" s="83"/>
-    </row>
-    <row r="42" spans="24:44" x14ac:dyDescent="0.25">
+      <c r="Y41" s="99"/>
+      <c r="Z41" s="92"/>
+      <c r="AA41" s="93"/>
+      <c r="AB41" s="94"/>
+      <c r="AC41" s="95"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="95"/>
+      <c r="AF41" s="99"/>
+      <c r="AG41" s="99"/>
+      <c r="AH41" s="99"/>
+      <c r="AI41" s="96"/>
+      <c r="AJ41" s="107"/>
+      <c r="AK41" s="107"/>
+      <c r="AL41" s="107"/>
+      <c r="AM41" s="18"/>
+      <c r="AN41" s="18"/>
+      <c r="AO41" s="18"/>
+      <c r="AQ41" s="17"/>
+      <c r="AR41" s="17"/>
+      <c r="AS41" s="17"/>
+    </row>
+    <row r="42" spans="16:45" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="X42" s="18"/>
-      <c r="Y42" s="22"/>
-      <c r="Z42" s="15"/>
-      <c r="AA42" s="25"/>
-      <c r="AB42" s="16"/>
-      <c r="AC42" s="16"/>
-      <c r="AD42" s="16"/>
-      <c r="AE42" s="16"/>
-      <c r="AF42" s="83"/>
-      <c r="AG42" s="83"/>
-      <c r="AH42" s="83"/>
-      <c r="AI42" s="83"/>
-      <c r="AJ42" s="83"/>
-      <c r="AK42" s="93"/>
-      <c r="AL42" s="93"/>
-      <c r="AM42" s="93"/>
-      <c r="AN42" s="83"/>
-      <c r="AO42" s="84"/>
-      <c r="AP42" s="84"/>
-      <c r="AQ42" s="84"/>
-      <c r="AR42" s="83"/>
-    </row>
-    <row r="43" spans="24:44" x14ac:dyDescent="0.25">
-      <c r="Y43" s="35"/>
-      <c r="Z43" s="35"/>
-      <c r="AF43" s="83"/>
-      <c r="AG43" s="83"/>
-      <c r="AH43" s="83"/>
-      <c r="AI43" s="83"/>
-      <c r="AJ43" s="83"/>
-      <c r="AK43" s="93"/>
-      <c r="AL43" s="93"/>
-      <c r="AM43" s="95"/>
-      <c r="AN43" s="83"/>
-      <c r="AO43" s="84"/>
-      <c r="AP43" s="84"/>
-      <c r="AQ43" s="84"/>
-      <c r="AR43" s="83"/>
-    </row>
-    <row r="44" spans="24:44" x14ac:dyDescent="0.25">
-      <c r="Y44" s="36"/>
-      <c r="Z44" s="35"/>
-      <c r="AA44" s="16"/>
-      <c r="AB44" s="24"/>
-      <c r="AC44" s="24"/>
-      <c r="AD44" s="24"/>
-      <c r="AF44" s="83"/>
-      <c r="AG44" s="83"/>
-      <c r="AH44" s="83"/>
-      <c r="AI44" s="83"/>
-      <c r="AJ44" s="83"/>
-      <c r="AK44" s="93"/>
-      <c r="AL44" s="93"/>
-      <c r="AM44" s="93"/>
-      <c r="AN44" s="83"/>
-      <c r="AO44" s="84"/>
-      <c r="AP44" s="84"/>
-      <c r="AQ44" s="84"/>
-      <c r="AR44" s="83"/>
-    </row>
-    <row r="45" spans="24:44" x14ac:dyDescent="0.25">
-      <c r="Y45" s="35"/>
-      <c r="Z45" s="35"/>
-      <c r="AF45" s="83"/>
-      <c r="AG45" s="83"/>
-      <c r="AH45" s="83"/>
-      <c r="AI45" s="83"/>
-      <c r="AJ45" s="83"/>
-      <c r="AK45" s="93"/>
-      <c r="AL45" s="93"/>
-      <c r="AM45" s="93"/>
-      <c r="AN45" s="83"/>
-      <c r="AO45" s="84"/>
-      <c r="AP45" s="84"/>
-      <c r="AQ45" s="84"/>
-      <c r="AR45" s="83"/>
-    </row>
-    <row r="46" spans="24:44" x14ac:dyDescent="0.25">
-      <c r="Y46" s="35"/>
-      <c r="Z46" s="35"/>
-      <c r="AF46" s="83"/>
-      <c r="AG46" s="83"/>
-      <c r="AH46" s="83"/>
-      <c r="AI46" s="83"/>
-      <c r="AJ46" s="83"/>
-      <c r="AK46" s="93"/>
-      <c r="AL46" s="93"/>
-      <c r="AM46" s="93"/>
-      <c r="AN46" s="83"/>
-      <c r="AO46" s="84"/>
-      <c r="AP46" s="84"/>
-      <c r="AQ46" s="84"/>
-      <c r="AR46" s="83"/>
-    </row>
-    <row r="47" spans="24:44" x14ac:dyDescent="0.25">
-      <c r="AF47" s="83"/>
-      <c r="AG47" s="83"/>
-      <c r="AH47" s="83"/>
-      <c r="AI47" s="83"/>
-      <c r="AJ47" s="83"/>
-      <c r="AK47" s="93"/>
-      <c r="AL47" s="93"/>
-      <c r="AM47" s="93"/>
-      <c r="AN47" s="83"/>
-      <c r="AO47" s="84"/>
-      <c r="AP47" s="84"/>
-      <c r="AQ47" s="84"/>
-      <c r="AR47" s="83"/>
-    </row>
-    <row r="48" spans="24:44" x14ac:dyDescent="0.25">
-      <c r="AF48" s="83"/>
-      <c r="AG48" s="83"/>
-      <c r="AH48" s="83"/>
-      <c r="AI48" s="83"/>
-      <c r="AJ48" s="83"/>
-      <c r="AK48" s="93"/>
-      <c r="AL48" s="93"/>
-      <c r="AM48" s="93"/>
-      <c r="AN48" s="83"/>
-      <c r="AO48" s="84"/>
-      <c r="AP48" s="84"/>
-      <c r="AQ48" s="84"/>
-      <c r="AR48" s="83"/>
-    </row>
-    <row r="49" spans="32:44" x14ac:dyDescent="0.25">
-      <c r="AF49" s="83"/>
-      <c r="AG49" s="83"/>
-      <c r="AH49" s="83"/>
-      <c r="AI49" s="83"/>
-      <c r="AJ49" s="83"/>
-      <c r="AK49" s="93"/>
-      <c r="AL49" s="93"/>
-      <c r="AM49" s="93"/>
-      <c r="AN49" s="83"/>
-      <c r="AO49" s="84"/>
-      <c r="AP49" s="84"/>
-      <c r="AQ49" s="84"/>
-      <c r="AR49" s="83"/>
-    </row>
-    <row r="50" spans="32:44" x14ac:dyDescent="0.25">
-      <c r="AF50" s="83"/>
-      <c r="AG50" s="83"/>
-      <c r="AH50" s="83"/>
-      <c r="AI50" s="83"/>
-      <c r="AJ50" s="83"/>
-      <c r="AK50" s="93"/>
-      <c r="AL50" s="93"/>
-      <c r="AM50" s="93"/>
-      <c r="AN50" s="83"/>
-      <c r="AO50" s="84"/>
-      <c r="AP50" s="84"/>
-      <c r="AQ50" s="84"/>
-      <c r="AR50" s="83"/>
-    </row>
-    <row r="51" spans="32:44" x14ac:dyDescent="0.25">
-      <c r="AF51" s="83"/>
-      <c r="AG51" s="83"/>
-      <c r="AH51" s="83"/>
-      <c r="AI51" s="83"/>
-      <c r="AJ51" s="83"/>
-      <c r="AK51" s="93"/>
-      <c r="AL51" s="93"/>
-      <c r="AM51" s="93"/>
-      <c r="AN51" s="83"/>
-      <c r="AO51" s="84"/>
-      <c r="AP51" s="84"/>
-      <c r="AQ51" s="84"/>
-      <c r="AR51" s="83"/>
-    </row>
-    <row r="52" spans="32:44" x14ac:dyDescent="0.2">
-      <c r="AF52" s="83"/>
-      <c r="AG52" s="83"/>
-      <c r="AH52" s="83"/>
-      <c r="AI52" s="83"/>
-      <c r="AJ52" s="83"/>
-      <c r="AK52" s="83"/>
-      <c r="AL52" s="83"/>
-      <c r="AM52" s="83"/>
-      <c r="AN52" s="83"/>
-      <c r="AO52" s="83"/>
-      <c r="AP52" s="83"/>
-      <c r="AQ52" s="83"/>
-      <c r="AR52" s="83"/>
-    </row>
-    <row r="53" spans="32:44" x14ac:dyDescent="0.2">
-      <c r="AF53" s="83"/>
-      <c r="AG53" s="83"/>
-      <c r="AH53" s="83"/>
-      <c r="AI53" s="83"/>
-      <c r="AJ53" s="83"/>
-      <c r="AK53" s="83"/>
-      <c r="AL53" s="83"/>
-      <c r="AM53" s="83"/>
-      <c r="AN53" s="83"/>
-      <c r="AO53" s="83"/>
-      <c r="AP53" s="83"/>
-      <c r="AQ53" s="83"/>
-      <c r="AR53" s="83"/>
+      <c r="Y42" s="99"/>
+      <c r="Z42" s="92"/>
+      <c r="AA42" s="93"/>
+      <c r="AB42" s="94"/>
+      <c r="AC42" s="95"/>
+      <c r="AD42" s="95"/>
+      <c r="AE42" s="95"/>
+      <c r="AF42" s="99"/>
+      <c r="AG42" s="99"/>
+      <c r="AH42" s="99"/>
+      <c r="AI42" s="96"/>
+      <c r="AJ42" s="107"/>
+      <c r="AK42" s="107"/>
+      <c r="AL42" s="107"/>
+      <c r="AM42" s="18"/>
+      <c r="AN42" s="18"/>
+      <c r="AO42" s="18"/>
+      <c r="AQ42" s="17"/>
+      <c r="AR42" s="17"/>
+      <c r="AS42" s="17"/>
+    </row>
+    <row r="43" spans="16:45" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X43" s="18"/>
+      <c r="Y43" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z43" s="71"/>
+      <c r="AA43" s="71"/>
+      <c r="AB43" s="71"/>
+      <c r="AC43" s="71"/>
+      <c r="AD43" s="71"/>
+      <c r="AE43" s="71"/>
+      <c r="AF43" s="71"/>
+      <c r="AG43" s="71"/>
+      <c r="AH43" s="72"/>
+      <c r="AI43" s="96"/>
+      <c r="AJ43" s="107"/>
+      <c r="AK43" s="107"/>
+      <c r="AL43" s="107"/>
+      <c r="AM43" s="18"/>
+      <c r="AN43" s="18"/>
+      <c r="AO43" s="18"/>
+      <c r="AQ43" s="17"/>
+      <c r="AR43" s="17"/>
+      <c r="AS43" s="17"/>
+    </row>
+    <row r="44" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="X44" s="18"/>
+      <c r="Y44" s="37"/>
+      <c r="Z44" s="38"/>
+      <c r="AA44" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB44" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC44" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD44" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE44" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG44" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH44" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI44" s="96"/>
+      <c r="AJ44" s="107"/>
+      <c r="AK44" s="107"/>
+      <c r="AL44" s="107"/>
+      <c r="AM44" s="18"/>
+      <c r="AN44" s="18"/>
+      <c r="AO44" s="18"/>
+      <c r="AQ44" s="17"/>
+      <c r="AR44" s="17"/>
+      <c r="AS44" s="17"/>
+    </row>
+    <row r="45" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="Y45" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z45" s="91">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB45" s="62">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="AC45" s="101"/>
+      <c r="AD45" s="30"/>
+      <c r="AE45" s="16">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AF45" s="30">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="AG45" s="16"/>
+      <c r="AH45" s="30"/>
+      <c r="AI45" s="96"/>
+      <c r="AJ45" s="107"/>
+      <c r="AK45" s="107"/>
+      <c r="AL45" s="107"/>
+      <c r="AM45" s="18"/>
+      <c r="AN45" s="18"/>
+      <c r="AO45" s="14"/>
+      <c r="AQ45" s="17"/>
+      <c r="AR45" s="17"/>
+      <c r="AS45" s="17"/>
+    </row>
+    <row r="46" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="Y46" s="66"/>
+      <c r="Z46" s="91"/>
+      <c r="AA46" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB46" s="62"/>
+      <c r="AC46" s="101"/>
+      <c r="AD46" s="30"/>
+      <c r="AE46" s="16">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="AF46" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AG46" s="16"/>
+      <c r="AH46" s="30"/>
+      <c r="AI46" s="96"/>
+      <c r="AJ46" s="107"/>
+      <c r="AK46" s="107"/>
+      <c r="AL46" s="107"/>
+      <c r="AM46" s="18"/>
+      <c r="AN46" s="18"/>
+      <c r="AO46" s="18"/>
+      <c r="AQ46" s="17"/>
+      <c r="AR46" s="17"/>
+      <c r="AS46" s="17"/>
+    </row>
+    <row r="47" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="Y47" s="66"/>
+      <c r="Z47" s="91">
+        <v>2</v>
+      </c>
+      <c r="AA47" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB47" s="62">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="AC47" s="101"/>
+      <c r="AD47" s="30"/>
+      <c r="AE47" s="16">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AF47" s="30">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AG47" s="16"/>
+      <c r="AH47" s="30"/>
+      <c r="AI47" s="96"/>
+      <c r="AJ47" s="107"/>
+      <c r="AK47" s="107"/>
+      <c r="AL47" s="107"/>
+      <c r="AM47" s="18"/>
+      <c r="AN47" s="18"/>
+      <c r="AO47" s="18"/>
+      <c r="AQ47" s="17"/>
+      <c r="AR47" s="17"/>
+      <c r="AS47" s="17"/>
+    </row>
+    <row r="48" spans="16:45" x14ac:dyDescent="0.25">
+      <c r="Y48" s="66"/>
+      <c r="Z48" s="91"/>
+      <c r="AA48" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB48" s="62"/>
+      <c r="AC48" s="101"/>
+      <c r="AD48" s="30"/>
+      <c r="AE48" s="16">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="AF48" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="30"/>
+      <c r="AI48" s="96"/>
+      <c r="AJ48" s="107"/>
+      <c r="AK48" s="107"/>
+      <c r="AL48" s="107"/>
+      <c r="AM48" s="18"/>
+      <c r="AN48" s="18"/>
+      <c r="AO48" s="18"/>
+      <c r="AQ48" s="17"/>
+      <c r="AR48" s="17"/>
+      <c r="AS48" s="17"/>
+    </row>
+    <row r="49" spans="25:45" x14ac:dyDescent="0.25">
+      <c r="Y49" s="66"/>
+      <c r="Z49" s="91">
+        <v>5</v>
+      </c>
+      <c r="AA49" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB49" s="62">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AC49" s="101"/>
+      <c r="AD49" s="30"/>
+      <c r="AE49" s="16">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AF49" s="30">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AG49" s="16"/>
+      <c r="AH49" s="30"/>
+      <c r="AI49" s="96"/>
+      <c r="AJ49" s="107"/>
+      <c r="AK49" s="107"/>
+      <c r="AL49" s="107"/>
+      <c r="AM49" s="18"/>
+      <c r="AN49" s="18"/>
+      <c r="AO49" s="18"/>
+      <c r="AQ49" s="17"/>
+      <c r="AR49" s="17"/>
+      <c r="AS49" s="17"/>
+    </row>
+    <row r="50" spans="25:45" x14ac:dyDescent="0.25">
+      <c r="Y50" s="66"/>
+      <c r="Z50" s="91"/>
+      <c r="AA50" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB50" s="62"/>
+      <c r="AC50" s="101"/>
+      <c r="AD50" s="30"/>
+      <c r="AE50" s="16">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="AF50" s="30">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="AG50" s="16"/>
+      <c r="AH50" s="30"/>
+      <c r="AI50" s="96"/>
+      <c r="AJ50" s="107"/>
+      <c r="AK50" s="107"/>
+      <c r="AL50" s="107"/>
+      <c r="AM50" s="18"/>
+      <c r="AN50" s="18"/>
+      <c r="AO50" s="18"/>
+      <c r="AQ50" s="17"/>
+      <c r="AR50" s="17"/>
+      <c r="AS50" s="17"/>
+    </row>
+    <row r="51" spans="25:45" x14ac:dyDescent="0.25">
+      <c r="Y51" s="66"/>
+      <c r="Z51" s="91">
+        <v>10</v>
+      </c>
+      <c r="AA51" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB51" s="62">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AC51" s="101"/>
+      <c r="AD51" s="30"/>
+      <c r="AE51" s="16">
+        <v>0.95</v>
+      </c>
+      <c r="AF51" s="30">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AG51" s="16"/>
+      <c r="AH51" s="30"/>
+      <c r="AI51" s="96"/>
+      <c r="AJ51" s="107"/>
+      <c r="AK51" s="107"/>
+      <c r="AL51" s="107"/>
+      <c r="AM51" s="18"/>
+      <c r="AN51" s="18"/>
+      <c r="AO51" s="18"/>
+      <c r="AQ51" s="17"/>
+      <c r="AR51" s="17"/>
+      <c r="AS51" s="17"/>
+    </row>
+    <row r="52" spans="25:45" x14ac:dyDescent="0.25">
+      <c r="Y52" s="66"/>
+      <c r="Z52" s="91"/>
+      <c r="AA52" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB52" s="62"/>
+      <c r="AC52" s="101"/>
+      <c r="AD52" s="30"/>
+      <c r="AE52" s="16">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AF52" s="30">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="AG52" s="16"/>
+      <c r="AH52" s="30"/>
+      <c r="AI52" s="96"/>
+      <c r="AJ52" s="96"/>
+      <c r="AK52" s="96"/>
+      <c r="AL52" s="96"/>
+      <c r="AM52" s="18"/>
+      <c r="AN52" s="18"/>
+      <c r="AO52" s="18"/>
+      <c r="AQ52" s="17"/>
+      <c r="AR52" s="17"/>
+      <c r="AS52" s="17"/>
+    </row>
+    <row r="53" spans="25:45" x14ac:dyDescent="0.25">
+      <c r="Y53" s="66"/>
+      <c r="Z53" s="91">
+        <v>20</v>
+      </c>
+      <c r="AA53" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB53" s="62">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="AC53" s="101"/>
+      <c r="AD53" s="30"/>
+      <c r="AE53" s="16">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AF53" s="30">
+        <v>0.94</v>
+      </c>
+      <c r="AG53" s="16"/>
+      <c r="AH53" s="30"/>
+      <c r="AI53" s="96"/>
+      <c r="AJ53" s="96"/>
+      <c r="AK53" s="96"/>
+      <c r="AL53" s="96"/>
+      <c r="AM53" s="18"/>
+      <c r="AN53" s="18"/>
+      <c r="AO53" s="18"/>
+      <c r="AQ53" s="17"/>
+      <c r="AR53" s="17"/>
+      <c r="AS53" s="17"/>
+    </row>
+    <row r="54" spans="25:45" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Y54" s="67"/>
+      <c r="Z54" s="88"/>
+      <c r="AA54" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB54" s="86"/>
+      <c r="AC54" s="102"/>
+      <c r="AD54" s="40"/>
+      <c r="AE54" s="39">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AF54" s="40">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AG54" s="39"/>
+      <c r="AH54" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="40">
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="Y43:AH43"/>
+    <mergeCell ref="Y45:Y54"/>
+    <mergeCell ref="Z45:Z46"/>
+    <mergeCell ref="AB45:AB46"/>
+    <mergeCell ref="Z47:Z48"/>
+    <mergeCell ref="AB47:AB48"/>
+    <mergeCell ref="Z49:Z50"/>
+    <mergeCell ref="AB49:AB50"/>
+    <mergeCell ref="Z51:Z52"/>
+    <mergeCell ref="AB51:AB52"/>
+    <mergeCell ref="Z53:Z54"/>
+    <mergeCell ref="AB53:AB54"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="P24:P41"/>
+    <mergeCell ref="Q24:Q32"/>
+    <mergeCell ref="R29:R32"/>
+    <mergeCell ref="Q33:Q41"/>
+    <mergeCell ref="R34:R37"/>
+    <mergeCell ref="R38:R41"/>
+    <mergeCell ref="P13:V13"/>
+    <mergeCell ref="P14:S15"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="P16:Q23"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="T17:V17"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="T19:V19"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="AM2:AQ2"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:I3"/>
     <mergeCell ref="R25:R28"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="P2:V2"/>
-    <mergeCell ref="Y2:AF2"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="P3:S4"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="P5:Q10"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="P11:P28"/>
-    <mergeCell ref="Q11:Q19"/>
-    <mergeCell ref="R12:R15"/>
-    <mergeCell ref="R16:R19"/>
-    <mergeCell ref="Q20:Q28"/>
-    <mergeCell ref="R21:R24"/>
-    <mergeCell ref="Y4:Y13"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="AB12:AB13"/>
   </mergeCells>
   <conditionalFormatting sqref="K5:K6 D8:N10 D5:I5 D6:K7">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5404,8 +5869,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB4:AF13">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="AB16:AH16">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5416,8 +5881,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB18:AF18">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="AR36:AR53">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR28:AS30 AS36:AS53 AQ28:AQ53">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB36:AE42">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5428,7 +5917,43 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP34:AP51">
+  <conditionalFormatting sqref="AK34:AK51">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK28:AL30 AL34:AL51 AJ28:AJ51">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U24:U41">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U16:V18 V24:V41 T16:T41">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -5440,8 +5965,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP28:AQ30 AQ34:AQ51 AO28:AO51">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="AB45:AH54">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color theme="2"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U11:U12">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5452,8 +5989,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U11:U28">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="U5:V7 V11:V12 T5:T12">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5464,14 +6001,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U5:V7 V11:V28 T5:T28">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="AB4:AH11">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFFF0000"/>
-        <color rgb="FFFCFCFF"/>
+        <color theme="2"/>
         <color theme="6"/>
       </colorScale>
     </cfRule>

</xml_diff>